<commit_message>
Updated as per discussion with Anadi
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{21C8D0A5-F31B-4008-B7D1-03AE52A3AD06}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{44576A71-BDD6-49A1-A037-B88E6822002B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="279">
   <si>
     <t>S.No.</t>
   </si>
@@ -612,42 +612,6 @@
   </si>
   <si>
     <t>Discussion with GoM/PwC on 24-Oct-18</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mode of login to client, Mode of local duplicate check on client, Mode of officer authentication at end of each registration on client: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Backlog</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Support multifactor authentication using username + password and/or OTP, fingerprint - Iris and Face is a new inclusion as requested by GoM/PwC</t>
-    </r>
   </si>
   <si>
     <t>Resham</t>
@@ -3118,23 +3082,111 @@
   </si>
   <si>
     <t>&lt;22Jan19&gt;
-Not needed by GoM but demoed and hence to be included</t>
+OK</t>
   </si>
   <si>
     <t>&lt;22Jan19&gt;
-OK</t>
+Prioritize GoM req with stubbed config/modularity in v1. Config perspective, the parameter will not be marked and only GoM required modes of login should be the primary focus. If the config is marked, then MOSIP should respond with "Feature not available".
+Scope the other peices (Other modes) in v1+.</t>
   </si>
   <si>
     <t>&lt;22Jan19&gt;
-Need Design and Effort</t>
+Prioritize GoM req with stubbed config/modularity in v1. Scope the other peices in v1+. My problem is with effort estimate, why so much?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;22Jan19&gt;
+Prioritize GoM req with stubbed config/modularity in v1. Scope the other peices in v1+. My problem is with effort estimate, why so much? </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Mode of local duplicate check on client, 
+2. Mode of officer authentication at end of each registration on client: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Backlog</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Support multifactor authentication using username + password and/or OTP, fingerprint - Iris and Face is a new inclusion as requested by GoM/PwC</t>
+    </r>
   </si>
   <si>
     <t>&lt;22Jan19&gt;
-Infra as code is not a change request. It was always a part of design as Kubernets. Refer email from me on the same subject. Shravan to explain.</t>
+Infra as code is not a change request, it was always a part of design as K8. Refer my email on the subject. Shravan to explain.</t>
   </si>
   <si>
     <t>&lt;22Jan19&gt;
-OK. Go as per Sanjay's inputs.</t>
+Discuss Change Desc with Ramesh, Sanjays inputs look good.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+OK. Go as per Sanjay's inputs.
+Correct the change description. Above threshold match for biometric and exact match for demographic data.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+As discussed with Sanjay, there is no change request. Please take it off the list.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+As discussed with Sanjay, there is no change request, exact match is the limited match. Please take it off the list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;22Jan19&gt;
+Biometric image is for v1+. </t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+small time changes. Include in v1. 12 days of PD needed for these! I need justification for estimate.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+If face is in scope of GoM keep it, else for v1+</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+Its an essential part of eKYC security. Should be implemented for v1. Need design and effort estimate.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+Not really needed by GoM, but has been demoed to them. So do it.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+It is really subset of 61, please merge the two. Needs to be implemented for v1.</t>
+  </si>
+  <si>
+    <t>&lt;22Jan19&gt;
+It is in scope of v1. Need design (using modularity principles) and effort estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;22Jan19&gt;
+We need to do it. Need to see design &amp; Effort estimate
+</t>
   </si>
 </sst>
 </file>
@@ -4886,7 +4938,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -5235,12 +5287,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -5257,7 +5308,7 @@
     <col min="11" max="11" width="20.85546875" style="3" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" style="3" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="29" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="15.85546875" style="11" customWidth="1"/>
     <col min="17" max="17" width="15.85546875" style="2" customWidth="1"/>
@@ -5267,7 +5318,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -5313,7 +5364,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J2" s="21" t="s">
         <v>8</v>
@@ -5328,22 +5379,22 @@
         <v>11</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O2" s="21" t="s">
         <v>12</v>
       </c>
       <c r="P2" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q2" s="21" t="s">
         <v>204</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>205</v>
       </c>
       <c r="R2" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5368,7 +5419,9 @@
       <c r="H3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="34" t="s">
+        <v>262</v>
+      </c>
       <c r="J3" s="34">
         <v>1</v>
       </c>
@@ -5385,7 +5438,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P3" s="32"/>
       <c r="Q3" s="32"/>
@@ -5393,7 +5446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="4" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -5418,7 +5471,9 @@
       <c r="H4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="34" t="s">
+        <v>263</v>
+      </c>
       <c r="J4" s="34">
         <v>1</v>
       </c>
@@ -5435,7 +5490,7 @@
         <v>12</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
@@ -5443,7 +5498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="4" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5468,7 +5523,9 @@
       <c r="H5" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="34"/>
+      <c r="I5" s="34" t="s">
+        <v>264</v>
+      </c>
       <c r="J5" s="34">
         <v>1</v>
       </c>
@@ -5485,7 +5542,7 @@
         <v>35</v>
       </c>
       <c r="O5" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P5" s="32"/>
       <c r="Q5" s="32"/>
@@ -5493,7 +5550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="4" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -5535,7 +5592,7 @@
         <v>30</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
@@ -5543,7 +5600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5585,13 +5642,13 @@
         <v>0</v>
       </c>
       <c r="O7" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
       <c r="R7" s="22"/>
     </row>
-    <row r="8" spans="1:18" s="1" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -5633,7 +5690,7 @@
         <v>36</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
@@ -5686,7 +5743,7 @@
       <c r="Q9" s="32"/>
       <c r="R9" s="22"/>
     </row>
-    <row r="10" spans="1:18" s="1" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -5703,10 +5760,10 @@
         <v>31</v>
       </c>
       <c r="F10" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="20" t="s">
         <v>29</v>
@@ -5728,15 +5785,15 @@
         <v>20</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="1" customFormat="1" ht="120" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -5747,19 +5804,19 @@
         <v>43</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34">
@@ -5775,22 +5832,22 @@
         <v>43419</v>
       </c>
       <c r="N11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O11" s="43">
         <v>36</v>
       </c>
       <c r="P11" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q11" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="Q11" s="32" t="s">
-        <v>200</v>
-      </c>
       <c r="R11" s="22" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="1" customFormat="1" ht="126.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="1" customFormat="1" ht="126.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -5801,19 +5858,19 @@
         <v>43</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34">
@@ -5835,16 +5892,16 @@
         <v>54</v>
       </c>
       <c r="P12" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q12" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="Q12" s="32" t="s">
-        <v>200</v>
-      </c>
       <c r="R12" s="22" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -5855,19 +5912,19 @@
         <v>43</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20">
@@ -5883,22 +5940,22 @@
         <v>43419</v>
       </c>
       <c r="N13" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O13" s="43">
         <v>72</v>
       </c>
       <c r="P13" s="63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q13" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R13" s="22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -5909,19 +5966,19 @@
         <v>43</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>54</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>55</v>
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="25">
@@ -5943,16 +6000,16 @@
         <v>0</v>
       </c>
       <c r="P14" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q14" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R14" s="22" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -5963,19 +6020,19 @@
         <v>43</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="34" t="s">
         <v>57</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>58</v>
       </c>
       <c r="I15" s="34"/>
       <c r="J15" s="34">
@@ -5994,40 +6051,40 @@
         <v>10</v>
       </c>
       <c r="O15" s="57" t="s">
+        <v>210</v>
+      </c>
+      <c r="P15" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q15" s="57" t="s">
         <v>211</v>
       </c>
-      <c r="P15" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q15" s="57" t="s">
-        <v>212</v>
-      </c>
       <c r="R15" s="58" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>59</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>60</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>62</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34">
@@ -6048,28 +6105,28 @@
       <c r="Q16" s="32"/>
       <c r="R16" s="22"/>
     </row>
-    <row r="17" spans="1:18" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>59</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>60</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>63</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>64</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34">
@@ -6090,7 +6147,7 @@
       <c r="Q17" s="32"/>
       <c r="R17" s="22"/>
     </row>
-    <row r="18" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -6098,7 +6155,7 @@
         <v>43402</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>15</v>
@@ -6107,13 +6164,13 @@
         <v>31</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="34"/>
       <c r="J18" s="34">
@@ -6132,15 +6189,15 @@
         <v>10</v>
       </c>
       <c r="O18" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -6148,7 +6205,7 @@
         <v>43402</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>15</v>
@@ -6157,13 +6214,13 @@
         <v>31</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="34"/>
       <c r="J19" s="34">
@@ -6182,15 +6239,15 @@
         <v>5</v>
       </c>
       <c r="O19" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
       <c r="R19" s="22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -6198,22 +6255,22 @@
         <v>43402</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15">
@@ -6235,16 +6292,16 @@
         <v>30</v>
       </c>
       <c r="P20" s="65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q20" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R20" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -6252,22 +6309,22 @@
         <v>43402</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="34"/>
       <c r="J21" s="34">
@@ -6288,7 +6345,7 @@
       <c r="Q21" s="32"/>
       <c r="R21" s="22"/>
     </row>
-    <row r="22" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -6296,22 +6353,22 @@
         <v>43402</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="25">
@@ -6332,7 +6389,7 @@
       <c r="Q22" s="32"/>
       <c r="R22" s="22"/>
     </row>
-    <row r="23" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -6340,7 +6397,7 @@
         <v>43402</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>15</v>
@@ -6349,13 +6406,13 @@
         <v>31</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I23" s="34"/>
       <c r="J23" s="34">
@@ -6374,15 +6431,15 @@
         <v>10</v>
       </c>
       <c r="O23" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P23" s="32"/>
       <c r="Q23" s="32"/>
       <c r="R23" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -6390,7 +6447,7 @@
         <v>43418</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>15</v>
@@ -6399,13 +6456,13 @@
         <v>31</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I24" s="34"/>
       <c r="J24" s="15">
@@ -6424,15 +6481,15 @@
         <v>5</v>
       </c>
       <c r="O24" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P24" s="32"/>
       <c r="Q24" s="32"/>
       <c r="R24" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -6440,22 +6497,22 @@
         <v>43418</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I25" s="34"/>
       <c r="J25" s="15">
@@ -6476,7 +6533,7 @@
       <c r="Q25" s="32"/>
       <c r="R25" s="22"/>
     </row>
-    <row r="26" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -6484,34 +6541,34 @@
         <v>43418</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J26" s="15">
         <v>1</v>
       </c>
       <c r="K26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>86</v>
       </c>
       <c r="M26" s="22">
         <v>43419</v>
@@ -6520,13 +6577,13 @@
         <v>30</v>
       </c>
       <c r="O26" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P26" s="32"/>
       <c r="Q26" s="32"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" ht="101.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -6534,32 +6591,32 @@
         <v>43418</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F27" s="48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H27" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I27" s="34"/>
       <c r="J27" s="15">
         <v>1</v>
       </c>
       <c r="K27" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>86</v>
       </c>
       <c r="M27" s="22">
         <v>43419</v>
@@ -6571,16 +6628,16 @@
         <v>30</v>
       </c>
       <c r="P27" s="66" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q27" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="Q27" s="32" t="s">
-        <v>214</v>
-      </c>
       <c r="R27" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -6588,31 +6645,31 @@
         <v>43430</v>
       </c>
       <c r="C28" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="34" t="s">
         <v>90</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>91</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J28" s="34">
         <v>1</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L28" s="34" t="s">
         <v>21</v>
@@ -6624,13 +6681,13 @@
         <v>6</v>
       </c>
       <c r="O28" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P28" s="32"/>
       <c r="Q28" s="32"/>
       <c r="R28" s="34"/>
     </row>
-    <row r="29" spans="1:18" s="8" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" s="8" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6638,7 +6695,7 @@
         <v>43430</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>15</v>
@@ -6647,20 +6704,20 @@
         <v>31</v>
       </c>
       <c r="F29" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>94</v>
       </c>
       <c r="I29" s="34"/>
       <c r="J29" s="34">
         <v>1</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L29" s="34" t="s">
         <v>21</v>
@@ -6672,15 +6729,15 @@
         <v>10</v>
       </c>
       <c r="O29" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P29" s="32"/>
       <c r="Q29" s="32"/>
       <c r="R29" s="34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" s="8" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -6688,7 +6745,7 @@
         <v>43430</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>15</v>
@@ -6697,20 +6754,20 @@
         <v>31</v>
       </c>
       <c r="F30" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="34" t="s">
         <v>96</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>97</v>
       </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34">
         <v>1</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L30" s="34" t="s">
         <v>21</v>
@@ -6722,15 +6779,15 @@
         <v>15</v>
       </c>
       <c r="O30" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P30" s="32"/>
       <c r="Q30" s="32"/>
       <c r="R30" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -6738,7 +6795,7 @@
         <v>43430</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>15</v>
@@ -6747,20 +6804,20 @@
         <v>31</v>
       </c>
       <c r="F31" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="34" t="s">
         <v>99</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>100</v>
       </c>
       <c r="I31" s="34"/>
       <c r="J31" s="34">
         <v>1</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L31" s="34" t="s">
         <v>21</v>
@@ -6772,7 +6829,7 @@
         <v>1</v>
       </c>
       <c r="O31" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P31" s="32"/>
       <c r="Q31" s="32"/>
@@ -6786,7 +6843,7 @@
         <v>43430</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>38</v>
@@ -6795,22 +6852,22 @@
         <v>31</v>
       </c>
       <c r="F32" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="G32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="30" t="s">
-        <v>103</v>
-      </c>
       <c r="I32" s="30" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J32" s="16">
         <v>1</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L32" s="34" t="s">
         <v>21</v>
@@ -6822,12 +6879,12 @@
         <v>0</v>
       </c>
       <c r="O32" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P32" s="32"/>
       <c r="Q32" s="32"/>
       <c r="R32" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
@@ -6838,7 +6895,7 @@
         <v>43430</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="34" t="s">
         <v>38</v>
@@ -6847,22 +6904,22 @@
         <v>31</v>
       </c>
       <c r="F33" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>106</v>
-      </c>
       <c r="I33" s="30" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="J33" s="16">
         <v>1</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L33" s="34" t="s">
         <v>21</v>
@@ -6874,12 +6931,12 @@
         <v>10</v>
       </c>
       <c r="O33" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
       <c r="R33" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="142.5" x14ac:dyDescent="0.25">
@@ -6890,7 +6947,7 @@
         <v>43430</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>38</v>
@@ -6899,20 +6956,22 @@
         <v>31</v>
       </c>
       <c r="F34" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="G34" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="I34" s="34"/>
+      <c r="I34" s="30" t="s">
+        <v>269</v>
+      </c>
       <c r="J34" s="34">
         <v>1</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L34" s="34" t="s">
         <v>21</v>
@@ -6924,12 +6983,12 @@
         <v>0</v>
       </c>
       <c r="O34" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P34" s="32"/>
       <c r="Q34" s="32"/>
       <c r="R34" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
@@ -6940,7 +6999,7 @@
         <v>43430</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="34" t="s">
         <v>38</v>
@@ -6949,20 +7008,22 @@
         <v>31</v>
       </c>
       <c r="F35" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" s="34"/>
+        <v>107</v>
+      </c>
+      <c r="I35" s="30" t="s">
+        <v>270</v>
+      </c>
       <c r="J35" s="34">
         <v>1</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L35" s="34" t="s">
         <v>21</v>
@@ -6974,15 +7035,15 @@
         <v>0</v>
       </c>
       <c r="O35" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P35" s="32"/>
       <c r="Q35" s="32"/>
       <c r="R35" s="34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -6990,31 +7051,31 @@
         <v>43430</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E36" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F36" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="34" t="s">
-        <v>112</v>
-      </c>
       <c r="I36" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J36" s="34">
         <v>2</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L36" s="34" t="s">
         <v>21</v>
@@ -7028,7 +7089,7 @@
       <c r="Q36" s="32"/>
       <c r="R36" s="34"/>
     </row>
-    <row r="37" spans="1:18" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -7036,7 +7097,7 @@
         <v>43430</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>15</v>
@@ -7045,20 +7106,20 @@
         <v>39</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H37" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I37" s="34"/>
       <c r="J37" s="34">
         <v>2</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L37" s="34" t="s">
         <v>21</v>
@@ -7075,7 +7136,7 @@
       <c r="Q37" s="32"/>
       <c r="R37" s="34"/>
     </row>
-    <row r="38" spans="1:18" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -7083,7 +7144,7 @@
         <v>43427</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>15</v>
@@ -7092,20 +7153,20 @@
         <v>39</v>
       </c>
       <c r="F38" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="34" t="s">
         <v>115</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="34" t="s">
-        <v>116</v>
       </c>
       <c r="I38" s="34"/>
       <c r="J38" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L38" s="34" t="s">
         <v>21</v>
@@ -7124,7 +7185,7 @@
       <c r="Q38" s="32"/>
       <c r="R38" s="34"/>
     </row>
-    <row r="39" spans="1:18" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -7132,7 +7193,7 @@
         <v>43427</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>15</v>
@@ -7141,20 +7202,20 @@
         <v>39</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H39" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I39" s="34"/>
       <c r="J39" s="34">
         <v>2</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L39" s="34" t="s">
         <v>21</v>
@@ -7171,7 +7232,7 @@
       <c r="Q39" s="32"/>
       <c r="R39" s="34"/>
     </row>
-    <row r="40" spans="1:18" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -7179,29 +7240,29 @@
         <v>43427</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H40" s="34" t="s">
         <v>118</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" s="34" t="s">
-        <v>119</v>
       </c>
       <c r="I40" s="34"/>
       <c r="J40" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L40" s="34" t="s">
         <v>21</v>
@@ -7216,14 +7277,14 @@
         <v>90</v>
       </c>
       <c r="P40" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q40" s="32"/>
       <c r="R40" s="34" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -7231,29 +7292,29 @@
         <v>43427</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H41" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I41" s="34"/>
       <c r="J41" s="34">
         <v>2</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L41" s="34" t="s">
         <v>21</v>
@@ -7268,10 +7329,10 @@
       <c r="P41" s="32"/>
       <c r="Q41" s="32"/>
       <c r="R41" s="34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="83.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="83.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -7279,29 +7340,29 @@
         <v>43427</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F42" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" s="34" t="s">
         <v>121</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H42" s="34" t="s">
-        <v>122</v>
       </c>
       <c r="I42" s="34"/>
       <c r="J42" s="34">
         <v>1</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L42" s="34" t="s">
         <v>21</v>
@@ -7313,19 +7374,19 @@
         <v>18</v>
       </c>
       <c r="O42" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P42" s="66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q42" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R42" s="34" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -7333,29 +7394,29 @@
         <v>43427</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I43" s="34"/>
       <c r="J43" s="34">
         <v>1</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L43" s="34" t="s">
         <v>21</v>
@@ -7370,16 +7431,16 @@
         <v>30</v>
       </c>
       <c r="P43" s="64" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q43" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="R43" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="Q43" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="R43" s="34" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>45</v>
       </c>
@@ -7387,32 +7448,32 @@
         <v>43427</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E44" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I44" s="34"/>
       <c r="J44" s="34">
         <v>2</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L44" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M44" s="22">
         <v>43452</v>
@@ -7423,7 +7484,7 @@
       <c r="Q44" s="32"/>
       <c r="R44" s="34"/>
     </row>
-    <row r="45" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>46</v>
       </c>
@@ -7431,29 +7492,29 @@
         <v>43427</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34">
         <v>1</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L45" s="34" t="s">
         <v>21</v>
@@ -7468,13 +7529,13 @@
         <v>8</v>
       </c>
       <c r="P45" s="67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q45" s="57" t="s">
+        <v>229</v>
+      </c>
+      <c r="R45" s="20" t="s">
         <v>230</v>
-      </c>
-      <c r="R45" s="20" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="57" x14ac:dyDescent="0.25">
@@ -7485,7 +7546,7 @@
         <v>43427</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D46" s="34" t="s">
         <v>38</v>
@@ -7494,20 +7555,22 @@
         <v>31</v>
       </c>
       <c r="F46" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H46" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="G46" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="I46" s="20"/>
+      <c r="I46" s="30" t="s">
+        <v>271</v>
+      </c>
       <c r="J46" s="34">
         <v>1</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L46" s="34" t="s">
         <v>21</v>
@@ -7519,15 +7582,15 @@
         <v>0</v>
       </c>
       <c r="O46" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P46" s="32"/>
       <c r="Q46" s="32"/>
       <c r="R46" s="34" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>48</v>
       </c>
@@ -7535,7 +7598,7 @@
         <v>43427</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>15</v>
@@ -7544,20 +7607,20 @@
         <v>39</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H47" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I47" s="34"/>
       <c r="J47" s="34">
         <v>2</v>
       </c>
       <c r="K47" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L47" s="34" t="s">
         <v>21</v>
@@ -7574,7 +7637,7 @@
       <c r="Q47" s="32"/>
       <c r="R47" s="34"/>
     </row>
-    <row r="48" spans="1:18" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>49</v>
       </c>
@@ -7582,29 +7645,29 @@
         <v>43427</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H48" s="34" t="s">
         <v>128</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H48" s="34" t="s">
-        <v>129</v>
       </c>
       <c r="I48" s="34"/>
       <c r="J48" s="34">
         <v>1</v>
       </c>
       <c r="K48" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L48" s="34" t="s">
         <v>21</v>
@@ -7618,7 +7681,7 @@
       <c r="Q48" s="32"/>
       <c r="R48" s="34"/>
     </row>
-    <row r="49" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>50</v>
       </c>
@@ -7626,7 +7689,7 @@
         <v>43427</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D49" s="34" t="s">
         <v>15</v>
@@ -7635,20 +7698,20 @@
         <v>31</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I49" s="34"/>
       <c r="J49" s="34">
         <v>1</v>
       </c>
       <c r="K49" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L49" s="34" t="s">
         <v>21</v>
@@ -7660,15 +7723,15 @@
         <v>12</v>
       </c>
       <c r="O49" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P49" s="32"/>
       <c r="Q49" s="32"/>
       <c r="R49" s="34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>51</v>
       </c>
@@ -7676,29 +7739,29 @@
         <v>43427</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E50" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I50" s="34"/>
       <c r="J50" s="34">
         <v>1</v>
       </c>
       <c r="K50" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L50" s="34" t="s">
         <v>21</v>
@@ -7712,7 +7775,7 @@
       <c r="Q50" s="32"/>
       <c r="R50" s="34"/>
     </row>
-    <row r="51" spans="1:18" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>52</v>
       </c>
@@ -7720,7 +7783,7 @@
         <v>43427</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>15</v>
@@ -7729,20 +7792,20 @@
         <v>39</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I51" s="34"/>
       <c r="J51" s="34">
         <v>2</v>
       </c>
       <c r="K51" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L51" s="34" t="s">
         <v>21</v>
@@ -7759,7 +7822,7 @@
       <c r="Q51" s="32"/>
       <c r="R51" s="34"/>
     </row>
-    <row r="52" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>53</v>
       </c>
@@ -7767,7 +7830,7 @@
         <v>43427</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D52" s="34" t="s">
         <v>15</v>
@@ -7776,20 +7839,20 @@
         <v>31</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I52" s="34"/>
       <c r="J52" s="34">
         <v>1</v>
       </c>
       <c r="K52" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L52" s="34" t="s">
         <v>21</v>
@@ -7801,15 +7864,15 @@
         <v>20</v>
       </c>
       <c r="O52" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P52" s="32"/>
       <c r="Q52" s="32"/>
       <c r="R52" s="34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>54</v>
       </c>
@@ -7817,7 +7880,7 @@
         <v>43427</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D53" s="34" t="s">
         <v>15</v>
@@ -7826,20 +7889,20 @@
         <v>31</v>
       </c>
       <c r="F53" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53" s="34" t="s">
         <v>135</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>136</v>
       </c>
       <c r="I53" s="34"/>
       <c r="J53" s="34">
         <v>1</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L53" s="34" t="s">
         <v>21</v>
@@ -7851,15 +7914,15 @@
         <v>40</v>
       </c>
       <c r="O53" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P53" s="32"/>
       <c r="Q53" s="32"/>
       <c r="R53" s="34" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>55</v>
       </c>
@@ -7867,7 +7930,7 @@
         <v>43427</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" s="34" t="s">
         <v>15</v>
@@ -7876,20 +7939,20 @@
         <v>39</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H54" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I54" s="34"/>
       <c r="J54" s="34">
         <v>2</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L54" s="34" t="s">
         <v>21</v>
@@ -7906,7 +7969,7 @@
       <c r="Q54" s="32"/>
       <c r="R54" s="34"/>
     </row>
-    <row r="55" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>56</v>
       </c>
@@ -7914,7 +7977,7 @@
         <v>43427</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="34" t="s">
         <v>15</v>
@@ -7923,20 +7986,20 @@
         <v>39</v>
       </c>
       <c r="F55" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H55" s="34" t="s">
         <v>139</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H55" s="34" t="s">
-        <v>140</v>
       </c>
       <c r="I55" s="34"/>
       <c r="J55" s="34">
         <v>2</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L55" s="34" t="s">
         <v>21</v>
@@ -7953,7 +8016,7 @@
       <c r="Q55" s="32"/>
       <c r="R55" s="34"/>
     </row>
-    <row r="56" spans="1:18" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>57</v>
       </c>
@@ -7961,29 +8024,31 @@
         <v>43432</v>
       </c>
       <c r="C56" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" s="34" t="s">
         <v>141</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>142</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I56" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="I56" s="34" t="s">
+        <v>272</v>
+      </c>
       <c r="J56" s="34">
         <v>1</v>
       </c>
       <c r="K56" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L56" s="34" t="s">
         <v>21</v>
@@ -7995,7 +8060,7 @@
         <v>4</v>
       </c>
       <c r="O56" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P56" s="32"/>
       <c r="Q56" s="32"/>
@@ -8009,7 +8074,7 @@
         <v>43432</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D57" s="34" t="s">
         <v>38</v>
@@ -8018,20 +8083,22 @@
         <v>31</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I57" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>273</v>
+      </c>
       <c r="J57" s="34">
         <v>1</v>
       </c>
       <c r="K57" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L57" s="34" t="s">
         <v>21</v>
@@ -8048,10 +8115,10 @@
       <c r="P57" s="32"/>
       <c r="Q57" s="32"/>
       <c r="R57" s="34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>59</v>
       </c>
@@ -8059,29 +8126,29 @@
         <v>43432</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E58" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H58" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="34">
         <v>1</v>
       </c>
       <c r="K58" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L58" s="34" t="s">
         <v>21</v>
@@ -8096,16 +8163,16 @@
         <v>30</v>
       </c>
       <c r="P58" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q58" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="R58" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="R58" s="34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>60</v>
       </c>
@@ -8113,29 +8180,31 @@
         <v>43432</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E59" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F59" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="G59" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H59" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="I59" s="34"/>
+      <c r="I59" s="34" t="s">
+        <v>261</v>
+      </c>
       <c r="J59" s="34">
         <v>2</v>
       </c>
       <c r="K59" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L59" s="34" t="s">
         <v>21</v>
@@ -8149,7 +8218,7 @@
       <c r="Q59" s="35"/>
       <c r="R59" s="34"/>
     </row>
-    <row r="60" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>61</v>
       </c>
@@ -8157,29 +8226,31 @@
         <v>43432</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D60" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F60" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H60" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="I60" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="J60" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="G60" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H60" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34" t="s">
-        <v>183</v>
-      </c>
       <c r="K60" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L60" s="34" t="s">
         <v>21</v>
@@ -8201,7 +8272,7 @@
         <v>43440</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D61" s="34" t="s">
         <v>38</v>
@@ -8210,23 +8281,25 @@
         <v>31</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H61" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I61" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="I61" s="34" t="s">
+        <v>274</v>
+      </c>
       <c r="J61" s="34">
         <v>1</v>
       </c>
       <c r="K61" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L61" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M61" s="22">
         <v>43452</v>
@@ -8240,10 +8313,10 @@
       <c r="P61" s="5"/>
       <c r="Q61" s="5"/>
       <c r="R61" s="34" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>63</v>
       </c>
@@ -8251,7 +8324,7 @@
         <v>43440</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D62" s="34" t="s">
         <v>15</v>
@@ -8260,20 +8333,20 @@
         <v>31</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H62" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I62" s="34"/>
       <c r="J62" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K62" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L62" s="34" t="s">
         <v>21</v>
@@ -8290,10 +8363,10 @@
       <c r="P62" s="5"/>
       <c r="Q62" s="5"/>
       <c r="R62" s="34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>64</v>
       </c>
@@ -8301,31 +8374,31 @@
         <v>43440</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H63" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I63" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J63" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K63" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L63" s="34" t="s">
         <v>21</v>
@@ -8342,10 +8415,10 @@
       <c r="P63" s="5"/>
       <c r="Q63" s="5"/>
       <c r="R63" s="34" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="228" hidden="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="228" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>65</v>
       </c>
@@ -8353,7 +8426,7 @@
         <v>43446</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D64" s="34" t="s">
         <v>15</v>
@@ -8362,20 +8435,20 @@
         <v>31</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H64" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I64" s="34"/>
       <c r="J64" s="34">
         <v>1</v>
       </c>
       <c r="K64" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L64" s="34" t="s">
         <v>21</v>
@@ -8390,10 +8463,10 @@
       <c r="P64" s="5"/>
       <c r="Q64" s="5"/>
       <c r="R64" s="34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>66</v>
       </c>
@@ -8401,7 +8474,7 @@
         <v>43446</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D65" s="34" t="s">
         <v>15</v>
@@ -8410,20 +8483,20 @@
         <v>31</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H65" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I65" s="34"/>
       <c r="J65" s="34">
         <v>1</v>
       </c>
       <c r="K65" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L65" s="34" t="s">
         <v>21</v>
@@ -8439,7 +8512,7 @@
       <c r="Q65" s="5"/>
       <c r="R65" s="34"/>
     </row>
-    <row r="66" spans="1:20" ht="106.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>67</v>
       </c>
@@ -8447,7 +8520,7 @@
         <v>43451</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D66" s="34" t="s">
         <v>15</v>
@@ -8456,20 +8529,20 @@
         <v>31</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H66" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I66" s="34"/>
       <c r="J66" s="34">
         <v>1</v>
       </c>
       <c r="K66" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L66" s="34" t="s">
         <v>21</v>
@@ -8484,10 +8557,10 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="5"/>
       <c r="R66" s="34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="114" hidden="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="114" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>68</v>
       </c>
@@ -8495,31 +8568,31 @@
         <v>43451</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D67" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H67" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I67" s="34" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="J67" s="34">
         <v>1</v>
       </c>
       <c r="K67" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L67" s="34" t="s">
         <v>21</v>
@@ -8536,12 +8609,12 @@
       <c r="P67" s="5"/>
       <c r="Q67" s="5"/>
       <c r="R67" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S67" s="5"/>
       <c r="T67" s="34"/>
     </row>
-    <row r="68" spans="1:20" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>69</v>
       </c>
@@ -8549,7 +8622,7 @@
         <v>43451</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D68" s="34" t="s">
         <v>15</v>
@@ -8558,20 +8631,20 @@
         <v>31</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H68" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I68" s="34"/>
       <c r="J68" s="34">
         <v>1</v>
       </c>
       <c r="K68" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L68" s="34" t="s">
         <v>21</v>
@@ -8589,7 +8662,7 @@
       <c r="S68" s="41"/>
       <c r="T68" s="30"/>
     </row>
-    <row r="69" spans="1:20" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>70</v>
       </c>
@@ -8597,7 +8670,7 @@
         <v>43454</v>
       </c>
       <c r="C69" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D69" s="30" t="s">
         <v>15</v>
@@ -8606,20 +8679,20 @@
         <v>39</v>
       </c>
       <c r="F69" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H69" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I69" s="30"/>
       <c r="J69" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K69" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L69" s="30" t="s">
         <v>21</v>
@@ -8639,7 +8712,7 @@
       <c r="S69" s="5"/>
       <c r="T69" s="34"/>
     </row>
-    <row r="70" spans="1:20" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>71</v>
       </c>
@@ -8647,29 +8720,29 @@
         <v>43454</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E70" s="30" t="s">
         <v>31</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I70" s="30"/>
       <c r="J70" s="30">
         <v>1</v>
       </c>
       <c r="K70" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L70" s="30" t="s">
         <v>21</v>
@@ -8684,16 +8757,16 @@
         <v>30</v>
       </c>
       <c r="P70" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q70" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="Q70" s="41" t="s">
-        <v>200</v>
-      </c>
       <c r="R70" s="68" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>72</v>
       </c>
@@ -8701,29 +8774,29 @@
         <v>43454</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D71" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E71" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F71" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H71" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I71" s="34"/>
       <c r="J71" s="34">
         <v>1</v>
       </c>
       <c r="K71" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L71" s="34" t="s">
         <v>21</v>
@@ -8738,16 +8811,16 @@
         <v>15</v>
       </c>
       <c r="P71" s="78" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q71" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R71" s="68" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>73</v>
       </c>
@@ -8755,7 +8828,7 @@
         <v>43465</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D72" s="34" t="s">
         <v>15</v>
@@ -8764,23 +8837,23 @@
         <v>31</v>
       </c>
       <c r="F72" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H72" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I72" s="34"/>
       <c r="J72" s="34">
         <v>1</v>
       </c>
       <c r="K72" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L72" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M72" s="22">
         <v>43465</v>
@@ -8793,7 +8866,7 @@
       <c r="S72" s="5"/>
       <c r="T72" s="34"/>
     </row>
-    <row r="73" spans="1:20" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>74</v>
       </c>
@@ -8801,7 +8874,7 @@
         <v>43465</v>
       </c>
       <c r="C73" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D73" s="34" t="s">
         <v>15</v>
@@ -8810,23 +8883,23 @@
         <v>31</v>
       </c>
       <c r="F73" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H73" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I73" s="34"/>
       <c r="J73" s="34">
         <v>1</v>
       </c>
       <c r="K73" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L73" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M73" s="22">
         <v>43465</v>
@@ -8839,7 +8912,7 @@
       <c r="S73" s="5"/>
       <c r="T73" s="34"/>
     </row>
-    <row r="74" spans="1:20" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="57" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>75</v>
       </c>
@@ -8847,7 +8920,7 @@
         <v>43465</v>
       </c>
       <c r="C74" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D74" s="34" t="s">
         <v>15</v>
@@ -8856,23 +8929,23 @@
         <v>31</v>
       </c>
       <c r="F74" s="34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H74" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I74" s="34"/>
       <c r="J74" s="34">
         <v>1</v>
       </c>
       <c r="K74" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L74" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M74" s="22">
         <v>43465</v>
@@ -8885,7 +8958,7 @@
       <c r="S74" s="5"/>
       <c r="T74" s="34"/>
     </row>
-    <row r="75" spans="1:20" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="57" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>76</v>
       </c>
@@ -8893,7 +8966,7 @@
         <v>43465</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D75" s="34" t="s">
         <v>15</v>
@@ -8902,23 +8975,23 @@
         <v>31</v>
       </c>
       <c r="F75" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H75" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I75" s="34"/>
       <c r="J75" s="34">
         <v>1</v>
       </c>
       <c r="K75" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L75" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M75" s="22">
         <v>43465</v>
@@ -8931,7 +9004,7 @@
       <c r="S75" s="77"/>
       <c r="T75" s="34"/>
     </row>
-    <row r="76" spans="1:20" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>77</v>
       </c>
@@ -8939,7 +9012,7 @@
         <v>43465</v>
       </c>
       <c r="C76" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D76" s="34" t="s">
         <v>15</v>
@@ -8948,23 +9021,23 @@
         <v>31</v>
       </c>
       <c r="F76" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H76" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I76" s="34"/>
       <c r="J76" s="34">
         <v>1</v>
       </c>
       <c r="K76" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L76" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M76" s="22">
         <v>43465</v>
@@ -8977,7 +9050,7 @@
       <c r="S76" s="77"/>
       <c r="T76" s="34"/>
     </row>
-    <row r="77" spans="1:20" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="114" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>78</v>
       </c>
@@ -8985,32 +9058,32 @@
         <v>43477</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D77" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E77" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H77" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I77" s="34"/>
       <c r="J77" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K77" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L77" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M77" s="22">
         <v>43477</v>
@@ -9022,16 +9095,16 @@
         <v>0</v>
       </c>
       <c r="P77" s="64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q77" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R77" s="34" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>79</v>
       </c>
@@ -9039,7 +9112,7 @@
         <v>43477</v>
       </c>
       <c r="C78" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D78" s="34" t="s">
         <v>15</v>
@@ -9048,23 +9121,23 @@
         <v>31</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H78" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I78" s="34"/>
       <c r="J78" s="34">
         <v>1</v>
       </c>
       <c r="K78" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L78" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M78" s="22">
         <v>43477</v>
@@ -9075,7 +9148,7 @@
       <c r="Q78" s="5"/>
       <c r="R78" s="34"/>
     </row>
-    <row r="79" spans="1:20" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="57" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>80</v>
       </c>
@@ -9083,7 +9156,7 @@
         <v>43477</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D79" s="34" t="s">
         <v>15</v>
@@ -9092,23 +9165,23 @@
         <v>31</v>
       </c>
       <c r="F79" s="34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H79" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I79" s="34"/>
       <c r="J79" s="34">
         <v>1</v>
       </c>
       <c r="K79" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L79" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M79" s="22">
         <v>43477</v>
@@ -9119,7 +9192,7 @@
       <c r="Q79" s="5"/>
       <c r="R79" s="34"/>
     </row>
-    <row r="80" spans="1:20" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>81</v>
       </c>
@@ -9127,7 +9200,7 @@
         <v>43477</v>
       </c>
       <c r="C80" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D80" s="34" t="s">
         <v>15</v>
@@ -9136,23 +9209,23 @@
         <v>31</v>
       </c>
       <c r="F80" s="34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H80" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I80" s="34"/>
       <c r="J80" s="34">
         <v>1</v>
       </c>
       <c r="K80" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L80" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M80" s="22">
         <v>43477</v>
@@ -9171,7 +9244,7 @@
         <v>43477</v>
       </c>
       <c r="C81" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D81" s="34" t="s">
         <v>38</v>
@@ -9180,23 +9253,25 @@
         <v>31</v>
       </c>
       <c r="F81" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H81" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I81" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="I81" s="34" t="s">
+        <v>276</v>
+      </c>
       <c r="J81" s="34">
         <v>1</v>
       </c>
       <c r="K81" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L81" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M81" s="22">
         <v>43477</v>
@@ -9215,7 +9290,7 @@
         <v>43477</v>
       </c>
       <c r="C82" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D82" s="34" t="s">
         <v>38</v>
@@ -9224,23 +9299,25 @@
         <v>31</v>
       </c>
       <c r="F82" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H82" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I82" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="I82" s="34" t="s">
+        <v>277</v>
+      </c>
       <c r="J82" s="34">
         <v>1</v>
       </c>
       <c r="K82" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L82" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M82" s="22">
         <v>43477</v>
@@ -9251,7 +9328,7 @@
       <c r="Q82" s="5"/>
       <c r="R82" s="34"/>
     </row>
-    <row r="83" spans="1:18" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>84</v>
       </c>
@@ -9259,34 +9336,34 @@
         <v>43477</v>
       </c>
       <c r="C83" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D83" s="34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F83" s="34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H83" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I83" s="34" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="J83" s="34">
         <v>1</v>
       </c>
       <c r="K83" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L83" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M83" s="22">
         <v>43477</v>
@@ -9297,7 +9374,7 @@
       <c r="Q83" s="5"/>
       <c r="R83" s="34"/>
     </row>
-    <row r="84" spans="1:18" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="57" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>85</v>
       </c>
@@ -9305,32 +9382,32 @@
         <v>43477</v>
       </c>
       <c r="C84" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D84" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E84" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F84" s="34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H84" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I84" s="34"/>
       <c r="J84" s="34">
         <v>1</v>
       </c>
       <c r="K84" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L84" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M84" s="22">
         <v>43477</v>
@@ -9341,7 +9418,7 @@
       <c r="Q84" s="5"/>
       <c r="R84" s="34"/>
     </row>
-    <row r="85" spans="1:18" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>86</v>
       </c>
@@ -9349,7 +9426,7 @@
         <v>43486</v>
       </c>
       <c r="C85" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D85" s="34" t="s">
         <v>15</v>
@@ -9358,23 +9435,23 @@
         <v>31</v>
       </c>
       <c r="F85" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H85" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I85" s="34"/>
       <c r="J85" s="34">
         <v>1</v>
       </c>
       <c r="K85" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L85" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M85" s="22">
         <v>43486</v>
@@ -9386,14 +9463,7 @@
       <c r="R85" s="34"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R85" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="DevOps"/>
-        <filter val="ID Authentication"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:R85" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:R1"/>
   </mergeCells>
@@ -9420,7 +9490,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -9430,7 +9500,7 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -9440,17 +9510,17 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -9477,18 +9547,18 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
         <v>171</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="38">
         <v>1</v>
@@ -9510,7 +9580,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="38">
         <v>3</v>
@@ -9521,7 +9591,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="38">
         <v>3</v>
@@ -9543,7 +9613,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="38">
         <v>15</v>
@@ -9554,7 +9624,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="38">
         <v>7</v>
@@ -9565,7 +9635,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="38">
         <v>64</v>
@@ -9593,34 +9663,34 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="69" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1" s="70" t="s">
         <v>240</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="71"/>
       <c r="C2" s="72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="73"/>
       <c r="C3" s="72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="74"/>
       <c r="C4" s="72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="75"/>
       <c r="C5" s="76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -9630,6 +9700,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9801,39 +9903,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9849,28 +9943,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated as per inputs from Reg. Client-Akshaya
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{44576A71-BDD6-49A1-A037-B88E6822002B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C065AD6C-6BFE-4260-9930-C8E88E23283C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="288">
   <si>
     <t>S.No.</t>
   </si>
@@ -3187,6 +3187,54 @@
     <t xml:space="preserve">&lt;22Jan19&gt;
 We need to do it. Need to see design &amp; Effort estimate
 </t>
+  </si>
+  <si>
+    <t>Delete pre-reg packet if not consumed in client after 15 days of appointment date.</t>
+  </si>
+  <si>
+    <t>Vivek/Akshaya</t>
+  </si>
+  <si>
+    <t>Enter Pre-registration ID: Addendum to MOS-1204:
+1. Provide ability to scan the pre-reg ID using a QR code scanner and populate the ID on the registration page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document upload: Addendum to MOS-1214:
+1. Document Categories + Types applicable for an individual are driven by configuration per Applicant Type + Gender + Foreigner/Local.
+2. Applicable documents are always mandatory. There is no optional document.  
+</t>
+  </si>
+  <si>
+    <t>Preview page: Addendum to MOS-1214:
+1. Provide a timer (default 30 sec). User can proceed to the next step only after expiry of the timer.
+2. Preview page should display actual scanned images of fingerprints and irises.
+2. On navigating to Registration Preview &gt; Edit &gt; Modify ‘Biometric Exception’ from ‘On’ to ‘Off’ or ‘Off’ to ‘On': All biometrics previously captured (including photos) should be cleared and fresh captures will need to be made.</t>
+  </si>
+  <si>
+    <t>Acknowledgement page: Addendum to MOS-338:
+Render dummy images of left hand, right hand, thumbs, left iris and right iris. A tick or cross against each finger/Iris should indicate if the respective biometric was captured or was marked as an exception. Show fingerprint quality ranks.</t>
+  </si>
+  <si>
+    <t>UIN Update: Addendum to MOS-1299:
+1. The mandatory biometrics should be configurable. For v1 we will implement the following rules.
+1.1. UIN Update - Adult
+- Update of demographic data only: Capture at least one biometric (fingerprint or iris). More than one can be captured at the operator’s discretion.
+- Update of fingerprints: Capture all ten fingerprints minus any exceptions.
+- Update of irises: Capture both irises minus any exceptions.
+1.2. UIN Update - Child - for the first time after turning 5
+- Capture all ten fingerprints and both irises minus any exceptions.
+- Capture at least one biometric of the parent.
+1.3. UIN Update - Child - before 5 years of age
+- Only demographic data update is allowed. Capture at least one biometric of the parent.
+2. Mandatory fields to be captured and sent in the packet: UIN, List of attributes marked for update, New values of attributes, Full Name, Face photo.</t>
+  </si>
+  <si>
+    <t>Upload Packets: Addendum to MOS-559:
+1. Provide the ability for the Officer to first view packet IDs pending upload and select which ones to upload.</t>
+  </si>
+  <si>
+    <t>Device status:
+Display device status on the header.</t>
   </si>
 </sst>
 </file>
@@ -4938,7 +4986,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -5287,11 +5335,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T85"/>
+  <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:R1"/>
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -5302,7 +5350,7 @@
     <col min="4" max="4" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="71.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="17" customWidth="1"/>
     <col min="8" max="9" width="44.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" style="3" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" style="3" customWidth="1"/>
@@ -9461,6 +9509,270 @@
       <c r="P85" s="35"/>
       <c r="Q85" s="5"/>
       <c r="R85" s="34"/>
+    </row>
+    <row r="86" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <f>1+A85</f>
+        <v>87</v>
+      </c>
+      <c r="B86" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E86" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F86" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="G86" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H86" s="34"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="34"/>
+      <c r="K86" s="34"/>
+      <c r="L86" s="34"/>
+      <c r="M86" s="34"/>
+      <c r="N86" s="33"/>
+      <c r="O86" s="5"/>
+      <c r="P86" s="35"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="34"/>
+    </row>
+    <row r="87" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <f t="shared" ref="A87:A93" si="1">1+A86</f>
+        <v>88</v>
+      </c>
+      <c r="B87" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E87" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F87" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H87" s="34"/>
+      <c r="I87" s="34"/>
+      <c r="J87" s="34"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="34"/>
+      <c r="M87" s="34"/>
+      <c r="N87" s="33"/>
+      <c r="O87" s="5"/>
+      <c r="P87" s="35"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="34"/>
+    </row>
+    <row r="88" spans="1:18" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B88" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F88" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H88" s="34"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="34"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34"/>
+      <c r="M88" s="34"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="5"/>
+      <c r="P88" s="35"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="34"/>
+    </row>
+    <row r="89" spans="1:18" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B89" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F89" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="G89" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H89" s="34"/>
+      <c r="I89" s="34"/>
+      <c r="J89" s="34"/>
+      <c r="K89" s="34"/>
+      <c r="L89" s="34"/>
+      <c r="M89" s="34"/>
+      <c r="N89" s="33"/>
+      <c r="O89" s="5"/>
+      <c r="P89" s="35"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="34"/>
+    </row>
+    <row r="90" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B90" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F90" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="G90" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="34"/>
+      <c r="K90" s="34"/>
+      <c r="L90" s="34"/>
+      <c r="M90" s="34"/>
+      <c r="N90" s="33"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="35"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="34"/>
+    </row>
+    <row r="91" spans="1:18" ht="270.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B91" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E91" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F91" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="G91" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H91" s="34"/>
+      <c r="I91" s="34"/>
+      <c r="J91" s="34"/>
+      <c r="K91" s="34"/>
+      <c r="L91" s="34"/>
+      <c r="M91" s="34"/>
+      <c r="N91" s="33"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="35"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="34"/>
+    </row>
+    <row r="92" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B92" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F92" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="34"/>
+      <c r="K92" s="34"/>
+      <c r="L92" s="34"/>
+      <c r="M92" s="34"/>
+      <c r="N92" s="33"/>
+      <c r="O92" s="5"/>
+      <c r="P92" s="35"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="34"/>
+    </row>
+    <row r="93" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B93" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F93" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="H93" s="34"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="34"/>
+      <c r="K93" s="34"/>
+      <c r="L93" s="34"/>
+      <c r="M93" s="34"/>
+      <c r="N93" s="33"/>
+      <c r="O93" s="5"/>
+      <c r="P93" s="35"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="34"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:R85" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -9700,29 +10012,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9731,7 +10020,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9903,23 +10192,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9927,7 +10223,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9943,4 +10239,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated CR for ID-Auth
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C065AD6C-6BFE-4260-9930-C8E88E23283C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D3F298A-B6B8-4D55-A754-98D8960048FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="290">
   <si>
     <t>S.No.</t>
   </si>
@@ -3235,6 +3235,25 @@
   <si>
     <t>Device status:
 Display device status on the header.</t>
+  </si>
+  <si>
+    <t>Requirements Review of FIT2 stories</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fingerprint and IRIS Auth Composite Score Logic
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>For the Fingerprint and IRIS Composite Authentication, the composite score logic for two fingerprints/IRIS to be provided by SDK
+MOSIP to integrate with SDK provided by the country to retrieve the composite score</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3542,7 +3561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3777,6 +3796,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4986,7 +5008,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -5335,11 +5357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T93"/>
+  <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
+      <pane ySplit="2" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -9774,6 +9796,44 @@
       <c r="Q93" s="5"/>
       <c r="R93" s="34"/>
     </row>
+    <row r="94" spans="1:18" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>95</v>
+      </c>
+      <c r="B94" s="6">
+        <v>43448</v>
+      </c>
+      <c r="C94" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E94" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F94" s="83" t="s">
+        <v>289</v>
+      </c>
+      <c r="G94" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H94" s="34"/>
+      <c r="I94" s="34"/>
+      <c r="J94" s="34"/>
+      <c r="K94" s="34"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="33">
+        <v>20</v>
+      </c>
+      <c r="N94" s="5">
+        <v>40</v>
+      </c>
+      <c r="O94" s="35"/>
+      <c r="P94" s="5"/>
+      <c r="Q94" s="34"/>
+      <c r="R94" s="11"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:R85" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
@@ -10021,6 +10081,29 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10192,29 +10275,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
@@ -10224,6 +10284,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10239,20 +10315,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MOS-5771 Reg client CR estimate updated
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$R$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$R$104</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="314">
   <si>
     <t>S.No.</t>
   </si>
@@ -3306,6 +3306,29 @@
   </si>
   <si>
     <t>Mobile has different OS. Integrate and getting infromation from IOS might become challenges.  Need to do the POC on multiple mobile platform [IOS, Android, Black berry, Simbion OS and windows]. Implementation Approach to be finalized. Highlevel estimation provided.</t>
+  </si>
+  <si>
+    <t>Cbeff update applicable.</t>
+  </si>
+  <si>
+    <t>QR - hardware - SDK - integration. 
+[Need to identify the open source lib + drivers + hardware]</t>
+  </si>
+  <si>
+    <t>Stub for QR data retrieval. UI + Api changes.</t>
+  </si>
+  <si>
+    <t>if the Registration client software is a docker then we have to check the feasibility of the same.</t>
+  </si>
+  <si>
+    <t>Stubbed data.</t>
+  </si>
+  <si>
+    <t>Need some analysis on this area. Approximate effort provided. Based on R&amp;D this effort would vary.
+[TPM + Bitlocker + Windows + Docker]</t>
+  </si>
+  <si>
+    <t>This functionality has been removed. Need confirmation.</t>
   </si>
 </sst>
 </file>
@@ -3613,7 +3636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3752,9 +3775,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5409,18 +5429,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N77" sqref="N77"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36.08984375" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
@@ -5441,26 +5460,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="83"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="82"/>
     </row>
     <row r="2" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
@@ -5508,7 +5527,7 @@
       <c r="O2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="60" t="s">
+      <c r="P2" s="59" t="s">
         <v>198</v>
       </c>
       <c r="Q2" s="21" t="s">
@@ -5572,7 +5591,7 @@
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>43362</v>
@@ -5622,9 +5641,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" s="4" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6">
         <v>43362</v>
@@ -5674,9 +5693,9 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" s="4" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6">
         <v>43362</v>
@@ -5728,7 +5747,7 @@
     </row>
     <row r="7" spans="1:18" s="4" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" s="6">
         <v>43362</v>
@@ -5780,7 +5799,7 @@
     </row>
     <row r="8" spans="1:18" s="4" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6">
         <v>43362</v>
@@ -5832,7 +5851,7 @@
     </row>
     <row r="9" spans="1:18" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>43362</v>
@@ -5882,7 +5901,7 @@
     </row>
     <row r="10" spans="1:18" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>43362</v>
@@ -5932,7 +5951,7 @@
     </row>
     <row r="11" spans="1:18" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6">
         <v>43362</v>
@@ -5980,7 +5999,7 @@
     </row>
     <row r="12" spans="1:18" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6">
         <v>43362</v>
@@ -6028,9 +6047,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="1" customFormat="1" ht="350" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="1" customFormat="1" ht="350" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B13" s="6">
         <v>43395</v>
@@ -6077,7 +6096,7 @@
     </row>
     <row r="14" spans="1:18" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B14" s="6">
         <v>43397</v>
@@ -6127,7 +6146,7 @@
     </row>
     <row r="15" spans="1:18" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B15" s="6">
         <v>43397</v>
@@ -6177,7 +6196,7 @@
     </row>
     <row r="16" spans="1:18" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B16" s="6">
         <v>43397</v>
@@ -6191,7 +6210,7 @@
       <c r="E16" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="52" t="s">
         <v>201</v>
       </c>
       <c r="G16" s="15" t="s">
@@ -6213,13 +6232,13 @@
       <c r="M16" s="22">
         <v>43419</v>
       </c>
-      <c r="N16" s="52" t="s">
+      <c r="N16" s="51" t="s">
         <v>45</v>
       </c>
       <c r="O16" s="42">
         <v>36</v>
       </c>
-      <c r="P16" s="62" t="s">
+      <c r="P16" s="61" t="s">
         <v>193</v>
       </c>
       <c r="Q16" s="31" t="s">
@@ -6231,7 +6250,7 @@
     </row>
     <row r="17" spans="1:18" s="1" customFormat="1" ht="210" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B17" s="6">
         <v>43397</v>
@@ -6245,7 +6264,7 @@
       <c r="E17" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="52" t="s">
         <v>200</v>
       </c>
       <c r="G17" s="15" t="s">
@@ -6267,13 +6286,13 @@
       <c r="M17" s="22">
         <v>43419</v>
       </c>
-      <c r="N17" s="54">
+      <c r="N17" s="53">
         <v>36</v>
       </c>
       <c r="O17" s="42">
         <v>54</v>
       </c>
-      <c r="P17" s="62" t="s">
+      <c r="P17" s="61" t="s">
         <v>193</v>
       </c>
       <c r="Q17" s="31" t="s">
@@ -6285,7 +6304,7 @@
     </row>
     <row r="18" spans="1:18" s="4" customFormat="1" ht="238" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6">
         <v>43397</v>
@@ -6321,13 +6340,13 @@
       <c r="M18" s="22">
         <v>43419</v>
       </c>
-      <c r="N18" s="52" t="s">
+      <c r="N18" s="51" t="s">
         <v>49</v>
       </c>
       <c r="O18" s="42">
         <v>72</v>
       </c>
-      <c r="P18" s="62" t="s">
+      <c r="P18" s="61" t="s">
         <v>193</v>
       </c>
       <c r="Q18" s="31" t="s">
@@ -6339,7 +6358,7 @@
     </row>
     <row r="19" spans="1:18" s="1" customFormat="1" ht="182" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6">
         <v>43397</v>
@@ -6381,7 +6400,7 @@
       <c r="O19" s="42">
         <v>0</v>
       </c>
-      <c r="P19" s="63" t="s">
+      <c r="P19" s="62" t="s">
         <v>220</v>
       </c>
       <c r="Q19" s="31" t="s">
@@ -6393,7 +6412,7 @@
     </row>
     <row r="20" spans="1:18" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B20" s="6">
         <v>43397</v>
@@ -6429,25 +6448,25 @@
       <c r="M20" s="22">
         <v>43419</v>
       </c>
-      <c r="N20" s="55">
+      <c r="N20" s="54">
         <v>10</v>
       </c>
-      <c r="O20" s="56" t="s">
+      <c r="O20" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="P20" s="64" t="s">
+      <c r="P20" s="63" t="s">
         <v>193</v>
       </c>
-      <c r="Q20" s="56" t="s">
+      <c r="Q20" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="R20" s="57" t="s">
+      <c r="R20" s="56" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="13" t="s">
@@ -6489,7 +6508,7 @@
     </row>
     <row r="22" spans="1:18" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="13" t="s">
@@ -6531,7 +6550,7 @@
     </row>
     <row r="23" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6">
         <v>43402</v>
@@ -6581,7 +6600,7 @@
     </row>
     <row r="24" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B24" s="6">
         <v>43402</v>
@@ -6631,7 +6650,7 @@
     </row>
     <row r="25" spans="1:18" ht="112" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6">
         <v>43402</v>
@@ -6667,13 +6686,13 @@
       <c r="M25" s="22">
         <v>43419</v>
       </c>
-      <c r="N25" s="54">
+      <c r="N25" s="53">
         <v>20</v>
       </c>
       <c r="O25" s="42">
         <v>30</v>
       </c>
-      <c r="P25" s="64" t="s">
+      <c r="P25" s="63" t="s">
         <v>193</v>
       </c>
       <c r="Q25" s="31" t="s">
@@ -6685,7 +6704,7 @@
     </row>
     <row r="26" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6">
         <v>43402</v>
@@ -6729,7 +6748,7 @@
     </row>
     <row r="27" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B27" s="6">
         <v>43402</v>
@@ -6773,7 +6792,7 @@
     </row>
     <row r="28" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B28" s="6">
         <v>43402</v>
@@ -6823,7 +6842,7 @@
     </row>
     <row r="29" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B29" s="6">
         <v>43418</v>
@@ -6873,7 +6892,7 @@
     </row>
     <row r="30" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B30" s="6">
         <v>43418</v>
@@ -6917,7 +6936,7 @@
     </row>
     <row r="31" spans="1:18" ht="84" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B31" s="6">
         <v>43418</v>
@@ -6967,7 +6986,7 @@
     </row>
     <row r="32" spans="1:18" ht="126" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6">
         <v>43418</v>
@@ -7003,13 +7022,13 @@
       <c r="M32" s="22">
         <v>43419</v>
       </c>
-      <c r="N32" s="54">
+      <c r="N32" s="53">
         <v>20</v>
       </c>
       <c r="O32" s="42">
         <v>30</v>
       </c>
-      <c r="P32" s="65" t="s">
+      <c r="P32" s="64" t="s">
         <v>207</v>
       </c>
       <c r="Q32" s="31" t="s">
@@ -7021,7 +7040,7 @@
     </row>
     <row r="33" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6">
         <v>43430</v>
@@ -7071,7 +7090,7 @@
     </row>
     <row r="34" spans="1:18" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B34" s="6">
         <v>43430</v>
@@ -7121,7 +7140,7 @@
     </row>
     <row r="35" spans="1:18" s="8" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B35" s="6">
         <v>43430</v>
@@ -7171,7 +7190,7 @@
     </row>
     <row r="36" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B36" s="6">
         <v>43430</v>
@@ -7219,7 +7238,7 @@
     </row>
     <row r="37" spans="1:18" ht="182" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B37" s="6">
         <v>43430</v>
@@ -7271,7 +7290,7 @@
     </row>
     <row r="38" spans="1:18" ht="126" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B38" s="6">
         <v>43430</v>
@@ -7323,7 +7342,7 @@
     </row>
     <row r="39" spans="1:18" ht="224" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B39" s="6">
         <v>43430</v>
@@ -7375,7 +7394,7 @@
     </row>
     <row r="40" spans="1:18" ht="126" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B40" s="6">
         <v>43430</v>
@@ -7425,9 +7444,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B41" s="6">
         <v>43430</v>
@@ -7471,9 +7490,9 @@
       <c r="Q41" s="31"/>
       <c r="R41" s="33"/>
     </row>
-    <row r="42" spans="1:18" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6">
         <v>43430</v>
@@ -7518,9 +7537,9 @@
       <c r="Q42" s="31"/>
       <c r="R42" s="33"/>
     </row>
-    <row r="43" spans="1:18" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B43" s="6">
         <v>43427</v>
@@ -7567,9 +7586,9 @@
       <c r="Q43" s="31"/>
       <c r="R43" s="33"/>
     </row>
-    <row r="44" spans="1:18" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B44" s="6">
         <v>43427</v>
@@ -7616,7 +7635,7 @@
     </row>
     <row r="45" spans="1:18" ht="322" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B45" s="6">
         <v>43427</v>
@@ -7652,13 +7671,13 @@
       <c r="M45" s="22">
         <v>43440</v>
       </c>
-      <c r="N45" s="54">
+      <c r="N45" s="53">
         <v>60</v>
       </c>
       <c r="O45" s="42">
         <v>90</v>
       </c>
-      <c r="P45" s="61" t="s">
+      <c r="P45" s="60" t="s">
         <v>193</v>
       </c>
       <c r="Q45" s="31"/>
@@ -7666,9 +7685,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="140" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B46" s="6">
         <v>43427</v>
@@ -7716,7 +7735,7 @@
     </row>
     <row r="47" spans="1:18" ht="28" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B47" s="6">
         <v>43427</v>
@@ -7758,7 +7777,7 @@
       <c r="O47" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="P47" s="65" t="s">
+      <c r="P47" s="64" t="s">
         <v>210</v>
       </c>
       <c r="Q47" s="31" t="s">
@@ -7770,7 +7789,7 @@
     </row>
     <row r="48" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B48" s="6">
         <v>43427</v>
@@ -7812,7 +7831,7 @@
       <c r="O48" s="42">
         <v>30</v>
       </c>
-      <c r="P48" s="63" t="s">
+      <c r="P48" s="62" t="s">
         <v>222</v>
       </c>
       <c r="Q48" s="31" t="s">
@@ -7824,7 +7843,7 @@
     </row>
     <row r="49" spans="1:18" ht="84" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B49" s="6">
         <v>43427</v>
@@ -7868,7 +7887,7 @@
     </row>
     <row r="50" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B50" s="6">
         <v>43427</v>
@@ -7904,16 +7923,16 @@
       <c r="M50" s="22">
         <v>43440</v>
       </c>
-      <c r="N50" s="58">
+      <c r="N50" s="57">
         <v>5</v>
       </c>
-      <c r="O50" s="59">
+      <c r="O50" s="58">
         <v>8</v>
       </c>
-      <c r="P50" s="66" t="s">
+      <c r="P50" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="Q50" s="56" t="s">
+      <c r="Q50" s="55" t="s">
         <v>224</v>
       </c>
       <c r="R50" s="20" t="s">
@@ -7922,7 +7941,7 @@
     </row>
     <row r="51" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B51" s="6">
         <v>43427</v>
@@ -7972,9 +7991,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B52" s="6">
         <v>43427</v>
@@ -8021,7 +8040,7 @@
     </row>
     <row r="53" spans="1:18" ht="224" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B53" s="6">
         <v>43427</v>
@@ -8065,7 +8084,7 @@
     </row>
     <row r="54" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B54" s="6">
         <v>43427</v>
@@ -8115,7 +8134,7 @@
     </row>
     <row r="55" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B55" s="6">
         <v>43427</v>
@@ -8157,9 +8176,9 @@
       <c r="Q55" s="31"/>
       <c r="R55" s="33"/>
     </row>
-    <row r="56" spans="1:18" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B56" s="6">
         <v>43427</v>
@@ -8206,7 +8225,7 @@
     </row>
     <row r="57" spans="1:18" ht="84" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B57" s="6">
         <v>43427</v>
@@ -8256,7 +8275,7 @@
     </row>
     <row r="58" spans="1:18" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B58" s="6">
         <v>43427</v>
@@ -8304,9 +8323,9 @@
         <v>306</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="70" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B59" s="6">
         <v>43427</v>
@@ -8351,9 +8370,9 @@
       <c r="Q59" s="31"/>
       <c r="R59" s="33"/>
     </row>
-    <row r="60" spans="1:18" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" ht="98" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B60" s="6">
         <v>43427</v>
@@ -8400,7 +8419,7 @@
     </row>
     <row r="61" spans="1:18" ht="140" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B61" s="6">
         <v>43432</v>
@@ -8450,7 +8469,7 @@
     </row>
     <row r="62" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B62" s="6">
         <v>43432</v>
@@ -8502,7 +8521,7 @@
     </row>
     <row r="63" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B63" s="6">
         <v>43432</v>
@@ -8544,7 +8563,7 @@
       <c r="O63" s="42">
         <v>30</v>
       </c>
-      <c r="P63" s="65" t="s">
+      <c r="P63" s="64" t="s">
         <v>207</v>
       </c>
       <c r="Q63" s="31" t="s">
@@ -8554,9 +8573,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B64" s="6">
         <v>43432</v>
@@ -8600,9 +8619,9 @@
       <c r="Q64" s="34"/>
       <c r="R64" s="33"/>
     </row>
-    <row r="65" spans="1:20" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" ht="56" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B65" s="6">
         <v>43432</v>
@@ -8648,7 +8667,7 @@
     </row>
     <row r="66" spans="1:20" ht="280" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B66" s="6">
         <v>43440</v>
@@ -8700,7 +8719,7 @@
     </row>
     <row r="67" spans="1:20" ht="154" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B67" s="6">
         <v>43440</v>
@@ -8750,7 +8769,7 @@
     </row>
     <row r="68" spans="1:20" ht="154" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B68" s="6">
         <v>43440</v>
@@ -8802,7 +8821,7 @@
     </row>
     <row r="69" spans="1:20" ht="350" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B69" s="6">
         <v>43446</v>
@@ -8838,7 +8857,9 @@
       <c r="M69" s="22">
         <v>43446</v>
       </c>
-      <c r="N69" s="32"/>
+      <c r="N69" s="32">
+        <v>12</v>
+      </c>
       <c r="O69" s="5">
         <v>24</v>
       </c>
@@ -8850,7 +8871,7 @@
     </row>
     <row r="70" spans="1:20" ht="42" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B70" s="6">
         <v>43446</v>
@@ -8886,9 +8907,11 @@
       <c r="M70" s="22">
         <v>43446</v>
       </c>
-      <c r="N70" s="32"/>
+      <c r="N70" s="32">
+        <v>4</v>
+      </c>
       <c r="O70" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
@@ -8896,7 +8919,7 @@
     </row>
     <row r="71" spans="1:20" ht="154" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B71" s="6">
         <v>43451</v>
@@ -8946,7 +8969,7 @@
     </row>
     <row r="72" spans="1:20" ht="182" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B72" s="6">
         <v>43451</v>
@@ -9000,7 +9023,7 @@
     </row>
     <row r="73" spans="1:20" ht="196" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B73" s="6">
         <v>43451</v>
@@ -9048,9 +9071,9 @@
       <c r="S73" s="40"/>
       <c r="T73" s="29"/>
     </row>
-    <row r="74" spans="1:20" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" ht="126" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B74" s="6">
         <v>43454</v>
@@ -9100,7 +9123,7 @@
     </row>
     <row r="75" spans="1:20" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B75" s="38">
         <v>43454</v>
@@ -9142,19 +9165,19 @@
       <c r="O75" s="40">
         <v>30</v>
       </c>
-      <c r="P75" s="64" t="s">
+      <c r="P75" s="63" t="s">
         <v>193</v>
       </c>
       <c r="Q75" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="R75" s="67" t="s">
+      <c r="R75" s="66" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="182" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B76" s="6">
         <v>43454</v>
@@ -9196,19 +9219,19 @@
       <c r="O76" s="42">
         <v>15</v>
       </c>
-      <c r="P76" s="77" t="s">
+      <c r="P76" s="76" t="s">
         <v>251</v>
       </c>
       <c r="Q76" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="R76" s="67" t="s">
+      <c r="R76" s="66" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:20" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B77" s="6">
         <v>43465</v>
@@ -9260,7 +9283,7 @@
     </row>
     <row r="78" spans="1:20" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B78" s="6">
         <v>43465</v>
@@ -9296,8 +9319,12 @@
       <c r="M78" s="22">
         <v>43465</v>
       </c>
-      <c r="N78" s="51"/>
-      <c r="O78" s="5"/>
+      <c r="N78" s="5">
+        <v>30</v>
+      </c>
+      <c r="O78" s="5">
+        <v>60</v>
+      </c>
       <c r="P78" s="5"/>
       <c r="Q78" s="5"/>
       <c r="R78" s="5"/>
@@ -9306,7 +9333,7 @@
     </row>
     <row r="79" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B79" s="6">
         <v>43465</v>
@@ -9342,17 +9369,23 @@
       <c r="M79" s="22">
         <v>43465</v>
       </c>
-      <c r="N79" s="51"/>
-      <c r="O79" s="5"/>
+      <c r="N79" s="31">
+        <v>20</v>
+      </c>
+      <c r="O79" s="5">
+        <v>40</v>
+      </c>
       <c r="P79" s="5"/>
       <c r="Q79" s="5"/>
-      <c r="R79" s="5"/>
+      <c r="R79" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="S79" s="5"/>
       <c r="T79" s="33"/>
     </row>
     <row r="80" spans="1:20" ht="84" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B80" s="6">
         <v>43465</v>
@@ -9388,17 +9421,21 @@
       <c r="M80" s="22">
         <v>43465</v>
       </c>
-      <c r="N80" s="51"/>
-      <c r="O80" s="5"/>
+      <c r="N80" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="O80" s="5">
+        <v>12</v>
+      </c>
       <c r="P80" s="5"/>
       <c r="Q80" s="5"/>
       <c r="R80" s="5"/>
-      <c r="S80" s="76"/>
+      <c r="S80" s="75"/>
       <c r="T80" s="33"/>
     </row>
     <row r="81" spans="1:20" ht="224" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B81" s="6">
         <v>43465</v>
@@ -9434,17 +9471,23 @@
       <c r="M81" s="22">
         <v>43465</v>
       </c>
-      <c r="N81" s="51"/>
-      <c r="O81" s="5"/>
+      <c r="N81" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="O81" s="5">
+        <v>40</v>
+      </c>
       <c r="P81" s="5"/>
       <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="76"/>
+      <c r="R81" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="S81" s="75"/>
       <c r="T81" s="33"/>
     </row>
-    <row r="82" spans="1:20" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B82" s="6">
         <v>43477</v>
@@ -9486,7 +9529,7 @@
       <c r="O82" s="5">
         <v>0</v>
       </c>
-      <c r="P82" s="63" t="s">
+      <c r="P82" s="62" t="s">
         <v>222</v>
       </c>
       <c r="Q82" s="5" t="s">
@@ -9496,15 +9539,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="70" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" ht="224" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B83" s="6">
-        <v>43477</v>
+        <v>43465</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="D83" s="33" t="s">
         <v>15</v>
@@ -9512,8 +9555,8 @@
       <c r="E83" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F83" s="20" t="s">
-        <v>242</v>
+      <c r="F83" s="33" t="s">
+        <v>217</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>42</v>
@@ -9529,20 +9572,28 @@
         <v>80</v>
       </c>
       <c r="L83" s="33" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="M83" s="22">
-        <v>43477</v>
-      </c>
-      <c r="N83" s="32"/>
-      <c r="O83" s="5"/>
-      <c r="P83" s="34"/>
+        <v>43465</v>
+      </c>
+      <c r="N83" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="O83" s="5">
+        <v>20</v>
+      </c>
+      <c r="P83" s="5"/>
       <c r="Q83" s="5"/>
-      <c r="R83" s="33"/>
-    </row>
-    <row r="84" spans="1:20" ht="84" x14ac:dyDescent="0.35">
+      <c r="R83" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="S83" s="75"/>
+      <c r="T83" s="33"/>
+    </row>
+    <row r="84" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B84" s="6">
         <v>43477</v>
@@ -9556,8 +9607,8 @@
       <c r="E84" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F84" s="33" t="s">
-        <v>243</v>
+      <c r="F84" s="20" t="s">
+        <v>242</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>42</v>
@@ -9578,15 +9629,21 @@
       <c r="M84" s="22">
         <v>43477</v>
       </c>
-      <c r="N84" s="32"/>
-      <c r="O84" s="5"/>
+      <c r="N84" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="O84" s="5">
+        <v>40</v>
+      </c>
       <c r="P84" s="34"/>
       <c r="Q84" s="5"/>
-      <c r="R84" s="33"/>
-    </row>
-    <row r="85" spans="1:20" ht="140" x14ac:dyDescent="0.35">
+      <c r="R84" s="33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="84" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B85" s="6">
         <v>43477</v>
@@ -9601,7 +9658,7 @@
         <v>29</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>42</v>
@@ -9617,20 +9674,24 @@
         <v>80</v>
       </c>
       <c r="L85" s="33" t="s">
-        <v>238</v>
+        <v>174</v>
       </c>
       <c r="M85" s="22">
         <v>43477</v>
       </c>
-      <c r="N85" s="32"/>
-      <c r="O85" s="5"/>
+      <c r="N85" s="32">
+        <v>6</v>
+      </c>
+      <c r="O85" s="5">
+        <v>12</v>
+      </c>
       <c r="P85" s="34"/>
       <c r="Q85" s="5"/>
       <c r="R85" s="33"/>
     </row>
-    <row r="86" spans="1:20" ht="168" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" ht="140" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B86" s="6">
         <v>43477</v>
@@ -9639,13 +9700,13 @@
         <v>237</v>
       </c>
       <c r="D86" s="33" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E86" s="33" t="s">
         <v>29</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>42</v>
@@ -9653,9 +9714,7 @@
       <c r="H86" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="I86" s="33" t="s">
-        <v>271</v>
-      </c>
+      <c r="I86" s="33"/>
       <c r="J86" s="33">
         <v>1</v>
       </c>
@@ -9668,15 +9727,21 @@
       <c r="M86" s="22">
         <v>43477</v>
       </c>
-      <c r="N86" s="32"/>
-      <c r="O86" s="5"/>
+      <c r="N86" s="32">
+        <v>0</v>
+      </c>
+      <c r="O86" s="5">
+        <v>0</v>
+      </c>
       <c r="P86" s="34"/>
       <c r="Q86" s="5"/>
-      <c r="R86" s="33"/>
-    </row>
-    <row r="87" spans="1:20" ht="210" x14ac:dyDescent="0.35">
+      <c r="R86" s="33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" ht="168" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B87" s="6">
         <v>43477</v>
@@ -9691,7 +9756,7 @@
         <v>29</v>
       </c>
       <c r="F87" s="33" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>42</v>
@@ -9700,7 +9765,7 @@
         <v>92</v>
       </c>
       <c r="I87" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J87" s="33">
         <v>1</v>
@@ -9720,9 +9785,9 @@
       <c r="Q87" s="5"/>
       <c r="R87" s="33"/>
     </row>
-    <row r="88" spans="1:20" ht="98" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" ht="210" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B88" s="6">
         <v>43477</v>
@@ -9731,13 +9796,13 @@
         <v>237</v>
       </c>
       <c r="D88" s="33" t="s">
-        <v>239</v>
+        <v>36</v>
       </c>
       <c r="E88" s="33" t="s">
         <v>29</v>
       </c>
       <c r="F88" s="33" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="G88" s="15" t="s">
         <v>42</v>
@@ -9746,7 +9811,7 @@
         <v>92</v>
       </c>
       <c r="I88" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J88" s="33">
         <v>1</v>
@@ -9766,9 +9831,9 @@
       <c r="Q88" s="5"/>
       <c r="R88" s="33"/>
     </row>
-    <row r="89" spans="1:20" ht="70" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" ht="98" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B89" s="6">
         <v>43477</v>
@@ -9777,13 +9842,13 @@
         <v>237</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E89" s="33" t="s">
         <v>29</v>
       </c>
       <c r="F89" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G89" s="15" t="s">
         <v>42</v>
@@ -9791,7 +9856,9 @@
       <c r="H89" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="I89" s="33"/>
+      <c r="I89" s="33" t="s">
+        <v>273</v>
+      </c>
       <c r="J89" s="33">
         <v>1</v>
       </c>
@@ -9810,24 +9877,24 @@
       <c r="Q89" s="5"/>
       <c r="R89" s="33"/>
     </row>
-    <row r="90" spans="1:20" ht="238" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B90" s="6">
-        <v>43486</v>
+        <v>43477</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="D90" s="33" t="s">
-        <v>15</v>
+        <v>240</v>
       </c>
       <c r="E90" s="33" t="s">
         <v>29</v>
       </c>
       <c r="F90" s="33" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="G90" s="15" t="s">
         <v>42</v>
@@ -9843,10 +9910,10 @@
         <v>80</v>
       </c>
       <c r="L90" s="33" t="s">
-        <v>174</v>
+        <v>238</v>
       </c>
       <c r="M90" s="22">
-        <v>43486</v>
+        <v>43477</v>
       </c>
       <c r="N90" s="32"/>
       <c r="O90" s="5"/>
@@ -9854,15 +9921,16 @@
       <c r="Q90" s="5"/>
       <c r="R90" s="33"/>
     </row>
-    <row r="91" spans="1:20" ht="28" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" ht="238" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
-        <f>1+A90</f>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B91" s="6">
-        <v>43489</v>
-      </c>
-      <c r="C91" s="32"/>
+        <v>43486</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>253</v>
+      </c>
       <c r="D91" s="33" t="s">
         <v>15</v>
       </c>
@@ -9870,29 +9938,42 @@
         <v>29</v>
       </c>
       <c r="F91" s="33" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="H91" s="33"/>
+        <v>42</v>
+      </c>
+      <c r="H91" s="33" t="s">
+        <v>92</v>
+      </c>
       <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
-      <c r="K91" s="33"/>
-      <c r="L91" s="33"/>
-      <c r="M91" s="33"/>
+      <c r="J91" s="33">
+        <v>1</v>
+      </c>
+      <c r="K91" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="L91" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="M91" s="22">
+        <v>43486</v>
+      </c>
       <c r="N91" s="32">
-        <v>4</v>
-      </c>
-      <c r="O91" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="O91" s="5">
+        <v>60</v>
+      </c>
       <c r="P91" s="34"/>
       <c r="Q91" s="5"/>
-      <c r="R91" s="33"/>
-    </row>
-    <row r="92" spans="1:20" ht="70" x14ac:dyDescent="0.35">
+      <c r="R91" s="29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" ht="28" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
-        <f t="shared" ref="A92:A101" si="1">1+A91</f>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B92" s="6">
         <v>43489</v>
@@ -9905,7 +9986,7 @@
         <v>29</v>
       </c>
       <c r="F92" s="33" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G92" s="15" t="s">
         <v>275</v>
@@ -9917,19 +9998,18 @@
       <c r="L92" s="33"/>
       <c r="M92" s="33"/>
       <c r="N92" s="32">
-        <v>30</v>
-      </c>
-      <c r="O92" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="O92" s="5">
+        <v>8</v>
+      </c>
       <c r="P92" s="34"/>
       <c r="Q92" s="5"/>
-      <c r="R92" s="33" t="s">
-        <v>291</v>
-      </c>
+      <c r="R92" s="33"/>
     </row>
     <row r="93" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
-        <f t="shared" si="1"/>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B93" s="6">
         <v>43489</v>
@@ -9954,19 +10034,20 @@
       <c r="L93" s="33"/>
       <c r="M93" s="33"/>
       <c r="N93" s="32">
-        <v>10</v>
-      </c>
-      <c r="O93" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="O93" s="5">
+        <v>50</v>
+      </c>
       <c r="P93" s="34"/>
       <c r="Q93" s="5"/>
       <c r="R93" s="33" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" ht="140" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
-        <f>1+A92</f>
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B94" s="6">
         <v>43489</v>
@@ -9979,7 +10060,7 @@
         <v>29</v>
       </c>
       <c r="F94" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G94" s="15" t="s">
         <v>275</v>
@@ -9991,17 +10072,20 @@
       <c r="L94" s="33"/>
       <c r="M94" s="33"/>
       <c r="N94" s="32">
+        <v>6</v>
+      </c>
+      <c r="O94" s="5">
         <v>12</v>
       </c>
-      <c r="O94" s="5"/>
       <c r="P94" s="34"/>
       <c r="Q94" s="5"/>
-      <c r="R94" s="33"/>
-    </row>
-    <row r="95" spans="1:20" ht="182" x14ac:dyDescent="0.35">
+      <c r="R94" s="33" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" ht="70" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B95" s="6">
         <v>43489</v>
@@ -10014,7 +10098,7 @@
         <v>29</v>
       </c>
       <c r="F95" s="33" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G95" s="15" t="s">
         <v>275</v>
@@ -10028,15 +10112,18 @@
       <c r="N95" s="32">
         <v>10</v>
       </c>
-      <c r="O95" s="5"/>
+      <c r="O95" s="5">
+        <v>20</v>
+      </c>
       <c r="P95" s="34"/>
       <c r="Q95" s="5"/>
-      <c r="R95" s="33"/>
-    </row>
-    <row r="96" spans="1:20" ht="126" x14ac:dyDescent="0.35">
+      <c r="R95" s="33" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" ht="140" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
-        <f t="shared" si="1"/>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B96" s="6">
         <v>43489</v>
@@ -10049,7 +10136,7 @@
         <v>29</v>
       </c>
       <c r="F96" s="33" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G96" s="15" t="s">
         <v>275</v>
@@ -10061,19 +10148,18 @@
       <c r="L96" s="33"/>
       <c r="M96" s="33"/>
       <c r="N96" s="32">
-        <v>6</v>
-      </c>
-      <c r="O96" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="O96" s="5">
+        <v>24</v>
+      </c>
       <c r="P96" s="34"/>
       <c r="Q96" s="5"/>
-      <c r="R96" s="33" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" ht="406" x14ac:dyDescent="0.35">
+      <c r="R96" s="33"/>
+    </row>
+    <row r="97" spans="1:18" ht="182" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
-        <f t="shared" si="1"/>
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B97" s="6">
         <v>43489</v>
@@ -10086,7 +10172,7 @@
         <v>29</v>
       </c>
       <c r="F97" s="33" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G97" s="15" t="s">
         <v>275</v>
@@ -10098,19 +10184,18 @@
       <c r="L97" s="33"/>
       <c r="M97" s="33"/>
       <c r="N97" s="32">
+        <v>10</v>
+      </c>
+      <c r="O97" s="5">
         <v>20</v>
       </c>
-      <c r="O97" s="5"/>
       <c r="P97" s="34"/>
       <c r="Q97" s="5"/>
-      <c r="R97" s="33" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" ht="406" x14ac:dyDescent="0.35">
+      <c r="R97" s="33"/>
+    </row>
+    <row r="98" spans="1:18" ht="126" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
-        <f t="shared" si="1"/>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B98" s="6">
         <v>43489</v>
@@ -10123,7 +10208,7 @@
         <v>29</v>
       </c>
       <c r="F98" s="33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G98" s="15" t="s">
         <v>275</v>
@@ -10135,19 +10220,20 @@
       <c r="L98" s="33"/>
       <c r="M98" s="33"/>
       <c r="N98" s="32">
-        <v>8</v>
-      </c>
-      <c r="O98" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="O98" s="5">
+        <v>12</v>
+      </c>
       <c r="P98" s="34"/>
       <c r="Q98" s="5"/>
       <c r="R98" s="33" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" ht="56" x14ac:dyDescent="0.35">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" ht="406" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
-        <f>1+A97</f>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B99" s="6">
         <v>43489</v>
@@ -10160,7 +10246,7 @@
         <v>29</v>
       </c>
       <c r="F99" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G99" s="15" t="s">
         <v>275</v>
@@ -10172,17 +10258,20 @@
       <c r="L99" s="33"/>
       <c r="M99" s="33"/>
       <c r="N99" s="32">
-        <v>6</v>
-      </c>
-      <c r="O99" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="O99" s="5">
+        <v>40</v>
+      </c>
       <c r="P99" s="34"/>
       <c r="Q99" s="5"/>
-      <c r="R99" s="33"/>
-    </row>
-    <row r="100" spans="1:18" ht="28" x14ac:dyDescent="0.35">
+      <c r="R99" s="33" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" ht="406" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
-        <f t="shared" si="1"/>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B100" s="6">
         <v>43489</v>
@@ -10195,7 +10284,7 @@
         <v>29</v>
       </c>
       <c r="F100" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G100" s="15" t="s">
         <v>275</v>
@@ -10207,19 +10296,20 @@
       <c r="L100" s="33"/>
       <c r="M100" s="33"/>
       <c r="N100" s="32">
-        <v>10</v>
-      </c>
-      <c r="O100" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="O100" s="5">
+        <v>16</v>
+      </c>
       <c r="P100" s="34"/>
       <c r="Q100" s="5"/>
       <c r="R100" s="33" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" ht="28" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" ht="56" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
-        <f t="shared" si="1"/>
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B101" s="6">
         <v>43489</v>
@@ -10232,7 +10322,7 @@
         <v>29</v>
       </c>
       <c r="F101" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G101" s="15" t="s">
         <v>275</v>
@@ -10244,61 +10334,131 @@
       <c r="L101" s="33"/>
       <c r="M101" s="33"/>
       <c r="N101" s="32">
-        <v>4</v>
-      </c>
-      <c r="O101" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="O101" s="5">
+        <v>12</v>
+      </c>
       <c r="P101" s="34"/>
       <c r="Q101" s="5"/>
-      <c r="R101" s="33" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" ht="126" x14ac:dyDescent="0.35">
+      <c r="R101" s="33"/>
+    </row>
+    <row r="102" spans="1:18" ht="28" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B102" s="6">
-        <v>43448</v>
-      </c>
-      <c r="C102" s="33" t="s">
-        <v>283</v>
-      </c>
+        <v>43489</v>
+      </c>
+      <c r="C102" s="32"/>
       <c r="D102" s="33" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E102" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F102" s="78" t="s">
-        <v>284</v>
+      <c r="F102" s="33" t="s">
+        <v>282</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>39</v>
+        <v>275</v>
       </c>
       <c r="H102" s="33"/>
       <c r="I102" s="33"/>
       <c r="J102" s="33"/>
       <c r="K102" s="33"/>
-      <c r="L102" s="22"/>
-      <c r="M102" s="32">
+      <c r="L102" s="33"/>
+      <c r="M102" s="33"/>
+      <c r="N102" s="32">
+        <v>10</v>
+      </c>
+      <c r="O102" s="5">
         <v>20</v>
       </c>
-      <c r="N102" s="5">
+      <c r="P102" s="34"/>
+      <c r="Q102" s="5"/>
+      <c r="R102" s="33" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" ht="28" x14ac:dyDescent="0.35">
+      <c r="A103" s="5">
+        <v>101</v>
+      </c>
+      <c r="B103" s="6">
+        <v>43489</v>
+      </c>
+      <c r="C103" s="32"/>
+      <c r="D103" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F103" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="G103" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="H103" s="33"/>
+      <c r="I103" s="33"/>
+      <c r="J103" s="33"/>
+      <c r="K103" s="33"/>
+      <c r="L103" s="33"/>
+      <c r="M103" s="33"/>
+      <c r="N103" s="32">
+        <v>4</v>
+      </c>
+      <c r="O103" s="5">
+        <v>8</v>
+      </c>
+      <c r="P103" s="34"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" ht="126" x14ac:dyDescent="0.35">
+      <c r="A104" s="5">
+        <v>102</v>
+      </c>
+      <c r="B104" s="6">
+        <v>43448</v>
+      </c>
+      <c r="C104" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F104" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="G104" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H104" s="33"/>
+      <c r="I104" s="33"/>
+      <c r="J104" s="33"/>
+      <c r="K104" s="33"/>
+      <c r="L104" s="22"/>
+      <c r="M104" s="32">
+        <v>20</v>
+      </c>
+      <c r="N104" s="5">
         <v>40</v>
       </c>
-      <c r="O102" s="34"/>
-      <c r="P102" s="5"/>
-      <c r="Q102" s="33"/>
-      <c r="R102" s="11"/>
+      <c r="O104" s="34"/>
+      <c r="P104" s="5"/>
+      <c r="Q104" s="33"/>
+      <c r="R104" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R102">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="New"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:R104"/>
   <mergeCells count="1">
     <mergeCell ref="A1:R1"/>
   </mergeCells>
@@ -10497,34 +10657,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="67" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="68" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="70"/>
-      <c r="C2" s="71" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="70" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="72"/>
-      <c r="C3" s="71" t="s">
+      <c r="B3" s="71"/>
+      <c r="C3" s="70" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="73"/>
-      <c r="C4" s="71" t="s">
+      <c r="B4" s="72"/>
+      <c r="C4" s="70" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="74"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="73"/>
+      <c r="C5" s="74" t="s">
         <v>233</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MOS-5771 Reg client CR estimate updated with stub value
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="315">
   <si>
     <t>S.No.</t>
   </si>
@@ -3329,6 +3329,12 @@
   </si>
   <si>
     <t>This functionality has been removed. Need confirmation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;22Jan19&gt;
+Prioritize GoM req with stubbed config/modularity in v1. Config perspective, the parameter will not be marked and only GoM required modes of login should be the primary focus. If the config is marked, then MOSIP should respond with "Feature not available".
+Scope the other peices (Other modes) in v1+.
+</t>
   </si>
 </sst>
 </file>
@@ -5433,7 +5439,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -5615,7 +5621,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>257</v>
+        <v>314</v>
       </c>
       <c r="J4" s="33">
         <v>1</v>

</xml_diff>

<commit_message>
MOS-5771 Registration client CR estimation updated with Stub data.
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="316">
   <si>
     <t>S.No.</t>
   </si>
@@ -3334,6 +3334,10 @@
     <t xml:space="preserve">&lt;22Jan19&gt;
 Prioritize GoM req with stubbed config/modularity in v1. Config perspective, the parameter will not be marked and only GoM required modes of login should be the primary focus. If the config is marked, then MOSIP should respond with "Feature not available".
 Scope the other peices (Other modes) in v1+.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build as per Backlog, Morocco will remove what it does not want, as part of its configuration. 
 </t>
   </si>
 </sst>
@@ -5086,7 +5090,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -5439,7 +5443,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -5618,7 +5622,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>19</v>
+        <v>315</v>
       </c>
       <c r="I4" s="33" t="s">
         <v>314</v>
@@ -10701,15 +10705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -10730,6 +10725,15 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10905,14 +10909,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -10924,6 +10920,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
MOS-5685 - CR estimation doc updated
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mindtree\Projects\MOSIP\IDA\Code\git-repo\0.8.0-branch1\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56F2E489-27C1-490B-A070-22D155AF6197}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7700"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,9 +20,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$S$105</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="15" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="324">
   <si>
     <t>S.No.</t>
   </si>
@@ -3353,11 +3352,23 @@
   <si>
     <t>90</t>
   </si>
+  <si>
+    <t>Awaiting requirement clarification from Anadi for CR estimation</t>
+  </si>
+  <si>
+    <t>Awating requirement clarification from GoM for CR estimation</t>
+  </si>
+  <si>
+    <t>Auth API spec changes based on technical Review</t>
+  </si>
+  <si>
+    <t>Awaiting clarifications for CR #85 and #86</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -3877,6 +3888,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3890,12 +3907,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3928,7 +3939,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -3945,7 +3956,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:S70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -5106,7 +5117,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -5454,62 +5465,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R104" sqref="R104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="20.28515625" style="10"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="20.26953125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="79" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="81"/>
-    </row>
-    <row r="2" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="80"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="83"/>
+    </row>
+    <row r="2" spans="1:19" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -5568,7 +5580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" ht="228" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="4" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5623,7 +5635,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" ht="228" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="4" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -5678,7 +5690,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="4" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5733,7 +5745,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="4" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -5788,7 +5800,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="4" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5843,7 +5855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="4" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -5898,7 +5910,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -5951,7 +5963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="4" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -6004,7 +6016,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -6055,7 +6067,7 @@
       <c r="R11" s="30"/>
       <c r="S11" s="21"/>
     </row>
-    <row r="12" spans="1:19" s="1" customFormat="1" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" s="1" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -6108,7 +6120,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="1" customFormat="1" ht="384.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="1" customFormat="1" ht="350" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -6146,12 +6158,11 @@
       <c r="M13" s="21">
         <v>43419</v>
       </c>
-      <c r="N13" s="82" t="s">
-        <v>156</v>
-      </c>
-      <c r="O13" s="30">
-        <f t="shared" ref="N13:O60" si="0">N13*1.5</f>
-        <v>0</v>
+      <c r="N13" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>177</v>
       </c>
       <c r="P13" s="30" t="s">
         <v>177</v>
@@ -6160,7 +6171,7 @@
       <c r="R13" s="30"/>
       <c r="S13" s="21"/>
     </row>
-    <row r="14" spans="1:19" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -6213,7 +6224,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -6266,7 +6277,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -6323,7 +6334,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="1" customFormat="1" ht="213.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" s="1" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -6380,7 +6391,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="4" customFormat="1" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="4" customFormat="1" ht="238" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -6437,7 +6448,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="1" customFormat="1" ht="199.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" s="1" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -6494,7 +6505,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -6551,7 +6562,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -6594,7 +6605,7 @@
       <c r="R21" s="30"/>
       <c r="S21" s="21"/>
     </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -6637,7 +6648,7 @@
       <c r="R22" s="30"/>
       <c r="S22" s="21"/>
     </row>
-    <row r="23" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -6690,7 +6701,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -6743,7 +6754,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -6800,7 +6811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -6845,7 +6856,7 @@
       <c r="R26" s="30"/>
       <c r="S26" s="21"/>
     </row>
-    <row r="27" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -6890,7 +6901,7 @@
       <c r="R27" s="30"/>
       <c r="S27" s="21"/>
     </row>
-    <row r="28" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -6943,7 +6954,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6996,7 +7007,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -7041,7 +7052,7 @@
       <c r="R30" s="30"/>
       <c r="S30" s="21"/>
     </row>
-    <row r="31" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -7094,7 +7105,7 @@
       <c r="R31" s="30"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -7151,7 +7162,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -7204,7 +7215,7 @@
       <c r="R33" s="30"/>
       <c r="S33" s="32"/>
     </row>
-    <row r="34" spans="1:19" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -7257,7 +7268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="8" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="8" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -7310,7 +7321,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -7361,7 +7372,7 @@
       <c r="R36" s="30"/>
       <c r="S36" s="14"/>
     </row>
-    <row r="37" spans="1:19" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="182" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -7416,7 +7427,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="126" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -7471,7 +7482,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="224" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -7526,7 +7537,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="126" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -7581,7 +7592,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -7628,7 +7639,7 @@
       <c r="R41" s="30"/>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -7666,11 +7677,11 @@
       <c r="M42" s="21">
         <v>43440</v>
       </c>
-      <c r="N42" s="83" t="s">
+      <c r="N42" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O42" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="O13:O60" si="0">N42*1.5</f>
         <v>0</v>
       </c>
       <c r="P42" s="30" t="s">
@@ -7680,7 +7691,7 @@
       <c r="R42" s="30"/>
       <c r="S42" s="32"/>
     </row>
-    <row r="43" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -7732,7 +7743,7 @@
       <c r="R43" s="30"/>
       <c r="S43" s="32"/>
     </row>
-    <row r="44" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -7770,7 +7781,7 @@
       <c r="M44" s="21">
         <v>43452</v>
       </c>
-      <c r="N44" s="83" t="s">
+      <c r="N44" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O44" s="30">
@@ -7784,7 +7795,7 @@
       <c r="R44" s="30"/>
       <c r="S44" s="32"/>
     </row>
-    <row r="45" spans="1:19" ht="327.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="322" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -7839,7 +7850,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -7892,7 +7903,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -7949,7 +7960,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -8006,7 +8017,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -8051,7 +8062,7 @@
       <c r="R49" s="30"/>
       <c r="S49" s="32"/>
     </row>
-    <row r="50" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -8108,7 +8119,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="56" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -8163,7 +8174,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -8201,7 +8212,7 @@
       <c r="M52" s="21">
         <v>43440</v>
       </c>
-      <c r="N52" s="83" t="s">
+      <c r="N52" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O52" s="30">
@@ -8215,7 +8226,7 @@
       <c r="R52" s="30"/>
       <c r="S52" s="32"/>
     </row>
-    <row r="53" spans="1:19" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="224" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -8260,7 +8271,7 @@
       <c r="R53" s="30"/>
       <c r="S53" s="32"/>
     </row>
-    <row r="54" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -8313,7 +8324,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -8358,7 +8369,7 @@
       <c r="R55" s="30"/>
       <c r="S55" s="32"/>
     </row>
-    <row r="56" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -8396,7 +8407,7 @@
       <c r="M56" s="21">
         <v>43452</v>
       </c>
-      <c r="N56" s="83" t="s">
+      <c r="N56" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O56" s="30">
@@ -8410,7 +8421,7 @@
       <c r="R56" s="30"/>
       <c r="S56" s="32"/>
     </row>
-    <row r="57" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -8463,7 +8474,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -8516,7 +8527,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -8554,7 +8565,7 @@
       <c r="M59" s="21">
         <v>43440</v>
       </c>
-      <c r="N59" s="83" t="s">
+      <c r="N59" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O59" s="30">
@@ -8568,7 +8579,7 @@
       <c r="R59" s="30"/>
       <c r="S59" s="32"/>
     </row>
-    <row r="60" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -8606,7 +8617,7 @@
       <c r="M60" s="21">
         <v>43440</v>
       </c>
-      <c r="N60" s="83" t="s">
+      <c r="N60" s="78" t="s">
         <v>156</v>
       </c>
       <c r="O60" s="30">
@@ -8620,7 +8631,7 @@
       <c r="R60" s="30"/>
       <c r="S60" s="32"/>
     </row>
-    <row r="61" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -8673,7 +8684,7 @@
       <c r="R61" s="30"/>
       <c r="S61" s="32"/>
     </row>
-    <row r="62" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="56" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -8728,7 +8739,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -8785,7 +8796,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="114" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -8832,7 +8843,7 @@
       <c r="R64" s="33"/>
       <c r="S64" s="32"/>
     </row>
-    <row r="65" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -8879,7 +8890,7 @@
       <c r="R65" s="33"/>
       <c r="S65" s="32"/>
     </row>
-    <row r="66" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="280" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -8920,7 +8931,7 @@
         <v>43452</v>
       </c>
       <c r="N66" s="31">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O66" s="5">
         <v>40</v>
@@ -8934,7 +8945,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -8987,7 +8998,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -9042,7 +9053,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="370.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="350" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -9095,7 +9106,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -9146,7 +9157,7 @@
       <c r="R70" s="5"/>
       <c r="S70" s="32"/>
     </row>
-    <row r="71" spans="1:21" ht="171" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -9199,7 +9210,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -9256,7 +9267,7 @@
       <c r="T72" s="5"/>
       <c r="U72" s="32"/>
     </row>
-    <row r="73" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -9309,7 +9320,7 @@
       <c r="T73" s="39"/>
       <c r="U73" s="28"/>
     </row>
-    <row r="74" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -9362,7 +9373,7 @@
       <c r="T74" s="5"/>
       <c r="U74" s="32"/>
     </row>
-    <row r="75" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -9419,7 +9430,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -9476,7 +9487,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -9531,7 +9542,7 @@
       <c r="T77" s="5"/>
       <c r="U77" s="32"/>
     </row>
-    <row r="78" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -9584,7 +9595,7 @@
       <c r="T78" s="5"/>
       <c r="U78" s="32"/>
     </row>
-    <row r="79" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -9639,7 +9650,7 @@
       <c r="T79" s="5"/>
       <c r="U79" s="32"/>
     </row>
-    <row r="80" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -9692,7 +9703,7 @@
       <c r="T80" s="74"/>
       <c r="U80" s="32"/>
     </row>
-    <row r="81" spans="1:21" ht="228" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="224" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -9747,7 +9758,7 @@
       <c r="T81" s="74"/>
       <c r="U81" s="32"/>
     </row>
-    <row r="82" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -9804,7 +9815,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="228" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="224" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -9859,7 +9870,7 @@
       <c r="T83" s="74"/>
       <c r="U83" s="32"/>
     </row>
-    <row r="84" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -9912,7 +9923,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -9963,7 +9974,7 @@
       <c r="R85" s="5"/>
       <c r="S85" s="32"/>
     </row>
-    <row r="86" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -10016,7 +10027,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="168" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -10061,9 +10072,11 @@
       <c r="P87" s="5"/>
       <c r="Q87" s="33"/>
       <c r="R87" s="5"/>
-      <c r="S87" s="32"/>
-    </row>
-    <row r="88" spans="1:21" ht="228" x14ac:dyDescent="0.25">
+      <c r="S87" s="32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" ht="210" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -10108,9 +10121,11 @@
       <c r="P88" s="5"/>
       <c r="Q88" s="33"/>
       <c r="R88" s="5"/>
-      <c r="S88" s="32"/>
-    </row>
-    <row r="89" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="S88" s="32" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -10157,7 +10172,7 @@
       <c r="R89" s="5"/>
       <c r="S89" s="32"/>
     </row>
-    <row r="90" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -10202,7 +10217,7 @@
       <c r="R90" s="5"/>
       <c r="S90" s="32"/>
     </row>
-    <row r="91" spans="1:21" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="238" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -10255,7 +10270,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -10294,7 +10309,7 @@
       <c r="R92" s="5"/>
       <c r="S92" s="32"/>
     </row>
-    <row r="93" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -10335,7 +10350,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -10376,7 +10391,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -10417,7 +10432,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -10456,7 +10471,7 @@
       <c r="R96" s="5"/>
       <c r="S96" s="32"/>
     </row>
-    <row r="97" spans="1:19" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -10495,7 +10510,7 @@
       <c r="R97" s="5"/>
       <c r="S97" s="32"/>
     </row>
-    <row r="98" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -10536,7 +10551,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="406" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -10577,7 +10592,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="406" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -10618,7 +10633,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -10657,7 +10672,7 @@
       <c r="R101" s="5"/>
       <c r="S101" s="32"/>
     </row>
-    <row r="102" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -10698,7 +10713,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -10739,7 +10754,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="126" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -10763,10 +10778,18 @@
       </c>
       <c r="H104" s="32"/>
       <c r="I104" s="32"/>
-      <c r="J104" s="32"/>
-      <c r="K104" s="32"/>
-      <c r="L104" s="21"/>
-      <c r="M104" s="31"/>
+      <c r="J104" s="32">
+        <v>1</v>
+      </c>
+      <c r="K104" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L104" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="M104" s="6">
+        <v>43448</v>
+      </c>
       <c r="N104" s="31">
         <v>20</v>
       </c>
@@ -10778,9 +10801,9 @@
       </c>
       <c r="Q104" s="5"/>
       <c r="R104" s="32"/>
-      <c r="S104" s="10"/>
-    </row>
-    <row r="105" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S104" s="33"/>
+    </row>
+    <row r="105" spans="1:19" ht="28" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -10788,7 +10811,7 @@
         <v>43447</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="D105" s="32" t="s">
         <v>36</v>
@@ -10804,19 +10827,35 @@
       </c>
       <c r="H105" s="32"/>
       <c r="I105" s="32"/>
-      <c r="J105" s="32"/>
-      <c r="K105" s="32"/>
-      <c r="L105" s="21"/>
-      <c r="M105" s="31"/>
+      <c r="J105" s="32">
+        <v>1</v>
+      </c>
+      <c r="K105" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L105" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="M105" s="6">
+        <v>43447</v>
+      </c>
       <c r="N105" s="5"/>
       <c r="O105" s="33"/>
       <c r="P105" s="33"/>
       <c r="Q105" s="5"/>
       <c r="R105" s="32"/>
-      <c r="S105" s="10"/>
+      <c r="S105" s="33" t="s">
+        <v>323</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:S105" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:S105">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="ID Authentication"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:S1"/>
   </mergeCells>
@@ -10826,57 +10865,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -10886,19 +10925,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>163</v>
       </c>
@@ -10909,7 +10948,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>78</v>
       </c>
@@ -10920,7 +10959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>36</v>
       </c>
@@ -10931,7 +10970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>136</v>
       </c>
@@ -10942,7 +10981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>86</v>
       </c>
@@ -10953,7 +10992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -10964,7 +11003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>43</v>
       </c>
@@ -10975,7 +11014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
@@ -10986,7 +11025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>164</v>
       </c>
@@ -11004,17 +11043,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="66" t="s">
         <v>234</v>
       </c>
@@ -11022,25 +11061,25 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>233</v>
@@ -11053,6 +11092,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -11073,15 +11121,6 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11257,6 +11296,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -11268,14 +11315,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
JIRA added for S. No. 125
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\PROJECTS\MOSIP\UX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE170024-1E19-447F-AD03-721BCA697AE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFB5E03-DD4E-4948-B3E2-2CAD726D1BF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2655" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$120</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -30,12 +30,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="468">
   <si>
     <t>S.No.</t>
   </si>
@@ -4736,10 +4741,6 @@
 </t>
   </si>
   <si>
-    <t>Via Registration Client software, Collection of Persons Demographic &amp; Biometric Data, performing a Dedupe and identify the Duplicate and proceed to issue of letter. 
-• At the back end - as first step use the demographic data as filter and then perform a biometric dedupe with the limited set of records, in case of unsuccessful match ignore the demographic data and perform a complete biometric dedupe to identify the duplicate.</t>
-  </si>
-  <si>
     <t>Discussion with Shrikant, Ramesh and Sasi - 04-Mar-19</t>
   </si>
   <si>
@@ -4749,6 +4750,32 @@
   </si>
   <si>
     <t>E-mail from Shrikant dated 05-Mar-19</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lost UIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Via Registration Client software, Collection of Persons Demographic &amp; Biometric Data, performing a Dedupe and identify the Duplicate and proceed to issue of letter. 
+• At the back end - as first step use the demographic data as filter and then perform a biometric dedupe with the limited set of records, in case of unsuccessful match ignore the demographic data and perform a complete biometric dedupe to identify the duplicate.</t>
+    </r>
+  </si>
+  <si>
+    <t>MOS-17830</t>
   </si>
 </sst>
 </file>
@@ -6917,37 +6944,37 @@
   <dimension ref="A1:W125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="2" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="49" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.44140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.42578125" style="10"/>
+    <col min="12" max="12" width="11.109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.88671875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.44140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="90" t="s">
         <v>210</v>
       </c>
@@ -6972,7 +6999,7 @@
       <c r="T1" s="92"/>
       <c r="U1" s="94"/>
     </row>
-    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7037,7 +7064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="138" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7099,7 +7126,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7160,7 +7187,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7222,7 +7249,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7284,7 +7311,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -7346,7 +7373,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="138" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -7408,7 +7435,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -7468,7 +7495,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -7528,7 +7555,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7582,7 +7609,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -7639,7 +7666,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="276" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7690,7 +7717,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -7750,7 +7777,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -7812,7 +7839,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -7874,7 +7901,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="207" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -7936,7 +7963,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="138" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -7996,7 +8023,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8058,7 +8085,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8106,7 +8133,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8154,7 +8181,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8214,7 +8241,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8272,7 +8299,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8334,7 +8361,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8384,7 +8411,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8434,7 +8461,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -8492,7 +8519,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -8552,7 +8579,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8602,7 +8629,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8658,7 +8685,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8720,7 +8747,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -8778,7 +8805,7 @@
       <c r="T32" s="30"/>
       <c r="U32" s="32"/>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -8836,7 +8863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -8898,7 +8925,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -8953,7 +8980,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9017,7 +9044,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9081,7 +9108,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="171" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9145,7 +9172,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9209,7 +9236,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9263,7 +9290,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9319,7 +9346,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9373,7 +9400,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -9429,7 +9456,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="262.2" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9489,7 +9516,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9547,7 +9574,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9609,7 +9636,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9671,7 +9698,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -9721,7 +9748,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -9783,7 +9810,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -9846,7 +9873,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -9900,7 +9927,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -9950,7 +9977,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10010,7 +10037,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10060,7 +10087,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10114,7 +10141,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10171,7 +10198,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10228,7 +10255,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -10286,7 +10313,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10340,7 +10367,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10394,7 +10421,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10449,7 +10476,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10512,7 +10539,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10573,7 +10600,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10622,7 +10649,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10671,7 +10698,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="207" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10734,7 +10761,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -10794,7 +10821,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -10853,7 +10880,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="285" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="276" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -10911,7 +10938,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -10967,7 +10994,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11025,7 +11052,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11086,7 +11113,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11146,7 +11173,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11201,7 +11228,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11262,7 +11289,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11323,7 +11350,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -11383,7 +11410,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -11445,7 +11472,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -11505,7 +11532,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -11567,7 +11594,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -11627,7 +11654,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -11689,7 +11716,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -11748,7 +11775,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -11810,7 +11837,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="69" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -11870,7 +11897,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="69" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -11930,7 +11957,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -11989,7 +12016,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12050,7 +12077,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12105,7 +12132,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12154,7 +12181,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12201,7 +12228,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -12261,7 +12288,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -12317,7 +12344,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -12377,7 +12404,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="69" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -12437,7 +12464,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="69" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -12497,7 +12524,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -12555,7 +12582,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12604,7 +12631,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="138" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -12660,7 +12687,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -12720,7 +12747,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="342" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="317.39999999999998" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -12780,7 +12807,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -12838,7 +12865,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -12898,7 +12925,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -12958,7 +12985,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13017,7 +13044,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13076,7 +13103,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13125,7 +13152,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13184,7 +13211,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13239,7 +13266,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13294,7 +13321,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13351,7 +13378,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13408,7 +13435,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13465,7 +13492,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13522,7 +13549,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13577,7 +13604,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13623,7 +13650,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -13671,7 +13698,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13716,7 +13743,7 @@
       <c r="T118" s="5"/>
       <c r="U118" s="32"/>
     </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -13763,7 +13790,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -13809,7 +13836,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -13852,7 +13879,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="69" x14ac:dyDescent="0.3">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -13895,16 +13922,18 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="138" x14ac:dyDescent="0.3">
       <c r="A123" s="5">
         <v>125</v>
       </c>
-      <c r="B123" s="31"/>
+      <c r="B123" s="31" t="s">
+        <v>467</v>
+      </c>
       <c r="C123" s="6">
         <v>43528</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E123" s="32" t="s">
         <v>15</v>
@@ -13913,7 +13942,7 @@
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="32"/>
@@ -13938,7 +13967,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="138" x14ac:dyDescent="0.3">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -13947,7 +13976,7 @@
         <v>43528</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>39</v>
@@ -13956,7 +13985,7 @@
         <v>26</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="H124" s="14"/>
       <c r="I124" s="32"/>
@@ -13981,7 +14010,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -13990,7 +14019,7 @@
         <v>43529</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E125" s="32" t="s">
         <v>80</v>
@@ -13999,7 +14028,7 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I125" s="32"/>
       <c r="J125" s="32"/>
@@ -14038,52 +14067,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -14098,14 +14127,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -14116,7 +14145,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -14127,7 +14156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -14138,7 +14167,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -14149,7 +14178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -14160,7 +14189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -14171,7 +14200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -14182,7 +14211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -14193,7 +14222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -14216,12 +14245,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="66" t="s">
         <v>208</v>
       </c>
@@ -14229,25 +14258,25 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="30.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>207</v>
@@ -14260,6 +14289,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -14280,15 +14318,6 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14464,6 +14493,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -14475,14 +14512,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added dates for registration client
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Documents\GitHub\mosip\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$126</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="486">
   <si>
     <t>S.No.</t>
   </si>
@@ -4819,6 +4819,48 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>MOS-14566</t>
+  </si>
+  <si>
+    <t>MOS-8641</t>
+  </si>
+  <si>
+    <t>MOS-12112</t>
+  </si>
+  <si>
+    <t>MOS-5482</t>
+  </si>
+  <si>
+    <t>MOS-18117</t>
+  </si>
+  <si>
+    <t>MOS 9090</t>
+  </si>
+  <si>
+    <t>MOS 1226</t>
+  </si>
+  <si>
+    <t>MOS 16545</t>
+  </si>
+  <si>
+    <t>MOS-13661</t>
+  </si>
+  <si>
+    <t>MOS-12961</t>
+  </si>
+  <si>
+    <t>MOS-12874</t>
+  </si>
+  <si>
+    <t>MOS 1204</t>
+  </si>
+  <si>
+    <t>MOS-8942</t>
+  </si>
+  <si>
+    <t>MOS-1316</t>
   </si>
 </sst>
 </file>
@@ -6987,11 +7029,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O64" sqref="O64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -7601,7 +7644,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7712,7 +7755,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7823,7 +7866,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -7885,7 +7928,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="182" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -7947,7 +7990,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8009,7 +8052,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8069,7 +8112,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8131,7 +8174,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8179,7 +8222,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8291,7 +8334,9 @@
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="31"/>
+      <c r="B23" s="31" t="s">
+        <v>472</v>
+      </c>
       <c r="C23" s="6">
         <v>43402</v>
       </c>
@@ -8345,7 +8390,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8407,7 +8452,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8457,7 +8502,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8511,7 +8556,9 @@
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="83"/>
+      <c r="B27" s="83" t="s">
+        <v>473</v>
+      </c>
       <c r="C27" s="6">
         <v>43402</v>
       </c>
@@ -8569,7 +8616,9 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="83"/>
+      <c r="B28" s="83" t="s">
+        <v>474</v>
+      </c>
       <c r="C28" s="6">
         <v>43418</v>
       </c>
@@ -8625,7 +8674,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8675,7 +8724,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8731,7 +8780,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8793,7 +8842,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -8851,7 +8900,7 @@
       <c r="T32" s="30"/>
       <c r="U32" s="32"/>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -8975,7 +9024,9 @@
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="83"/>
+      <c r="B35" s="83" t="s">
+        <v>477</v>
+      </c>
       <c r="C35" s="6">
         <v>43430</v>
       </c>
@@ -9026,7 +9077,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="182" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9090,7 +9141,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9154,7 +9205,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="168" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="168" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9218,7 +9269,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9282,7 +9333,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9340,7 +9391,9 @@
       <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="31" t="s">
+        <v>475</v>
+      </c>
       <c r="C41" s="6">
         <v>43430</v>
       </c>
@@ -9392,7 +9445,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9450,7 +9503,9 @@
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="87"/>
+      <c r="B43" s="87" t="s">
+        <v>476</v>
+      </c>
       <c r="C43" s="6">
         <v>43427</v>
       </c>
@@ -9502,7 +9557,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="252" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9562,7 +9617,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9620,7 +9675,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9682,7 +9737,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9744,7 +9799,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -9794,7 +9849,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -9856,7 +9911,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -9919,7 +9974,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -9973,7 +10028,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10083,7 +10138,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10133,7 +10188,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10191,7 +10246,9 @@
       <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="83"/>
+      <c r="B56" s="83" t="s">
+        <v>478</v>
+      </c>
       <c r="C56" s="6">
         <v>43427</v>
       </c>
@@ -10248,7 +10305,9 @@
       <c r="A57" s="5">
         <v>55</v>
       </c>
-      <c r="B57" s="83"/>
+      <c r="B57" s="83" t="s">
+        <v>479</v>
+      </c>
       <c r="C57" s="6">
         <v>43427</v>
       </c>
@@ -10305,7 +10364,9 @@
       <c r="A58" s="5">
         <v>56</v>
       </c>
-      <c r="B58" s="84"/>
+      <c r="B58" s="84" t="s">
+        <v>480</v>
+      </c>
       <c r="C58" s="6">
         <v>43427</v>
       </c>
@@ -10359,7 +10420,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10413,7 +10474,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10467,7 +10528,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10524,7 +10585,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10587,7 +10648,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10648,7 +10709,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10699,7 +10760,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10750,7 +10811,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="210" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10873,7 +10934,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -10936,7 +10997,9 @@
       <c r="A69" s="5">
         <v>67</v>
       </c>
-      <c r="B69" s="83"/>
+      <c r="B69" s="83" t="s">
+        <v>481</v>
+      </c>
       <c r="C69" s="6">
         <v>43446</v>
       </c>
@@ -10994,7 +11057,9 @@
       <c r="A70" s="5">
         <v>68</v>
       </c>
-      <c r="B70" s="83"/>
+      <c r="B70" s="83" t="s">
+        <v>482</v>
+      </c>
       <c r="C70" s="6">
         <v>43446</v>
       </c>
@@ -11050,7 +11115,9 @@
       <c r="A71" s="5">
         <v>69</v>
       </c>
-      <c r="B71" s="83"/>
+      <c r="B71" s="83" t="s">
+        <v>483</v>
+      </c>
       <c r="C71" s="6">
         <v>43451</v>
       </c>
@@ -11104,7 +11171,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="168" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11225,7 +11292,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="98" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11280,7 +11347,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11341,7 +11408,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="154" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11768,7 +11835,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -11893,7 +11960,9 @@
       <c r="A85" s="5">
         <v>82</v>
       </c>
-      <c r="B85" s="31"/>
+      <c r="B85" s="83" t="s">
+        <v>295</v>
+      </c>
       <c r="C85" s="6">
         <v>43477</v>
       </c>
@@ -12009,7 +12078,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12068,7 +12137,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12129,7 +12198,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="168" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12184,7 +12253,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="84" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12233,7 +12302,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12344,7 +12413,9 @@
       <c r="A93" s="5">
         <v>90</v>
       </c>
-      <c r="B93" s="83"/>
+      <c r="B93" s="83" t="s">
+        <v>484</v>
+      </c>
       <c r="C93" s="6">
         <v>43489</v>
       </c>
@@ -12634,7 +12705,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12687,7 +12758,9 @@
       <c r="A99" s="5">
         <v>96</v>
       </c>
-      <c r="B99" s="31"/>
+      <c r="B99" s="31" t="s">
+        <v>485</v>
+      </c>
       <c r="C99" s="6">
         <v>43489</v>
       </c>
@@ -13037,7 +13110,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13096,7 +13169,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13155,7 +13228,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13263,7 +13336,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13318,7 +13391,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13373,7 +13446,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13430,7 +13503,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13487,7 +13560,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13544,7 +13617,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13601,7 +13674,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13656,7 +13729,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13702,7 +13775,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -13750,7 +13823,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13888,7 +13961,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -13931,7 +14004,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14019,7 +14092,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="140" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14062,7 +14135,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14147,7 +14220,18 @@
       <c r="U126" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U126"/>
+  <autoFilter ref="A2:U126">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Registration Client"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="New"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
@@ -14387,12 +14471,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14568,32 +14666,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14617,17 +14709,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MOS-16536 Update Feature Road Map
Updated Feature Road Map for Registration Processor
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1012602\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip_new_master\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{26626B09-0D32-4C66-9225-F99C54493136}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01CCFC6-BCAB-47F6-ADEF-867B59F1E775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$126</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
@@ -30,12 +30,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="495">
   <si>
     <t>S.No.</t>
   </si>
@@ -4874,6 +4879,21 @@
   </si>
   <si>
     <t>MOS-18215</t>
+  </si>
+  <si>
+    <t>MOS-17678</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Creating ABIS Middle-ware for Registration Processor (ABIS Middle ware is inclusive of Face De-Dupe, Iris De-Dupe and Finger Print De-Dupe Combined)</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>MOS-13140</t>
   </si>
 </sst>
 </file>
@@ -5212,7 +5232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5484,6 +5504,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7046,37 +7069,37 @@
   <dimension ref="A1:W126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121:B122"/>
+      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="49" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.42578125" style="10"/>
+    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="91" t="s">
         <v>209</v>
       </c>
@@ -7101,7 +7124,7 @@
       <c r="T1" s="93"/>
       <c r="U1" s="95"/>
     </row>
-    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7166,7 +7189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7228,7 +7251,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7289,7 +7312,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7351,7 +7374,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7413,7 +7436,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -7475,7 +7498,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -7537,7 +7560,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -7597,7 +7620,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -7657,7 +7680,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7711,7 +7734,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -7768,7 +7791,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7819,7 +7842,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -7879,7 +7902,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -7924,7 +7947,7 @@
       <c r="P15" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="Q15" s="79">
+      <c r="Q15" s="96">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -7941,7 +7964,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="182" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -7986,7 +8009,7 @@
       <c r="P16" s="52">
         <v>36</v>
       </c>
-      <c r="Q16" s="79">
+      <c r="Q16" s="96">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -8003,7 +8026,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="210" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8048,7 +8071,7 @@
       <c r="P17" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="79">
+      <c r="Q17" s="96">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
@@ -8065,11 +8088,13 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="C18" s="6">
         <v>43397</v>
       </c>
@@ -8108,7 +8133,7 @@
       <c r="P18" s="41">
         <v>0</v>
       </c>
-      <c r="Q18" s="79">
+      <c r="Q18" s="96">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8125,7 +8150,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8170,7 +8195,7 @@
       <c r="P19" s="53">
         <v>10</v>
       </c>
-      <c r="Q19" s="79">
+      <c r="Q19" s="96">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -8187,7 +8212,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8235,7 +8260,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8283,7 +8308,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8343,7 +8368,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8403,7 +8428,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8448,7 +8473,7 @@
       <c r="P24" s="52">
         <v>20</v>
       </c>
-      <c r="Q24" s="79">
+      <c r="Q24" s="96">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -8465,7 +8490,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8515,7 +8540,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8565,7 +8590,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -8625,7 +8650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -8687,7 +8712,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8737,7 +8762,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8793,7 +8818,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8838,7 +8863,7 @@
       <c r="P31" s="52">
         <v>20</v>
       </c>
-      <c r="Q31" s="79">
+      <c r="Q31" s="96">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -8855,7 +8880,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -8913,7 +8938,7 @@
       <c r="T32" s="30"/>
       <c r="U32" s="32"/>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -8971,7 +8996,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9033,7 +9058,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9090,7 +9115,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9154,7 +9179,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9218,7 +9243,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="171" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="168" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9282,7 +9307,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9346,7 +9371,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9400,7 +9425,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9458,7 +9483,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9512,7 +9537,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -9570,7 +9595,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="299.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9615,7 +9640,7 @@
       <c r="P44" s="52">
         <v>60</v>
       </c>
-      <c r="Q44" s="79">
+      <c r="Q44" s="96">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -9630,7 +9655,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9688,7 +9713,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9733,7 +9758,7 @@
       <c r="P46" s="31">
         <v>18</v>
       </c>
-      <c r="Q46" s="79">
+      <c r="Q46" s="96">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -9750,7 +9775,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9795,7 +9820,7 @@
       <c r="P47" s="40">
         <v>20</v>
       </c>
-      <c r="Q47" s="79">
+      <c r="Q47" s="96">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -9812,11 +9837,13 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>494</v>
+      </c>
       <c r="C48" s="6">
         <v>43427</v>
       </c>
@@ -9853,16 +9880,23 @@
         <v>43452</v>
       </c>
       <c r="P48" s="31"/>
-      <c r="Q48" s="79">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R48" s="30"/>
-      <c r="S48" s="30"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="32"/>
-    </row>
-    <row r="49" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q48" s="82" t="s">
+        <v>493</v>
+      </c>
+      <c r="R48" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="S48" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="T48" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="U48" s="32" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -9907,7 +9941,7 @@
       <c r="P49" s="56">
         <v>5</v>
       </c>
-      <c r="Q49" s="79">
+      <c r="Q49" s="96">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -9924,7 +9958,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -9987,7 +10021,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10041,7 +10075,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10091,7 +10125,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10151,7 +10185,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10201,7 +10235,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10255,7 +10289,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10314,7 +10348,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10373,7 +10407,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -10433,7 +10467,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10487,7 +10521,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10541,7 +10575,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10598,7 +10632,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10661,7 +10695,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10722,7 +10756,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10773,7 +10807,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10824,7 +10858,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10887,7 +10921,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -10947,7 +10981,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11006,7 +11040,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="266" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11066,7 +11100,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11124,7 +11158,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11184,7 +11218,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11245,7 +11279,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11305,7 +11339,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11360,7 +11394,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11421,7 +11455,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11482,7 +11516,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -11542,7 +11576,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -11604,7 +11638,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -11664,7 +11698,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -11726,7 +11760,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -11786,7 +11820,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -11848,7 +11882,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -11907,7 +11941,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="270.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -11969,7 +12003,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12031,7 +12065,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12091,7 +12125,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12150,7 +12184,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12211,7 +12245,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12266,7 +12300,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12315,7 +12349,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12362,7 +12396,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -12422,7 +12456,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -12480,7 +12514,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -12540,7 +12574,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -12600,7 +12634,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -12660,7 +12694,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="182" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -12718,7 +12752,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12767,7 +12801,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -12825,7 +12859,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -12885,7 +12919,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="342" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="322" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -12945,7 +12979,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13003,7 +13037,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13063,7 +13097,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13123,7 +13157,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13182,7 +13216,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13241,7 +13275,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13290,7 +13324,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13349,7 +13383,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13404,7 +13438,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13459,7 +13493,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13516,7 +13550,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13573,7 +13607,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13630,7 +13664,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13687,7 +13721,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13742,7 +13776,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13788,7 +13822,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -13836,7 +13870,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13883,7 +13917,7 @@
       <c r="T118" s="5"/>
       <c r="U118" s="32"/>
     </row>
-    <row r="119" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -13930,7 +13964,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -13976,7 +14010,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -14021,7 +14055,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14066,7 +14100,7 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>125</v>
       </c>
@@ -14111,11 +14145,13 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>126</v>
       </c>
-      <c r="B124" s="31"/>
+      <c r="B124" s="31" t="s">
+        <v>490</v>
+      </c>
       <c r="C124" s="6">
         <v>43528</v>
       </c>
@@ -14149,12 +14185,14 @@
       </c>
       <c r="P124" s="31"/>
       <c r="Q124" s="5"/>
-      <c r="R124" s="5"/>
+      <c r="R124" s="5" t="s">
+        <v>491</v>
+      </c>
       <c r="S124" s="33"/>
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14197,7 +14235,7 @@
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>128</v>
       </c>
@@ -14242,11 +14280,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:U126" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="ID Authentication"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="New"/>
@@ -14270,52 +14303,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -14330,14 +14363,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -14348,7 +14381,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -14359,7 +14392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -14370,7 +14403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -14381,7 +14414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -14392,7 +14425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -14403,7 +14436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -14414,7 +14447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -14425,7 +14458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -14448,12 +14481,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -14461,25 +14494,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -14492,6 +14525,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14663,39 +14728,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14711,28 +14768,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MOS-18236 Updated Feature Road Map
Update with VID Feature
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip_new_master\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01CCFC6-BCAB-47F6-ADEF-867B59F1E775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C058286-5D59-472C-B790-449CE6759AE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="498">
   <si>
     <t>S.No.</t>
   </si>
@@ -4894,6 +4894,17 @@
   </si>
   <si>
     <t>MOS-13140</t>
+  </si>
+  <si>
+    <t>Disucssion with Srikant
+Dated 13-Mar-19
+Queries on Pre-registration and Reg. Client - UIN Update | Lost UIN | Auto-Logout</t>
+  </si>
+  <si>
+    <t>UIN Update: Support entry of VIN (also called VID) instead of the UIN</t>
+  </si>
+  <si>
+    <t>[Shrikant] This is a good thought. Analyze the impact to understand the effort involved from Reg. Client and Reg. Processor perspective, so that a decision could be made on whether it should be part of v1 or v1.5</t>
   </si>
 </sst>
 </file>
@@ -5232,7 +5243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5490,6 +5501,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5505,8 +5519,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6716,7 +6730,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7065,12 +7079,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:W126"/>
+  <dimension ref="A1:W127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -7100,29 +7113,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="95"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="96"/>
     </row>
     <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -7680,7 +7693,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7791,7 +7804,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7947,7 +7960,7 @@
       <c r="P15" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="Q15" s="96">
+      <c r="Q15" s="91">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -8009,7 +8022,7 @@
       <c r="P16" s="52">
         <v>36</v>
       </c>
-      <c r="Q16" s="96">
+      <c r="Q16" s="91">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
@@ -8071,7 +8084,7 @@
       <c r="P17" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="96">
+      <c r="Q17" s="91">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
@@ -8133,7 +8146,7 @@
       <c r="P18" s="41">
         <v>0</v>
       </c>
-      <c r="Q18" s="96">
+      <c r="Q18" s="91">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -8195,7 +8208,7 @@
       <c r="P19" s="53">
         <v>10</v>
       </c>
-      <c r="Q19" s="96">
+      <c r="Q19" s="91">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -8473,7 +8486,7 @@
       <c r="P24" s="52">
         <v>20</v>
       </c>
-      <c r="Q24" s="96">
+      <c r="Q24" s="91">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -8863,7 +8876,7 @@
       <c r="P31" s="52">
         <v>20</v>
       </c>
-      <c r="Q31" s="96">
+      <c r="Q31" s="91">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -8938,7 +8951,7 @@
       <c r="T32" s="30"/>
       <c r="U32" s="32"/>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9371,7 +9384,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9483,7 +9496,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9640,7 +9653,7 @@
       <c r="P44" s="52">
         <v>60</v>
       </c>
-      <c r="Q44" s="96">
+      <c r="Q44" s="91">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -9655,7 +9668,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9758,7 +9771,7 @@
       <c r="P46" s="31">
         <v>18</v>
       </c>
-      <c r="Q46" s="96">
+      <c r="Q46" s="91">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
@@ -9820,7 +9833,7 @@
       <c r="P47" s="40">
         <v>20</v>
       </c>
-      <c r="Q47" s="96">
+      <c r="Q47" s="91">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -9941,7 +9954,7 @@
       <c r="P49" s="56">
         <v>5</v>
       </c>
-      <c r="Q49" s="96">
+      <c r="Q49" s="91">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -10021,7 +10034,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10235,7 +10248,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10467,7 +10480,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10521,7 +10534,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10756,7 +10769,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10807,7 +10820,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11339,7 +11352,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11882,7 +11895,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -13387,7 +13400,7 @@
       <c r="A109" s="5">
         <v>111</v>
       </c>
-      <c r="B109" s="32" t="s">
+      <c r="B109" s="31" t="s">
         <v>421</v>
       </c>
       <c r="C109" s="6">
@@ -13497,7 +13510,7 @@
       <c r="A111" s="5">
         <v>113</v>
       </c>
-      <c r="B111" s="32" t="s">
+      <c r="B111" s="31" t="s">
         <v>312</v>
       </c>
       <c r="C111" s="6">
@@ -13554,7 +13567,7 @@
       <c r="A112" s="5">
         <v>114</v>
       </c>
-      <c r="B112" s="32" t="s">
+      <c r="B112" s="31" t="s">
         <v>313</v>
       </c>
       <c r="C112" s="6">
@@ -13611,7 +13624,7 @@
       <c r="A113" s="5">
         <v>115</v>
       </c>
-      <c r="B113" s="32" t="s">
+      <c r="B113" s="31" t="s">
         <v>315</v>
       </c>
       <c r="C113" s="6">
@@ -13668,7 +13681,7 @@
       <c r="A114" s="5">
         <v>116</v>
       </c>
-      <c r="B114" s="32" t="s">
+      <c r="B114" s="31" t="s">
         <v>316</v>
       </c>
       <c r="C114" s="6">
@@ -13725,7 +13738,7 @@
       <c r="A115" s="5">
         <v>117</v>
       </c>
-      <c r="B115" s="32" t="s">
+      <c r="B115" s="31" t="s">
         <v>420</v>
       </c>
       <c r="C115" s="6">
@@ -13780,7 +13793,7 @@
       <c r="A116" s="5">
         <v>118</v>
       </c>
-      <c r="B116" s="32" t="s">
+      <c r="B116" s="31" t="s">
         <v>422</v>
       </c>
       <c r="C116" s="6">
@@ -13826,7 +13839,7 @@
       <c r="A117" s="39">
         <v>119</v>
       </c>
-      <c r="B117" s="28" t="s">
+      <c r="B117" s="97" t="s">
         <v>425</v>
       </c>
       <c r="C117" s="37">
@@ -14278,14 +14291,51 @@
       <c r="T126" s="5"/>
       <c r="U126" s="32"/>
     </row>
+    <row r="127" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+      <c r="A127" s="5">
+        <v>129</v>
+      </c>
+      <c r="B127" s="31"/>
+      <c r="C127" s="6">
+        <v>43537</v>
+      </c>
+      <c r="D127" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="E127" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F127" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G127" s="32" t="s">
+        <v>496</v>
+      </c>
+      <c r="I127" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="J127" s="32"/>
+      <c r="K127" s="32"/>
+      <c r="L127" s="32"/>
+      <c r="M127" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N127" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="O127" s="21">
+        <v>43537</v>
+      </c>
+      <c r="Q127" s="5"/>
+      <c r="R127" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="S127" s="33"/>
+      <c r="T127" s="5"/>
+      <c r="U127" s="32"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:U126" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="New"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:U126" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
@@ -14525,38 +14575,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14728,31 +14746,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14768,4 +14794,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Feature Roadmap for a feature for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C4F30-B4AF-40AB-A852-3C0AA775C827}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{47EF2CD7-D492-4498-B964-2976E0432E73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$128</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -30,17 +30,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="500">
   <si>
     <t>S.No.</t>
   </si>
@@ -4919,6 +4914,15 @@
   </si>
   <si>
     <t>MOS-18319</t>
+  </si>
+  <si>
+    <t>MOS-18511</t>
+  </si>
+  <si>
+    <t>DOB Type Authentication Implementation to be revalidated in v1+</t>
+  </si>
+  <si>
+    <t>Auth API specs Review</t>
   </si>
 </sst>
 </file>
@@ -7091,40 +7095,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:W127"/>
+  <dimension ref="A1:W128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C134" sqref="C134"/>
+      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="13.8" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="49" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.21875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.77734375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.21875" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.77734375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.44140625" style="10"/>
+    <col min="12" max="12" width="11.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>209</v>
       </c>
@@ -7149,7 +7153,7 @@
       <c r="T1" s="94"/>
       <c r="U1" s="96"/>
     </row>
-    <row r="2" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7214,7 +7218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="138" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7276,7 +7280,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7337,7 +7341,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7399,7 +7403,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7461,7 +7465,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -7523,7 +7527,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="138" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -7585,7 +7589,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -7645,7 +7649,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -7705,7 +7709,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="41.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7759,7 +7763,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="124.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -7816,7 +7820,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="276" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7867,7 +7871,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -7927,7 +7931,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="96.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -7989,7 +7993,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="179.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8051,7 +8055,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8113,7 +8117,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="138" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8175,7 +8179,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8237,7 +8241,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8285,7 +8289,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8333,7 +8337,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8393,7 +8397,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8453,7 +8457,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8515,7 +8519,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8565,7 +8569,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8615,7 +8619,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -8675,7 +8679,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -8737,7 +8741,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8787,7 +8791,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8843,7 +8847,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8905,7 +8909,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -8963,7 +8967,7 @@
       <c r="T32" s="30"/>
       <c r="U32" s="32"/>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9021,7 +9025,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9083,7 +9087,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9140,7 +9144,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9204,7 +9208,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9268,7 +9272,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="171" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9332,7 +9336,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9396,7 +9400,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="41.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9450,7 +9454,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9508,7 +9512,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="41.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9562,7 +9566,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -9620,7 +9624,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="262.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="299.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9680,7 +9684,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9738,7 +9742,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9800,7 +9804,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9862,7 +9866,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -9921,7 +9925,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -9983,7 +9987,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10046,7 +10050,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="55.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10100,7 +10104,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10150,7 +10154,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10210,7 +10214,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10260,7 +10264,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="55.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10314,7 +10318,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10373,7 +10377,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10432,7 +10436,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -10492,7 +10496,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="55.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10546,7 +10550,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10600,7 +10604,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10657,7 +10661,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10720,7 +10724,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10781,7 +10785,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10832,7 +10836,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="41.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10883,7 +10887,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="207" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="228" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10946,7 +10950,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11006,7 +11010,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11065,7 +11069,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="276" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11125,7 +11129,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11183,7 +11187,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11243,7 +11247,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11304,7 +11308,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11364,7 +11368,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11419,7 +11423,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11480,7 +11484,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11541,7 +11545,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -11601,7 +11605,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -11663,7 +11667,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -11723,7 +11727,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -11785,7 +11789,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -11845,7 +11849,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -11907,7 +11911,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -11966,7 +11970,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="248.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="270.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12028,7 +12032,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="69" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12090,7 +12094,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="69" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12150,7 +12154,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12209,7 +12213,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12270,7 +12274,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12325,7 +12329,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12374,7 +12378,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12421,7 +12425,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -12481,7 +12485,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -12539,7 +12543,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -12599,7 +12603,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="69" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -12659,7 +12663,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="69" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -12719,7 +12723,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -12777,7 +12781,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12826,7 +12830,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="138" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -12884,7 +12888,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -12944,7 +12948,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="317.39999999999998" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" ht="342" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13004,7 +13008,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13062,7 +13066,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13122,7 +13126,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13182,7 +13186,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13241,7 +13245,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13300,7 +13304,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13349,7 +13353,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13408,7 +13412,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13463,7 +13467,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13518,7 +13522,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13575,7 +13579,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13632,7 +13636,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13689,7 +13693,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13746,7 +13750,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13801,7 +13805,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13847,7 +13851,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -13895,7 +13899,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13942,7 +13946,7 @@
       <c r="T118" s="5"/>
       <c r="U118" s="32"/>
     </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -13989,7 +13993,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -14035,7 +14039,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -14080,7 +14084,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="69" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14125,7 +14129,7 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="138" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>125</v>
       </c>
@@ -14170,7 +14174,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="138" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14217,7 +14221,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14260,7 +14264,7 @@
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>128</v>
       </c>
@@ -14303,7 +14307,7 @@
       <c r="T126" s="5"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>129</v>
       </c>
@@ -14344,8 +14348,49 @@
       <c r="R127" s="5"/>
       <c r="S127" s="32"/>
     </row>
+    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
+        <v>130</v>
+      </c>
+      <c r="B128" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="C128" s="6">
+        <v>43539</v>
+      </c>
+      <c r="D128" s="32" t="s">
+        <v>499</v>
+      </c>
+      <c r="E128" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F128" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G128" s="32" t="s">
+        <v>498</v>
+      </c>
+      <c r="H128" s="32"/>
+      <c r="I128" s="32"/>
+      <c r="J128" s="32"/>
+      <c r="K128" s="32"/>
+      <c r="L128" s="32"/>
+      <c r="M128" s="21"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="33"/>
+      <c r="P128" s="5"/>
+      <c r="Q128" s="32"/>
+      <c r="S128" s="3"/>
+      <c r="T128" s="10"/>
+      <c r="U128" s="10"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:U126" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A2:U128" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="ID Authentication"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="New"/>
@@ -14369,52 +14414,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -14429,14 +14474,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -14447,7 +14492,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -14458,7 +14503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -14469,7 +14514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -14480,7 +14525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -14491,7 +14536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -14502,7 +14547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -14513,7 +14558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -14524,7 +14569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -14547,12 +14592,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="52.21875" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -14560,25 +14605,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="31.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -14763,15 +14808,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -14794,6 +14830,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
@@ -14813,14 +14858,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -14834,4 +14871,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated new CR for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1036862\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{88D4578C-9F13-40A6-B466-28DCFF632FEE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6C8FA60-FB1A-4E56-B8AE-9484F806D9D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="514">
   <si>
     <t>S.No.</t>
   </si>
@@ -4940,6 +4940,18 @@
   </si>
   <si>
     <t>VD needs to changed/ any other intuitive way should be decided</t>
+  </si>
+  <si>
+    <t>MOS-20783</t>
+  </si>
+  <si>
+    <t>ID-Authentication</t>
+  </si>
+  <si>
+    <t>Update Biometric Authentication design independent of the biometric provider/type</t>
+  </si>
+  <si>
+    <t>MOS-1145 - Review of Sprint 10 stories</t>
   </si>
 </sst>
 </file>
@@ -5278,7 +5290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5556,6 +5568,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7117,38 +7132,38 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:W133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S128" sqref="S128:S132"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="49" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.81640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.453125" style="10"/>
+    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="93" t="s">
         <v>209</v>
       </c>
@@ -7173,7 +7188,7 @@
       <c r="T1" s="95"/>
       <c r="U1" s="97"/>
     </row>
-    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7238,7 +7253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7300,7 +7315,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7361,7 +7376,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7423,7 +7438,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7485,7 +7500,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -7547,7 +7562,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -7609,7 +7624,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -7669,7 +7684,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -7729,7 +7744,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7783,7 +7798,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -7840,7 +7855,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7891,7 +7906,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -7951,7 +7966,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -8013,7 +8028,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8075,7 +8090,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8137,7 +8152,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8197,7 +8212,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8259,7 +8274,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8307,7 +8322,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8355,7 +8370,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8415,7 +8430,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8475,7 +8490,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8537,7 +8552,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8587,7 +8602,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8637,7 +8652,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -8697,7 +8712,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -8759,7 +8774,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8809,7 +8824,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8865,7 +8880,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8927,7 +8942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -8989,7 +9004,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9047,7 +9062,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9109,7 +9124,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9166,7 +9181,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9230,7 +9245,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9294,7 +9309,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="171" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9358,7 +9373,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9422,7 +9437,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9476,7 +9491,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9534,7 +9549,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9588,7 +9603,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -9646,7 +9661,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="252" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9706,7 +9721,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9764,7 +9779,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9826,7 +9841,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9888,7 +9903,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -9938,7 +9953,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10000,7 +10015,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10063,7 +10078,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10117,7 +10132,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10167,7 +10182,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10227,7 +10242,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10277,7 +10292,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10331,7 +10346,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10390,7 +10405,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10449,7 +10464,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -10509,7 +10524,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10563,7 +10578,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10617,7 +10632,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10674,7 +10689,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10737,7 +10752,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10798,7 +10813,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10849,7 +10864,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10900,7 +10915,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" ht="228" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10963,7 +10978,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11023,7 +11038,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11084,7 +11099,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="266" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" ht="285" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11144,7 +11159,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11202,7 +11217,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11262,7 +11277,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="168" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" ht="171" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11325,7 +11340,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" ht="171" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11385,7 +11400,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11440,7 +11455,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11501,7 +11516,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11562,7 +11577,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -11622,7 +11637,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" ht="171" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -11684,7 +11699,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -11744,7 +11759,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -11806,7 +11821,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -11866,7 +11881,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="171" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -11928,7 +11943,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -11987,7 +12002,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="252" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12049,7 +12064,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12111,7 +12126,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12171,7 +12186,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12230,7 +12245,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12291,7 +12306,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12346,7 +12361,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12395,7 +12410,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12442,7 +12457,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -12502,7 +12517,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -12560,7 +12575,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -12620,7 +12635,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -12680,7 +12695,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -12740,7 +12755,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -12798,7 +12813,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12849,7 +12864,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -12907,7 +12922,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -12967,7 +12982,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="322" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:21" ht="342" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13027,7 +13042,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13085,7 +13100,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13145,7 +13160,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13205,7 +13220,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13264,7 +13279,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13323,7 +13338,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13374,7 +13389,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13433,7 +13448,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13488,7 +13503,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13543,7 +13558,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13600,7 +13615,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13657,7 +13672,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13714,7 +13729,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13771,7 +13786,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13826,7 +13841,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13872,7 +13887,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -13920,7 +13935,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13971,7 +13986,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -14018,7 +14033,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -14064,7 +14079,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -14111,7 +14126,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14158,7 +14173,7 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>125</v>
       </c>
@@ -14205,7 +14220,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14250,7 +14265,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14297,7 +14312,7 @@
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>128</v>
       </c>
@@ -14342,7 +14357,7 @@
       <c r="T126" s="5"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>129</v>
       </c>
@@ -14391,7 +14406,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>130</v>
       </c>
@@ -14441,7 +14456,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>131</v>
       </c>
@@ -14488,7 +14503,7 @@
       </c>
       <c r="T129" s="32"/>
     </row>
-    <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>132</v>
       </c>
@@ -14535,7 +14550,7 @@
       </c>
       <c r="T130" s="32"/>
     </row>
-    <row r="131" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>133</v>
       </c>
@@ -14582,7 +14597,7 @@
       </c>
       <c r="T131" s="32"/>
     </row>
-    <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>134</v>
       </c>
@@ -14629,22 +14644,55 @@
       </c>
       <c r="T132" s="32"/>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="H133" s="3"/>
-      <c r="O133" s="2"/>
-      <c r="P133" s="2"/>
-      <c r="Q133" s="10"/>
-      <c r="S133" s="3"/>
-      <c r="T133" s="10"/>
+    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
+        <v>135</v>
+      </c>
+      <c r="B133" s="90" t="s">
+        <v>510</v>
+      </c>
+      <c r="C133" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D133" s="98" t="s">
+        <v>513</v>
+      </c>
+      <c r="E133" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F133" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133" s="32" t="s">
+        <v>512</v>
+      </c>
+      <c r="H133" s="32"/>
+      <c r="I133" s="91"/>
+      <c r="J133" s="32"/>
+      <c r="K133" s="32"/>
+      <c r="L133" s="32">
+        <v>1</v>
+      </c>
+      <c r="M133" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N133" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O133" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P133" s="33"/>
+      <c r="Q133" s="14"/>
+      <c r="R133" s="32"/>
+      <c r="S133" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="T133" s="32"/>
       <c r="U133" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:U132" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Pre-registration"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="New"/>
@@ -14662,9 +14710,11 @@
     <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{BB9E9B3E-0E03-4659-A85C-01809F67F8D6}"/>
     <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{1915143A-B9C2-4A24-8FB6-E88C8544E2D0}"/>
     <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{FB48445D-D2D0-4064-9DBB-4BA93CE53469}"/>
+    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{21F8C533-9ACB-4C1F-B101-E6D8754F93FF}"/>
+    <hyperlink ref="D133" r:id="rId9" xr:uid="{AD45D360-3EBC-4492-9C71-A4AF6DC87609}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -14674,52 +14724,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -14734,14 +14784,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -14752,7 +14802,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -14763,7 +14813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -14774,7 +14824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -14785,7 +14835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -14796,7 +14846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -14807,7 +14857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -14818,7 +14868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -14829,7 +14879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -14852,12 +14902,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -14865,25 +14915,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -14896,29 +14946,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15090,6 +15117,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15100,22 +15150,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15133,6 +15167,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
MOS-21370 Added Changes after Discussion with Sasi
Added Changes after Discussion with Sasi.

Sl. No. 136 to 150
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6C8FA60-FB1A-4E56-B8AE-9484F806D9D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416BF122-1AE7-40D7-B58C-EE3D1FCD33FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$132</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -30,12 +30,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="531">
   <si>
     <t>S.No.</t>
   </si>
@@ -4952,6 +4957,387 @@
   </si>
   <si>
     <t>MOS-1145 - Review of Sprint 10 stories</t>
+  </si>
+  <si>
+    <t>Email 
+Dated: 28th Mar 2019
+Subject: Detailed out the Suggestions that were Provided by Sasi for Registration Processor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Filesystem must have permissions.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Both Internal File System (HDFS/CEPH) and External File System (File System
+in DMZ) should have permissions enabled for Upload/Fetch/Delete Files from File
+System.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hash Check for Encrypted Packet (RID, Hash Sequence, Packet Size, Optional Values – Anything Required for Integration, PRID)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>a.	Registration Client needs to send a Hash Sequence for the Encrypted Packet, Size of the Packet, PRID, Any Optional Attributes which would be required for Integration with External System during Packet Meta Data Sync.
+b.	Whenever Registration Processor Stage fetches the Encrypted Packet they need to perform a Check Sum Validation for the Encrypted Packet against the Hashed Sequence received during Packet Metadata Sync.
+i.	Receiving the Packet from Reg Client.
+ii.	Fetching the File from DMZ Zone to Store in HDFS (Secure Zone) File System.
+c.	Encrypt the whole Request Body for the Packet Metadata Sync Request (Same as Encryption Logic used for Packet).
+d.	Center ID should be passed in the Header.
+e.	While Receiving the Packet from Reg Client, Registration Processor can perform size validation using the Packet Size received during Packet Metadata Sync.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Digital Signature of the Response received by Client (One Key Pair can be used for Whole MOSIP Application)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	Server Signs the response with a MOSIP Private Key.
+b.	Client Validates the Request using the MOSIP Public Key.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Virus Scanning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	Virus Scanning should be done In-Memory.
+b.	Virus Scanning should be done before even Storing the File in the File System (even in DMZ Zone).
+c.	Virus Scanning should be done twice, first in Untrusted Zone and Again in Trusted Zone.
+d.	First Virus Scan, for the encrypted and decrypted file should be done in-memory, but it should not be unzipped as Antivirus should take care of unzipping and performing Virus Scan.
+e.	Second Virus Scan can be done on unzipped Files in Pre-Processing Stage (Secure Zone). 
+f.	If Virus Scan Fails, we should not Store the file at all in MOSIP System, the Virus Scanner will store the File in Quarantine Zone. We should not worry about it. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fetching Files from DMZ to HDFS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	The Connector Stage (in Secure Zone) gets triggered and gets a RID.
+b.	The Connector Stage now performs a Check Sum Validation on the File in DMZ Zone.
+c.	Post Successful Validation, the Connector Stage should Pull the File from DMZ File System and Store in HDFS (in Secure Zone).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>OTP Validation for Officer and Supervisor (Can be part of Version 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	Registration Processor should receive a Token from Registration Client, when Officer or Supervisor authenticate the them self during Packet Creation.
+b.	Registration Processor validates the Token in Server and Authenticates the Officer and Supervisor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Parent or Guardian (Introducer) Biometric Validation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+          Scenario 1:
+a.	If RID of the Parent is not found or UIN has not been generated, then wait for Y hrs. and retry for X number of days.
+b.	Even if after X number of days, you don't find the Parent RID, then Perform a Bio De-Dupe for Parent's captured biometrics (Can be taken as part of Version 2)
+I.	if match found in Bio Dedupe, generate Child's UIN.
+II.	if match not found in Bio Dedupe, then reject the Child's UIN.
+          Scenario 2:
+a. If RID of the Parent is Processed or UIN of the Parent is received, Perform 1:1 Match,
+i.	if match found in 1:1 Match, generate Child's UIN.
+ii.	if match not found in 1:1 Match, then reject the Child's UIN.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Parent or Guardian (Introducer) Biometric Validation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+For Current Implementation,	
+a.	For New child registration, capture one slapstick of one biometric of the Parent/Guardian
+b.	For UIN Update of Child, capture the UIN, Name and one slapstick of one biometric of the Parent/Guardian (It could be any Parent/guardian – Same Parent/guardian as during registration or another Parent/guardian)
+c.	Perform 1:1 match of the biometric captured with the biometric of the parent/guardian’s associated with the provided UIN
+I.	If matched - Honor Child’s UIN’s Update request
+II.	If not matched – Reject Child’s UIN’s Update request
+d.	If Parent/guardian’s RID is never received by Registration Processor, then Reject the UIN of the Resident.</t>
+    </r>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Manual Verification after 1:1 Biometric Match Failure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+In the event of demo dedupe potential match and bio 1:1 match failure, manual verification is not required. Such packets can be rejected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>UIN generation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	For New Registration, Inserting Data in ID Database should be handled by Registration Processor.
+b.	For Update Registration, Updating Data in ID Database should be handled by Registration Processor.
+c.	ID Repository API should only perform GET/SEARCH operations.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator and Supervisor Logins should have VIDs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	User ID, Password is present in LDAP.
+b.	Create a Mapping of User ID and VID internally and Authenticate the User.
+c.	Even though the mapped VID is inactive/revoked, the operator can continue with registrations
+d.	What happens when VID gets Expired or Changed by Operator? - TBD </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Adding Trained Flag for Operator or Supervisor in User Table/LDAP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Add Trained/Certified flag in LDAP/User table for Operator or Supervisor who have completed the Training for MOSIP.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Blacklisted Operators and Supervisors in User Table/LDAP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	Add Blacklisted flag in LDAP/User table for Operator or Supervisor, if the Admin Blacklists the User.
+b.	If an Operator/Supervisor is found to be Black Listed in the Packet, then the Packet goes On Hold.
+c.	User History should be stored in MOSIP DB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Use Reference ID instead of UIN,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+We should use UIN Reference ID instead of UIN in Registration Processor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Integration with External System and Appending /Combining the Packets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+a.	Store Multiple Packets in Packet Store (DFS) for Processing.
+b.	The Additional Packets coming in should be as per MOSIP Standards (Pre-Decided).
+c.	Update Section in the Update Packet – Should have only Update Values. 
+d.	Combination of Packet Function to Combine multiple Packets.
+e.	Verify the Combined packet using Check Sum.
+f.	This can be used for Correction Packet Integration.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5136,7 +5522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -5285,12 +5671,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5548,11 +5969,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5569,8 +5990,32 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7130,40 +7575,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:W133"/>
+  <dimension ref="A1:W148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O148" sqref="O148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="60" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.42578125" style="10"/>
+    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="93" t="s">
         <v>209</v>
       </c>
@@ -7177,7 +7622,7 @@
       <c r="I1" s="95"/>
       <c r="J1" s="95"/>
       <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
+      <c r="L1" s="106"/>
       <c r="M1" s="95"/>
       <c r="N1" s="95"/>
       <c r="O1" s="95"/>
@@ -7188,7 +7633,7 @@
       <c r="T1" s="95"/>
       <c r="U1" s="97"/>
     </row>
-    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7253,7 +7698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7315,7 +7760,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7376,7 +7821,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7438,7 +7883,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7500,7 +7945,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -7562,7 +8007,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -7624,7 +8069,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -7684,7 +8129,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -7744,7 +8189,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -7798,7 +8243,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -7855,7 +8300,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -7906,7 +8351,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -7966,7 +8411,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -8028,7 +8473,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8090,7 +8535,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8152,7 +8597,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8212,7 +8657,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8274,7 +8719,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8322,7 +8767,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8370,7 +8815,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8430,7 +8875,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8490,7 +8935,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -8552,7 +8997,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -8602,7 +9047,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -8652,7 +9097,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -8712,7 +9157,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -8774,7 +9219,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -8824,7 +9269,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -8880,7 +9325,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -8942,7 +9387,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9004,7 +9449,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9062,7 +9507,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9124,7 +9569,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9181,7 +9626,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9245,7 +9690,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9309,7 +9754,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="171" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9373,7 +9818,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9437,7 +9882,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9491,7 +9936,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -9549,7 +9994,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -9603,7 +10048,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -9661,7 +10106,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -9721,7 +10166,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -9779,7 +10224,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -9841,7 +10286,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -9903,7 +10348,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -9953,7 +10398,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10015,7 +10460,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10078,7 +10523,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10132,7 +10577,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10182,7 +10627,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10242,7 +10687,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10292,7 +10737,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10346,7 +10791,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10405,7 +10850,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10464,7 +10909,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -10524,7 +10969,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -10578,7 +11023,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -10632,7 +11077,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -10689,7 +11134,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -10752,7 +11197,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -10813,7 +11258,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -10864,7 +11309,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -10915,7 +11360,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -10978,7 +11423,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11038,7 +11483,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11099,7 +11544,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="285" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11159,7 +11604,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11217,7 +11662,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11277,7 +11722,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11340,7 +11785,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11400,7 +11845,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11455,7 +11900,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -11516,7 +11961,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -11577,7 +12022,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -11637,7 +12082,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -11699,7 +12144,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -11759,7 +12204,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -11821,7 +12266,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -11881,7 +12326,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -11943,7 +12388,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -12002,7 +12447,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12064,7 +12509,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12126,7 +12571,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12186,7 +12631,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12245,7 +12690,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12306,7 +12751,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12361,7 +12806,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12410,7 +12855,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12457,7 +12902,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -12517,7 +12962,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -12575,7 +13020,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -12635,7 +13080,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -12695,7 +13140,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -12755,7 +13200,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -12813,7 +13258,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -12864,7 +13309,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -12922,7 +13367,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -12982,7 +13427,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="342" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13042,7 +13487,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13100,7 +13545,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13160,7 +13605,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13220,7 +13665,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13279,7 +13724,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13338,7 +13783,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13389,7 +13834,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13448,7 +13893,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13503,7 +13948,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -13558,7 +14003,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -13615,7 +14060,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -13672,7 +14117,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -13729,7 +14174,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -13786,7 +14231,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -13841,7 +14286,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -13887,11 +14332,11 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
-      <c r="B117" s="92" t="s">
+      <c r="B117" s="91" t="s">
         <v>425</v>
       </c>
       <c r="C117" s="37">
@@ -13935,7 +14380,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -13986,7 +14431,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -14033,7 +14478,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -14079,7 +14524,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -14126,7 +14571,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14173,7 +14618,7 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>125</v>
       </c>
@@ -14220,7 +14665,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14265,7 +14710,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14312,7 +14757,7 @@
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>128</v>
       </c>
@@ -14357,7 +14802,7 @@
       <c r="T126" s="5"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>129</v>
       </c>
@@ -14406,58 +14851,58 @@
         <v>508</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>130</v>
       </c>
-      <c r="B128" s="90" t="s">
+      <c r="B128" s="104" t="s">
         <v>493</v>
       </c>
-      <c r="C128" s="6">
+      <c r="C128" s="37">
         <v>43550</v>
       </c>
-      <c r="D128" s="32" t="s">
+      <c r="D128" s="28" t="s">
         <v>491</v>
       </c>
-      <c r="E128" s="32" t="s">
+      <c r="E128" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F128" s="32" t="s">
+      <c r="F128" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G128" s="32" t="s">
+      <c r="G128" s="28" t="s">
         <v>494</v>
       </c>
-      <c r="I128" s="32" t="s">
+      <c r="I128" s="28" t="s">
         <v>433</v>
       </c>
-      <c r="J128" s="91"/>
-      <c r="K128" s="32"/>
-      <c r="L128" s="32">
+      <c r="J128" s="105"/>
+      <c r="K128" s="28"/>
+      <c r="L128" s="28">
         <v>1</v>
       </c>
-      <c r="M128" s="32" t="s">
+      <c r="M128" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N128" s="32" t="s">
+      <c r="N128" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O128" s="21">
+      <c r="O128" s="38">
         <v>43550</v>
       </c>
       <c r="P128" s="5"/>
-      <c r="Q128" s="5"/>
-      <c r="R128" s="33"/>
-      <c r="S128" s="14" t="s">
+      <c r="Q128" s="39"/>
+      <c r="R128" s="89"/>
+      <c r="S128" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="T128" s="32"/>
+      <c r="T128" s="28"/>
       <c r="U128" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="5">
+    <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="A129" s="98">
         <v>131</v>
       </c>
       <c r="B129" s="90" t="s">
@@ -14481,7 +14926,7 @@
       <c r="I129" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="J129" s="91"/>
+      <c r="J129" s="32"/>
       <c r="K129" s="32"/>
       <c r="L129" s="32">
         <v>1</v>
@@ -14495,16 +14940,17 @@
       <c r="O129" s="21">
         <v>43550</v>
       </c>
-      <c r="P129" s="5"/>
+      <c r="P129" s="102"/>
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
         <v>505</v>
       </c>
       <c r="T129" s="32"/>
-    </row>
-    <row r="130" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="5">
+      <c r="U129" s="32"/>
+    </row>
+    <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A130" s="98">
         <v>132</v>
       </c>
       <c r="B130" s="90" t="s">
@@ -14528,7 +14974,7 @@
       <c r="I130" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="J130" s="91"/>
+      <c r="J130" s="32"/>
       <c r="K130" s="32"/>
       <c r="L130" s="32">
         <v>1</v>
@@ -14542,16 +14988,17 @@
       <c r="O130" s="21">
         <v>43550</v>
       </c>
-      <c r="P130" s="5"/>
+      <c r="P130" s="102"/>
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
         <v>505</v>
       </c>
       <c r="T130" s="32"/>
-    </row>
-    <row r="131" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="5">
+      <c r="U130" s="32"/>
+    </row>
+    <row r="131" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A131" s="98">
         <v>133</v>
       </c>
       <c r="B131" s="90" t="s">
@@ -14575,7 +15022,7 @@
       <c r="I131" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="J131" s="91"/>
+      <c r="J131" s="32"/>
       <c r="K131" s="32"/>
       <c r="L131" s="32">
         <v>1</v>
@@ -14589,16 +15036,17 @@
       <c r="O131" s="21">
         <v>43550</v>
       </c>
-      <c r="P131" s="5"/>
+      <c r="P131" s="102"/>
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
         <v>505</v>
       </c>
       <c r="T131" s="32"/>
-    </row>
-    <row r="132" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
+      <c r="U131" s="32"/>
+    </row>
+    <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A132" s="98">
         <v>134</v>
       </c>
       <c r="B132" s="90" t="s">
@@ -14622,7 +15070,7 @@
       <c r="I132" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="J132" s="91"/>
+      <c r="J132" s="32"/>
       <c r="K132" s="32"/>
       <c r="L132" s="32">
         <v>1</v>
@@ -14636,16 +15084,17 @@
       <c r="O132" s="21">
         <v>43550</v>
       </c>
-      <c r="P132" s="5"/>
+      <c r="P132" s="102"/>
       <c r="Q132" s="5"/>
       <c r="R132" s="33"/>
       <c r="S132" s="14" t="s">
         <v>505</v>
       </c>
       <c r="T132" s="32"/>
-    </row>
-    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
+      <c r="U132" s="32"/>
+    </row>
+    <row r="133" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="A133" s="98">
         <v>135</v>
       </c>
       <c r="B133" s="90" t="s">
@@ -14654,7 +15103,7 @@
       <c r="C133" s="6">
         <v>43552</v>
       </c>
-      <c r="D133" s="98" t="s">
+      <c r="D133" s="92" t="s">
         <v>513</v>
       </c>
       <c r="E133" s="32" t="s">
@@ -14666,8 +15115,8 @@
       <c r="G133" s="32" t="s">
         <v>512</v>
       </c>
-      <c r="H133" s="32"/>
-      <c r="I133" s="91"/>
+      <c r="H133" s="100"/>
+      <c r="I133" s="32"/>
       <c r="J133" s="32"/>
       <c r="K133" s="32"/>
       <c r="L133" s="32">
@@ -14682,14 +15131,689 @@
       <c r="O133" s="21">
         <v>43552</v>
       </c>
-      <c r="P133" s="33"/>
+      <c r="P133" s="103"/>
       <c r="Q133" s="14"/>
       <c r="R133" s="32"/>
       <c r="S133" s="14" t="s">
         <v>505</v>
       </c>
       <c r="T133" s="32"/>
-      <c r="U133" s="10"/>
+      <c r="U133" s="33"/>
+    </row>
+    <row r="134" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+      <c r="A134" s="98">
+        <v>136</v>
+      </c>
+      <c r="B134" s="31"/>
+      <c r="C134" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D134" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E134" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F134" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G134" s="32" t="s">
+        <v>515</v>
+      </c>
+      <c r="H134" s="100"/>
+      <c r="I134" s="32"/>
+      <c r="J134" s="32"/>
+      <c r="K134" s="32"/>
+      <c r="L134" s="32">
+        <v>1</v>
+      </c>
+      <c r="M134" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N134" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O134" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P134" s="102"/>
+      <c r="Q134" s="33"/>
+      <c r="R134" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="S134" s="32"/>
+      <c r="T134" s="33"/>
+      <c r="U134" s="33"/>
+    </row>
+    <row r="135" spans="1:21" ht="266" x14ac:dyDescent="0.35">
+      <c r="A135" s="98">
+        <v>137</v>
+      </c>
+      <c r="B135" s="31"/>
+      <c r="C135" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D135" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E135" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F135" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G135" s="32" t="s">
+        <v>516</v>
+      </c>
+      <c r="H135" s="100"/>
+      <c r="I135" s="32"/>
+      <c r="J135" s="32"/>
+      <c r="K135" s="32"/>
+      <c r="L135" s="32">
+        <v>1</v>
+      </c>
+      <c r="M135" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N135" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O135" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P135" s="102"/>
+      <c r="Q135" s="32"/>
+      <c r="R135" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="S135" s="33"/>
+      <c r="T135" s="33"/>
+      <c r="U135" s="33"/>
+    </row>
+    <row r="136" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+      <c r="A136" s="98">
+        <v>138</v>
+      </c>
+      <c r="B136" s="31"/>
+      <c r="C136" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D136" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E136" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F136" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" s="32" t="s">
+        <v>517</v>
+      </c>
+      <c r="H136" s="100"/>
+      <c r="I136" s="32"/>
+      <c r="J136" s="32"/>
+      <c r="K136" s="32"/>
+      <c r="L136" s="32">
+        <v>1</v>
+      </c>
+      <c r="M136" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N136" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O136" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P136" s="10"/>
+      <c r="Q136" s="33"/>
+      <c r="R136" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S136" s="33"/>
+      <c r="T136" s="33"/>
+      <c r="U136" s="33"/>
+    </row>
+    <row r="137" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+      <c r="A137" s="98">
+        <v>139</v>
+      </c>
+      <c r="B137" s="31"/>
+      <c r="C137" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D137" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E137" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F137" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G137" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="H137" s="100"/>
+      <c r="I137" s="32"/>
+      <c r="J137" s="32"/>
+      <c r="K137" s="21"/>
+      <c r="L137" s="14">
+        <v>1</v>
+      </c>
+      <c r="M137" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N137" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O137" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P137" s="10"/>
+      <c r="Q137" s="33"/>
+      <c r="R137" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S137" s="33"/>
+      <c r="T137" s="33"/>
+      <c r="U137" s="33"/>
+    </row>
+    <row r="138" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+      <c r="A138" s="98">
+        <v>140</v>
+      </c>
+      <c r="B138" s="31"/>
+      <c r="C138" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D138" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E138" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F138" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G138" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="H138" s="100"/>
+      <c r="I138" s="32"/>
+      <c r="J138" s="21"/>
+      <c r="K138" s="5"/>
+      <c r="L138" s="14">
+        <v>1</v>
+      </c>
+      <c r="M138" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N138" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O138" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P138" s="10"/>
+      <c r="Q138" s="33"/>
+      <c r="R138" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S138" s="33"/>
+      <c r="T138" s="33"/>
+      <c r="U138" s="33"/>
+    </row>
+    <row r="139" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+      <c r="A139" s="98">
+        <v>141</v>
+      </c>
+      <c r="B139" s="31"/>
+      <c r="C139" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D139" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E139" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F139" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G139" s="32" t="s">
+        <v>520</v>
+      </c>
+      <c r="H139" s="100"/>
+      <c r="I139" s="21"/>
+      <c r="J139" s="5"/>
+      <c r="K139" s="33"/>
+      <c r="L139" s="32">
+        <v>2</v>
+      </c>
+      <c r="M139" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N139" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O139" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P139" s="10"/>
+      <c r="Q139" s="33"/>
+      <c r="R139" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S139" s="33"/>
+      <c r="T139" s="33"/>
+      <c r="U139" s="33"/>
+    </row>
+    <row r="140" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+      <c r="A140" s="98">
+        <v>142</v>
+      </c>
+      <c r="B140" s="31"/>
+      <c r="C140" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D140" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E140" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F140" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G140" s="32" t="s">
+        <v>521</v>
+      </c>
+      <c r="H140" s="101"/>
+      <c r="I140" s="5"/>
+      <c r="J140" s="33"/>
+      <c r="K140" s="32"/>
+      <c r="L140" s="14">
+        <v>2</v>
+      </c>
+      <c r="M140" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N140" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O140" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="33"/>
+      <c r="R140" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S140" s="33"/>
+      <c r="T140" s="33"/>
+      <c r="U140" s="33"/>
+    </row>
+    <row r="141" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+      <c r="A141" s="98">
+        <v>143</v>
+      </c>
+      <c r="B141" s="31"/>
+      <c r="C141" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D141" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E141" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F141" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G141" s="32" t="s">
+        <v>522</v>
+      </c>
+      <c r="H141" s="102"/>
+      <c r="I141" s="33"/>
+      <c r="J141" s="32"/>
+      <c r="K141" s="33"/>
+      <c r="L141" s="14">
+        <v>1</v>
+      </c>
+      <c r="M141" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N141" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O141" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P141" s="10"/>
+      <c r="Q141" s="33"/>
+      <c r="R141" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S141" s="33"/>
+      <c r="T141" s="33"/>
+      <c r="U141" s="33"/>
+    </row>
+    <row r="142" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+      <c r="A142" s="98">
+        <v>144</v>
+      </c>
+      <c r="B142" s="31"/>
+      <c r="C142" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D142" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E142" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F142" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G142" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="H142" s="33"/>
+      <c r="I142" s="32"/>
+      <c r="J142" s="33"/>
+      <c r="K142" s="14"/>
+      <c r="L142" s="14">
+        <v>1</v>
+      </c>
+      <c r="M142" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N142" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O142" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P142" s="99"/>
+      <c r="Q142" s="33"/>
+      <c r="R142" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S142" s="33"/>
+      <c r="T142" s="33"/>
+      <c r="U142" s="33"/>
+    </row>
+    <row r="143" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+      <c r="A143" s="98">
+        <v>145</v>
+      </c>
+      <c r="B143" s="31"/>
+      <c r="C143" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D143" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E143" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F143" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G143" s="32" t="s">
+        <v>525</v>
+      </c>
+      <c r="H143" s="32"/>
+      <c r="I143" s="33"/>
+      <c r="J143" s="14"/>
+      <c r="K143" s="14"/>
+      <c r="L143" s="32">
+        <v>1</v>
+      </c>
+      <c r="M143" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N143" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O143" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P143" s="99"/>
+      <c r="Q143" s="33"/>
+      <c r="R143" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S143" s="33"/>
+      <c r="T143" s="33"/>
+      <c r="U143" s="33"/>
+    </row>
+    <row r="144" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+      <c r="A144" s="98">
+        <v>146</v>
+      </c>
+      <c r="B144" s="31"/>
+      <c r="C144" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D144" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E144" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F144" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G144" s="32" t="s">
+        <v>526</v>
+      </c>
+      <c r="H144" s="33"/>
+      <c r="I144" s="14"/>
+      <c r="J144" s="14"/>
+      <c r="K144" s="32"/>
+      <c r="L144" s="32">
+        <v>1</v>
+      </c>
+      <c r="M144" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N144" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O144" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="33"/>
+      <c r="R144" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S144" s="33"/>
+      <c r="T144" s="33"/>
+      <c r="U144" s="33"/>
+    </row>
+    <row r="145" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+      <c r="A145" s="98">
+        <v>147</v>
+      </c>
+      <c r="B145" s="31"/>
+      <c r="C145" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D145" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E145" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="F145" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G145" s="32" t="s">
+        <v>528</v>
+      </c>
+      <c r="H145" s="14"/>
+      <c r="I145" s="14"/>
+      <c r="J145" s="32"/>
+      <c r="K145" s="32"/>
+      <c r="L145" s="32">
+        <v>1</v>
+      </c>
+      <c r="M145" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N145" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O145" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P145" s="10"/>
+      <c r="Q145" s="33"/>
+      <c r="R145" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S145" s="33"/>
+      <c r="T145" s="33"/>
+      <c r="U145" s="33"/>
+    </row>
+    <row r="146" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+      <c r="A146" s="98">
+        <v>148</v>
+      </c>
+      <c r="B146" s="31"/>
+      <c r="C146" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D146" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E146" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="F146" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G146" s="32" t="s">
+        <v>527</v>
+      </c>
+      <c r="H146" s="14"/>
+      <c r="I146" s="32"/>
+      <c r="J146" s="32"/>
+      <c r="K146" s="21"/>
+      <c r="L146" s="32">
+        <v>1</v>
+      </c>
+      <c r="M146" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N146" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O146" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="33"/>
+      <c r="R146" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S146" s="33"/>
+      <c r="T146" s="33"/>
+      <c r="U146" s="33"/>
+    </row>
+    <row r="147" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+      <c r="A147" s="98">
+        <v>149</v>
+      </c>
+      <c r="B147" s="31"/>
+      <c r="C147" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D147" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E147" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F147" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G147" s="32" t="s">
+        <v>529</v>
+      </c>
+      <c r="H147" s="32"/>
+      <c r="I147" s="32"/>
+      <c r="J147" s="21"/>
+      <c r="K147" s="21"/>
+      <c r="L147" s="32">
+        <v>1</v>
+      </c>
+      <c r="M147" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N147" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O147" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P147" s="10"/>
+      <c r="Q147" s="33"/>
+      <c r="R147" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S147" s="33"/>
+      <c r="T147" s="33"/>
+      <c r="U147" s="33"/>
+    </row>
+    <row r="148" spans="1:21" ht="140" x14ac:dyDescent="0.35">
+      <c r="A148" s="98">
+        <v>150</v>
+      </c>
+      <c r="B148" s="31"/>
+      <c r="C148" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D148" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E148" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F148" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G148" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="H148" s="32"/>
+      <c r="I148" s="21"/>
+      <c r="J148" s="21"/>
+      <c r="K148" s="21"/>
+      <c r="L148" s="32">
+        <v>1</v>
+      </c>
+      <c r="M148" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N148" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O148" s="21">
+        <v>43552</v>
+      </c>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="33"/>
+      <c r="R148" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="S148" s="33"/>
+      <c r="T148" s="33"/>
+      <c r="U148" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:U132" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -14724,52 +15848,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -14784,14 +15908,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -14802,7 +15926,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -14813,7 +15937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -14824,7 +15948,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -14835,7 +15959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -14846,7 +15970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -14857,7 +15981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -14868,7 +15992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -14879,7 +16003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -14902,12 +16026,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -14915,25 +16039,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -14946,6 +16070,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15117,52 +16273,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15184,9 +16298,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added few CR's for Reg client
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416BF122-1AE7-40D7-B58C-EE3D1FCD33FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -19,9 +18,9 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$148</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="542">
   <si>
     <t>S.No.</t>
   </si>
@@ -5339,11 +5338,44 @@
 f.	This can be used for Correction Packet Integration.</t>
     </r>
   </si>
+  <si>
+    <t>MOS-21461</t>
+  </si>
+  <si>
+    <t>MOS-21470</t>
+  </si>
+  <si>
+    <t>MOS-21517</t>
+  </si>
+  <si>
+    <t>MOS-21523</t>
+  </si>
+  <si>
+    <t>MOS-21573</t>
+  </si>
+  <si>
+    <t>Registration processor discussion with Sasi</t>
+  </si>
+  <si>
+    <t>Tech story - Send a Hash Sequence for the Encrypted Packet</t>
+  </si>
+  <si>
+    <t>As MOSIP registration client, for UIN Update of Child, capture the UIN, Name and one biometric of the Parent/Guardian</t>
+  </si>
+  <si>
+    <t>As MOSIP registration client, for new registration of child capture any one biometric of the Parent/Guardian</t>
+  </si>
+  <si>
+    <t>Tech story - Registration Client should send a token to Registration processor, when Officer or Supervisor authenticate themselves during Packet Creation</t>
+  </si>
+  <si>
+    <t>Tech story--Generate packet using centre id and unique machine id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -5522,7 +5554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -5706,12 +5738,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5975,21 +6018,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6014,8 +6042,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6047,7 +6093,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6064,7 +6110,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:U70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7225,7 +7271,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7573,13 +7619,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:W148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:W161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O148" sqref="O148"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -7609,29 +7655,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="101" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="97"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="106"/>
     </row>
     <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -8189,7 +8235,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8300,7 +8346,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="280" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8935,7 +8981,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9449,7 +9495,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9690,7 +9736,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9882,7 +9928,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9994,7 +10040,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10166,7 +10212,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10523,7 +10569,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10737,7 +10783,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10969,7 +11015,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11023,7 +11069,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11258,7 +11304,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11309,7 +11355,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11845,7 +11891,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12388,7 +12434,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -14761,7 +14807,7 @@
       <c r="A126" s="5">
         <v>128</v>
       </c>
-      <c r="B126" s="90" t="s">
+      <c r="B126" s="31" t="s">
         <v>468</v>
       </c>
       <c r="C126" s="6">
@@ -14796,10 +14842,7 @@
       <c r="O126" s="21">
         <v>43531</v>
       </c>
-      <c r="Q126" s="5"/>
-      <c r="R126" s="5"/>
       <c r="S126" s="33"/>
-      <c r="T126" s="5"/>
       <c r="U126" s="32"/>
     </row>
     <row r="127" spans="1:21" ht="70" x14ac:dyDescent="0.35">
@@ -14855,7 +14898,7 @@
       <c r="A128" s="5">
         <v>130</v>
       </c>
-      <c r="B128" s="104" t="s">
+      <c r="B128" s="99" t="s">
         <v>493</v>
       </c>
       <c r="C128" s="37">
@@ -14876,7 +14919,7 @@
       <c r="I128" s="28" t="s">
         <v>433</v>
       </c>
-      <c r="J128" s="105"/>
+      <c r="J128" s="100"/>
       <c r="K128" s="28"/>
       <c r="L128" s="28">
         <v>1</v>
@@ -14902,7 +14945,7 @@
       </c>
     </row>
     <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A129" s="98">
+      <c r="A129" s="93">
         <v>131</v>
       </c>
       <c r="B129" s="90" t="s">
@@ -14940,7 +14983,7 @@
       <c r="O129" s="21">
         <v>43550</v>
       </c>
-      <c r="P129" s="102"/>
+      <c r="P129" s="97"/>
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
@@ -14950,7 +14993,7 @@
       <c r="U129" s="32"/>
     </row>
     <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A130" s="98">
+      <c r="A130" s="93">
         <v>132</v>
       </c>
       <c r="B130" s="90" t="s">
@@ -14988,7 +15031,7 @@
       <c r="O130" s="21">
         <v>43550</v>
       </c>
-      <c r="P130" s="102"/>
+      <c r="P130" s="97"/>
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
@@ -14998,7 +15041,7 @@
       <c r="U130" s="32"/>
     </row>
     <row r="131" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A131" s="98">
+      <c r="A131" s="93">
         <v>133</v>
       </c>
       <c r="B131" s="90" t="s">
@@ -15036,7 +15079,7 @@
       <c r="O131" s="21">
         <v>43550</v>
       </c>
-      <c r="P131" s="102"/>
+      <c r="P131" s="97"/>
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
@@ -15046,7 +15089,7 @@
       <c r="U131" s="32"/>
     </row>
     <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A132" s="98">
+      <c r="A132" s="93">
         <v>134</v>
       </c>
       <c r="B132" s="90" t="s">
@@ -15084,7 +15127,7 @@
       <c r="O132" s="21">
         <v>43550</v>
       </c>
-      <c r="P132" s="102"/>
+      <c r="P132" s="97"/>
       <c r="Q132" s="5"/>
       <c r="R132" s="33"/>
       <c r="S132" s="14" t="s">
@@ -15094,7 +15137,7 @@
       <c r="U132" s="32"/>
     </row>
     <row r="133" spans="1:21" ht="29" x14ac:dyDescent="0.35">
-      <c r="A133" s="98">
+      <c r="A133" s="93">
         <v>135</v>
       </c>
       <c r="B133" s="90" t="s">
@@ -15115,7 +15158,7 @@
       <c r="G133" s="32" t="s">
         <v>512</v>
       </c>
-      <c r="H133" s="100"/>
+      <c r="H133" s="95"/>
       <c r="I133" s="32"/>
       <c r="J133" s="32"/>
       <c r="K133" s="32"/>
@@ -15131,7 +15174,7 @@
       <c r="O133" s="21">
         <v>43552</v>
       </c>
-      <c r="P133" s="103"/>
+      <c r="P133" s="98"/>
       <c r="Q133" s="14"/>
       <c r="R133" s="32"/>
       <c r="S133" s="14" t="s">
@@ -15141,7 +15184,7 @@
       <c r="U133" s="33"/>
     </row>
     <row r="134" spans="1:21" ht="84" x14ac:dyDescent="0.35">
-      <c r="A134" s="98">
+      <c r="A134" s="93">
         <v>136</v>
       </c>
       <c r="B134" s="31"/>
@@ -15160,7 +15203,7 @@
       <c r="G134" s="32" t="s">
         <v>515</v>
       </c>
-      <c r="H134" s="100"/>
+      <c r="H134" s="95"/>
       <c r="I134" s="32"/>
       <c r="J134" s="32"/>
       <c r="K134" s="32"/>
@@ -15176,7 +15219,7 @@
       <c r="O134" s="21">
         <v>43552</v>
       </c>
-      <c r="P134" s="102"/>
+      <c r="P134" s="97"/>
       <c r="Q134" s="33"/>
       <c r="R134" s="5" t="s">
         <v>523</v>
@@ -15186,7 +15229,7 @@
       <c r="U134" s="33"/>
     </row>
     <row r="135" spans="1:21" ht="266" x14ac:dyDescent="0.35">
-      <c r="A135" s="98">
+      <c r="A135" s="93">
         <v>137</v>
       </c>
       <c r="B135" s="31"/>
@@ -15205,7 +15248,7 @@
       <c r="G135" s="32" t="s">
         <v>516</v>
       </c>
-      <c r="H135" s="100"/>
+      <c r="H135" s="95"/>
       <c r="I135" s="32"/>
       <c r="J135" s="32"/>
       <c r="K135" s="32"/>
@@ -15221,7 +15264,7 @@
       <c r="O135" s="21">
         <v>43552</v>
       </c>
-      <c r="P135" s="102"/>
+      <c r="P135" s="97"/>
       <c r="Q135" s="32"/>
       <c r="R135" s="5" t="s">
         <v>523</v>
@@ -15231,7 +15274,7 @@
       <c r="U135" s="33"/>
     </row>
     <row r="136" spans="1:21" ht="70" x14ac:dyDescent="0.35">
-      <c r="A136" s="98">
+      <c r="A136" s="93">
         <v>138</v>
       </c>
       <c r="B136" s="31"/>
@@ -15250,7 +15293,7 @@
       <c r="G136" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="H136" s="100"/>
+      <c r="H136" s="95"/>
       <c r="I136" s="32"/>
       <c r="J136" s="32"/>
       <c r="K136" s="32"/>
@@ -15276,7 +15319,7 @@
       <c r="U136" s="33"/>
     </row>
     <row r="137" spans="1:21" ht="196" x14ac:dyDescent="0.35">
-      <c r="A137" s="98">
+      <c r="A137" s="93">
         <v>139</v>
       </c>
       <c r="B137" s="31"/>
@@ -15295,7 +15338,7 @@
       <c r="G137" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="H137" s="100"/>
+      <c r="H137" s="95"/>
       <c r="I137" s="32"/>
       <c r="J137" s="32"/>
       <c r="K137" s="21"/>
@@ -15321,7 +15364,7 @@
       <c r="U137" s="33"/>
     </row>
     <row r="138" spans="1:21" ht="98" x14ac:dyDescent="0.35">
-      <c r="A138" s="98">
+      <c r="A138" s="93">
         <v>140</v>
       </c>
       <c r="B138" s="31"/>
@@ -15340,7 +15383,7 @@
       <c r="G138" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="H138" s="100"/>
+      <c r="H138" s="95"/>
       <c r="I138" s="32"/>
       <c r="J138" s="21"/>
       <c r="K138" s="5"/>
@@ -15366,7 +15409,7 @@
       <c r="U138" s="33"/>
     </row>
     <row r="139" spans="1:21" ht="84" x14ac:dyDescent="0.35">
-      <c r="A139" s="98">
+      <c r="A139" s="93">
         <v>141</v>
       </c>
       <c r="B139" s="31"/>
@@ -15385,7 +15428,7 @@
       <c r="G139" s="32" t="s">
         <v>520</v>
       </c>
-      <c r="H139" s="100"/>
+      <c r="H139" s="95"/>
       <c r="I139" s="21"/>
       <c r="J139" s="5"/>
       <c r="K139" s="33"/>
@@ -15411,7 +15454,7 @@
       <c r="U139" s="33"/>
     </row>
     <row r="140" spans="1:21" ht="196" x14ac:dyDescent="0.35">
-      <c r="A140" s="98">
+      <c r="A140" s="93">
         <v>142</v>
       </c>
       <c r="B140" s="31"/>
@@ -15430,7 +15473,7 @@
       <c r="G140" s="32" t="s">
         <v>521</v>
       </c>
-      <c r="H140" s="101"/>
+      <c r="H140" s="96"/>
       <c r="I140" s="5"/>
       <c r="J140" s="33"/>
       <c r="K140" s="32"/>
@@ -15456,7 +15499,7 @@
       <c r="U140" s="33"/>
     </row>
     <row r="141" spans="1:21" ht="196" x14ac:dyDescent="0.35">
-      <c r="A141" s="98">
+      <c r="A141" s="93">
         <v>143</v>
       </c>
       <c r="B141" s="31"/>
@@ -15475,7 +15518,7 @@
       <c r="G141" s="32" t="s">
         <v>522</v>
       </c>
-      <c r="H141" s="102"/>
+      <c r="H141" s="97"/>
       <c r="I141" s="33"/>
       <c r="J141" s="32"/>
       <c r="K141" s="33"/>
@@ -15501,7 +15544,7 @@
       <c r="U141" s="33"/>
     </row>
     <row r="142" spans="1:21" ht="70" x14ac:dyDescent="0.35">
-      <c r="A142" s="98">
+      <c r="A142" s="93">
         <v>144</v>
       </c>
       <c r="B142" s="31"/>
@@ -15536,7 +15579,7 @@
       <c r="O142" s="21">
         <v>43552</v>
       </c>
-      <c r="P142" s="99"/>
+      <c r="P142" s="94"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
         <v>523</v>
@@ -15546,7 +15589,7 @@
       <c r="U142" s="33"/>
     </row>
     <row r="143" spans="1:21" ht="84" x14ac:dyDescent="0.35">
-      <c r="A143" s="98">
+      <c r="A143" s="93">
         <v>145</v>
       </c>
       <c r="B143" s="31"/>
@@ -15581,7 +15624,7 @@
       <c r="O143" s="21">
         <v>43552</v>
       </c>
-      <c r="P143" s="99"/>
+      <c r="P143" s="94"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
         <v>523</v>
@@ -15591,7 +15634,7 @@
       <c r="U143" s="33"/>
     </row>
     <row r="144" spans="1:21" ht="112" x14ac:dyDescent="0.35">
-      <c r="A144" s="98">
+      <c r="A144" s="93">
         <v>146</v>
       </c>
       <c r="B144" s="31"/>
@@ -15636,7 +15679,7 @@
       <c r="U144" s="33"/>
     </row>
     <row r="145" spans="1:21" ht="84" x14ac:dyDescent="0.35">
-      <c r="A145" s="98">
+      <c r="A145" s="93">
         <v>147</v>
       </c>
       <c r="B145" s="31"/>
@@ -15681,7 +15724,7 @@
       <c r="U145" s="33"/>
     </row>
     <row r="146" spans="1:21" ht="70" x14ac:dyDescent="0.35">
-      <c r="A146" s="98">
+      <c r="A146" s="93">
         <v>148</v>
       </c>
       <c r="B146" s="31"/>
@@ -15726,7 +15769,7 @@
       <c r="U146" s="33"/>
     </row>
     <row r="147" spans="1:21" ht="70" x14ac:dyDescent="0.35">
-      <c r="A147" s="98">
+      <c r="A147" s="93">
         <v>149</v>
       </c>
       <c r="B147" s="31"/>
@@ -15771,71 +15814,442 @@
       <c r="U147" s="33"/>
     </row>
     <row r="148" spans="1:21" ht="140" x14ac:dyDescent="0.35">
-      <c r="A148" s="98">
+      <c r="A148" s="107">
         <v>150</v>
       </c>
-      <c r="B148" s="31"/>
-      <c r="C148" s="6">
+      <c r="B148" s="91"/>
+      <c r="C148" s="37">
         <v>43552</v>
       </c>
-      <c r="D148" s="32" t="s">
+      <c r="D148" s="28" t="s">
         <v>514</v>
       </c>
-      <c r="E148" s="32" t="s">
+      <c r="E148" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F148" s="32" t="s">
+      <c r="F148" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G148" s="32" t="s">
+      <c r="G148" s="28" t="s">
         <v>530</v>
       </c>
       <c r="H148" s="32"/>
-      <c r="I148" s="21"/>
-      <c r="J148" s="21"/>
-      <c r="K148" s="21"/>
-      <c r="L148" s="32">
+      <c r="I148" s="38"/>
+      <c r="J148" s="38"/>
+      <c r="K148" s="38"/>
+      <c r="L148" s="28">
         <v>1</v>
       </c>
-      <c r="M148" s="21" t="s">
+      <c r="M148" s="38" t="s">
         <v>74</v>
       </c>
       <c r="N148" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="O148" s="21">
+      <c r="O148" s="38">
         <v>43552</v>
       </c>
       <c r="P148" s="10"/>
-      <c r="Q148" s="33"/>
-      <c r="R148" s="33" t="s">
+      <c r="Q148" s="89"/>
+      <c r="R148" s="89" t="s">
         <v>523</v>
       </c>
-      <c r="S148" s="33"/>
-      <c r="T148" s="33"/>
-      <c r="U148" s="33"/>
+      <c r="S148" s="89"/>
+      <c r="T148" s="89"/>
+      <c r="U148" s="89"/>
+    </row>
+    <row r="149" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A149" s="5">
+        <f>1+A126</f>
+        <v>129</v>
+      </c>
+      <c r="B149" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="C149" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D149" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="E149" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F149" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G149" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="I149" s="32"/>
+      <c r="J149" s="32"/>
+      <c r="K149" s="32"/>
+      <c r="L149" s="32">
+        <v>1</v>
+      </c>
+      <c r="M149" s="32"/>
+      <c r="N149" s="32"/>
+      <c r="O149" s="32"/>
+      <c r="Q149" s="5">
+        <v>15</v>
+      </c>
+      <c r="R149" s="5">
+        <v>10</v>
+      </c>
+      <c r="S149" s="33"/>
+      <c r="T149" s="5">
+        <v>11</v>
+      </c>
+      <c r="U149" s="32"/>
+    </row>
+    <row r="150" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A150" s="5">
+        <f t="shared" ref="A150:A153" si="8">1+A127</f>
+        <v>130</v>
+      </c>
+      <c r="B150" s="31" t="s">
+        <v>532</v>
+      </c>
+      <c r="C150" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D150" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="E150" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F150" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G150" s="32" t="s">
+        <v>538</v>
+      </c>
+      <c r="I150" s="32"/>
+      <c r="J150" s="32"/>
+      <c r="K150" s="32"/>
+      <c r="L150" s="32">
+        <v>1</v>
+      </c>
+      <c r="M150" s="32"/>
+      <c r="N150" s="32"/>
+      <c r="O150" s="32"/>
+      <c r="Q150" s="5">
+        <v>12</v>
+      </c>
+      <c r="R150" s="5">
+        <v>8</v>
+      </c>
+      <c r="S150" s="33"/>
+      <c r="T150" s="5">
+        <v>11</v>
+      </c>
+      <c r="U150" s="32"/>
+    </row>
+    <row r="151" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A151" s="5">
+        <f t="shared" si="8"/>
+        <v>131</v>
+      </c>
+      <c r="B151" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="C151" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D151" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="E151" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F151" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G151" s="32" t="s">
+        <v>539</v>
+      </c>
+      <c r="I151" s="32"/>
+      <c r="J151" s="32"/>
+      <c r="K151" s="32"/>
+      <c r="L151" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="M151" s="32"/>
+      <c r="N151" s="32"/>
+      <c r="O151" s="32"/>
+      <c r="Q151" s="5">
+        <v>12</v>
+      </c>
+      <c r="R151" s="5">
+        <v>8</v>
+      </c>
+      <c r="U151" s="32"/>
+    </row>
+    <row r="152" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="A152" s="5">
+        <f t="shared" si="8"/>
+        <v>132</v>
+      </c>
+      <c r="B152" s="31" t="s">
+        <v>534</v>
+      </c>
+      <c r="C152" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D152" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="E152" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F152" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G152" s="32" t="s">
+        <v>540</v>
+      </c>
+      <c r="I152" s="32"/>
+      <c r="J152" s="32"/>
+      <c r="K152" s="32"/>
+      <c r="L152" s="32">
+        <v>2</v>
+      </c>
+      <c r="M152" s="32"/>
+      <c r="N152" s="32"/>
+      <c r="O152" s="32"/>
+      <c r="Q152" s="5"/>
+      <c r="R152" s="5"/>
+      <c r="S152" s="33"/>
+      <c r="T152" s="5"/>
+      <c r="U152" s="32"/>
+    </row>
+    <row r="153" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A153" s="5">
+        <f t="shared" si="8"/>
+        <v>133</v>
+      </c>
+      <c r="B153" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="C153" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D153" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="E153" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G153" s="32" t="s">
+        <v>541</v>
+      </c>
+      <c r="I153" s="32"/>
+      <c r="J153" s="32"/>
+      <c r="K153" s="32"/>
+      <c r="L153" s="32">
+        <v>1</v>
+      </c>
+      <c r="M153" s="32"/>
+      <c r="N153" s="32"/>
+      <c r="O153" s="32"/>
+      <c r="Q153" s="5">
+        <v>15</v>
+      </c>
+      <c r="R153" s="5">
+        <v>10</v>
+      </c>
+      <c r="S153" s="33"/>
+      <c r="T153" s="5">
+        <v>11</v>
+      </c>
+      <c r="U153" s="32"/>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A154" s="5"/>
+      <c r="B154" s="31"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="32"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="32"/>
+      <c r="G154" s="32"/>
+      <c r="I154" s="32"/>
+      <c r="J154" s="32"/>
+      <c r="K154" s="32"/>
+      <c r="L154" s="32"/>
+      <c r="M154" s="32"/>
+      <c r="N154" s="32"/>
+      <c r="O154" s="32"/>
+      <c r="Q154" s="5"/>
+      <c r="R154" s="5"/>
+      <c r="S154" s="33"/>
+      <c r="T154" s="5"/>
+      <c r="U154" s="32"/>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A155" s="5"/>
+      <c r="B155" s="31"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="32"/>
+      <c r="E155" s="32"/>
+      <c r="F155" s="32"/>
+      <c r="G155" s="32"/>
+      <c r="I155" s="32"/>
+      <c r="J155" s="32"/>
+      <c r="K155" s="32"/>
+      <c r="L155" s="32"/>
+      <c r="M155" s="32"/>
+      <c r="N155" s="32"/>
+      <c r="O155" s="32"/>
+      <c r="Q155" s="5"/>
+      <c r="R155" s="5"/>
+      <c r="S155" s="33"/>
+      <c r="T155" s="5"/>
+      <c r="U155" s="32"/>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A156" s="5"/>
+      <c r="B156" s="31"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="32"/>
+      <c r="E156" s="32"/>
+      <c r="F156" s="32"/>
+      <c r="G156" s="32"/>
+      <c r="I156" s="32"/>
+      <c r="J156" s="32"/>
+      <c r="K156" s="32"/>
+      <c r="L156" s="32"/>
+      <c r="M156" s="32"/>
+      <c r="N156" s="32"/>
+      <c r="O156" s="32"/>
+      <c r="Q156" s="5"/>
+      <c r="R156" s="5"/>
+      <c r="S156" s="33"/>
+      <c r="T156" s="5"/>
+      <c r="U156" s="32"/>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A157" s="5"/>
+      <c r="B157" s="31"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="32"/>
+      <c r="E157" s="32"/>
+      <c r="F157" s="32"/>
+      <c r="G157" s="32"/>
+      <c r="I157" s="32"/>
+      <c r="J157" s="32"/>
+      <c r="K157" s="32"/>
+      <c r="L157" s="32"/>
+      <c r="M157" s="32"/>
+      <c r="N157" s="32"/>
+      <c r="O157" s="32"/>
+      <c r="Q157" s="5"/>
+      <c r="R157" s="5"/>
+      <c r="S157" s="33"/>
+      <c r="T157" s="5"/>
+      <c r="U157" s="32"/>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A158" s="5"/>
+      <c r="B158" s="31"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="32"/>
+      <c r="E158" s="32"/>
+      <c r="F158" s="32"/>
+      <c r="G158" s="32"/>
+      <c r="I158" s="32"/>
+      <c r="J158" s="32"/>
+      <c r="K158" s="32"/>
+      <c r="L158" s="32"/>
+      <c r="M158" s="32"/>
+      <c r="N158" s="32"/>
+      <c r="O158" s="32"/>
+      <c r="Q158" s="5"/>
+      <c r="R158" s="5"/>
+      <c r="S158" s="33"/>
+      <c r="T158" s="5"/>
+      <c r="U158" s="32"/>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A159" s="5"/>
+      <c r="B159" s="31"/>
+      <c r="C159" s="5"/>
+      <c r="D159" s="32"/>
+      <c r="E159" s="32"/>
+      <c r="F159" s="32"/>
+      <c r="G159" s="32"/>
+      <c r="I159" s="32"/>
+      <c r="J159" s="32"/>
+      <c r="K159" s="32"/>
+      <c r="L159" s="32"/>
+      <c r="M159" s="32"/>
+      <c r="N159" s="32"/>
+      <c r="O159" s="32"/>
+      <c r="Q159" s="5"/>
+      <c r="R159" s="5"/>
+      <c r="S159" s="33"/>
+      <c r="T159" s="5"/>
+      <c r="U159" s="32"/>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A160" s="5"/>
+      <c r="B160" s="31"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="32"/>
+      <c r="E160" s="32"/>
+      <c r="F160" s="32"/>
+      <c r="G160" s="32"/>
+      <c r="I160" s="32"/>
+      <c r="J160" s="32"/>
+      <c r="K160" s="32"/>
+      <c r="L160" s="32"/>
+      <c r="M160" s="32"/>
+      <c r="N160" s="32"/>
+      <c r="O160" s="32"/>
+      <c r="Q160" s="5"/>
+      <c r="R160" s="5"/>
+      <c r="S160" s="33"/>
+      <c r="T160" s="5"/>
+      <c r="U160" s="32"/>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A161" s="5"/>
+      <c r="B161" s="31"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="32"/>
+      <c r="E161" s="32"/>
+      <c r="F161" s="32"/>
+      <c r="G161" s="32"/>
+      <c r="I161" s="32"/>
+      <c r="J161" s="32"/>
+      <c r="K161" s="32"/>
+      <c r="L161" s="32"/>
+      <c r="M161" s="32"/>
+      <c r="N161" s="32"/>
+      <c r="O161" s="32"/>
+      <c r="Q161" s="5"/>
+      <c r="R161" s="5"/>
+      <c r="S161" s="33"/>
+      <c r="T161" s="5"/>
+      <c r="U161" s="32"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U132" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="New"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{5E9F328A-0AF8-40D7-BB8D-E321F49730D1}"/>
-    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{A1590941-EEAB-4213-9D06-59D7B83D50D7}"/>
-    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{3322D43E-EC4E-4060-8ACF-C2509E74D154}"/>
-    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{BB9E9B3E-0E03-4659-A85C-01809F67F8D6}"/>
-    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{1915143A-B9C2-4A24-8FB6-E88C8544E2D0}"/>
-    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{FB48445D-D2D0-4064-9DBB-4BA93CE53469}"/>
-    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{21F8C533-9ACB-4C1F-B101-E6D8754F93FF}"/>
-    <hyperlink ref="D133" r:id="rId9" xr:uid="{AD45D360-3EBC-4492-9C71-A4AF6DC87609}"/>
+    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D133" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -15843,7 +16257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15903,7 +16317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16021,7 +16435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16070,38 +16484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16273,10 +16655,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16298,19 +16722,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Features Roadmap for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{28CCE309-41FF-44FC-A43B-75C8554F6959}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -20,26 +21,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$148</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="554">
   <si>
     <t>S.No.</t>
   </si>
@@ -5371,11 +5367,47 @@
   <si>
     <t>Tech story--Generate packet using centre id and unique machine id</t>
   </si>
+  <si>
+    <t>MOS-21582</t>
+  </si>
+  <si>
+    <t>API Specification Changes for IDA based on MDS review by Sasi/Ramesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional or Modification of attributes in API Specs based on review </t>
+  </si>
+  <si>
+    <t>MOS-21583</t>
+  </si>
+  <si>
+    <t>Design Change of ID-Repo based on Security review by Sasi/Ramesh</t>
+  </si>
+  <si>
+    <t>MOS-21584</t>
+  </si>
+  <si>
+    <t>Design Change of IDA based on Security review by Sasi/Ramesh</t>
+  </si>
+  <si>
+    <t>MOS-21585</t>
+  </si>
+  <si>
+    <t>Mapping of platform address attributes in IDA based on Morrocco Address Structure</t>
+  </si>
+  <si>
+    <t>MOS-21327</t>
+  </si>
+  <si>
+    <t>Integrate with new VID Generator API</t>
+  </si>
+  <si>
+    <t>Integrate with the new VID generator component based on the VID policy/type defined</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -5754,7 +5786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6042,6 +6074,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6060,8 +6095,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6093,7 +6128,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6110,7 +6145,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:U70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7271,7 +7306,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7619,67 +7654,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="2" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="60" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.81640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.453125" style="10"/>
+    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="102" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="106"/>
-    </row>
-    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="B1" s="103"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="107"/>
+    </row>
+    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7744,7 +7779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7806,7 +7841,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -7867,7 +7902,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7929,7 +7964,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -7991,7 +8026,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8053,7 +8088,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8115,7 +8150,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8175,7 +8210,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -8235,7 +8270,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8289,7 +8324,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8346,7 +8381,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8397,7 +8432,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8457,7 +8492,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -8519,7 +8554,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8581,7 +8616,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8643,7 +8678,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8703,7 +8738,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8765,7 +8800,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8813,7 +8848,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8861,7 +8896,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8921,7 +8956,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -8981,7 +9016,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9043,7 +9078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9093,7 +9128,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9143,7 +9178,7 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -9203,7 +9238,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9265,7 +9300,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9315,7 +9350,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9371,7 +9406,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9433,7 +9468,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9495,7 +9530,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9553,7 +9588,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9615,7 +9650,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9672,7 +9707,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="182" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9736,7 +9771,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9800,7 +9835,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="154" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -9864,7 +9899,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -9928,7 +9963,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -9982,7 +10017,7 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -10040,7 +10075,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10094,7 +10129,7 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10152,7 +10187,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="252" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10212,7 +10247,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10270,7 +10305,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10332,7 +10367,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10394,7 +10429,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10444,7 +10479,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10506,7 +10541,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10569,7 +10604,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10623,7 +10658,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="154" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10673,7 +10708,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10733,7 +10768,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10783,7 +10818,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10837,7 +10872,7 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -10896,7 +10931,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -10955,7 +10990,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11015,7 +11050,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11069,7 +11104,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11123,7 +11158,7 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -11180,7 +11215,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -11243,7 +11278,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -11304,7 +11339,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11355,7 +11390,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11406,7 +11441,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="182" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -11469,7 +11504,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11529,7 +11564,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11590,7 +11625,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="252" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11650,7 +11685,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11708,7 +11743,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -11768,7 +11803,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="140" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -11831,7 +11866,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="140" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11891,7 +11926,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11946,7 +11981,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -12007,7 +12042,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -12068,7 +12103,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -12128,7 +12163,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="154" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -12190,7 +12225,7 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -12250,7 +12285,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -12312,7 +12347,7 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -12372,7 +12407,7 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="140" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -12434,7 +12469,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="98" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -12493,7 +12528,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="210" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" ht="228" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12555,7 +12590,7 @@
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12617,7 +12652,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12677,7 +12712,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="98" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12736,7 +12771,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12797,7 +12832,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -12852,7 +12887,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12901,7 +12936,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12948,7 +12983,7 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="168" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" ht="171" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -13008,7 +13043,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -13066,7 +13101,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -13126,7 +13161,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -13186,7 +13221,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" ht="57" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -13246,7 +13281,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="154" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -13304,7 +13339,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -13355,7 +13390,7 @@
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="126" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -13413,7 +13448,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -13473,7 +13508,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="280" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13533,7 +13568,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13591,7 +13626,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13651,7 +13686,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13711,7 +13746,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13770,7 +13805,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -13829,7 +13864,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -13880,7 +13915,7 @@
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="126" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -13939,7 +13974,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -13994,7 +14029,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -14049,7 +14084,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -14106,7 +14141,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -14163,7 +14198,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -14220,7 +14255,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -14277,7 +14312,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -14332,7 +14367,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -14378,7 +14413,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -14426,7 +14461,7 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -14477,7 +14512,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -14524,7 +14559,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -14570,7 +14605,7 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>123</v>
       </c>
@@ -14617,7 +14652,7 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>124</v>
       </c>
@@ -14664,7 +14699,7 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>125</v>
       </c>
@@ -14711,7 +14746,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14756,7 +14791,7 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>127</v>
       </c>
@@ -14803,7 +14838,7 @@
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>128</v>
       </c>
@@ -14845,7 +14880,7 @@
       <c r="S126" s="33"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>129</v>
       </c>
@@ -14894,7 +14929,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>130</v>
       </c>
@@ -14944,7 +14979,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A129" s="93">
         <v>131</v>
       </c>
@@ -14992,7 +15027,7 @@
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
     </row>
-    <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A130" s="93">
         <v>132</v>
       </c>
@@ -15040,7 +15075,7 @@
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
     </row>
-    <row r="131" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A131" s="93">
         <v>133</v>
       </c>
@@ -15088,7 +15123,7 @@
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
     </row>
-    <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A132" s="93">
         <v>134</v>
       </c>
@@ -15136,7 +15171,7 @@
       <c r="T132" s="32"/>
       <c r="U132" s="32"/>
     </row>
-    <row r="133" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="93">
         <v>135</v>
       </c>
@@ -15183,7 +15218,7 @@
       <c r="T133" s="32"/>
       <c r="U133" s="33"/>
     </row>
-    <row r="134" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A134" s="93">
         <v>136</v>
       </c>
@@ -15228,7 +15263,7 @@
       <c r="T134" s="33"/>
       <c r="U134" s="33"/>
     </row>
-    <row r="135" spans="1:21" ht="266" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:21" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A135" s="93">
         <v>137</v>
       </c>
@@ -15273,7 +15308,7 @@
       <c r="T135" s="33"/>
       <c r="U135" s="33"/>
     </row>
-    <row r="136" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A136" s="93">
         <v>138</v>
       </c>
@@ -15318,7 +15353,7 @@
       <c r="T136" s="33"/>
       <c r="U136" s="33"/>
     </row>
-    <row r="137" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A137" s="93">
         <v>139</v>
       </c>
@@ -15363,7 +15398,7 @@
       <c r="T137" s="33"/>
       <c r="U137" s="33"/>
     </row>
-    <row r="138" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A138" s="93">
         <v>140</v>
       </c>
@@ -15408,7 +15443,7 @@
       <c r="T138" s="33"/>
       <c r="U138" s="33"/>
     </row>
-    <row r="139" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A139" s="93">
         <v>141</v>
       </c>
@@ -15453,7 +15488,7 @@
       <c r="T139" s="33"/>
       <c r="U139" s="33"/>
     </row>
-    <row r="140" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A140" s="93">
         <v>142</v>
       </c>
@@ -15498,7 +15533,7 @@
       <c r="T140" s="33"/>
       <c r="U140" s="33"/>
     </row>
-    <row r="141" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:21" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A141" s="93">
         <v>143</v>
       </c>
@@ -15543,7 +15578,7 @@
       <c r="T141" s="33"/>
       <c r="U141" s="33"/>
     </row>
-    <row r="142" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A142" s="93">
         <v>144</v>
       </c>
@@ -15588,7 +15623,7 @@
       <c r="T142" s="33"/>
       <c r="U142" s="33"/>
     </row>
-    <row r="143" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A143" s="93">
         <v>145</v>
       </c>
@@ -15633,7 +15668,7 @@
       <c r="T143" s="33"/>
       <c r="U143" s="33"/>
     </row>
-    <row r="144" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:21" ht="114" x14ac:dyDescent="0.25">
       <c r="A144" s="93">
         <v>146</v>
       </c>
@@ -15678,7 +15713,7 @@
       <c r="T144" s="33"/>
       <c r="U144" s="33"/>
     </row>
-    <row r="145" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A145" s="93">
         <v>147</v>
       </c>
@@ -15723,7 +15758,7 @@
       <c r="T145" s="33"/>
       <c r="U145" s="33"/>
     </row>
-    <row r="146" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A146" s="93">
         <v>148</v>
       </c>
@@ -15768,7 +15803,7 @@
       <c r="T146" s="33"/>
       <c r="U146" s="33"/>
     </row>
-    <row r="147" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A147" s="93">
         <v>149</v>
       </c>
@@ -15813,8 +15848,8 @@
       <c r="T147" s="33"/>
       <c r="U147" s="33"/>
     </row>
-    <row r="148" spans="1:21" ht="140" x14ac:dyDescent="0.35">
-      <c r="A148" s="107">
+    <row r="148" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="101">
         <v>150</v>
       </c>
       <c r="B148" s="91"/>
@@ -15858,7 +15893,7 @@
       <c r="T148" s="89"/>
       <c r="U148" s="89"/>
     </row>
-    <row r="149" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <f>1+A126</f>
         <v>129</v>
@@ -15902,7 +15937,7 @@
       </c>
       <c r="U149" s="32"/>
     </row>
-    <row r="150" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <f t="shared" ref="A150:A153" si="8">1+A127</f>
         <v>130</v>
@@ -15946,7 +15981,7 @@
       </c>
       <c r="U150" s="32"/>
     </row>
-    <row r="151" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <f t="shared" si="8"/>
         <v>131</v>
@@ -15986,7 +16021,7 @@
       </c>
       <c r="U151" s="32"/>
     </row>
-    <row r="152" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <f t="shared" si="8"/>
         <v>132</v>
@@ -16024,7 +16059,7 @@
       <c r="T152" s="5"/>
       <c r="U152" s="32"/>
     </row>
-    <row r="153" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <f t="shared" si="8"/>
         <v>133</v>
@@ -16068,112 +16103,232 @@
       </c>
       <c r="U153" s="32"/>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A154" s="5"/>
-      <c r="B154" s="31"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="32"/>
-      <c r="E154" s="32"/>
-      <c r="F154" s="32"/>
-      <c r="G154" s="32"/>
-      <c r="I154" s="32"/>
+    <row r="154" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A154" s="93">
+        <v>151</v>
+      </c>
+      <c r="B154" s="31" t="s">
+        <v>542</v>
+      </c>
+      <c r="C154" s="6">
+        <v>43550</v>
+      </c>
+      <c r="D154" s="32" t="s">
+        <v>543</v>
+      </c>
+      <c r="E154" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F154" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G154" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="H154" s="21"/>
+      <c r="I154" s="21"/>
       <c r="J154" s="32"/>
       <c r="K154" s="32"/>
-      <c r="L154" s="32"/>
-      <c r="M154" s="32"/>
-      <c r="N154" s="32"/>
-      <c r="O154" s="32"/>
+      <c r="L154" s="32">
+        <v>1</v>
+      </c>
+      <c r="M154" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="N154" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O154" s="21">
+        <v>43550</v>
+      </c>
+      <c r="P154" s="33"/>
       <c r="Q154" s="5"/>
       <c r="R154" s="5"/>
       <c r="S154" s="33"/>
       <c r="T154" s="5"/>
       <c r="U154" s="32"/>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A155" s="5"/>
-      <c r="B155" s="31"/>
-      <c r="C155" s="5"/>
-      <c r="D155" s="32"/>
-      <c r="E155" s="32"/>
-      <c r="F155" s="32"/>
-      <c r="G155" s="32"/>
+    <row r="155" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="93">
+        <v>152</v>
+      </c>
+      <c r="B155" s="31" t="s">
+        <v>545</v>
+      </c>
+      <c r="C155" s="6">
+        <v>43550</v>
+      </c>
+      <c r="D155" s="32" t="s">
+        <v>546</v>
+      </c>
+      <c r="E155" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F155" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G155" s="32" t="s">
+        <v>546</v>
+      </c>
+      <c r="H155" s="21"/>
       <c r="I155" s="32"/>
       <c r="J155" s="32"/>
       <c r="K155" s="32"/>
-      <c r="L155" s="32"/>
-      <c r="M155" s="32"/>
-      <c r="N155" s="32"/>
-      <c r="O155" s="32"/>
+      <c r="L155" s="32">
+        <v>1</v>
+      </c>
+      <c r="M155" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N155" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O155" s="108">
+        <v>43550</v>
+      </c>
+      <c r="P155" s="33"/>
       <c r="Q155" s="5"/>
       <c r="R155" s="5"/>
       <c r="S155" s="33"/>
       <c r="T155" s="5"/>
       <c r="U155" s="32"/>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A156" s="5"/>
-      <c r="B156" s="31"/>
-      <c r="C156" s="5"/>
-      <c r="D156" s="32"/>
-      <c r="E156" s="32"/>
-      <c r="F156" s="32"/>
-      <c r="G156" s="32"/>
+    <row r="156" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="93">
+        <v>153</v>
+      </c>
+      <c r="B156" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="C156" s="6">
+        <v>43550</v>
+      </c>
+      <c r="D156" s="32" t="s">
+        <v>548</v>
+      </c>
+      <c r="E156" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F156" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G156" s="32" t="s">
+        <v>548</v>
+      </c>
+      <c r="H156" s="32"/>
       <c r="I156" s="32"/>
       <c r="J156" s="32"/>
       <c r="K156" s="32"/>
-      <c r="L156" s="32"/>
-      <c r="M156" s="32"/>
-      <c r="N156" s="32"/>
-      <c r="O156" s="32"/>
+      <c r="L156" s="32">
+        <v>1</v>
+      </c>
+      <c r="M156" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N156" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O156" s="108">
+        <v>43550</v>
+      </c>
+      <c r="P156" s="33"/>
       <c r="Q156" s="5"/>
       <c r="R156" s="5"/>
       <c r="S156" s="33"/>
       <c r="T156" s="5"/>
       <c r="U156" s="32"/>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A157" s="5"/>
-      <c r="B157" s="31"/>
-      <c r="C157" s="5"/>
-      <c r="D157" s="32"/>
-      <c r="E157" s="32"/>
-      <c r="F157" s="32"/>
-      <c r="G157" s="32"/>
+    <row r="157" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="93">
+        <v>154</v>
+      </c>
+      <c r="B157" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="C157" s="6">
+        <v>43556</v>
+      </c>
+      <c r="D157" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="E157" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F157" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G157" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="H157" s="32"/>
       <c r="I157" s="32"/>
       <c r="J157" s="32"/>
       <c r="K157" s="32"/>
-      <c r="L157" s="32"/>
-      <c r="M157" s="32"/>
-      <c r="N157" s="32"/>
-      <c r="O157" s="32"/>
+      <c r="L157" s="32">
+        <v>1</v>
+      </c>
+      <c r="M157" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N157" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="O157" s="108">
+        <v>43556</v>
+      </c>
+      <c r="P157" s="33"/>
       <c r="Q157" s="5"/>
       <c r="R157" s="5"/>
       <c r="S157" s="33"/>
       <c r="T157" s="5"/>
       <c r="U157" s="32"/>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A158" s="5"/>
-      <c r="B158" s="31"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="32"/>
-      <c r="E158" s="32"/>
-      <c r="F158" s="32"/>
-      <c r="G158" s="32"/>
+    <row r="158" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="93">
+        <v>155</v>
+      </c>
+      <c r="B158" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="C158" s="6">
+        <v>43552</v>
+      </c>
+      <c r="D158" s="32" t="s">
+        <v>552</v>
+      </c>
+      <c r="E158" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="F158" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G158" s="32" t="s">
+        <v>553</v>
+      </c>
+      <c r="H158" s="32"/>
       <c r="I158" s="32"/>
       <c r="J158" s="32"/>
       <c r="K158" s="32"/>
-      <c r="L158" s="32"/>
-      <c r="M158" s="32"/>
-      <c r="N158" s="32"/>
-      <c r="O158" s="32"/>
+      <c r="L158" s="32">
+        <v>1</v>
+      </c>
+      <c r="M158" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N158" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O158" s="108">
+        <v>43552</v>
+      </c>
+      <c r="P158" s="33"/>
       <c r="Q158" s="5"/>
       <c r="R158" s="5"/>
       <c r="S158" s="33"/>
       <c r="T158" s="5"/>
       <c r="U158" s="32"/>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="31"/>
       <c r="C159" s="5"/>
@@ -16194,7 +16349,7 @@
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="31"/>
       <c r="C160" s="5"/>
@@ -16215,7 +16370,7 @@
       <c r="T160" s="5"/>
       <c r="U160" s="32"/>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="31"/>
       <c r="C161" s="5"/>
@@ -16241,15 +16396,15 @@
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
-    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
-    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
-    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
-    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
-    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
-    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
-    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
-    <hyperlink ref="D133" r:id="rId9"/>
+    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D133" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -16257,57 +16412,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -16317,19 +16472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -16340,7 +16495,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -16351,7 +16506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -16362,7 +16517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -16373,7 +16528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -16384,7 +16539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -16395,7 +16550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -16406,7 +16561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -16417,7 +16572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -16435,17 +16590,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -16453,25 +16608,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -16484,6 +16639,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16655,52 +16842,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16722,9 +16867,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added CR's for reg client
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{28CCE309-41FF-44FC-A43B-75C8554F6959}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -19,9 +18,9 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$158</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="560">
   <si>
     <t>S.No.</t>
   </si>
@@ -2749,25 +2748,16 @@
     <t>MOS-12989</t>
   </si>
   <si>
-    <t>MOS-13518</t>
-  </si>
-  <si>
     <t>MOS-13519</t>
   </si>
   <si>
     <t>MOS-13522</t>
   </si>
   <si>
-    <t>MOS-13524</t>
-  </si>
-  <si>
     <t>MOS-13526</t>
   </si>
   <si>
     <t>MOS-13528</t>
-  </si>
-  <si>
-    <t>MOS-13527</t>
   </si>
   <si>
     <t>MOS-13556</t>
@@ -5403,11 +5393,43 @@
   <si>
     <t>Integrate with the new VID generator component based on the VID policy/type defined</t>
   </si>
+  <si>
+    <t>MOS-13518
+MOS-19886
+MOS-16109</t>
+  </si>
+  <si>
+    <t>MOS-13524
+MOS-19014</t>
+  </si>
+  <si>
+    <t>MOS-13527
+MOS-16120</t>
+  </si>
+  <si>
+    <t>MOS-20066</t>
+  </si>
+  <si>
+    <t>Comments from Shrikant on Mar 22 nd in JIRA</t>
+  </si>
+  <si>
+    <t>As the MOSIP Registration Client, I should validate there are no blacklisted words in demographic data</t>
+  </si>
+  <si>
+    <t>MOS-15324
+MOS-14999</t>
+  </si>
+  <si>
+    <t>New visual designs created by UI team</t>
+  </si>
+  <si>
+    <t>Visual design changes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -6077,6 +6099,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6094,9 +6119,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6128,7 +6150,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6145,7 +6167,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:U70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7306,7 +7328,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7654,67 +7676,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:W161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
+      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A159" sqref="A159:S160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="60" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.42578125" style="10"/>
+    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="103" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="104"/>
-      <c r="U1" s="107"/>
-    </row>
-    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="104"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="108"/>
+    </row>
+    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7746,7 +7768,7 @@
         <v>228</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>8</v>
@@ -7779,7 +7801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7799,7 +7821,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>17</v>
@@ -7808,13 +7830,13 @@
         <v>18</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="L3" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M3" s="32" t="s">
         <v>19</v>
@@ -7838,15 +7860,15 @@
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
       <c r="U3" s="21" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="84" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C4" s="6">
         <v>43362</v>
@@ -7861,7 +7883,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>17</v>
@@ -7873,7 +7895,7 @@
         <v>265</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="L4" s="32">
         <v>1</v>
@@ -7899,10 +7921,10 @@
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="21" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -7934,10 +7956,10 @@
         <v>230</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="L5" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>19</v>
@@ -7964,12 +7986,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C6" s="6">
         <v>43362</v>
@@ -7984,7 +8006,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>17</v>
@@ -7996,10 +8018,10 @@
         <v>230</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L6" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M6" s="32" t="s">
         <v>19</v>
@@ -8023,10 +8045,10 @@
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
       <c r="U6" s="21" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8058,10 +8080,10 @@
         <v>231</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="L7" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M7" s="32" t="s">
         <v>19</v>
@@ -8085,15 +8107,15 @@
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
       <c r="U7" s="21" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C8" s="6">
         <v>43362</v>
@@ -8108,7 +8130,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>17</v>
@@ -8120,10 +8142,10 @@
         <v>231</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="L8" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>19</v>
@@ -8147,10 +8169,10 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="21" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8180,10 +8202,10 @@
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L9" s="85" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M9" s="32" t="s">
         <v>19</v>
@@ -8207,15 +8229,15 @@
       <c r="S9" s="30"/>
       <c r="T9" s="30"/>
       <c r="U9" s="22" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C10" s="6">
         <v>43362</v>
@@ -8230,7 +8252,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>17</v>
@@ -8240,7 +8262,7 @@
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="L10" s="19">
         <v>1</v>
@@ -8267,10 +8289,10 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="22" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8324,7 +8346,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8342,7 +8364,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>17</v>
@@ -8352,7 +8374,7 @@
       </c>
       <c r="J12" s="32"/>
       <c r="K12" s="32" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="L12" s="32">
         <v>1</v>
@@ -8378,15 +8400,15 @@
       <c r="S12" s="30"/>
       <c r="T12" s="30"/>
       <c r="U12" s="21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C13" s="6">
         <v>43395</v>
@@ -8432,7 +8454,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8452,7 +8474,7 @@
         <v>26</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>38</v>
@@ -8462,7 +8484,7 @@
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L14" s="32">
         <v>1</v>
@@ -8489,15 +8511,15 @@
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="21" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C15" s="6">
         <v>43397</v>
@@ -8554,12 +8576,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C16" s="6">
         <v>43397</v>
@@ -8616,12 +8638,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C17" s="6">
         <v>43397</v>
@@ -8678,7 +8700,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8738,12 +8760,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C19" s="6">
         <v>43397</v>
@@ -8800,7 +8822,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -8848,7 +8870,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -8896,7 +8918,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -8926,7 +8948,7 @@
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L22" s="32">
         <v>1</v>
@@ -8953,15 +8975,15 @@
       <c r="S22" s="30"/>
       <c r="T22" s="30"/>
       <c r="U22" s="21" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C23" s="6">
         <v>43402</v>
@@ -8976,7 +8998,7 @@
         <v>26</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>38</v>
@@ -8986,7 +9008,7 @@
       </c>
       <c r="J23" s="32"/>
       <c r="K23" s="32" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="L23" s="32" t="s">
         <v>140</v>
@@ -9013,15 +9035,15 @@
       <c r="S23" s="30"/>
       <c r="T23" s="30"/>
       <c r="U23" s="21" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C24" s="6">
         <v>43402</v>
@@ -9078,7 +9100,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9128,7 +9150,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9178,12 +9200,12 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="83" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C27" s="6">
         <v>43402</v>
@@ -9208,7 +9230,7 @@
       </c>
       <c r="J27" s="32"/>
       <c r="K27" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L27" s="32">
         <v>1</v>
@@ -9238,12 +9260,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="83" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C28" s="6">
         <v>43418</v>
@@ -9267,10 +9289,10 @@
         <v>54</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L28" s="14">
         <v>1</v>
@@ -9300,7 +9322,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9350,7 +9372,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9406,7 +9428,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9468,7 +9490,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9523,14 +9545,14 @@
         <v>269</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="32" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9548,7 +9570,7 @@
         <v>33</v>
       </c>
       <c r="G33" s="46" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H33" s="14" t="s">
         <v>38</v>
@@ -9557,7 +9579,7 @@
         <v>82</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32">
@@ -9588,7 +9610,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9617,13 +9639,13 @@
         <v>85</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K34" s="32" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="L34" s="85" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="M34" s="32" t="s">
         <v>74</v>
@@ -9650,12 +9672,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" s="83" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C35" s="6">
         <v>43430</v>
@@ -9670,7 +9692,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="48" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>38</v>
@@ -9680,7 +9702,7 @@
       </c>
       <c r="J35" s="32"/>
       <c r="K35" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L35" s="32">
         <v>1</v>
@@ -9707,12 +9729,12 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C36" s="6">
         <v>43430</v>
@@ -9771,12 +9793,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C37" s="6">
         <v>43430</v>
@@ -9826,21 +9848,21 @@
         <v>269</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T37" s="30" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="U37" s="32" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C38" s="6">
         <v>43430</v>
@@ -9899,12 +9921,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C39" s="6">
         <v>43430</v>
@@ -9963,12 +9985,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C40" s="6">
         <v>43430</v>
@@ -10017,12 +10039,12 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C41" s="6">
         <v>43430</v>
@@ -10037,7 +10059,7 @@
         <v>26</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H41" s="14" t="s">
         <v>38</v>
@@ -10047,10 +10069,10 @@
       </c>
       <c r="J41" s="32"/>
       <c r="K41" s="32" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="L41" s="85" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M41" s="32" t="s">
         <v>74</v>
@@ -10075,7 +10097,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10129,12 +10151,12 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="87" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C43" s="6">
         <v>43427</v>
@@ -10149,7 +10171,7 @@
         <v>26</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="H43" s="14" t="s">
         <v>38</v>
@@ -10159,7 +10181,7 @@
       </c>
       <c r="J43" s="32"/>
       <c r="K43" s="32" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="L43" s="32">
         <v>2</v>
@@ -10187,12 +10209,12 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C44" s="6">
         <v>43427</v>
@@ -10247,12 +10269,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C45" s="6">
         <v>43427</v>
@@ -10305,12 +10327,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C46" s="6">
         <v>43427</v>
@@ -10367,12 +10389,12 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C47" s="6">
         <v>43427</v>
@@ -10420,7 +10442,7 @@
         <v>269</v>
       </c>
       <c r="S47" s="75" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="T47" s="30" t="s">
         <v>156</v>
@@ -10429,7 +10451,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10479,12 +10501,12 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C49" s="6">
         <v>43427</v>
@@ -10541,12 +10563,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C50" s="6">
         <v>43427</v>
@@ -10601,10 +10623,10 @@
         <v>156</v>
       </c>
       <c r="U50" s="32" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10658,7 +10680,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10708,7 +10730,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10738,7 +10760,7 @@
       </c>
       <c r="J53" s="32"/>
       <c r="K53" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L53" s="32">
         <v>1</v>
@@ -10768,7 +10790,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10818,7 +10840,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -10872,12 +10894,12 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="B56" s="83" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C56" s="6">
         <v>43427</v>
@@ -10892,7 +10914,7 @@
         <v>26</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>38</v>
@@ -10902,7 +10924,7 @@
       </c>
       <c r="J56" s="32"/>
       <c r="K56" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L56" s="32">
         <v>1</v>
@@ -10928,15 +10950,15 @@
       <c r="S56" s="30"/>
       <c r="T56" s="30"/>
       <c r="U56" s="32" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
       <c r="B57" s="83" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C57" s="6">
         <v>43427</v>
@@ -10951,7 +10973,7 @@
         <v>26</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>38</v>
@@ -10961,7 +10983,7 @@
       </c>
       <c r="J57" s="32"/>
       <c r="K57" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L57" s="32" t="s">
         <v>140</v>
@@ -10990,12 +11012,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
       <c r="B58" s="84" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C58" s="6">
         <v>43427</v>
@@ -11020,10 +11042,10 @@
       </c>
       <c r="J58" s="32"/>
       <c r="K58" s="32" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="L58" s="85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M58" s="32" t="s">
         <v>74</v>
@@ -11050,7 +11072,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11104,7 +11126,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11158,12 +11180,12 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C61" s="6">
         <v>43432</v>
@@ -11206,7 +11228,7 @@
         <v>4</v>
       </c>
       <c r="Q61" s="81" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="R61" s="30" t="s">
         <v>269</v>
@@ -11215,12 +11237,12 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C62" s="6">
         <v>43432</v>
@@ -11278,12 +11300,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C63" s="6">
         <v>43432</v>
@@ -11339,7 +11361,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11390,7 +11412,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11441,12 +11463,12 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C66" s="6">
         <v>43440</v>
@@ -11495,16 +11517,16 @@
         <v>269</v>
       </c>
       <c r="S66" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="T66" s="5" t="s">
         <v>172</v>
       </c>
       <c r="U66" s="32" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11534,7 +11556,7 @@
       </c>
       <c r="J67" s="32"/>
       <c r="K67" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L67" s="32" t="s">
         <v>140</v>
@@ -11564,12 +11586,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C68" s="6">
         <v>43440</v>
@@ -11618,19 +11640,19 @@
         <v>269</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T68" s="5"/>
       <c r="U68" s="32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
       <c r="B69" s="83" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C69" s="6">
         <v>43446</v>
@@ -11655,7 +11677,7 @@
       </c>
       <c r="J69" s="32"/>
       <c r="K69" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L69" s="32">
         <v>1</v>
@@ -11685,12 +11707,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
       <c r="B70" s="83" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C70" s="6">
         <v>43446</v>
@@ -11705,7 +11727,7 @@
         <v>26</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H70" s="14" t="s">
         <v>38</v>
@@ -11715,7 +11737,7 @@
       </c>
       <c r="J70" s="32"/>
       <c r="K70" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L70" s="32">
         <v>1</v>
@@ -11743,12 +11765,12 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
       <c r="B71" s="83" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C71" s="6">
         <v>43451</v>
@@ -11763,7 +11785,7 @@
         <v>26</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H71" s="14" t="s">
         <v>38</v>
@@ -11773,7 +11795,7 @@
       </c>
       <c r="J71" s="32"/>
       <c r="K71" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L71" s="32">
         <v>1</v>
@@ -11803,12 +11825,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C72" s="6">
         <v>43451</v>
@@ -11857,7 +11879,7 @@
         <v>269</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T72" s="5"/>
       <c r="U72" s="32" t="s">
@@ -11866,7 +11888,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -11896,7 +11918,7 @@
       </c>
       <c r="J73" s="32"/>
       <c r="K73" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L73" s="32">
         <v>1</v>
@@ -11926,7 +11948,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -11981,12 +12003,12 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C75" s="37">
         <v>43454</v>
@@ -12042,12 +12064,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C76" s="6">
         <v>43454</v>
@@ -12103,12 +12125,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
       <c r="B77" s="87" t="s">
-        <v>291</v>
+        <v>551</v>
       </c>
       <c r="C77" s="6">
         <v>43465</v>
@@ -12123,7 +12145,7 @@
         <v>26</v>
       </c>
       <c r="G77" s="32" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>38</v>
@@ -12133,10 +12155,10 @@
       </c>
       <c r="J77" s="32"/>
       <c r="K77" s="32" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="L77" s="85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M77" s="32" t="s">
         <v>74</v>
@@ -12163,12 +12185,12 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>75</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C78" s="6">
         <v>43465</v>
@@ -12183,7 +12205,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="32" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>38</v>
@@ -12193,10 +12215,10 @@
       </c>
       <c r="J78" s="32"/>
       <c r="K78" s="32" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L78" s="85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M78" s="32" t="s">
         <v>74</v>
@@ -12225,12 +12247,12 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>76</v>
       </c>
       <c r="B79" s="84" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C79" s="6">
         <v>43465</v>
@@ -12245,7 +12267,7 @@
         <v>26</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H79" s="14" t="s">
         <v>38</v>
@@ -12255,10 +12277,10 @@
       </c>
       <c r="J79" s="32"/>
       <c r="K79" s="32" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="L79" s="85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M79" s="32" t="s">
         <v>74</v>
@@ -12285,12 +12307,12 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>77</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C80" s="6">
         <v>43465</v>
@@ -12315,10 +12337,10 @@
       </c>
       <c r="J80" s="32"/>
       <c r="K80" s="32" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="L80" s="85" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="M80" s="32" t="s">
         <v>74</v>
@@ -12347,12 +12369,12 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>78</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C81" s="6">
         <v>43465</v>
@@ -12367,7 +12389,7 @@
         <v>26</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H81" s="14" t="s">
         <v>38</v>
@@ -12377,10 +12399,10 @@
       </c>
       <c r="J81" s="32"/>
       <c r="K81" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L81" s="85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M81" s="32" t="s">
         <v>74</v>
@@ -12407,12 +12429,12 @@
       <c r="V81" s="74"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>79</v>
       </c>
       <c r="B82" s="84" t="s">
-        <v>294</v>
+        <v>552</v>
       </c>
       <c r="C82" s="6">
         <v>43465</v>
@@ -12427,7 +12449,7 @@
         <v>26</v>
       </c>
       <c r="G82" s="32" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H82" s="14" t="s">
         <v>38</v>
@@ -12437,7 +12459,7 @@
       </c>
       <c r="J82" s="32"/>
       <c r="K82" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L82" s="32">
         <v>1</v>
@@ -12469,7 +12491,7 @@
       <c r="V82" s="74"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -12528,12 +12550,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>81</v>
       </c>
       <c r="B84" s="84" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C84" s="6">
         <v>43465</v>
@@ -12548,7 +12570,7 @@
         <v>26</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H84" s="14" t="s">
         <v>38</v>
@@ -12558,7 +12580,7 @@
       </c>
       <c r="J84" s="32"/>
       <c r="K84" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L84" s="32">
         <v>1</v>
@@ -12585,17 +12607,17 @@
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
       <c r="U84" s="32" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>82</v>
       </c>
       <c r="B85" s="83" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C85" s="6">
         <v>43477</v>
@@ -12619,10 +12641,10 @@
         <v>85</v>
       </c>
       <c r="J85" s="32" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K85" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L85" s="32">
         <v>1</v>
@@ -12652,12 +12674,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>83</v>
       </c>
       <c r="B86" s="83" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C86" s="6">
         <v>43477</v>
@@ -12681,10 +12703,10 @@
         <v>85</v>
       </c>
       <c r="J86" s="32" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K86" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L86" s="32">
         <v>1</v>
@@ -12712,12 +12734,12 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C87" s="6">
         <v>43477</v>
@@ -12741,7 +12763,7 @@
         <v>85</v>
       </c>
       <c r="J87" s="32" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32">
@@ -12771,12 +12793,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C88" s="6">
         <v>43477</v>
@@ -12823,21 +12845,21 @@
         <v>269</v>
       </c>
       <c r="S88" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="T88" s="5" t="s">
         <v>172</v>
       </c>
       <c r="U88" s="32" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="89" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C89" s="6">
         <v>43477</v>
@@ -12881,13 +12903,13 @@
       <c r="R89" s="5"/>
       <c r="S89" s="33"/>
       <c r="T89" s="5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="U89" s="32" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -12936,7 +12958,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -12983,12 +13005,12 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>89</v>
       </c>
       <c r="B92" s="84" t="s">
-        <v>297</v>
+        <v>553</v>
       </c>
       <c r="C92" s="6">
         <v>43486</v>
@@ -13043,12 +13065,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>90</v>
       </c>
       <c r="B93" s="83" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C93" s="6">
         <v>43489</v>
@@ -13063,7 +13085,7 @@
         <v>26</v>
       </c>
       <c r="G93" s="32" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H93" s="14" t="s">
         <v>245</v>
@@ -13073,7 +13095,7 @@
       </c>
       <c r="J93" s="32"/>
       <c r="K93" s="19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L93" s="32">
         <v>1</v>
@@ -13101,12 +13123,12 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>91</v>
       </c>
       <c r="B94" s="84" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C94" s="6">
         <v>43489</v>
@@ -13121,7 +13143,7 @@
         <v>26</v>
       </c>
       <c r="G94" s="32" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H94" s="14" t="s">
         <v>245</v>
@@ -13131,7 +13153,7 @@
       </c>
       <c r="J94" s="32"/>
       <c r="K94" s="32" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L94" s="85" t="s">
         <v>140</v>
@@ -13161,12 +13183,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>92</v>
       </c>
       <c r="B95" s="84" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C95" s="6">
         <v>43489</v>
@@ -13181,7 +13203,7 @@
         <v>26</v>
       </c>
       <c r="G95" s="32" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="H95" s="14" t="s">
         <v>245</v>
@@ -13221,12 +13243,12 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>93</v>
       </c>
       <c r="B96" s="84" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C96" s="6">
         <v>43489</v>
@@ -13241,7 +13263,7 @@
         <v>26</v>
       </c>
       <c r="G96" s="32" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="H96" s="14" t="s">
         <v>245</v>
@@ -13281,18 +13303,18 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>94</v>
       </c>
       <c r="B97" s="83" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C97" s="6">
         <v>43473</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E97" s="32" t="s">
         <v>15</v>
@@ -13301,7 +13323,7 @@
         <v>26</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H97" s="14" t="s">
         <v>245</v>
@@ -13311,7 +13333,7 @@
       </c>
       <c r="J97" s="32"/>
       <c r="K97" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L97" s="85">
         <v>1</v>
@@ -13339,18 +13361,18 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C98" s="6">
         <v>43473</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E98" s="32" t="s">
         <v>80</v>
@@ -13359,7 +13381,7 @@
         <v>26</v>
       </c>
       <c r="G98" s="32" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H98" s="14" t="s">
         <v>38</v>
@@ -13385,17 +13407,17 @@
       <c r="Q98" s="82"/>
       <c r="R98" s="5"/>
       <c r="S98" s="33" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>96</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C99" s="6">
         <v>43489</v>
@@ -13410,7 +13432,7 @@
         <v>26</v>
       </c>
       <c r="G99" s="32" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H99" s="14" t="s">
         <v>245</v>
@@ -13420,7 +13442,7 @@
       </c>
       <c r="J99" s="32"/>
       <c r="K99" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L99" s="85">
         <v>1</v>
@@ -13448,12 +13470,12 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>97</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C100" s="6">
         <v>43489</v>
@@ -13468,7 +13490,7 @@
         <v>26</v>
       </c>
       <c r="G100" s="32" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H100" s="14" t="s">
         <v>245</v>
@@ -13478,7 +13500,7 @@
       </c>
       <c r="J100" s="32"/>
       <c r="K100" s="32" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L100" s="85">
         <v>1</v>
@@ -13508,12 +13530,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>98</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C101" s="6">
         <v>43489</v>
@@ -13528,7 +13550,7 @@
         <v>26</v>
       </c>
       <c r="G101" s="32" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H101" s="14" t="s">
         <v>245</v>
@@ -13538,7 +13560,7 @@
       </c>
       <c r="J101" s="32"/>
       <c r="K101" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L101" s="85">
         <v>1</v>
@@ -13568,12 +13590,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>99</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C102" s="6">
         <v>43489</v>
@@ -13588,7 +13610,7 @@
         <v>26</v>
       </c>
       <c r="G102" s="32" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H102" s="14" t="s">
         <v>245</v>
@@ -13598,7 +13620,7 @@
       </c>
       <c r="J102" s="32"/>
       <c r="K102" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L102" s="85">
         <v>1</v>
@@ -13626,12 +13648,12 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>100</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C103" s="6">
         <v>43489</v>
@@ -13646,7 +13668,7 @@
         <v>26</v>
       </c>
       <c r="G103" s="32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H103" s="14" t="s">
         <v>245</v>
@@ -13656,7 +13678,7 @@
       </c>
       <c r="J103" s="32"/>
       <c r="K103" s="32" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="L103" s="85">
         <v>1</v>
@@ -13686,12 +13708,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>101</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C104" s="6">
         <v>43489</v>
@@ -13706,7 +13728,7 @@
         <v>26</v>
       </c>
       <c r="G104" s="32" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H104" s="14" t="s">
         <v>245</v>
@@ -13746,12 +13768,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C105" s="6">
         <v>43448</v>
@@ -13798,19 +13820,19 @@
         <v>269</v>
       </c>
       <c r="S105" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="T105" s="32" t="s">
         <v>406</v>
       </c>
-      <c r="T105" s="32" t="s">
-        <v>409</v>
-      </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C106" s="6">
         <v>43447</v>
@@ -13855,21 +13877,21 @@
         <v>269</v>
       </c>
       <c r="S106" s="5" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T106" s="32" t="s">
         <v>180</v>
       </c>
       <c r="U106" s="88" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C107" s="6">
         <v>43495</v>
@@ -13910,17 +13932,17 @@
       <c r="Q107" s="5"/>
       <c r="R107" s="5"/>
       <c r="S107" s="33" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>105</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C108" s="6">
         <v>43495</v>
@@ -13945,7 +13967,7 @@
       </c>
       <c r="J108" s="32"/>
       <c r="K108" s="32" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="L108" s="32">
         <v>1</v>
@@ -13971,21 +13993,21 @@
       <c r="S108" s="33"/>
       <c r="T108" s="5"/>
       <c r="U108" s="85" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C109" s="6">
         <v>43108</v>
       </c>
       <c r="D109" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E109" s="32" t="s">
         <v>125</v>
@@ -13994,10 +14016,10 @@
         <v>26</v>
       </c>
       <c r="G109" s="32" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I109" s="32" t="s">
         <v>85</v>
@@ -14029,18 +14051,18 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C110" s="6">
         <v>43108</v>
       </c>
       <c r="D110" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E110" s="32" t="s">
         <v>39</v>
@@ -14049,10 +14071,10 @@
         <v>26</v>
       </c>
       <c r="G110" s="32" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H110" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I110" s="32" t="s">
         <v>85</v>
@@ -14084,18 +14106,18 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
       <c r="B111" s="32" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C111" s="6">
         <v>43436</v>
       </c>
       <c r="D111" s="32" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E111" s="32" t="s">
         <v>125</v>
@@ -14104,10 +14126,10 @@
         <v>26</v>
       </c>
       <c r="G111" s="32" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H111" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I111" s="32" t="s">
         <v>85</v>
@@ -14137,22 +14159,22 @@
       </c>
       <c r="S111" s="33"/>
       <c r="T111" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
       <c r="B112" s="32" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C112" s="6">
         <v>43436</v>
       </c>
       <c r="D112" s="32" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E112" s="32" t="s">
         <v>125</v>
@@ -14161,10 +14183,10 @@
         <v>26</v>
       </c>
       <c r="G112" s="32" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I112" s="32" t="s">
         <v>85</v>
@@ -14194,22 +14216,22 @@
       </c>
       <c r="S112" s="33"/>
       <c r="T112" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
       <c r="B113" s="32" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C113" s="6">
         <v>43496</v>
       </c>
       <c r="D113" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E113" s="32" t="s">
         <v>125</v>
@@ -14218,10 +14240,10 @@
         <v>26</v>
       </c>
       <c r="G113" s="32" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H113" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I113" s="32" t="s">
         <v>85</v>
@@ -14251,22 +14273,22 @@
       </c>
       <c r="S113" s="33"/>
       <c r="T113" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
       <c r="B114" s="32" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C114" s="6">
         <v>43496</v>
       </c>
       <c r="D114" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E114" s="32" t="s">
         <v>125</v>
@@ -14275,10 +14297,10 @@
         <v>26</v>
       </c>
       <c r="G114" s="32" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I114" s="32" t="s">
         <v>85</v>
@@ -14308,22 +14330,22 @@
       </c>
       <c r="S114" s="33"/>
       <c r="T114" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
       <c r="B115" s="32" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C115" s="6">
         <v>43496</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E115" s="32" t="s">
         <v>125</v>
@@ -14332,10 +14354,10 @@
         <v>26</v>
       </c>
       <c r="G115" s="32" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I115" s="32" t="s">
         <v>85</v>
@@ -14367,18 +14389,18 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
       <c r="B116" s="32" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C116" s="6">
         <v>43496</v>
       </c>
       <c r="D116" s="32" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E116" s="32" t="s">
         <v>125</v>
@@ -14387,7 +14409,7 @@
         <v>26</v>
       </c>
       <c r="G116" s="32" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I116" s="32"/>
       <c r="J116" s="32"/>
@@ -14413,18 +14435,18 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
       <c r="B117" s="91" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C117" s="37">
         <v>43497</v>
       </c>
       <c r="D117" s="28" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E117" s="28" t="s">
         <v>125</v>
@@ -14433,10 +14455,10 @@
         <v>26</v>
       </c>
       <c r="G117" s="28" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="I117" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J117" s="28"/>
       <c r="L117" s="28">
@@ -14461,18 +14483,18 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C118" s="6">
         <v>43517</v>
       </c>
       <c r="D118" s="32" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E118" s="32" t="s">
         <v>80</v>
@@ -14481,11 +14503,11 @@
         <v>26</v>
       </c>
       <c r="G118" s="32" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H118" s="14"/>
       <c r="I118" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J118" s="32"/>
       <c r="K118" s="32"/>
@@ -14505,25 +14527,25 @@
       <c r="Q118" s="5"/>
       <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T118" s="5"/>
       <c r="U118" s="32" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>121</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C119" s="6">
         <v>43517</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E119" s="32" t="s">
         <v>15</v>
@@ -14532,11 +14554,11 @@
         <v>26</v>
       </c>
       <c r="G119" s="32" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H119" s="14"/>
       <c r="I119" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J119" s="32"/>
       <c r="K119" s="32"/>
@@ -14559,13 +14581,13 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C120" s="6">
         <v>43517</v>
@@ -14578,11 +14600,11 @@
         <v>26</v>
       </c>
       <c r="G120" s="32" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H120" s="14"/>
       <c r="I120" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J120" s="32"/>
       <c r="K120" s="32"/>
@@ -14605,18 +14627,18 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>123</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C121" s="6">
         <v>43525</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E121" s="32" t="s">
         <v>32</v>
@@ -14625,11 +14647,11 @@
         <v>26</v>
       </c>
       <c r="G121" s="32" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H121" s="14"/>
       <c r="I121" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J121" s="32"/>
       <c r="K121" s="32"/>
@@ -14652,18 +14674,18 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>124</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C122" s="6">
         <v>43525</v>
       </c>
       <c r="D122" s="32" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E122" s="32" t="s">
         <v>32</v>
@@ -14672,11 +14694,11 @@
         <v>26</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H122" s="14"/>
       <c r="I122" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J122" s="32"/>
       <c r="K122" s="32"/>
@@ -14699,18 +14721,18 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>125</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C123" s="6">
         <v>43528</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E123" s="32" t="s">
         <v>15</v>
@@ -14719,11 +14741,11 @@
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J123" s="32"/>
       <c r="K123" s="32"/>
@@ -14746,7 +14768,7 @@
       <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14755,7 +14777,7 @@
         <v>43528</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>39</v>
@@ -14764,11 +14786,11 @@
         <v>26</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H124" s="14"/>
       <c r="I124" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J124" s="32"/>
       <c r="K124" s="32"/>
@@ -14791,18 +14813,18 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>127</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C125" s="6">
         <v>43529</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E125" s="32" t="s">
         <v>80</v>
@@ -14811,10 +14833,10 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I125" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J125" s="32"/>
       <c r="K125" s="32"/>
@@ -14833,23 +14855,23 @@
       <c r="Q125" s="5"/>
       <c r="R125" s="5"/>
       <c r="S125" s="33" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>128</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C126" s="6">
         <v>43531</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E126" s="32" t="s">
         <v>15</v>
@@ -14858,10 +14880,10 @@
         <v>26</v>
       </c>
       <c r="G126" s="32" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I126" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J126" s="32"/>
       <c r="K126" s="32"/>
@@ -14880,18 +14902,18 @@
       <c r="S126" s="33"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>129</v>
       </c>
       <c r="B127" s="90" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C127" s="6">
         <v>43550</v>
       </c>
       <c r="D127" s="32" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E127" s="32" t="s">
         <v>80</v>
@@ -14900,10 +14922,10 @@
         <v>26</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I127" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J127" s="32"/>
       <c r="K127" s="32"/>
@@ -14922,25 +14944,25 @@
       <c r="Q127" s="5"/>
       <c r="R127" s="5"/>
       <c r="S127" s="33" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T127" s="5"/>
       <c r="U127" s="32" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>130</v>
       </c>
       <c r="B128" s="99" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C128" s="37">
         <v>43550</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E128" s="28" t="s">
         <v>80</v>
@@ -14949,10 +14971,10 @@
         <v>26</v>
       </c>
       <c r="G128" s="28" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I128" s="28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J128" s="100"/>
       <c r="K128" s="28"/>
@@ -14972,25 +14994,25 @@
       <c r="Q128" s="39"/>
       <c r="R128" s="89"/>
       <c r="S128" s="15" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T128" s="28"/>
       <c r="U128" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="129" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="93">
         <v>131</v>
       </c>
       <c r="B129" s="90" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C129" s="6">
         <v>43550</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>80</v>
@@ -14999,10 +15021,10 @@
         <v>26</v>
       </c>
       <c r="G129" s="32" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I129" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J129" s="32"/>
       <c r="K129" s="32"/>
@@ -15022,23 +15044,23 @@
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
     </row>
-    <row r="130" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="93">
         <v>132</v>
       </c>
       <c r="B130" s="90" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C130" s="6">
         <v>43550</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>80</v>
@@ -15047,10 +15069,10 @@
         <v>26</v>
       </c>
       <c r="G130" s="32" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I130" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J130" s="32"/>
       <c r="K130" s="32"/>
@@ -15070,23 +15092,23 @@
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
     </row>
-    <row r="131" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="93">
         <v>133</v>
       </c>
       <c r="B131" s="90" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C131" s="6">
         <v>43550</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>80</v>
@@ -15095,10 +15117,10 @@
         <v>26</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I131" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J131" s="32"/>
       <c r="K131" s="32"/>
@@ -15118,23 +15140,23 @@
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
     </row>
-    <row r="132" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="93">
         <v>134</v>
       </c>
       <c r="B132" s="90" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C132" s="6">
         <v>43550</v>
       </c>
       <c r="D132" s="32" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E132" s="32" t="s">
         <v>80</v>
@@ -15143,10 +15165,10 @@
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I132" s="32" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J132" s="32"/>
       <c r="K132" s="32"/>
@@ -15166,32 +15188,32 @@
       <c r="Q132" s="5"/>
       <c r="R132" s="33"/>
       <c r="S132" s="14" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T132" s="32"/>
       <c r="U132" s="32"/>
     </row>
-    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="93">
         <v>135</v>
       </c>
       <c r="B133" s="90" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C133" s="6">
         <v>43552</v>
       </c>
       <c r="D133" s="92" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F133" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H133" s="95"/>
       <c r="I133" s="32"/>
@@ -15213,12 +15235,12 @@
       <c r="Q133" s="14"/>
       <c r="R133" s="32"/>
       <c r="S133" s="14" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="T133" s="32"/>
       <c r="U133" s="33"/>
     </row>
-    <row r="134" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="93">
         <v>136</v>
       </c>
@@ -15227,7 +15249,7 @@
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15236,7 +15258,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H134" s="95"/>
       <c r="I134" s="32"/>
@@ -15257,13 +15279,13 @@
       <c r="P134" s="97"/>
       <c r="Q134" s="33"/>
       <c r="R134" s="5" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S134" s="32"/>
       <c r="T134" s="33"/>
       <c r="U134" s="33"/>
     </row>
-    <row r="135" spans="1:21" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="266" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="93">
         <v>137</v>
       </c>
@@ -15272,7 +15294,7 @@
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15281,7 +15303,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H135" s="95"/>
       <c r="I135" s="32"/>
@@ -15302,13 +15324,13 @@
       <c r="P135" s="97"/>
       <c r="Q135" s="32"/>
       <c r="R135" s="5" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S135" s="33"/>
       <c r="T135" s="33"/>
       <c r="U135" s="33"/>
     </row>
-    <row r="136" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="93">
         <v>138</v>
       </c>
@@ -15317,7 +15339,7 @@
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -15326,7 +15348,7 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H136" s="95"/>
       <c r="I136" s="32"/>
@@ -15347,13 +15369,13 @@
       <c r="P136" s="10"/>
       <c r="Q136" s="33"/>
       <c r="R136" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S136" s="33"/>
       <c r="T136" s="33"/>
       <c r="U136" s="33"/>
     </row>
-    <row r="137" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="93">
         <v>139</v>
       </c>
@@ -15362,7 +15384,7 @@
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -15371,7 +15393,7 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H137" s="95"/>
       <c r="I137" s="32"/>
@@ -15392,13 +15414,13 @@
       <c r="P137" s="10"/>
       <c r="Q137" s="33"/>
       <c r="R137" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S137" s="33"/>
       <c r="T137" s="33"/>
       <c r="U137" s="33"/>
     </row>
-    <row r="138" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="93">
         <v>140</v>
       </c>
@@ -15407,7 +15429,7 @@
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -15416,7 +15438,7 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H138" s="95"/>
       <c r="I138" s="32"/>
@@ -15437,13 +15459,13 @@
       <c r="P138" s="10"/>
       <c r="Q138" s="33"/>
       <c r="R138" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
       <c r="U138" s="33"/>
     </row>
-    <row r="139" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="93">
         <v>141</v>
       </c>
@@ -15452,7 +15474,7 @@
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -15461,7 +15483,7 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="H139" s="95"/>
       <c r="I139" s="21"/>
@@ -15482,13 +15504,13 @@
       <c r="P139" s="10"/>
       <c r="Q139" s="33"/>
       <c r="R139" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S139" s="33"/>
       <c r="T139" s="33"/>
       <c r="U139" s="33"/>
     </row>
-    <row r="140" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="93">
         <v>142</v>
       </c>
@@ -15497,7 +15519,7 @@
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -15506,7 +15528,7 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H140" s="96"/>
       <c r="I140" s="5"/>
@@ -15527,13 +15549,13 @@
       <c r="P140" s="10"/>
       <c r="Q140" s="33"/>
       <c r="R140" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S140" s="33"/>
       <c r="T140" s="33"/>
       <c r="U140" s="33"/>
     </row>
-    <row r="141" spans="1:21" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="93">
         <v>143</v>
       </c>
@@ -15542,7 +15564,7 @@
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -15551,7 +15573,7 @@
         <v>26</v>
       </c>
       <c r="G141" s="32" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H141" s="97"/>
       <c r="I141" s="33"/>
@@ -15572,13 +15594,13 @@
       <c r="P141" s="10"/>
       <c r="Q141" s="33"/>
       <c r="R141" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S141" s="33"/>
       <c r="T141" s="33"/>
       <c r="U141" s="33"/>
     </row>
-    <row r="142" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="93">
         <v>144</v>
       </c>
@@ -15587,7 +15609,7 @@
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -15596,7 +15618,7 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H142" s="33"/>
       <c r="I142" s="32"/>
@@ -15617,13 +15639,13 @@
       <c r="P142" s="94"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S142" s="33"/>
       <c r="T142" s="33"/>
       <c r="U142" s="33"/>
     </row>
-    <row r="143" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="93">
         <v>145</v>
       </c>
@@ -15632,7 +15654,7 @@
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -15641,7 +15663,7 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H143" s="32"/>
       <c r="I143" s="33"/>
@@ -15662,13 +15684,13 @@
       <c r="P143" s="94"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S143" s="33"/>
       <c r="T143" s="33"/>
       <c r="U143" s="33"/>
     </row>
-    <row r="144" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="93">
         <v>146</v>
       </c>
@@ -15677,7 +15699,7 @@
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>39</v>
@@ -15686,7 +15708,7 @@
         <v>26</v>
       </c>
       <c r="G144" s="32" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H144" s="33"/>
       <c r="I144" s="14"/>
@@ -15707,13 +15729,13 @@
       <c r="P144" s="10"/>
       <c r="Q144" s="33"/>
       <c r="R144" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S144" s="33"/>
       <c r="T144" s="33"/>
       <c r="U144" s="33"/>
     </row>
-    <row r="145" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="93">
         <v>147</v>
       </c>
@@ -15722,7 +15744,7 @@
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>212</v>
@@ -15731,7 +15753,7 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
@@ -15752,13 +15774,13 @@
       <c r="P145" s="10"/>
       <c r="Q145" s="33"/>
       <c r="R145" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S145" s="33"/>
       <c r="T145" s="33"/>
       <c r="U145" s="33"/>
     </row>
-    <row r="146" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="93">
         <v>148</v>
       </c>
@@ -15767,7 +15789,7 @@
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>212</v>
@@ -15776,7 +15798,7 @@
         <v>26</v>
       </c>
       <c r="G146" s="32" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H146" s="14"/>
       <c r="I146" s="32"/>
@@ -15797,13 +15819,13 @@
       <c r="P146" s="10"/>
       <c r="Q146" s="33"/>
       <c r="R146" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S146" s="33"/>
       <c r="T146" s="33"/>
       <c r="U146" s="33"/>
     </row>
-    <row r="147" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="93">
         <v>149</v>
       </c>
@@ -15812,7 +15834,7 @@
         <v>43552</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E147" s="32" t="s">
         <v>39</v>
@@ -15821,7 +15843,7 @@
         <v>26</v>
       </c>
       <c r="G147" s="32" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H147" s="32"/>
       <c r="I147" s="32"/>
@@ -15842,13 +15864,13 @@
       <c r="P147" s="10"/>
       <c r="Q147" s="33"/>
       <c r="R147" s="33" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S147" s="33"/>
       <c r="T147" s="33"/>
       <c r="U147" s="33"/>
     </row>
-    <row r="148" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="101">
         <v>150</v>
       </c>
@@ -15857,7 +15879,7 @@
         <v>43552</v>
       </c>
       <c r="D148" s="28" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E148" s="28" t="s">
         <v>39</v>
@@ -15866,7 +15888,7 @@
         <v>26</v>
       </c>
       <c r="G148" s="28" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H148" s="32"/>
       <c r="I148" s="38"/>
@@ -15887,25 +15909,25 @@
       <c r="P148" s="10"/>
       <c r="Q148" s="89"/>
       <c r="R148" s="89" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="S148" s="89"/>
       <c r="T148" s="89"/>
       <c r="U148" s="89"/>
     </row>
-    <row r="149" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <f>1+A126</f>
         <v>129</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C149" s="6">
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -15914,7 +15936,7 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I149" s="32"/>
       <c r="J149" s="32"/>
@@ -15937,19 +15959,19 @@
       </c>
       <c r="U149" s="32"/>
     </row>
-    <row r="150" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <f t="shared" ref="A150:A153" si="8">1+A127</f>
         <v>130</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C150" s="6">
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -15958,7 +15980,7 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I150" s="32"/>
       <c r="J150" s="32"/>
@@ -15981,19 +16003,19 @@
       </c>
       <c r="U150" s="32"/>
     </row>
-    <row r="151" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <f t="shared" si="8"/>
         <v>131</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C151" s="6">
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16002,7 +16024,7 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="I151" s="32"/>
       <c r="J151" s="32"/>
@@ -16021,19 +16043,19 @@
       </c>
       <c r="U151" s="32"/>
     </row>
-    <row r="152" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <f t="shared" si="8"/>
         <v>132</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C152" s="6">
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16042,7 +16064,7 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I152" s="32"/>
       <c r="J152" s="32"/>
@@ -16059,19 +16081,19 @@
       <c r="T152" s="5"/>
       <c r="U152" s="32"/>
     </row>
-    <row r="153" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <f t="shared" si="8"/>
         <v>133</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C153" s="6">
         <v>43553</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E153" s="32" t="s">
         <v>15</v>
@@ -16080,7 +16102,7 @@
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="I153" s="32"/>
       <c r="J153" s="32"/>
@@ -16103,27 +16125,27 @@
       </c>
       <c r="U153" s="32"/>
     </row>
-    <row r="154" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="93">
         <v>151</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C154" s="6">
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E154" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F154" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G154" s="32" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H154" s="21"/>
       <c r="I154" s="21"/>
@@ -16148,27 +16170,27 @@
       <c r="T154" s="5"/>
       <c r="U154" s="32"/>
     </row>
-    <row r="155" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="93">
         <v>152</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C155" s="6">
         <v>43550</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E155" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F155" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G155" s="32" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H155" s="21"/>
       <c r="I155" s="32"/>
@@ -16183,7 +16205,7 @@
       <c r="N155" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="O155" s="108">
+      <c r="O155" s="102">
         <v>43550</v>
       </c>
       <c r="P155" s="33"/>
@@ -16193,27 +16215,27 @@
       <c r="T155" s="5"/>
       <c r="U155" s="32"/>
     </row>
-    <row r="156" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="93">
         <v>153</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C156" s="6">
         <v>43550</v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E156" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F156" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G156" s="32" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="H156" s="32"/>
       <c r="I156" s="32"/>
@@ -16228,7 +16250,7 @@
       <c r="N156" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="O156" s="108">
+      <c r="O156" s="102">
         <v>43550</v>
       </c>
       <c r="P156" s="33"/>
@@ -16238,27 +16260,27 @@
       <c r="T156" s="5"/>
       <c r="U156" s="32"/>
     </row>
-    <row r="157" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="93">
         <v>154</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C157" s="6">
         <v>43556</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E157" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F157" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H157" s="32"/>
       <c r="I157" s="32"/>
@@ -16273,7 +16295,7 @@
       <c r="N157" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O157" s="108">
+      <c r="O157" s="102">
         <v>43556</v>
       </c>
       <c r="P157" s="33"/>
@@ -16283,27 +16305,27 @@
       <c r="T157" s="5"/>
       <c r="U157" s="32"/>
     </row>
-    <row r="158" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="93">
         <v>155</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C158" s="6">
         <v>43552</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F158" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H158" s="32"/>
       <c r="I158" s="32"/>
@@ -16318,7 +16340,7 @@
       <c r="N158" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="O158" s="108">
+      <c r="O158" s="102">
         <v>43552</v>
       </c>
       <c r="P158" s="33"/>
@@ -16328,49 +16350,97 @@
       <c r="T158" s="5"/>
       <c r="U158" s="32"/>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A159" s="5"/>
-      <c r="B159" s="31"/>
-      <c r="C159" s="5"/>
-      <c r="D159" s="32"/>
-      <c r="E159" s="32"/>
-      <c r="F159" s="32"/>
-      <c r="G159" s="32"/>
+    <row r="159" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A159" s="5">
+        <v>134</v>
+      </c>
+      <c r="B159" s="31" t="s">
+        <v>554</v>
+      </c>
+      <c r="C159" s="6">
+        <v>43546</v>
+      </c>
+      <c r="D159" s="32" t="s">
+        <v>555</v>
+      </c>
+      <c r="E159" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F159" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G159" s="32" t="s">
+        <v>556</v>
+      </c>
+      <c r="H159" s="32"/>
       <c r="I159" s="32"/>
       <c r="J159" s="32"/>
-      <c r="K159" s="32"/>
+      <c r="K159" s="32">
+        <v>1</v>
+      </c>
       <c r="L159" s="32"/>
       <c r="M159" s="32"/>
       <c r="N159" s="32"/>
-      <c r="O159" s="32"/>
-      <c r="Q159" s="5"/>
-      <c r="R159" s="5"/>
-      <c r="S159" s="33"/>
+      <c r="O159" s="5">
+        <v>6</v>
+      </c>
+      <c r="P159" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q159" s="33"/>
+      <c r="R159" s="5">
+        <v>10</v>
+      </c>
+      <c r="S159" s="32"/>
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A160" s="5"/>
-      <c r="B160" s="31"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="32"/>
-      <c r="E160" s="32"/>
-      <c r="F160" s="32"/>
-      <c r="G160" s="32"/>
+    <row r="160" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A160" s="5">
+        <v>135</v>
+      </c>
+      <c r="B160" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C160" s="6">
+        <v>43528</v>
+      </c>
+      <c r="D160" s="32" t="s">
+        <v>558</v>
+      </c>
+      <c r="E160" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F160" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G160" s="32" t="s">
+        <v>559</v>
+      </c>
+      <c r="H160" s="32"/>
       <c r="I160" s="32"/>
       <c r="J160" s="32"/>
-      <c r="K160" s="32"/>
+      <c r="K160" s="32">
+        <v>1</v>
+      </c>
       <c r="L160" s="32"/>
       <c r="M160" s="32"/>
       <c r="N160" s="32"/>
-      <c r="O160" s="32"/>
-      <c r="Q160" s="5"/>
-      <c r="R160" s="5"/>
-      <c r="S160" s="33"/>
+      <c r="O160" s="5">
+        <v>6</v>
+      </c>
+      <c r="P160" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q160" s="33"/>
+      <c r="R160" s="5">
+        <v>9</v>
+      </c>
+      <c r="S160" s="32"/>
       <c r="T160" s="5"/>
       <c r="U160" s="32"/>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A161" s="5"/>
       <c r="B161" s="31"/>
       <c r="C161" s="5"/>
@@ -16392,19 +16462,26 @@
       <c r="U161" s="32"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:U158">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Registration Client"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D133" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D133" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -16412,57 +16489,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -16472,19 +16549,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -16495,7 +16572,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -16506,7 +16583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -16517,7 +16594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -16528,7 +16605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -16539,7 +16616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -16550,7 +16627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -16561,7 +16638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -16572,7 +16649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -16590,17 +16667,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="66" t="s">
         <v>207</v>
       </c>
@@ -16608,25 +16685,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="70"/>
       <c r="C3" s="69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="71"/>
       <c r="C4" s="69" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="72"/>
       <c r="C5" s="73" t="s">
         <v>206</v>
@@ -16639,15 +16716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -16668,6 +16736,15 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16843,14 +16920,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -16862,6 +16931,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Final file for Reg client
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="563">
   <si>
     <t>S.No.</t>
   </si>
@@ -2748,9 +2748,6 @@
     <t>MOS-12989</t>
   </si>
   <si>
-    <t>MOS-13519</t>
-  </si>
-  <si>
     <t>MOS-13522</t>
   </si>
   <si>
@@ -3597,20 +3594,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">MOS-13523, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>MOS-13659</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <u/>
         <sz val="11"/>
@@ -4812,9 +4795,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>MOS-14566</t>
-  </si>
-  <si>
     <t>MOS-8641</t>
   </si>
   <si>
@@ -5416,14 +5396,47 @@
     <t>As the MOSIP Registration Client, I should validate there are no blacklisted words in demographic data</t>
   </si>
   <si>
+    <t>New visual designs created by UI team</t>
+  </si>
+  <si>
+    <t>Visual design changes</t>
+  </si>
+  <si>
+    <t>MOS-14566
+MOS-14565</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MOS-13523, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>MOS-13659</t>
+    </r>
+  </si>
+  <si>
     <t>MOS-15324
-MOS-14999</t>
-  </si>
-  <si>
-    <t>New visual designs created by UI team</t>
-  </si>
-  <si>
-    <t>Visual design changes</t>
+MOS-14999
+MOS-13080</t>
+  </si>
+  <si>
+    <t>MOS-13519
+MOS-12999</t>
+  </si>
+  <si>
+    <t>MOS-12867</t>
+  </si>
+  <si>
+    <t>As the MOSIP registration client, I should enable registration only when packets pending EoD approval are within configured limits</t>
+  </si>
+  <si>
+    <t>CR for MOS 236</t>
   </si>
 </sst>
 </file>
@@ -7328,7 +7341,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7680,9 +7693,9 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:W161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159:S160"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W161" sqref="W161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -7768,7 +7781,7 @@
         <v>228</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>8</v>
@@ -7821,7 +7834,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>17</v>
@@ -7830,13 +7843,13 @@
         <v>18</v>
       </c>
       <c r="J3" s="32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="K3" s="32" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L3" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M3" s="32" t="s">
         <v>19</v>
@@ -7860,7 +7873,7 @@
       <c r="S3" s="30"/>
       <c r="T3" s="30"/>
       <c r="U3" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
@@ -7868,7 +7881,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="84" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C4" s="6">
         <v>43362</v>
@@ -7883,7 +7896,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>17</v>
@@ -7895,7 +7908,7 @@
         <v>265</v>
       </c>
       <c r="K4" s="32" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L4" s="32">
         <v>1</v>
@@ -7921,7 +7934,7 @@
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="21" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
@@ -7956,10 +7969,10 @@
         <v>230</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L5" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>19</v>
@@ -7991,7 +8004,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C6" s="6">
         <v>43362</v>
@@ -8006,7 +8019,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>17</v>
@@ -8018,10 +8031,10 @@
         <v>230</v>
       </c>
       <c r="K6" s="32" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L6" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M6" s="32" t="s">
         <v>19</v>
@@ -8045,7 +8058,7 @@
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
       <c r="U6" s="21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
@@ -8080,10 +8093,10 @@
         <v>231</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L7" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M7" s="32" t="s">
         <v>19</v>
@@ -8107,7 +8120,7 @@
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
       <c r="U7" s="21" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
@@ -8115,7 +8128,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C8" s="6">
         <v>43362</v>
@@ -8130,7 +8143,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>17</v>
@@ -8142,10 +8155,10 @@
         <v>231</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L8" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>19</v>
@@ -8169,7 +8182,7 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="21" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
@@ -8202,10 +8215,10 @@
       </c>
       <c r="J9" s="19"/>
       <c r="K9" s="32" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L9" s="85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M9" s="32" t="s">
         <v>19</v>
@@ -8229,7 +8242,7 @@
       <c r="S9" s="30"/>
       <c r="T9" s="30"/>
       <c r="U9" s="22" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
@@ -8237,7 +8250,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C10" s="6">
         <v>43362</v>
@@ -8252,7 +8265,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>17</v>
@@ -8262,7 +8275,7 @@
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L10" s="19">
         <v>1</v>
@@ -8289,7 +8302,7 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="22" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
@@ -8364,7 +8377,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>17</v>
@@ -8374,7 +8387,7 @@
       </c>
       <c r="J12" s="32"/>
       <c r="K12" s="32" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L12" s="32">
         <v>1</v>
@@ -8400,7 +8413,7 @@
       <c r="S12" s="30"/>
       <c r="T12" s="30"/>
       <c r="U12" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="1" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.35">
@@ -8408,7 +8421,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C13" s="6">
         <v>43395</v>
@@ -8474,7 +8487,7 @@
         <v>26</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>38</v>
@@ -8484,7 +8497,7 @@
       </c>
       <c r="J14" s="19"/>
       <c r="K14" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L14" s="32">
         <v>1</v>
@@ -8511,7 +8524,7 @@
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="21" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
@@ -8519,7 +8532,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C15" s="6">
         <v>43397</v>
@@ -8581,7 +8594,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C16" s="6">
         <v>43397</v>
@@ -8643,7 +8656,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C17" s="6">
         <v>43397</v>
@@ -8765,7 +8778,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C19" s="6">
         <v>43397</v>
@@ -8948,7 +8961,7 @@
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L22" s="32">
         <v>1</v>
@@ -8975,7 +8988,7 @@
       <c r="S22" s="30"/>
       <c r="T22" s="30"/>
       <c r="U22" s="21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
@@ -8983,7 +8996,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>469</v>
+        <v>556</v>
       </c>
       <c r="C23" s="6">
         <v>43402</v>
@@ -8998,7 +9011,7 @@
         <v>26</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>38</v>
@@ -9008,7 +9021,7 @@
       </c>
       <c r="J23" s="32"/>
       <c r="K23" s="32" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L23" s="32" t="s">
         <v>140</v>
@@ -9035,7 +9048,7 @@
       <c r="S23" s="30"/>
       <c r="T23" s="30"/>
       <c r="U23" s="21" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
@@ -9043,7 +9056,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C24" s="6">
         <v>43402</v>
@@ -9205,7 +9218,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="83" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C27" s="6">
         <v>43402</v>
@@ -9230,7 +9243,7 @@
       </c>
       <c r="J27" s="32"/>
       <c r="K27" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L27" s="32">
         <v>1</v>
@@ -9265,7 +9278,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="83" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C28" s="6">
         <v>43418</v>
@@ -9289,10 +9302,10 @@
         <v>54</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L28" s="14">
         <v>1</v>
@@ -9545,11 +9558,11 @@
         <v>269</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="32" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
@@ -9570,7 +9583,7 @@
         <v>33</v>
       </c>
       <c r="G33" s="46" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H33" s="14" t="s">
         <v>38</v>
@@ -9579,7 +9592,7 @@
         <v>82</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32">
@@ -9639,13 +9652,13 @@
         <v>85</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K34" s="32" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L34" s="85" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M34" s="32" t="s">
         <v>74</v>
@@ -9677,7 +9690,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="83" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C35" s="6">
         <v>43430</v>
@@ -9692,7 +9705,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>38</v>
@@ -9702,7 +9715,7 @@
       </c>
       <c r="J35" s="32"/>
       <c r="K35" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L35" s="32">
         <v>1</v>
@@ -9734,7 +9747,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C36" s="6">
         <v>43430</v>
@@ -9798,7 +9811,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C37" s="6">
         <v>43430</v>
@@ -9848,10 +9861,10 @@
         <v>269</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="T37" s="30" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="U37" s="32" t="s">
         <v>160</v>
@@ -9862,7 +9875,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C38" s="6">
         <v>43430</v>
@@ -9926,7 +9939,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C39" s="6">
         <v>43430</v>
@@ -9990,7 +10003,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C40" s="6">
         <v>43430</v>
@@ -10044,7 +10057,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C41" s="6">
         <v>43430</v>
@@ -10059,7 +10072,7 @@
         <v>26</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H41" s="14" t="s">
         <v>38</v>
@@ -10069,10 +10082,10 @@
       </c>
       <c r="J41" s="32"/>
       <c r="K41" s="32" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L41" s="85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M41" s="32" t="s">
         <v>74</v>
@@ -10156,7 +10169,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="87" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C43" s="6">
         <v>43427</v>
@@ -10171,7 +10184,7 @@
         <v>26</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H43" s="14" t="s">
         <v>38</v>
@@ -10181,7 +10194,7 @@
       </c>
       <c r="J43" s="32"/>
       <c r="K43" s="32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L43" s="32">
         <v>2</v>
@@ -10214,7 +10227,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C44" s="6">
         <v>43427</v>
@@ -10274,7 +10287,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C45" s="6">
         <v>43427</v>
@@ -10332,7 +10345,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C46" s="6">
         <v>43427</v>
@@ -10394,7 +10407,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C47" s="6">
         <v>43427</v>
@@ -10442,7 +10455,7 @@
         <v>269</v>
       </c>
       <c r="S47" s="75" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="T47" s="30" t="s">
         <v>156</v>
@@ -10506,7 +10519,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C49" s="6">
         <v>43427</v>
@@ -10568,7 +10581,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C50" s="6">
         <v>43427</v>
@@ -10623,7 +10636,7 @@
         <v>156</v>
       </c>
       <c r="U50" s="32" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="42" x14ac:dyDescent="0.35">
@@ -10760,7 +10773,7 @@
       </c>
       <c r="J53" s="32"/>
       <c r="K53" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L53" s="32">
         <v>1</v>
@@ -10899,7 +10912,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="83" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C56" s="6">
         <v>43427</v>
@@ -10914,7 +10927,7 @@
         <v>26</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>38</v>
@@ -10924,7 +10937,7 @@
       </c>
       <c r="J56" s="32"/>
       <c r="K56" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L56" s="32">
         <v>1</v>
@@ -10950,7 +10963,7 @@
       <c r="S56" s="30"/>
       <c r="T56" s="30"/>
       <c r="U56" s="32" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
@@ -10958,7 +10971,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="83" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C57" s="6">
         <v>43427</v>
@@ -10973,7 +10986,7 @@
         <v>26</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>38</v>
@@ -10983,7 +10996,7 @@
       </c>
       <c r="J57" s="32"/>
       <c r="K57" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L57" s="32" t="s">
         <v>140</v>
@@ -11017,7 +11030,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="84" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C58" s="6">
         <v>43427</v>
@@ -11042,10 +11055,10 @@
       </c>
       <c r="J58" s="32"/>
       <c r="K58" s="32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="L58" s="85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M58" s="32" t="s">
         <v>74</v>
@@ -11185,7 +11198,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C61" s="6">
         <v>43432</v>
@@ -11228,7 +11241,7 @@
         <v>4</v>
       </c>
       <c r="Q61" s="81" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="R61" s="30" t="s">
         <v>269</v>
@@ -11242,7 +11255,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C62" s="6">
         <v>43432</v>
@@ -11305,7 +11318,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C63" s="6">
         <v>43432</v>
@@ -11468,7 +11481,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C66" s="6">
         <v>43440</v>
@@ -11517,13 +11530,13 @@
         <v>269</v>
       </c>
       <c r="S66" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="T66" s="5" t="s">
         <v>172</v>
       </c>
       <c r="U66" s="32" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
@@ -11556,7 +11569,7 @@
       </c>
       <c r="J67" s="32"/>
       <c r="K67" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L67" s="32" t="s">
         <v>140</v>
@@ -11591,7 +11604,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C68" s="6">
         <v>43440</v>
@@ -11640,7 +11653,7 @@
         <v>269</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T68" s="5"/>
       <c r="U68" s="32" t="s">
@@ -11652,7 +11665,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="83" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C69" s="6">
         <v>43446</v>
@@ -11677,7 +11690,7 @@
       </c>
       <c r="J69" s="32"/>
       <c r="K69" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L69" s="32">
         <v>1</v>
@@ -11712,7 +11725,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="83" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C70" s="6">
         <v>43446</v>
@@ -11727,7 +11740,7 @@
         <v>26</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H70" s="14" t="s">
         <v>38</v>
@@ -11737,7 +11750,7 @@
       </c>
       <c r="J70" s="32"/>
       <c r="K70" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L70" s="32">
         <v>1</v>
@@ -11770,7 +11783,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="83" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C71" s="6">
         <v>43451</v>
@@ -11785,7 +11798,7 @@
         <v>26</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H71" s="14" t="s">
         <v>38</v>
@@ -11795,7 +11808,7 @@
       </c>
       <c r="J71" s="32"/>
       <c r="K71" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L71" s="32">
         <v>1</v>
@@ -11830,7 +11843,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C72" s="6">
         <v>43451</v>
@@ -11879,7 +11892,7 @@
         <v>269</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T72" s="5"/>
       <c r="U72" s="32" t="s">
@@ -11918,7 +11931,7 @@
       </c>
       <c r="J73" s="32"/>
       <c r="K73" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L73" s="32">
         <v>1</v>
@@ -12008,7 +12021,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C75" s="37">
         <v>43454</v>
@@ -12069,7 +12082,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C76" s="6">
         <v>43454</v>
@@ -12130,7 +12143,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="87" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C77" s="6">
         <v>43465</v>
@@ -12145,7 +12158,7 @@
         <v>26</v>
       </c>
       <c r="G77" s="32" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>38</v>
@@ -12155,10 +12168,10 @@
       </c>
       <c r="J77" s="32"/>
       <c r="K77" s="32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L77" s="85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M77" s="32" t="s">
         <v>74</v>
@@ -12190,7 +12203,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C78" s="6">
         <v>43465</v>
@@ -12205,7 +12218,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="32" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>38</v>
@@ -12215,10 +12228,10 @@
       </c>
       <c r="J78" s="32"/>
       <c r="K78" s="32" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L78" s="85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M78" s="32" t="s">
         <v>74</v>
@@ -12252,7 +12265,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="84" t="s">
-        <v>291</v>
+        <v>559</v>
       </c>
       <c r="C79" s="6">
         <v>43465</v>
@@ -12267,7 +12280,7 @@
         <v>26</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H79" s="14" t="s">
         <v>38</v>
@@ -12277,10 +12290,10 @@
       </c>
       <c r="J79" s="32"/>
       <c r="K79" s="32" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L79" s="85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M79" s="32" t="s">
         <v>74</v>
@@ -12312,7 +12325,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C80" s="6">
         <v>43465</v>
@@ -12337,10 +12350,10 @@
       </c>
       <c r="J80" s="32"/>
       <c r="K80" s="32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L80" s="85" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M80" s="32" t="s">
         <v>74</v>
@@ -12374,7 +12387,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>350</v>
+        <v>557</v>
       </c>
       <c r="C81" s="6">
         <v>43465</v>
@@ -12389,7 +12402,7 @@
         <v>26</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H81" s="14" t="s">
         <v>38</v>
@@ -12399,10 +12412,10 @@
       </c>
       <c r="J81" s="32"/>
       <c r="K81" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L81" s="85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M81" s="32" t="s">
         <v>74</v>
@@ -12434,7 +12447,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="84" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C82" s="6">
         <v>43465</v>
@@ -12449,7 +12462,7 @@
         <v>26</v>
       </c>
       <c r="G82" s="32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H82" s="14" t="s">
         <v>38</v>
@@ -12459,7 +12472,7 @@
       </c>
       <c r="J82" s="32"/>
       <c r="K82" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L82" s="32">
         <v>1</v>
@@ -12555,7 +12568,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="84" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C84" s="6">
         <v>43465</v>
@@ -12570,7 +12583,7 @@
         <v>26</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H84" s="14" t="s">
         <v>38</v>
@@ -12580,7 +12593,7 @@
       </c>
       <c r="J84" s="32"/>
       <c r="K84" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L84" s="32">
         <v>1</v>
@@ -12607,7 +12620,7 @@
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
       <c r="U84" s="32" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="V84" s="74"/>
       <c r="W84" s="32"/>
@@ -12617,7 +12630,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="83" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C85" s="6">
         <v>43477</v>
@@ -12641,10 +12654,10 @@
         <v>85</v>
       </c>
       <c r="J85" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K85" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L85" s="32">
         <v>1</v>
@@ -12679,7 +12692,7 @@
         <v>83</v>
       </c>
       <c r="B86" s="83" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C86" s="6">
         <v>43477</v>
@@ -12703,10 +12716,10 @@
         <v>85</v>
       </c>
       <c r="J86" s="32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K86" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L86" s="32">
         <v>1</v>
@@ -12739,7 +12752,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C87" s="6">
         <v>43477</v>
@@ -12763,7 +12776,7 @@
         <v>85</v>
       </c>
       <c r="J87" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32">
@@ -12798,7 +12811,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C88" s="6">
         <v>43477</v>
@@ -12845,13 +12858,13 @@
         <v>269</v>
       </c>
       <c r="S88" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="T88" s="5" t="s">
         <v>172</v>
       </c>
       <c r="U88" s="32" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
@@ -12859,7 +12872,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C89" s="6">
         <v>43477</v>
@@ -12903,7 +12916,7 @@
       <c r="R89" s="5"/>
       <c r="S89" s="33"/>
       <c r="T89" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="U89" s="32" t="s">
         <v>270</v>
@@ -13010,7 +13023,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="84" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C92" s="6">
         <v>43486</v>
@@ -13070,7 +13083,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="83" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C93" s="6">
         <v>43489</v>
@@ -13085,7 +13098,7 @@
         <v>26</v>
       </c>
       <c r="G93" s="32" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H93" s="14" t="s">
         <v>245</v>
@@ -13095,7 +13108,7 @@
       </c>
       <c r="J93" s="32"/>
       <c r="K93" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L93" s="32">
         <v>1</v>
@@ -13128,7 +13141,7 @@
         <v>91</v>
       </c>
       <c r="B94" s="84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C94" s="6">
         <v>43489</v>
@@ -13143,7 +13156,7 @@
         <v>26</v>
       </c>
       <c r="G94" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H94" s="14" t="s">
         <v>245</v>
@@ -13153,7 +13166,7 @@
       </c>
       <c r="J94" s="32"/>
       <c r="K94" s="32" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L94" s="85" t="s">
         <v>140</v>
@@ -13188,7 +13201,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C95" s="6">
         <v>43489</v>
@@ -13203,7 +13216,7 @@
         <v>26</v>
       </c>
       <c r="G95" s="32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H95" s="14" t="s">
         <v>245</v>
@@ -13248,7 +13261,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C96" s="6">
         <v>43489</v>
@@ -13263,7 +13276,7 @@
         <v>26</v>
       </c>
       <c r="G96" s="32" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H96" s="14" t="s">
         <v>245</v>
@@ -13308,13 +13321,13 @@
         <v>94</v>
       </c>
       <c r="B97" s="83" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C97" s="6">
         <v>43473</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E97" s="32" t="s">
         <v>15</v>
@@ -13323,7 +13336,7 @@
         <v>26</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H97" s="14" t="s">
         <v>245</v>
@@ -13333,7 +13346,7 @@
       </c>
       <c r="J97" s="32"/>
       <c r="K97" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L97" s="85">
         <v>1</v>
@@ -13366,13 +13379,13 @@
         <v>95</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C98" s="6">
         <v>43473</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E98" s="32" t="s">
         <v>80</v>
@@ -13381,7 +13394,7 @@
         <v>26</v>
       </c>
       <c r="G98" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H98" s="14" t="s">
         <v>38</v>
@@ -13407,7 +13420,7 @@
       <c r="Q98" s="82"/>
       <c r="R98" s="5"/>
       <c r="S98" s="33" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
@@ -13417,7 +13430,7 @@
         <v>96</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C99" s="6">
         <v>43489</v>
@@ -13432,7 +13445,7 @@
         <v>26</v>
       </c>
       <c r="G99" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H99" s="14" t="s">
         <v>245</v>
@@ -13442,7 +13455,7 @@
       </c>
       <c r="J99" s="32"/>
       <c r="K99" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L99" s="85">
         <v>1</v>
@@ -13475,7 +13488,7 @@
         <v>97</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C100" s="6">
         <v>43489</v>
@@ -13490,7 +13503,7 @@
         <v>26</v>
       </c>
       <c r="G100" s="32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H100" s="14" t="s">
         <v>245</v>
@@ -13500,7 +13513,7 @@
       </c>
       <c r="J100" s="32"/>
       <c r="K100" s="32" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="L100" s="85">
         <v>1</v>
@@ -13535,7 +13548,7 @@
         <v>98</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C101" s="6">
         <v>43489</v>
@@ -13550,7 +13563,7 @@
         <v>26</v>
       </c>
       <c r="G101" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H101" s="14" t="s">
         <v>245</v>
@@ -13560,7 +13573,7 @@
       </c>
       <c r="J101" s="32"/>
       <c r="K101" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L101" s="85">
         <v>1</v>
@@ -13595,7 +13608,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C102" s="6">
         <v>43489</v>
@@ -13610,7 +13623,7 @@
         <v>26</v>
       </c>
       <c r="G102" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H102" s="14" t="s">
         <v>245</v>
@@ -13620,7 +13633,7 @@
       </c>
       <c r="J102" s="32"/>
       <c r="K102" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L102" s="85">
         <v>1</v>
@@ -13653,7 +13666,7 @@
         <v>100</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C103" s="6">
         <v>43489</v>
@@ -13668,7 +13681,7 @@
         <v>26</v>
       </c>
       <c r="G103" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H103" s="14" t="s">
         <v>245</v>
@@ -13678,7 +13691,7 @@
       </c>
       <c r="J103" s="32"/>
       <c r="K103" s="32" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L103" s="85">
         <v>1</v>
@@ -13713,7 +13726,7 @@
         <v>101</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C104" s="6">
         <v>43489</v>
@@ -13728,7 +13741,7 @@
         <v>26</v>
       </c>
       <c r="G104" s="32" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H104" s="14" t="s">
         <v>245</v>
@@ -13773,7 +13786,7 @@
         <v>102</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C105" s="6">
         <v>43448</v>
@@ -13820,10 +13833,10 @@
         <v>269</v>
       </c>
       <c r="S105" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="T105" s="32" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="U105" s="33"/>
     </row>
@@ -13832,7 +13845,7 @@
         <v>103</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C106" s="6">
         <v>43447</v>
@@ -13877,13 +13890,13 @@
         <v>269</v>
       </c>
       <c r="S106" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="T106" s="32" t="s">
         <v>180</v>
       </c>
       <c r="U106" s="88" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="107" spans="1:21" ht="84" hidden="1" x14ac:dyDescent="0.35">
@@ -13891,7 +13904,7 @@
         <v>104</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C107" s="6">
         <v>43495</v>
@@ -13932,7 +13945,7 @@
       <c r="Q107" s="5"/>
       <c r="R107" s="5"/>
       <c r="S107" s="33" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
@@ -13942,7 +13955,7 @@
         <v>105</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C108" s="6">
         <v>43495</v>
@@ -13967,7 +13980,7 @@
       </c>
       <c r="J108" s="32"/>
       <c r="K108" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L108" s="32">
         <v>1</v>
@@ -13993,7 +14006,7 @@
       <c r="S108" s="33"/>
       <c r="T108" s="5"/>
       <c r="U108" s="85" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="109" spans="1:21" ht="98" hidden="1" x14ac:dyDescent="0.35">
@@ -14001,13 +14014,13 @@
         <v>111</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C109" s="6">
         <v>43108</v>
       </c>
       <c r="D109" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E109" s="32" t="s">
         <v>125</v>
@@ -14016,10 +14029,10 @@
         <v>26</v>
       </c>
       <c r="G109" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I109" s="32" t="s">
         <v>85</v>
@@ -14056,13 +14069,13 @@
         <v>112</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C110" s="6">
         <v>43108</v>
       </c>
       <c r="D110" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E110" s="32" t="s">
         <v>39</v>
@@ -14071,10 +14084,10 @@
         <v>26</v>
       </c>
       <c r="G110" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H110" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I110" s="32" t="s">
         <v>85</v>
@@ -14111,13 +14124,13 @@
         <v>113</v>
       </c>
       <c r="B111" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C111" s="6">
         <v>43436</v>
       </c>
       <c r="D111" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E111" s="32" t="s">
         <v>125</v>
@@ -14126,10 +14139,10 @@
         <v>26</v>
       </c>
       <c r="G111" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H111" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I111" s="32" t="s">
         <v>85</v>
@@ -14159,7 +14172,7 @@
       </c>
       <c r="S111" s="33"/>
       <c r="T111" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U111" s="32"/>
     </row>
@@ -14168,13 +14181,13 @@
         <v>114</v>
       </c>
       <c r="B112" s="32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C112" s="6">
         <v>43436</v>
       </c>
       <c r="D112" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E112" s="32" t="s">
         <v>125</v>
@@ -14183,10 +14196,10 @@
         <v>26</v>
       </c>
       <c r="G112" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I112" s="32" t="s">
         <v>85</v>
@@ -14216,7 +14229,7 @@
       </c>
       <c r="S112" s="33"/>
       <c r="T112" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U112" s="32"/>
     </row>
@@ -14225,13 +14238,13 @@
         <v>115</v>
       </c>
       <c r="B113" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C113" s="6">
         <v>43496</v>
       </c>
       <c r="D113" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E113" s="32" t="s">
         <v>125</v>
@@ -14240,10 +14253,10 @@
         <v>26</v>
       </c>
       <c r="G113" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H113" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I113" s="32" t="s">
         <v>85</v>
@@ -14273,7 +14286,7 @@
       </c>
       <c r="S113" s="33"/>
       <c r="T113" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U113" s="32"/>
     </row>
@@ -14282,13 +14295,13 @@
         <v>116</v>
       </c>
       <c r="B114" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C114" s="6">
         <v>43496</v>
       </c>
       <c r="D114" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E114" s="32" t="s">
         <v>125</v>
@@ -14297,10 +14310,10 @@
         <v>26</v>
       </c>
       <c r="G114" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I114" s="32" t="s">
         <v>85</v>
@@ -14330,7 +14343,7 @@
       </c>
       <c r="S114" s="33"/>
       <c r="T114" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="U114" s="32"/>
     </row>
@@ -14339,13 +14352,13 @@
         <v>117</v>
       </c>
       <c r="B115" s="32" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C115" s="6">
         <v>43496</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E115" s="32" t="s">
         <v>125</v>
@@ -14354,10 +14367,10 @@
         <v>26</v>
       </c>
       <c r="G115" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I115" s="32" t="s">
         <v>85</v>
@@ -14394,13 +14407,13 @@
         <v>118</v>
       </c>
       <c r="B116" s="32" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C116" s="6">
         <v>43496</v>
       </c>
       <c r="D116" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E116" s="32" t="s">
         <v>125</v>
@@ -14409,7 +14422,7 @@
         <v>26</v>
       </c>
       <c r="G116" s="32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I116" s="32"/>
       <c r="J116" s="32"/>
@@ -14440,13 +14453,13 @@
         <v>119</v>
       </c>
       <c r="B117" s="91" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C117" s="37">
         <v>43497</v>
       </c>
       <c r="D117" s="28" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E117" s="28" t="s">
         <v>125</v>
@@ -14455,10 +14468,10 @@
         <v>26</v>
       </c>
       <c r="G117" s="28" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I117" s="28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J117" s="28"/>
       <c r="L117" s="28">
@@ -14488,13 +14501,13 @@
         <v>120</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C118" s="6">
         <v>43517</v>
       </c>
       <c r="D118" s="32" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E118" s="32" t="s">
         <v>80</v>
@@ -14503,11 +14516,11 @@
         <v>26</v>
       </c>
       <c r="G118" s="32" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H118" s="14"/>
       <c r="I118" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J118" s="32"/>
       <c r="K118" s="32"/>
@@ -14527,11 +14540,11 @@
       <c r="Q118" s="5"/>
       <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T118" s="5"/>
       <c r="U118" s="32" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14539,13 +14552,13 @@
         <v>121</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C119" s="6">
         <v>43517</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E119" s="32" t="s">
         <v>15</v>
@@ -14554,11 +14567,11 @@
         <v>26</v>
       </c>
       <c r="G119" s="32" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H119" s="14"/>
       <c r="I119" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J119" s="32"/>
       <c r="K119" s="32"/>
@@ -14587,7 +14600,7 @@
         <v>122</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C120" s="6">
         <v>43517</v>
@@ -14600,11 +14613,11 @@
         <v>26</v>
       </c>
       <c r="G120" s="32" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H120" s="14"/>
       <c r="I120" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J120" s="32"/>
       <c r="K120" s="32"/>
@@ -14632,13 +14645,13 @@
         <v>123</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C121" s="6">
         <v>43525</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E121" s="32" t="s">
         <v>32</v>
@@ -14647,11 +14660,11 @@
         <v>26</v>
       </c>
       <c r="G121" s="32" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H121" s="14"/>
       <c r="I121" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J121" s="32"/>
       <c r="K121" s="32"/>
@@ -14679,13 +14692,13 @@
         <v>124</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C122" s="6">
         <v>43525</v>
       </c>
       <c r="D122" s="32" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E122" s="32" t="s">
         <v>32</v>
@@ -14694,11 +14707,11 @@
         <v>26</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H122" s="14"/>
       <c r="I122" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J122" s="32"/>
       <c r="K122" s="32"/>
@@ -14726,13 +14739,13 @@
         <v>125</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C123" s="6">
         <v>43528</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E123" s="32" t="s">
         <v>15</v>
@@ -14741,11 +14754,11 @@
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J123" s="32"/>
       <c r="K123" s="32"/>
@@ -14777,7 +14790,7 @@
         <v>43528</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>39</v>
@@ -14786,11 +14799,11 @@
         <v>26</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H124" s="14"/>
       <c r="I124" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J124" s="32"/>
       <c r="K124" s="32"/>
@@ -14818,13 +14831,13 @@
         <v>127</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C125" s="6">
         <v>43529</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E125" s="32" t="s">
         <v>80</v>
@@ -14833,10 +14846,10 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I125" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J125" s="32"/>
       <c r="K125" s="32"/>
@@ -14855,7 +14868,7 @@
       <c r="Q125" s="5"/>
       <c r="R125" s="5"/>
       <c r="S125" s="33" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
@@ -14865,13 +14878,13 @@
         <v>128</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C126" s="6">
         <v>43531</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E126" s="32" t="s">
         <v>15</v>
@@ -14880,10 +14893,10 @@
         <v>26</v>
       </c>
       <c r="G126" s="32" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I126" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J126" s="32"/>
       <c r="K126" s="32"/>
@@ -14907,13 +14920,13 @@
         <v>129</v>
       </c>
       <c r="B127" s="90" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C127" s="6">
         <v>43550</v>
       </c>
       <c r="D127" s="32" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E127" s="32" t="s">
         <v>80</v>
@@ -14922,10 +14935,10 @@
         <v>26</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I127" s="28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J127" s="32"/>
       <c r="K127" s="32"/>
@@ -14944,11 +14957,11 @@
       <c r="Q127" s="5"/>
       <c r="R127" s="5"/>
       <c r="S127" s="33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T127" s="5"/>
       <c r="U127" s="32" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="128" spans="1:21" ht="28" hidden="1" x14ac:dyDescent="0.35">
@@ -14956,13 +14969,13 @@
         <v>130</v>
       </c>
       <c r="B128" s="99" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C128" s="37">
         <v>43550</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E128" s="28" t="s">
         <v>80</v>
@@ -14971,10 +14984,10 @@
         <v>26</v>
       </c>
       <c r="G128" s="28" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="I128" s="28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J128" s="100"/>
       <c r="K128" s="28"/>
@@ -14994,11 +15007,11 @@
       <c r="Q128" s="39"/>
       <c r="R128" s="89"/>
       <c r="S128" s="15" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T128" s="28"/>
       <c r="U128" s="3" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="129" spans="1:21" ht="42" hidden="1" x14ac:dyDescent="0.35">
@@ -15006,13 +15019,13 @@
         <v>131</v>
       </c>
       <c r="B129" s="90" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C129" s="6">
         <v>43550</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>80</v>
@@ -15021,10 +15034,10 @@
         <v>26</v>
       </c>
       <c r="G129" s="32" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I129" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J129" s="32"/>
       <c r="K129" s="32"/>
@@ -15044,7 +15057,7 @@
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
@@ -15054,13 +15067,13 @@
         <v>132</v>
       </c>
       <c r="B130" s="90" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C130" s="6">
         <v>43550</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>80</v>
@@ -15069,10 +15082,10 @@
         <v>26</v>
       </c>
       <c r="G130" s="32" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I130" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J130" s="32"/>
       <c r="K130" s="32"/>
@@ -15092,7 +15105,7 @@
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
@@ -15102,13 +15115,13 @@
         <v>133</v>
       </c>
       <c r="B131" s="90" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C131" s="6">
         <v>43550</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>80</v>
@@ -15117,10 +15130,10 @@
         <v>26</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I131" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J131" s="32"/>
       <c r="K131" s="32"/>
@@ -15140,7 +15153,7 @@
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
@@ -15150,13 +15163,13 @@
         <v>134</v>
       </c>
       <c r="B132" s="90" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C132" s="6">
         <v>43550</v>
       </c>
       <c r="D132" s="32" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E132" s="32" t="s">
         <v>80</v>
@@ -15165,10 +15178,10 @@
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I132" s="32" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J132" s="32"/>
       <c r="K132" s="32"/>
@@ -15188,7 +15201,7 @@
       <c r="Q132" s="5"/>
       <c r="R132" s="33"/>
       <c r="S132" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T132" s="32"/>
       <c r="U132" s="32"/>
@@ -15198,22 +15211,22 @@
         <v>135</v>
       </c>
       <c r="B133" s="90" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C133" s="6">
         <v>43552</v>
       </c>
       <c r="D133" s="92" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F133" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H133" s="95"/>
       <c r="I133" s="32"/>
@@ -15235,7 +15248,7 @@
       <c r="Q133" s="14"/>
       <c r="R133" s="32"/>
       <c r="S133" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="T133" s="32"/>
       <c r="U133" s="33"/>
@@ -15249,7 +15262,7 @@
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15258,7 +15271,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H134" s="95"/>
       <c r="I134" s="32"/>
@@ -15279,7 +15292,7 @@
       <c r="P134" s="97"/>
       <c r="Q134" s="33"/>
       <c r="R134" s="5" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S134" s="32"/>
       <c r="T134" s="33"/>
@@ -15294,7 +15307,7 @@
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15303,7 +15316,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H135" s="95"/>
       <c r="I135" s="32"/>
@@ -15324,7 +15337,7 @@
       <c r="P135" s="97"/>
       <c r="Q135" s="32"/>
       <c r="R135" s="5" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S135" s="33"/>
       <c r="T135" s="33"/>
@@ -15339,7 +15352,7 @@
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -15348,7 +15361,7 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H136" s="95"/>
       <c r="I136" s="32"/>
@@ -15369,7 +15382,7 @@
       <c r="P136" s="10"/>
       <c r="Q136" s="33"/>
       <c r="R136" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S136" s="33"/>
       <c r="T136" s="33"/>
@@ -15384,7 +15397,7 @@
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -15393,7 +15406,7 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H137" s="95"/>
       <c r="I137" s="32"/>
@@ -15414,7 +15427,7 @@
       <c r="P137" s="10"/>
       <c r="Q137" s="33"/>
       <c r="R137" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S137" s="33"/>
       <c r="T137" s="33"/>
@@ -15429,7 +15442,7 @@
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -15438,7 +15451,7 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H138" s="95"/>
       <c r="I138" s="32"/>
@@ -15459,7 +15472,7 @@
       <c r="P138" s="10"/>
       <c r="Q138" s="33"/>
       <c r="R138" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
@@ -15474,7 +15487,7 @@
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -15483,7 +15496,7 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H139" s="95"/>
       <c r="I139" s="21"/>
@@ -15504,7 +15517,7 @@
       <c r="P139" s="10"/>
       <c r="Q139" s="33"/>
       <c r="R139" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S139" s="33"/>
       <c r="T139" s="33"/>
@@ -15519,7 +15532,7 @@
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -15528,7 +15541,7 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H140" s="96"/>
       <c r="I140" s="5"/>
@@ -15549,7 +15562,7 @@
       <c r="P140" s="10"/>
       <c r="Q140" s="33"/>
       <c r="R140" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S140" s="33"/>
       <c r="T140" s="33"/>
@@ -15564,7 +15577,7 @@
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -15573,7 +15586,7 @@
         <v>26</v>
       </c>
       <c r="G141" s="32" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H141" s="97"/>
       <c r="I141" s="33"/>
@@ -15594,7 +15607,7 @@
       <c r="P141" s="10"/>
       <c r="Q141" s="33"/>
       <c r="R141" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S141" s="33"/>
       <c r="T141" s="33"/>
@@ -15609,7 +15622,7 @@
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -15618,7 +15631,7 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H142" s="33"/>
       <c r="I142" s="32"/>
@@ -15639,7 +15652,7 @@
       <c r="P142" s="94"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S142" s="33"/>
       <c r="T142" s="33"/>
@@ -15654,7 +15667,7 @@
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -15663,7 +15676,7 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H143" s="32"/>
       <c r="I143" s="33"/>
@@ -15684,7 +15697,7 @@
       <c r="P143" s="94"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S143" s="33"/>
       <c r="T143" s="33"/>
@@ -15699,7 +15712,7 @@
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>39</v>
@@ -15708,7 +15721,7 @@
         <v>26</v>
       </c>
       <c r="G144" s="32" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="H144" s="33"/>
       <c r="I144" s="14"/>
@@ -15729,7 +15742,7 @@
       <c r="P144" s="10"/>
       <c r="Q144" s="33"/>
       <c r="R144" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S144" s="33"/>
       <c r="T144" s="33"/>
@@ -15744,7 +15757,7 @@
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>212</v>
@@ -15753,7 +15766,7 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
@@ -15774,7 +15787,7 @@
       <c r="P145" s="10"/>
       <c r="Q145" s="33"/>
       <c r="R145" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S145" s="33"/>
       <c r="T145" s="33"/>
@@ -15789,7 +15802,7 @@
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>212</v>
@@ -15798,7 +15811,7 @@
         <v>26</v>
       </c>
       <c r="G146" s="32" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H146" s="14"/>
       <c r="I146" s="32"/>
@@ -15819,7 +15832,7 @@
       <c r="P146" s="10"/>
       <c r="Q146" s="33"/>
       <c r="R146" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S146" s="33"/>
       <c r="T146" s="33"/>
@@ -15834,7 +15847,7 @@
         <v>43552</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E147" s="32" t="s">
         <v>39</v>
@@ -15843,7 +15856,7 @@
         <v>26</v>
       </c>
       <c r="G147" s="32" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H147" s="32"/>
       <c r="I147" s="32"/>
@@ -15864,7 +15877,7 @@
       <c r="P147" s="10"/>
       <c r="Q147" s="33"/>
       <c r="R147" s="33" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S147" s="33"/>
       <c r="T147" s="33"/>
@@ -15879,7 +15892,7 @@
         <v>43552</v>
       </c>
       <c r="D148" s="28" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E148" s="28" t="s">
         <v>39</v>
@@ -15888,7 +15901,7 @@
         <v>26</v>
       </c>
       <c r="G148" s="28" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H148" s="32"/>
       <c r="I148" s="38"/>
@@ -15909,7 +15922,7 @@
       <c r="P148" s="10"/>
       <c r="Q148" s="89"/>
       <c r="R148" s="89" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S148" s="89"/>
       <c r="T148" s="89"/>
@@ -15921,13 +15934,13 @@
         <v>129</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C149" s="6">
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -15936,7 +15949,7 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="I149" s="32"/>
       <c r="J149" s="32"/>
@@ -15965,13 +15978,13 @@
         <v>130</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C150" s="6">
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -15980,7 +15993,7 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="I150" s="32"/>
       <c r="J150" s="32"/>
@@ -16009,13 +16022,13 @@
         <v>131</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C151" s="6">
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16024,7 +16037,7 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="I151" s="32"/>
       <c r="J151" s="32"/>
@@ -16049,13 +16062,13 @@
         <v>132</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C152" s="6">
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16064,7 +16077,7 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I152" s="32"/>
       <c r="J152" s="32"/>
@@ -16087,13 +16100,13 @@
         <v>133</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C153" s="6">
         <v>43553</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E153" s="32" t="s">
         <v>15</v>
@@ -16102,7 +16115,7 @@
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I153" s="32"/>
       <c r="J153" s="32"/>
@@ -16130,22 +16143,22 @@
         <v>151</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C154" s="6">
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E154" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F154" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G154" s="32" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H154" s="21"/>
       <c r="I154" s="21"/>
@@ -16175,22 +16188,22 @@
         <v>152</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C155" s="6">
         <v>43550</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E155" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F155" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G155" s="32" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H155" s="21"/>
       <c r="I155" s="32"/>
@@ -16220,22 +16233,22 @@
         <v>153</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C156" s="6">
         <v>43550</v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E156" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F156" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G156" s="32" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H156" s="32"/>
       <c r="I156" s="32"/>
@@ -16265,22 +16278,22 @@
         <v>154</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C157" s="6">
         <v>43556</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E157" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F157" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="H157" s="32"/>
       <c r="I157" s="32"/>
@@ -16310,22 +16323,22 @@
         <v>155</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C158" s="6">
         <v>43552</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F158" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H158" s="32"/>
       <c r="I158" s="32"/>
@@ -16355,13 +16368,13 @@
         <v>134</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C159" s="6">
         <v>43546</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E159" s="32" t="s">
         <v>15</v>
@@ -16370,24 +16383,22 @@
         <v>26</v>
       </c>
       <c r="G159" s="32" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="H159" s="32"/>
       <c r="I159" s="32"/>
       <c r="J159" s="32"/>
-      <c r="K159" s="32">
+      <c r="L159" s="32">
         <v>1</v>
       </c>
-      <c r="L159" s="32"/>
       <c r="M159" s="32"/>
       <c r="N159" s="32"/>
-      <c r="O159" s="5">
-        <v>6</v>
-      </c>
       <c r="P159" s="5">
         <v>4</v>
       </c>
-      <c r="Q159" s="33"/>
+      <c r="Q159" s="5">
+        <v>6</v>
+      </c>
       <c r="R159" s="5">
         <v>10</v>
       </c>
@@ -16395,18 +16406,18 @@
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>135</v>
       </c>
       <c r="B160" s="31" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C160" s="6">
         <v>43528</v>
       </c>
       <c r="D160" s="32" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E160" s="32" t="s">
         <v>15</v>
@@ -16415,24 +16426,22 @@
         <v>26</v>
       </c>
       <c r="G160" s="32" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H160" s="32"/>
       <c r="I160" s="32"/>
       <c r="J160" s="32"/>
-      <c r="K160" s="32">
+      <c r="L160" s="32">
         <v>1</v>
       </c>
-      <c r="L160" s="32"/>
       <c r="M160" s="32"/>
       <c r="N160" s="32"/>
-      <c r="O160" s="5">
-        <v>6</v>
-      </c>
       <c r="P160" s="5">
         <v>4</v>
       </c>
-      <c r="Q160" s="33"/>
+      <c r="Q160" s="5">
+        <v>6</v>
+      </c>
       <c r="R160" s="5">
         <v>9</v>
       </c>
@@ -16440,25 +16449,47 @@
       <c r="T160" s="5"/>
       <c r="U160" s="32"/>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A161" s="5"/>
-      <c r="B161" s="31"/>
-      <c r="C161" s="5"/>
-      <c r="D161" s="32"/>
-      <c r="E161" s="32"/>
-      <c r="F161" s="32"/>
-      <c r="G161" s="32"/>
+    <row r="161" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A161" s="5">
+        <v>136</v>
+      </c>
+      <c r="B161" s="31" t="s">
+        <v>560</v>
+      </c>
+      <c r="C161" s="6">
+        <v>43481</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E161" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F161" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G161" s="32" t="s">
+        <v>561</v>
+      </c>
       <c r="I161" s="32"/>
       <c r="J161" s="32"/>
       <c r="K161" s="32"/>
-      <c r="L161" s="32"/>
+      <c r="L161" s="32">
+        <v>1</v>
+      </c>
       <c r="M161" s="32"/>
       <c r="N161" s="32"/>
       <c r="O161" s="32"/>
-      <c r="Q161" s="5"/>
-      <c r="R161" s="5"/>
+      <c r="Q161" s="5">
+        <v>12</v>
+      </c>
+      <c r="R161" s="5">
+        <v>8</v>
+      </c>
       <c r="S161" s="33"/>
-      <c r="T161" s="5"/>
+      <c r="T161" s="5">
+        <v>8</v>
+      </c>
       <c r="U161" s="32"/>
     </row>
   </sheetData>
@@ -16716,38 +16747,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16919,31 +16918,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16959,4 +16966,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lost UIN--added right JIRA id
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{69DDAA42-52DC-4475-86AD-4540993F9F1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,9 +20,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$171</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="589">
   <si>
     <t>S.No.</t>
   </si>
@@ -4736,9 +4735,6 @@
     </r>
   </si>
   <si>
-    <t>MOS-17830</t>
-  </si>
-  <si>
     <t>Sprint FIT-3 Demo feedback from Ramesh</t>
   </si>
   <si>
@@ -5554,7 +5550,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -6236,6 +6232,7 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6251,7 +6248,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6282,7 +6278,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6299,7 +6295,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:U70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7460,7 +7456,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7808,67 +7804,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R123" sqref="R123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="60" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="20.42578125" style="10"/>
+    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+    <row r="1" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="109"/>
-      <c r="R1" s="109"/>
-      <c r="S1" s="109"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="110"/>
-    </row>
-    <row r="2" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="109"/>
+      <c r="U1" s="111"/>
+    </row>
+    <row r="2" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7933,7 +7929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7995,7 +7991,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -8056,7 +8052,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8118,7 +8114,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -8180,7 +8176,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8242,7 +8238,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8304,7 +8300,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8364,7 +8360,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -8424,7 +8420,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8478,7 +8474,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:21" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8535,7 +8531,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="1" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8586,7 +8582,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
     </row>
-    <row r="14" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8646,7 +8642,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -8708,7 +8704,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8770,7 +8766,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8832,7 +8828,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8892,7 +8888,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8954,7 +8950,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9002,7 +8998,7 @@
       <c r="T20" s="30"/>
       <c r="U20" s="21"/>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9050,7 +9046,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9110,12 +9106,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C23" s="6">
         <v>43402</v>
@@ -9170,7 +9166,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9232,7 +9228,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9282,7 +9278,7 @@
       <c r="T25" s="30"/>
       <c r="U25" s="21"/>
     </row>
-    <row r="26" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9332,12 +9328,12 @@
       <c r="T26" s="30"/>
       <c r="U26" s="21"/>
     </row>
-    <row r="27" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="82" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C27" s="6">
         <v>43402</v>
@@ -9392,12 +9388,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="82" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C28" s="6">
         <v>43418</v>
@@ -9454,7 +9450,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9504,7 +9500,7 @@
       <c r="T29" s="30"/>
       <c r="U29" s="21"/>
     </row>
-    <row r="30" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9560,7 +9556,7 @@
       <c r="T30" s="30"/>
       <c r="U30" s="14"/>
     </row>
-    <row r="31" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9622,7 +9618,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9677,14 +9673,14 @@
         <v>269</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="32" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9742,7 +9738,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9804,12 +9800,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" s="82" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C35" s="6">
         <v>43430</v>
@@ -9861,7 +9857,7 @@
       <c r="T35" s="30"/>
       <c r="U35" s="14"/>
     </row>
-    <row r="36" spans="1:21" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9925,7 +9921,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -9989,7 +9985,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10053,7 +10049,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10117,7 +10113,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -10171,12 +10167,12 @@
       <c r="T40" s="30"/>
       <c r="U40" s="32"/>
     </row>
-    <row r="41" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C41" s="6">
         <v>43430</v>
@@ -10229,7 +10225,7 @@
       <c r="T41" s="30"/>
       <c r="U41" s="32"/>
     </row>
-    <row r="42" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10283,12 +10279,12 @@
       <c r="T42" s="30"/>
       <c r="U42" s="32"/>
     </row>
-    <row r="43" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="86" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C43" s="6">
         <v>43427</v>
@@ -10341,7 +10337,7 @@
       <c r="T43" s="30"/>
       <c r="U43" s="32"/>
     </row>
-    <row r="44" spans="1:21" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10401,7 +10397,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10459,7 +10455,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10521,7 +10517,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10583,7 +10579,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10633,7 +10629,7 @@
       <c r="T48" s="30"/>
       <c r="U48" s="32"/>
     </row>
-    <row r="49" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10695,7 +10691,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10758,7 +10754,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10812,7 +10808,7 @@
       <c r="T51" s="30"/>
       <c r="U51" s="32"/>
     </row>
-    <row r="52" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10862,7 +10858,7 @@
       <c r="T52" s="30"/>
       <c r="U52" s="32"/>
     </row>
-    <row r="53" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10922,7 +10918,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10972,7 +10968,7 @@
       <c r="T54" s="30"/>
       <c r="U54" s="32"/>
     </row>
-    <row r="55" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -11026,12 +11022,12 @@
       <c r="T55" s="30"/>
       <c r="U55" s="32"/>
     </row>
-    <row r="56" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
       <c r="B56" s="82" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C56" s="6">
         <v>43427</v>
@@ -11085,12 +11081,12 @@
         <v>452</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
       <c r="B57" s="82" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C57" s="6">
         <v>43427</v>
@@ -11144,12 +11140,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
       <c r="B58" s="83" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C58" s="6">
         <v>43427</v>
@@ -11204,7 +11200,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11258,7 +11254,7 @@
       <c r="T59" s="30"/>
       <c r="U59" s="32"/>
     </row>
-    <row r="60" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11312,12 +11308,12 @@
       <c r="T60" s="30"/>
       <c r="U60" s="32"/>
     </row>
-    <row r="61" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C61" s="6">
         <v>43432</v>
@@ -11360,7 +11356,7 @@
         <v>4</v>
       </c>
       <c r="Q61" s="80" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R61" s="30" t="s">
         <v>269</v>
@@ -11369,7 +11365,7 @@
       <c r="T61" s="30"/>
       <c r="U61" s="32"/>
     </row>
-    <row r="62" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -11432,7 +11428,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -11493,7 +11489,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11544,7 +11540,7 @@
       <c r="T64" s="33"/>
       <c r="U64" s="32"/>
     </row>
-    <row r="65" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11595,7 +11591,7 @@
       <c r="T65" s="33"/>
       <c r="U65" s="32"/>
     </row>
-    <row r="66" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -11658,7 +11654,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11718,7 +11714,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11772,19 +11768,19 @@
         <v>269</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T68" s="5"/>
       <c r="U68" s="32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
       <c r="B69" s="82" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C69" s="6">
         <v>43446</v>
@@ -11839,12 +11835,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
       <c r="B70" s="82" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C70" s="6">
         <v>43446</v>
@@ -11897,12 +11893,12 @@
       <c r="T70" s="5"/>
       <c r="U70" s="32"/>
     </row>
-    <row r="71" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
       <c r="B71" s="82" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C71" s="6">
         <v>43451</v>
@@ -11957,7 +11953,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -12011,7 +12007,7 @@
         <v>269</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T72" s="5"/>
       <c r="U72" s="32" t="s">
@@ -12020,7 +12016,7 @@
       <c r="V72" s="5"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -12080,7 +12076,7 @@
       <c r="V73" s="39"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12135,7 +12131,7 @@
       <c r="V74" s="5"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -12196,7 +12192,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -12257,12 +12253,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
       <c r="B77" s="86" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C77" s="6">
         <v>43465</v>
@@ -12317,7 +12313,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -12379,12 +12375,12 @@
       <c r="V78" s="5"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>76</v>
       </c>
       <c r="B79" s="83" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C79" s="6">
         <v>43465</v>
@@ -12439,7 +12435,7 @@
       <c r="V79" s="5"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -12501,12 +12497,12 @@
       <c r="V80" s="5"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>78</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C81" s="6">
         <v>43465</v>
@@ -12561,12 +12557,12 @@
       <c r="V81" s="73"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>79</v>
       </c>
       <c r="B82" s="83" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C82" s="6">
         <v>43465</v>
@@ -12623,7 +12619,7 @@
       <c r="V82" s="73"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -12682,7 +12678,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12744,7 +12740,7 @@
       <c r="V84" s="73"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12806,7 +12802,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12866,7 +12862,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="32"/>
     </row>
-    <row r="87" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -12925,7 +12921,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -12986,7 +12982,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -13041,7 +13037,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -13090,7 +13086,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="32"/>
     </row>
-    <row r="91" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -13137,12 +13133,12 @@
       <c r="T91" s="5"/>
       <c r="U91" s="32"/>
     </row>
-    <row r="92" spans="1:23" ht="171" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>89</v>
       </c>
       <c r="B92" s="83" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C92" s="6">
         <v>43486</v>
@@ -13197,12 +13193,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>90</v>
       </c>
       <c r="B93" s="82" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C93" s="6">
         <v>43489</v>
@@ -13255,7 +13251,7 @@
       <c r="T93" s="5"/>
       <c r="U93" s="32"/>
     </row>
-    <row r="94" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -13315,7 +13311,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -13375,7 +13371,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -13435,7 +13431,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -13493,7 +13489,7 @@
       <c r="T97" s="5"/>
       <c r="U97" s="32"/>
     </row>
-    <row r="98" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -13539,17 +13535,17 @@
       <c r="Q98" s="81"/>
       <c r="R98" s="5"/>
       <c r="S98" s="33" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
     </row>
-    <row r="99" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>96</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C99" s="6">
         <v>43489</v>
@@ -13602,7 +13598,7 @@
       <c r="T99" s="5"/>
       <c r="U99" s="32"/>
     </row>
-    <row r="100" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -13662,7 +13658,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13722,7 +13718,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13780,7 +13776,7 @@
       <c r="T102" s="5"/>
       <c r="U102" s="32"/>
     </row>
-    <row r="103" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13840,7 +13836,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -13900,7 +13896,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -13959,7 +13955,7 @@
       </c>
       <c r="U105" s="33"/>
     </row>
-    <row r="106" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -14018,7 +14014,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -14064,12 +14060,12 @@
       <c r="Q107" s="5"/>
       <c r="R107" s="5"/>
       <c r="S107" s="33" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
     </row>
-    <row r="108" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -14128,7 +14124,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -14183,7 +14179,7 @@
       </c>
       <c r="U109" s="32"/>
     </row>
-    <row r="110" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -14238,7 +14234,7 @@
       <c r="T110" s="5"/>
       <c r="U110" s="32"/>
     </row>
-    <row r="111" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -14295,7 +14291,7 @@
       </c>
       <c r="U111" s="32"/>
     </row>
-    <row r="112" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -14352,7 +14348,7 @@
       </c>
       <c r="U112" s="32"/>
     </row>
-    <row r="113" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -14409,7 +14405,7 @@
       </c>
       <c r="U113" s="32"/>
     </row>
-    <row r="114" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -14466,7 +14462,7 @@
       </c>
       <c r="U114" s="32"/>
     </row>
-    <row r="115" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -14521,7 +14517,7 @@
       </c>
       <c r="U115" s="32"/>
     </row>
-    <row r="116" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -14567,7 +14563,7 @@
       </c>
       <c r="U116" s="32"/>
     </row>
-    <row r="117" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -14615,12 +14611,12 @@
       </c>
       <c r="U117" s="28"/>
     </row>
-    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C118" s="6">
         <v>43517</v>
@@ -14659,14 +14655,14 @@
       <c r="Q118" s="5"/>
       <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T118" s="5"/>
       <c r="U118" s="32" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -14713,7 +14709,7 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <f>1+A119</f>
         <v>122</v>
@@ -14759,12 +14755,12 @@
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>123</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C121" s="6">
         <v>43525</v>
@@ -14806,12 +14802,12 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>124</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C122" s="6">
         <v>43525</v>
@@ -14853,12 +14849,12 @@
       <c r="T122" s="5"/>
       <c r="U122" s="32"/>
     </row>
-    <row r="123" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>125</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="C123" s="6">
         <v>43528</v>
@@ -14894,13 +14890,19 @@
         <v>43528</v>
       </c>
       <c r="P123" s="31"/>
-      <c r="Q123" s="5"/>
-      <c r="R123" s="5"/>
+      <c r="Q123" s="5">
+        <v>30</v>
+      </c>
+      <c r="R123" s="5">
+        <v>20</v>
+      </c>
       <c r="S123" s="33"/>
-      <c r="T123" s="5"/>
+      <c r="T123" s="5">
+        <v>10</v>
+      </c>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>126</v>
       </c>
@@ -14945,12 +14947,12 @@
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>127</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C125" s="6">
         <v>43529</v>
@@ -14965,7 +14967,7 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I125" s="32" t="s">
         <v>428</v>
@@ -14987,23 +14989,23 @@
       <c r="Q125" s="5"/>
       <c r="R125" s="5"/>
       <c r="S125" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T125" s="5"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>128</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C126" s="6">
         <v>43531</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E126" s="32" t="s">
         <v>15</v>
@@ -15012,7 +15014,7 @@
         <v>26</v>
       </c>
       <c r="G126" s="32" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I126" s="32" t="s">
         <v>428</v>
@@ -15036,18 +15038,18 @@
       <c r="S126" s="33"/>
       <c r="U126" s="32"/>
     </row>
-    <row r="127" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>129</v>
       </c>
       <c r="B127" s="89" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C127" s="6">
         <v>43550</v>
       </c>
       <c r="D127" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E127" s="32" t="s">
         <v>80</v>
@@ -15056,7 +15058,7 @@
         <v>26</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I127" s="28" t="s">
         <v>428</v>
@@ -15078,25 +15080,25 @@
       <c r="Q127" s="5"/>
       <c r="R127" s="5"/>
       <c r="S127" s="33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T127" s="5"/>
       <c r="U127" s="32" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>130</v>
       </c>
       <c r="B128" s="98" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C128" s="37">
         <v>43550</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E128" s="28" t="s">
         <v>80</v>
@@ -15105,7 +15107,7 @@
         <v>26</v>
       </c>
       <c r="G128" s="28" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I128" s="28" t="s">
         <v>428</v>
@@ -15128,25 +15130,25 @@
       <c r="Q128" s="39"/>
       <c r="R128" s="88"/>
       <c r="S128" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T128" s="28"/>
       <c r="U128" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="129" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A129" s="92">
         <v>131</v>
       </c>
       <c r="B129" s="89" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C129" s="6">
         <v>43550</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>80</v>
@@ -15155,7 +15157,7 @@
         <v>26</v>
       </c>
       <c r="G129" s="32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I129" s="32" t="s">
         <v>428</v>
@@ -15178,23 +15180,23 @@
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
     </row>
-    <row r="130" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="92">
         <v>132</v>
       </c>
       <c r="B130" s="89" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C130" s="6">
         <v>43550</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>80</v>
@@ -15203,7 +15205,7 @@
         <v>26</v>
       </c>
       <c r="G130" s="32" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I130" s="32" t="s">
         <v>428</v>
@@ -15226,23 +15228,23 @@
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
     </row>
-    <row r="131" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="92">
         <v>133</v>
       </c>
       <c r="B131" s="89" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C131" s="6">
         <v>43550</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>80</v>
@@ -15251,7 +15253,7 @@
         <v>26</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I131" s="32" t="s">
         <v>428</v>
@@ -15274,23 +15276,23 @@
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
     </row>
-    <row r="132" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A132" s="92">
         <v>134</v>
       </c>
       <c r="B132" s="89" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C132" s="6">
         <v>43550</v>
       </c>
       <c r="D132" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E132" s="32" t="s">
         <v>80</v>
@@ -15299,7 +15301,7 @@
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I132" s="32" t="s">
         <v>428</v>
@@ -15322,23 +15324,23 @@
       <c r="Q132" s="5"/>
       <c r="R132" s="33"/>
       <c r="S132" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T132" s="32"/>
       <c r="U132" s="32"/>
     </row>
-    <row r="133" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A133" s="92">
         <v>135</v>
       </c>
       <c r="B133" s="89" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C133" s="6">
         <v>43552</v>
       </c>
       <c r="D133" s="91" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E133" s="32" t="s">
         <v>32</v>
@@ -15347,7 +15349,7 @@
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H133" s="94"/>
       <c r="I133" s="32"/>
@@ -15369,12 +15371,12 @@
       <c r="Q133" s="14"/>
       <c r="R133" s="32"/>
       <c r="S133" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T133" s="32"/>
       <c r="U133" s="33"/>
     </row>
-    <row r="134" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A134" s="92">
         <v>136</v>
       </c>
@@ -15383,7 +15385,7 @@
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15392,7 +15394,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H134" s="94"/>
       <c r="I134" s="32"/>
@@ -15413,13 +15415,13 @@
       <c r="P134" s="96"/>
       <c r="Q134" s="33"/>
       <c r="R134" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S134" s="32"/>
       <c r="T134" s="33"/>
       <c r="U134" s="33"/>
     </row>
-    <row r="135" spans="1:21" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="266" x14ac:dyDescent="0.35">
       <c r="A135" s="92">
         <v>137</v>
       </c>
@@ -15428,7 +15430,7 @@
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15437,7 +15439,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H135" s="94"/>
       <c r="I135" s="32"/>
@@ -15458,13 +15460,13 @@
       <c r="P135" s="96"/>
       <c r="Q135" s="32"/>
       <c r="R135" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S135" s="33"/>
       <c r="T135" s="33"/>
       <c r="U135" s="33"/>
     </row>
-    <row r="136" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A136" s="92">
         <v>138</v>
       </c>
@@ -15473,7 +15475,7 @@
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -15482,7 +15484,7 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H136" s="94"/>
       <c r="I136" s="32"/>
@@ -15503,13 +15505,13 @@
       <c r="P136" s="10"/>
       <c r="Q136" s="33"/>
       <c r="R136" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S136" s="33"/>
       <c r="T136" s="33"/>
       <c r="U136" s="33"/>
     </row>
-    <row r="137" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A137" s="92">
         <v>139</v>
       </c>
@@ -15518,7 +15520,7 @@
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -15527,7 +15529,7 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H137" s="94"/>
       <c r="I137" s="32"/>
@@ -15548,13 +15550,13 @@
       <c r="P137" s="10"/>
       <c r="Q137" s="33"/>
       <c r="R137" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S137" s="33"/>
       <c r="T137" s="33"/>
       <c r="U137" s="33"/>
     </row>
-    <row r="138" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A138" s="92">
         <v>140</v>
       </c>
@@ -15563,7 +15565,7 @@
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -15572,7 +15574,7 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H138" s="94"/>
       <c r="I138" s="32"/>
@@ -15593,13 +15595,13 @@
       <c r="P138" s="10"/>
       <c r="Q138" s="33"/>
       <c r="R138" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
       <c r="U138" s="33"/>
     </row>
-    <row r="139" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A139" s="92">
         <v>141</v>
       </c>
@@ -15608,7 +15610,7 @@
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -15617,7 +15619,7 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H139" s="94"/>
       <c r="I139" s="21"/>
@@ -15638,13 +15640,13 @@
       <c r="P139" s="10"/>
       <c r="Q139" s="33"/>
       <c r="R139" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S139" s="33"/>
       <c r="T139" s="33"/>
       <c r="U139" s="33"/>
     </row>
-    <row r="140" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A140" s="92">
         <v>142</v>
       </c>
@@ -15653,7 +15655,7 @@
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -15662,7 +15664,7 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H140" s="95"/>
       <c r="I140" s="5"/>
@@ -15683,13 +15685,13 @@
       <c r="P140" s="10"/>
       <c r="Q140" s="33"/>
       <c r="R140" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S140" s="33"/>
       <c r="T140" s="33"/>
       <c r="U140" s="33"/>
     </row>
-    <row r="141" spans="1:21" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A141" s="92">
         <v>143</v>
       </c>
@@ -15698,7 +15700,7 @@
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -15707,7 +15709,7 @@
         <v>26</v>
       </c>
       <c r="G141" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H141" s="96"/>
       <c r="I141" s="33"/>
@@ -15728,13 +15730,13 @@
       <c r="P141" s="10"/>
       <c r="Q141" s="33"/>
       <c r="R141" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S141" s="33"/>
       <c r="T141" s="33"/>
       <c r="U141" s="33"/>
     </row>
-    <row r="142" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A142" s="92">
         <v>144</v>
       </c>
@@ -15743,7 +15745,7 @@
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -15752,7 +15754,7 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H142" s="33"/>
       <c r="I142" s="32"/>
@@ -15773,13 +15775,13 @@
       <c r="P142" s="93"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S142" s="33"/>
       <c r="T142" s="33"/>
       <c r="U142" s="33"/>
     </row>
-    <row r="143" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A143" s="92">
         <v>145</v>
       </c>
@@ -15788,7 +15790,7 @@
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -15797,7 +15799,7 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H143" s="32"/>
       <c r="I143" s="33"/>
@@ -15818,13 +15820,13 @@
       <c r="P143" s="93"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S143" s="33"/>
       <c r="T143" s="33"/>
       <c r="U143" s="33"/>
     </row>
-    <row r="144" spans="1:21" ht="114" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A144" s="92">
         <v>146</v>
       </c>
@@ -15833,7 +15835,7 @@
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>39</v>
@@ -15842,7 +15844,7 @@
         <v>26</v>
       </c>
       <c r="G144" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H144" s="33"/>
       <c r="I144" s="14"/>
@@ -15863,13 +15865,13 @@
       <c r="P144" s="10"/>
       <c r="Q144" s="33"/>
       <c r="R144" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S144" s="33"/>
       <c r="T144" s="33"/>
       <c r="U144" s="33"/>
     </row>
-    <row r="145" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A145" s="92">
         <v>147</v>
       </c>
@@ -15878,7 +15880,7 @@
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>212</v>
@@ -15887,7 +15889,7 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
@@ -15908,13 +15910,13 @@
       <c r="P145" s="10"/>
       <c r="Q145" s="33"/>
       <c r="R145" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S145" s="33"/>
       <c r="T145" s="33"/>
       <c r="U145" s="33"/>
     </row>
-    <row r="146" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A146" s="92">
         <v>148</v>
       </c>
@@ -15923,7 +15925,7 @@
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>212</v>
@@ -15932,7 +15934,7 @@
         <v>26</v>
       </c>
       <c r="G146" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H146" s="14"/>
       <c r="I146" s="32"/>
@@ -15953,13 +15955,13 @@
       <c r="P146" s="10"/>
       <c r="Q146" s="33"/>
       <c r="R146" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S146" s="33"/>
       <c r="T146" s="33"/>
       <c r="U146" s="33"/>
     </row>
-    <row r="147" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A147" s="92">
         <v>149</v>
       </c>
@@ -15968,7 +15970,7 @@
         <v>43552</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E147" s="32" t="s">
         <v>39</v>
@@ -15977,7 +15979,7 @@
         <v>26</v>
       </c>
       <c r="G147" s="32" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="H147" s="32"/>
       <c r="I147" s="32"/>
@@ -15998,13 +16000,13 @@
       <c r="P147" s="10"/>
       <c r="Q147" s="33"/>
       <c r="R147" s="33" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S147" s="33"/>
       <c r="T147" s="33"/>
       <c r="U147" s="33"/>
     </row>
-    <row r="148" spans="1:21" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A148" s="100">
         <v>150</v>
       </c>
@@ -16013,7 +16015,7 @@
         <v>43552</v>
       </c>
       <c r="D148" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E148" s="28" t="s">
         <v>39</v>
@@ -16022,7 +16024,7 @@
         <v>26</v>
       </c>
       <c r="G148" s="28" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H148" s="32"/>
       <c r="I148" s="38"/>
@@ -16043,25 +16045,25 @@
       <c r="P148" s="10"/>
       <c r="Q148" s="88"/>
       <c r="R148" s="88" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="S148" s="88"/>
       <c r="T148" s="88"/>
       <c r="U148" s="88"/>
     </row>
-    <row r="149" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <f>1+A126</f>
         <v>129</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C149" s="6">
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -16070,7 +16072,7 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I149" s="32"/>
       <c r="J149" s="32"/>
@@ -16082,7 +16084,7 @@
         <v>74</v>
       </c>
       <c r="N149" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O149" s="6">
         <v>43553</v>
@@ -16099,19 +16101,19 @@
       </c>
       <c r="U149" s="32"/>
     </row>
-    <row r="150" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <f t="shared" ref="A150:A153" si="8">1+A127</f>
         <v>130</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C150" s="6">
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -16120,7 +16122,7 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I150" s="32"/>
       <c r="J150" s="32"/>
@@ -16132,7 +16134,7 @@
         <v>74</v>
       </c>
       <c r="N150" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O150" s="6">
         <v>43553</v>
@@ -16149,19 +16151,19 @@
       </c>
       <c r="U150" s="32"/>
     </row>
-    <row r="151" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <f t="shared" si="8"/>
         <v>131</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C151" s="6">
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16170,7 +16172,7 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I151" s="32"/>
       <c r="J151" s="32"/>
@@ -16182,7 +16184,7 @@
         <v>74</v>
       </c>
       <c r="N151" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O151" s="6">
         <v>43553</v>
@@ -16196,19 +16198,19 @@
       <c r="S151" s="10"/>
       <c r="U151" s="32"/>
     </row>
-    <row r="152" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <f t="shared" si="8"/>
         <v>132</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C152" s="6">
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16217,7 +16219,7 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I152" s="32"/>
       <c r="J152" s="32"/>
@@ -16229,7 +16231,7 @@
         <v>74</v>
       </c>
       <c r="N152" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O152" s="6">
         <v>43553</v>
@@ -16240,19 +16242,19 @@
       <c r="T152" s="5"/>
       <c r="U152" s="32"/>
     </row>
-    <row r="153" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <f t="shared" si="8"/>
         <v>133</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C153" s="6">
         <v>43553</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E153" s="32" t="s">
         <v>15</v>
@@ -16261,7 +16263,7 @@
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I153" s="32"/>
       <c r="J153" s="32"/>
@@ -16273,7 +16275,7 @@
         <v>74</v>
       </c>
       <c r="N153" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="O153" s="6">
         <v>43553</v>
@@ -16290,18 +16292,18 @@
       </c>
       <c r="U153" s="32"/>
     </row>
-    <row r="154" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A154" s="92">
         <v>151</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C154" s="6">
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E154" s="32" t="s">
         <v>32</v>
@@ -16310,7 +16312,7 @@
         <v>26</v>
       </c>
       <c r="G154" s="32" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H154" s="21"/>
       <c r="I154" s="21"/>
@@ -16335,18 +16337,18 @@
       <c r="T154" s="5"/>
       <c r="U154" s="32"/>
     </row>
-    <row r="155" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A155" s="92">
         <v>152</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C155" s="6">
         <v>43550</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E155" s="32" t="s">
         <v>32</v>
@@ -16355,7 +16357,7 @@
         <v>26</v>
       </c>
       <c r="G155" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H155" s="21"/>
       <c r="I155" s="32"/>
@@ -16380,18 +16382,18 @@
       <c r="T155" s="5"/>
       <c r="U155" s="32"/>
     </row>
-    <row r="156" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A156" s="92">
         <v>153</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C156" s="6">
         <v>43550</v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E156" s="32" t="s">
         <v>32</v>
@@ -16400,7 +16402,7 @@
         <v>26</v>
       </c>
       <c r="G156" s="32" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H156" s="32"/>
       <c r="I156" s="32"/>
@@ -16425,18 +16427,18 @@
       <c r="T156" s="5"/>
       <c r="U156" s="32"/>
     </row>
-    <row r="157" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A157" s="92">
         <v>154</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C157" s="6">
         <v>43556</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E157" s="32" t="s">
         <v>32</v>
@@ -16445,7 +16447,7 @@
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H157" s="32"/>
       <c r="I157" s="32"/>
@@ -16470,18 +16472,18 @@
       <c r="T157" s="5"/>
       <c r="U157" s="32"/>
     </row>
-    <row r="158" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A158" s="92">
         <v>155</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C158" s="6">
         <v>43552</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E158" s="32" t="s">
         <v>32</v>
@@ -16490,7 +16492,7 @@
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H158" s="32"/>
       <c r="I158" s="32"/>
@@ -16515,18 +16517,18 @@
       <c r="T158" s="5"/>
       <c r="U158" s="32"/>
     </row>
-    <row r="159" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>134</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C159" s="6">
         <v>43546</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E159" s="32" t="s">
         <v>15</v>
@@ -16535,7 +16537,7 @@
         <v>26</v>
       </c>
       <c r="G159" s="32" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H159" s="32"/>
       <c r="I159" s="32"/>
@@ -16565,18 +16567,18 @@
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:21" ht="228" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="210" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>135</v>
       </c>
       <c r="B160" s="31" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C160" s="6">
         <v>43528</v>
       </c>
       <c r="D160" s="32" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E160" s="32" t="s">
         <v>15</v>
@@ -16585,7 +16587,7 @@
         <v>26</v>
       </c>
       <c r="G160" s="32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H160" s="32"/>
       <c r="I160" s="32"/>
@@ -16615,18 +16617,18 @@
       <c r="T160" s="5"/>
       <c r="U160" s="32"/>
     </row>
-    <row r="161" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A161" s="39">
         <v>136</v>
       </c>
       <c r="B161" s="90" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C161" s="37">
         <v>43481</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E161" s="28" t="s">
         <v>15</v>
@@ -16635,7 +16637,7 @@
         <v>26</v>
       </c>
       <c r="G161" s="28" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I161" s="28"/>
       <c r="J161" s="28"/>
@@ -16662,18 +16664,18 @@
       </c>
       <c r="U161" s="28"/>
     </row>
-    <row r="162" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>138</v>
       </c>
       <c r="B162" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C162" s="6">
         <v>43542</v>
       </c>
       <c r="D162" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E162" s="32" t="s">
         <v>80</v>
@@ -16682,7 +16684,7 @@
         <v>26</v>
       </c>
       <c r="G162" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H162" s="14"/>
       <c r="I162" s="32"/>
@@ -16706,25 +16708,25 @@
       </c>
       <c r="R162" s="5"/>
       <c r="S162" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T162" s="5">
         <v>10</v>
       </c>
       <c r="U162" s="32"/>
     </row>
-    <row r="163" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>140</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C163" s="6">
         <v>43542</v>
       </c>
       <c r="D163" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E163" s="32" t="s">
         <v>80</v>
@@ -16733,7 +16735,7 @@
         <v>26</v>
       </c>
       <c r="G163" s="32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H163" s="14"/>
       <c r="I163" s="32"/>
@@ -16757,25 +16759,25 @@
       </c>
       <c r="R163" s="5"/>
       <c r="S163" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T163" s="5">
         <v>10</v>
       </c>
       <c r="U163" s="32"/>
     </row>
-    <row r="164" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>141</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C164" s="6">
         <v>43542</v>
       </c>
       <c r="D164" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E164" s="32" t="s">
         <v>80</v>
@@ -16784,7 +16786,7 @@
         <v>26</v>
       </c>
       <c r="G164" s="32" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H164" s="14"/>
       <c r="I164" s="32"/>
@@ -16808,25 +16810,25 @@
       </c>
       <c r="R164" s="5"/>
       <c r="S164" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T164" s="5">
         <v>10</v>
       </c>
       <c r="U164" s="32"/>
     </row>
-    <row r="165" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>142</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C165" s="6">
         <v>43542</v>
       </c>
       <c r="D165" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E165" s="32" t="s">
         <v>80</v>
@@ -16835,7 +16837,7 @@
         <v>26</v>
       </c>
       <c r="G165" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H165" s="14"/>
       <c r="I165" s="32"/>
@@ -16859,25 +16861,25 @@
       </c>
       <c r="R165" s="5"/>
       <c r="S165" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T165" s="5">
         <v>10</v>
       </c>
       <c r="U165" s="32"/>
     </row>
-    <row r="166" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>143</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C166" s="6">
         <v>43542</v>
       </c>
       <c r="D166" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E166" s="32" t="s">
         <v>80</v>
@@ -16886,7 +16888,7 @@
         <v>26</v>
       </c>
       <c r="G166" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H166" s="14"/>
       <c r="I166" s="32"/>
@@ -16910,25 +16912,25 @@
       </c>
       <c r="R166" s="5"/>
       <c r="S166" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T166" s="5">
         <v>10</v>
       </c>
       <c r="U166" s="32"/>
     </row>
-    <row r="167" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>144</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C167" s="6">
         <v>43542</v>
       </c>
       <c r="D167" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E167" s="32" t="s">
         <v>80</v>
@@ -16937,7 +16939,7 @@
         <v>26</v>
       </c>
       <c r="G167" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H167" s="14"/>
       <c r="I167" s="32"/>
@@ -16961,25 +16963,25 @@
       </c>
       <c r="R167" s="5"/>
       <c r="S167" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T167" s="5">
         <v>10</v>
       </c>
       <c r="U167" s="32"/>
     </row>
-    <row r="168" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>145</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C168" s="6">
         <v>43542</v>
       </c>
       <c r="D168" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E168" s="32" t="s">
         <v>80</v>
@@ -16988,7 +16990,7 @@
         <v>26</v>
       </c>
       <c r="G168" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H168" s="14"/>
       <c r="I168" s="32"/>
@@ -17012,25 +17014,25 @@
       </c>
       <c r="R168" s="5"/>
       <c r="S168" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T168" s="5">
         <v>10</v>
       </c>
       <c r="U168" s="32"/>
     </row>
-    <row r="169" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>146</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C169" s="6">
         <v>43542</v>
       </c>
       <c r="D169" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E169" s="32" t="s">
         <v>80</v>
@@ -17039,7 +17041,7 @@
         <v>26</v>
       </c>
       <c r="G169" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H169" s="14"/>
       <c r="I169" s="32"/>
@@ -17063,25 +17065,25 @@
       </c>
       <c r="R169" s="5"/>
       <c r="S169" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T169" s="5">
         <v>10</v>
       </c>
       <c r="U169" s="32"/>
     </row>
-    <row r="170" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>148</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C170" s="6">
         <v>43542</v>
       </c>
       <c r="D170" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E170" s="32" t="s">
         <v>80</v>
@@ -17090,7 +17092,7 @@
         <v>26</v>
       </c>
       <c r="G170" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H170" s="14"/>
       <c r="I170" s="32"/>
@@ -17114,25 +17116,25 @@
       </c>
       <c r="R170" s="5"/>
       <c r="S170" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T170" s="5">
         <v>10</v>
       </c>
       <c r="U170" s="32"/>
     </row>
-    <row r="171" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>149</v>
       </c>
       <c r="B171" s="31" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C171" s="6">
         <v>43542</v>
       </c>
       <c r="D171" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E171" s="32" t="s">
         <v>80</v>
@@ -17141,7 +17143,7 @@
         <v>26</v>
       </c>
       <c r="G171" s="32" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H171" s="14"/>
       <c r="I171" s="32"/>
@@ -17165,14 +17167,14 @@
       </c>
       <c r="R171" s="5"/>
       <c r="S171" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T171" s="5">
         <v>10</v>
       </c>
       <c r="U171" s="32"/>
     </row>
-    <row r="172" spans="1:21" s="111" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" s="106" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>150</v>
       </c>
@@ -17181,7 +17183,7 @@
         <v>43552</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E172" s="14" t="s">
         <v>125</v>
@@ -17190,7 +17192,7 @@
         <v>26</v>
       </c>
       <c r="G172" s="32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H172" s="16"/>
       <c r="I172" s="14"/>
@@ -17203,7 +17205,7 @@
         <v>74</v>
       </c>
       <c r="N172" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O172" s="6">
         <v>43552</v>
@@ -17215,18 +17217,18 @@
       <c r="T172" s="5"/>
       <c r="U172" s="14"/>
     </row>
-    <row r="173" spans="1:21" s="111" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" s="106" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>151</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C173" s="6">
         <v>43552</v>
       </c>
       <c r="D173" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E173" s="14" t="s">
         <v>125</v>
@@ -17235,7 +17237,7 @@
         <v>26</v>
       </c>
       <c r="G173" s="32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H173" s="16"/>
       <c r="I173" s="14"/>
@@ -17248,7 +17250,7 @@
         <v>74</v>
       </c>
       <c r="N173" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O173" s="6">
         <v>43552</v>
@@ -17266,7 +17268,7 @@
       </c>
       <c r="U173" s="14"/>
     </row>
-    <row r="174" spans="1:21" s="111" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" s="106" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>152</v>
       </c>
@@ -17275,7 +17277,7 @@
         <v>43556</v>
       </c>
       <c r="D174" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>125</v>
@@ -17284,7 +17286,7 @@
         <v>26</v>
       </c>
       <c r="G174" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H174" s="16"/>
       <c r="I174" s="14"/>
@@ -17297,7 +17299,7 @@
         <v>74</v>
       </c>
       <c r="N174" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O174" s="6">
         <v>43556</v>
@@ -17309,7 +17311,7 @@
       <c r="T174" s="5"/>
       <c r="U174" s="14"/>
     </row>
-    <row r="175" spans="1:21" ht="57" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A175" s="2">
         <v>153</v>
       </c>
@@ -17318,7 +17320,7 @@
         <v>43556</v>
       </c>
       <c r="D175" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E175" s="14" t="s">
         <v>125</v>
@@ -17327,7 +17329,7 @@
         <v>26</v>
       </c>
       <c r="G175" s="32" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I175" s="14"/>
       <c r="J175" s="14"/>
@@ -17339,7 +17341,7 @@
         <v>74</v>
       </c>
       <c r="N175" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O175" s="6">
         <v>43556</v>
@@ -17351,20 +17353,20 @@
       <c r="U175" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U171" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:U171"/>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D133" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D133" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -17372,57 +17374,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -17432,19 +17434,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -17455,7 +17457,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -17466,7 +17468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -17477,7 +17479,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -17488,7 +17490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -17499,7 +17501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -17510,7 +17512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -17521,7 +17523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -17532,7 +17534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -17550,17 +17552,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="65" t="s">
         <v>207</v>
       </c>
@@ -17568,25 +17570,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69"/>
       <c r="C3" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="70"/>
       <c r="C4" s="68" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71"/>
       <c r="C5" s="72" t="s">
         <v>206</v>
@@ -17599,38 +17601,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17802,31 +17772,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17842,4 +17820,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Made few changes to Reg client
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -18,11 +18,11 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$U$174</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="587">
   <si>
     <t>S.No.</t>
   </si>
@@ -4273,12 +4273,6 @@
   </si>
   <si>
     <t>MOS-16544</t>
-  </si>
-  <si>
-    <t>RO’s biometrics exceptions to not be captured during User Onboarding</t>
-  </si>
-  <si>
-    <t>MOS-16545</t>
   </si>
   <si>
     <t>MOS-16040</t>
@@ -7456,7 +7450,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7806,11 +7800,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W175"/>
+  <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R123" sqref="R123"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q125" sqref="Q125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -7996,7 +7990,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C4" s="6">
         <v>43362</v>
@@ -8011,7 +8005,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>17</v>
@@ -8049,7 +8043,7 @@
       <c r="S4" s="30"/>
       <c r="T4" s="30"/>
       <c r="U4" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
@@ -8119,7 +8113,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C6" s="6">
         <v>43362</v>
@@ -8134,7 +8128,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>17</v>
@@ -8173,7 +8167,7 @@
       <c r="S6" s="30"/>
       <c r="T6" s="30"/>
       <c r="U6" s="21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
@@ -8243,7 +8237,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C8" s="6">
         <v>43362</v>
@@ -8258,7 +8252,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>17</v>
@@ -8297,7 +8291,7 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
@@ -8365,7 +8359,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C10" s="6">
         <v>43362</v>
@@ -8380,7 +8374,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>17</v>
@@ -8417,7 +8411,7 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
@@ -8639,7 +8633,7 @@
       <c r="S14" s="30"/>
       <c r="T14" s="30"/>
       <c r="U14" s="21" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
@@ -9111,7 +9105,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C23" s="6">
         <v>43402</v>
@@ -9333,7 +9327,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="82" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C27" s="6">
         <v>43402</v>
@@ -9393,7 +9387,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="82" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C28" s="6">
         <v>43418</v>
@@ -9673,11 +9667,11 @@
         <v>269</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="32" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="33" spans="1:21" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
@@ -9805,7 +9799,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="82" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C35" s="6">
         <v>43430</v>
@@ -10172,7 +10166,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C41" s="6">
         <v>43430</v>
@@ -10284,7 +10278,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="86" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C43" s="6">
         <v>43427</v>
@@ -11027,7 +11021,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="82" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C56" s="6">
         <v>43427</v>
@@ -11078,7 +11072,7 @@
       <c r="S56" s="30"/>
       <c r="T56" s="30"/>
       <c r="U56" s="32" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="56" x14ac:dyDescent="0.35">
@@ -11086,7 +11080,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="82" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C57" s="6">
         <v>43427</v>
@@ -11145,7 +11139,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="83" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C58" s="6">
         <v>43427</v>
@@ -11313,7 +11307,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C61" s="6">
         <v>43432</v>
@@ -11356,7 +11350,7 @@
         <v>4</v>
       </c>
       <c r="Q61" s="80" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="R61" s="30" t="s">
         <v>269</v>
@@ -11768,7 +11762,7 @@
         <v>269</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T68" s="5"/>
       <c r="U68" s="32" t="s">
@@ -11780,7 +11774,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C69" s="6">
         <v>43446</v>
@@ -11840,7 +11834,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="82" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C70" s="6">
         <v>43446</v>
@@ -11898,7 +11892,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="82" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C71" s="6">
         <v>43451</v>
@@ -12007,7 +12001,7 @@
         <v>269</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="T72" s="5"/>
       <c r="U72" s="32" t="s">
@@ -12258,7 +12252,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="86" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C77" s="6">
         <v>43465</v>
@@ -12318,7 +12312,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C78" s="6">
         <v>43465</v>
@@ -12333,7 +12327,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="32" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>38</v>
@@ -12380,7 +12374,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="83" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C79" s="6">
         <v>43465</v>
@@ -12502,7 +12496,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C81" s="6">
         <v>43465</v>
@@ -12562,7 +12556,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="83" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C82" s="6">
         <v>43465</v>
@@ -12683,7 +12677,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="83" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C84" s="6">
         <v>43465</v>
@@ -12698,7 +12692,7 @@
         <v>26</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H84" s="14" t="s">
         <v>38</v>
@@ -12735,7 +12729,7 @@
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
       <c r="U84" s="32" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="V84" s="73"/>
       <c r="W84" s="32"/>
@@ -13138,7 +13132,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="83" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C92" s="6">
         <v>43486</v>
@@ -13198,7 +13192,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="82" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C93" s="6">
         <v>43489</v>
@@ -13535,7 +13529,7 @@
       <c r="Q98" s="81"/>
       <c r="R98" s="5"/>
       <c r="S98" s="33" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
@@ -13545,7 +13539,7 @@
         <v>96</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C99" s="6">
         <v>43489</v>
@@ -13841,7 +13835,7 @@
         <v>101</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C104" s="6">
         <v>43489</v>
@@ -13856,7 +13850,7 @@
         <v>26</v>
       </c>
       <c r="G104" s="32" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H104" s="14" t="s">
         <v>245</v>
@@ -14060,7 +14054,7 @@
       <c r="Q107" s="5"/>
       <c r="R107" s="5"/>
       <c r="S107" s="33" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
@@ -14616,7 +14610,7 @@
         <v>120</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C118" s="6">
         <v>43517</v>
@@ -14655,11 +14649,11 @@
       <c r="Q118" s="5"/>
       <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T118" s="5"/>
       <c r="U118" s="32" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="119" spans="1:21" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14709,26 +14703,27 @@
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
     </row>
-    <row r="120" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
-        <f>1+A119</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>432</v>
+        <v>479</v>
       </c>
       <c r="C120" s="6">
-        <v>43517</v>
-      </c>
-      <c r="D120" s="32"/>
+        <v>43525</v>
+      </c>
+      <c r="D120" s="32" t="s">
+        <v>453</v>
+      </c>
       <c r="E120" s="32" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F120" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G120" s="32" t="s">
-        <v>431</v>
+        <v>452</v>
       </c>
       <c r="H120" s="14"/>
       <c r="I120" s="32" t="s">
@@ -14737,36 +14732,36 @@
       <c r="J120" s="32"/>
       <c r="K120" s="32"/>
       <c r="L120" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M120" s="32" t="s">
         <v>74</v>
       </c>
       <c r="N120" s="32" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="O120" s="21">
-        <v>43517</v>
+        <v>43525</v>
       </c>
       <c r="P120" s="31"/>
-      <c r="Q120" s="5"/>
-      <c r="R120" s="5"/>
-      <c r="S120" s="33"/>
+      <c r="Q120" s="14"/>
+      <c r="R120" s="14"/>
+      <c r="S120" s="14"/>
       <c r="T120" s="5"/>
       <c r="U120" s="32"/>
     </row>
-    <row r="121" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C121" s="6">
         <v>43525</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E121" s="32" t="s">
         <v>32</v>
@@ -14802,27 +14797,27 @@
       <c r="T121" s="5"/>
       <c r="U121" s="32"/>
     </row>
-    <row r="122" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="C122" s="6">
-        <v>43525</v>
+        <v>43528</v>
       </c>
       <c r="D122" s="32" t="s">
         <v>455</v>
       </c>
       <c r="E122" s="32" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F122" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H122" s="14"/>
       <c r="I122" s="32" t="s">
@@ -14837,39 +14832,43 @@
         <v>74</v>
       </c>
       <c r="N122" s="32" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="O122" s="21">
-        <v>43525</v>
+        <v>43528</v>
       </c>
       <c r="P122" s="31"/>
-      <c r="Q122" s="14"/>
-      <c r="R122" s="14"/>
-      <c r="S122" s="14"/>
-      <c r="T122" s="5"/>
+      <c r="Q122" s="5">
+        <v>30</v>
+      </c>
+      <c r="R122" s="5">
+        <v>20</v>
+      </c>
+      <c r="S122" s="33"/>
+      <c r="T122" s="5">
+        <v>10</v>
+      </c>
       <c r="U122" s="32"/>
     </row>
     <row r="123" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
-        <v>125</v>
-      </c>
-      <c r="B123" s="31" t="s">
-        <v>469</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B123" s="31"/>
       <c r="C123" s="6">
         <v>43528</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E123" s="32" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="F123" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="32" t="s">
@@ -14890,31 +14889,27 @@
         <v>43528</v>
       </c>
       <c r="P123" s="31"/>
-      <c r="Q123" s="5">
-        <v>30</v>
-      </c>
-      <c r="R123" s="5">
-        <v>20</v>
-      </c>
+      <c r="Q123" s="5"/>
+      <c r="R123" s="5"/>
       <c r="S123" s="33"/>
-      <c r="T123" s="5">
-        <v>10</v>
-      </c>
+      <c r="T123" s="5"/>
       <c r="U123" s="32"/>
     </row>
-    <row r="124" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
-        <v>126</v>
-      </c>
-      <c r="B124" s="31"/>
+        <v>127</v>
+      </c>
+      <c r="B124" s="31" t="s">
+        <v>478</v>
+      </c>
       <c r="C124" s="6">
-        <v>43528</v>
+        <v>43529</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E124" s="32" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="F124" s="32" t="s">
         <v>26</v>
@@ -14922,7 +14917,6 @@
       <c r="G124" s="32" t="s">
         <v>459</v>
       </c>
-      <c r="H124" s="14"/>
       <c r="I124" s="32" t="s">
         <v>428</v>
       </c>
@@ -14938,30 +14932,31 @@
         <v>20</v>
       </c>
       <c r="O124" s="21">
-        <v>43528</v>
-      </c>
-      <c r="P124" s="31"/>
+        <v>43529</v>
+      </c>
       <c r="Q124" s="5"/>
       <c r="R124" s="5"/>
-      <c r="S124" s="33"/>
+      <c r="S124" s="33" t="s">
+        <v>498</v>
+      </c>
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
     </row>
-    <row r="125" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="C125" s="6">
-        <v>43529</v>
+        <v>43531</v>
       </c>
       <c r="D125" s="32" t="s">
         <v>458</v>
       </c>
       <c r="E125" s="32" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="F125" s="32" t="s">
         <v>26</v>
@@ -14975,171 +14970,172 @@
       <c r="J125" s="32"/>
       <c r="K125" s="32"/>
       <c r="L125" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M125" s="32" t="s">
         <v>74</v>
       </c>
       <c r="N125" s="32" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="O125" s="21">
-        <v>43529</v>
-      </c>
-      <c r="Q125" s="5"/>
-      <c r="R125" s="5"/>
-      <c r="S125" s="33" t="s">
-        <v>500</v>
-      </c>
-      <c r="T125" s="5"/>
+        <v>43531</v>
+      </c>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="2"/>
+      <c r="S125" s="33"/>
       <c r="U125" s="32"/>
     </row>
-    <row r="126" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
-        <v>128</v>
-      </c>
-      <c r="B126" s="31" t="s">
-        <v>462</v>
+        <v>129</v>
+      </c>
+      <c r="B126" s="89" t="s">
+        <v>483</v>
       </c>
       <c r="C126" s="6">
-        <v>43531</v>
+        <v>43550</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>460</v>
+        <v>482</v>
       </c>
       <c r="E126" s="32" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="F126" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G126" s="32" t="s">
-        <v>463</v>
-      </c>
-      <c r="I126" s="32" t="s">
+      <c r="G126" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="I126" s="28" t="s">
         <v>428</v>
       </c>
       <c r="J126" s="32"/>
       <c r="K126" s="32"/>
       <c r="L126" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M126" s="32" t="s">
         <v>74</v>
       </c>
       <c r="N126" s="32" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="O126" s="21">
-        <v>43531</v>
-      </c>
-      <c r="Q126" s="2"/>
-      <c r="R126" s="2"/>
-      <c r="S126" s="33"/>
-      <c r="U126" s="32"/>
-    </row>
-    <row r="127" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+        <v>43550</v>
+      </c>
+      <c r="Q126" s="5"/>
+      <c r="R126" s="5"/>
+      <c r="S126" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="T126" s="5"/>
+      <c r="U126" s="32" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
-        <v>129</v>
-      </c>
-      <c r="B127" s="89" t="s">
+        <v>130</v>
+      </c>
+      <c r="B127" s="98" t="s">
+        <v>484</v>
+      </c>
+      <c r="C127" s="37">
+        <v>43550</v>
+      </c>
+      <c r="D127" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="E127" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F127" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G127" s="28" t="s">
         <v>485</v>
-      </c>
-      <c r="C127" s="6">
-        <v>43550</v>
-      </c>
-      <c r="D127" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="E127" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F127" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>483</v>
       </c>
       <c r="I127" s="28" t="s">
         <v>428</v>
       </c>
-      <c r="J127" s="32"/>
-      <c r="K127" s="32"/>
-      <c r="L127" s="32">
+      <c r="J127" s="99"/>
+      <c r="K127" s="28"/>
+      <c r="L127" s="28">
         <v>1</v>
       </c>
-      <c r="M127" s="32" t="s">
+      <c r="M127" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N127" s="32" t="s">
+      <c r="N127" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="O127" s="21">
+      <c r="O127" s="38">
         <v>43550</v>
       </c>
-      <c r="Q127" s="5"/>
-      <c r="R127" s="5"/>
-      <c r="S127" s="33" t="s">
-        <v>498</v>
-      </c>
-      <c r="T127" s="5"/>
-      <c r="U127" s="32" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A128" s="5">
-        <v>130</v>
-      </c>
-      <c r="B128" s="98" t="s">
+      <c r="P127" s="5"/>
+      <c r="Q127" s="39"/>
+      <c r="R127" s="88"/>
+      <c r="S127" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="T127" s="28"/>
+      <c r="U127" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="A128" s="92">
+        <v>131</v>
+      </c>
+      <c r="B128" s="89" t="s">
         <v>486</v>
       </c>
-      <c r="C128" s="37">
+      <c r="C128" s="6">
         <v>43550</v>
       </c>
-      <c r="D128" s="28" t="s">
-        <v>484</v>
-      </c>
-      <c r="E128" s="28" t="s">
+      <c r="D128" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="E128" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F128" s="28" t="s">
+      <c r="F128" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G128" s="28" t="s">
+      <c r="G128" s="32" t="s">
         <v>487</v>
       </c>
-      <c r="I128" s="28" t="s">
+      <c r="I128" s="32" t="s">
         <v>428</v>
       </c>
-      <c r="J128" s="99"/>
-      <c r="K128" s="28"/>
-      <c r="L128" s="28">
+      <c r="J128" s="32"/>
+      <c r="K128" s="32"/>
+      <c r="L128" s="32">
         <v>1</v>
       </c>
-      <c r="M128" s="28" t="s">
+      <c r="M128" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N128" s="28" t="s">
+      <c r="N128" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="O128" s="38">
+      <c r="O128" s="21">
         <v>43550</v>
       </c>
-      <c r="P128" s="5"/>
-      <c r="Q128" s="39"/>
-      <c r="R128" s="88"/>
-      <c r="S128" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="T128" s="28"/>
-      <c r="U128" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="129" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="P128" s="96"/>
+      <c r="Q128" s="5"/>
+      <c r="R128" s="33"/>
+      <c r="S128" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="T128" s="32"/>
+      <c r="U128" s="32"/>
+    </row>
+    <row r="129" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="92">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B129" s="89" t="s">
         <v>488</v>
@@ -15148,7 +15144,7 @@
         <v>43550</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>80</v>
@@ -15180,14 +15176,14 @@
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
     </row>
     <row r="130" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="92">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B130" s="89" t="s">
         <v>490</v>
@@ -15196,7 +15192,7 @@
         <v>43550</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>80</v>
@@ -15228,23 +15224,23 @@
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
     </row>
     <row r="131" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="92">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B131" s="89" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C131" s="6">
         <v>43550</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>80</v>
@@ -15253,7 +15249,7 @@
         <v>26</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I131" s="32" t="s">
         <v>428</v>
@@ -15276,36 +15272,35 @@
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
     </row>
-    <row r="132" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="92">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B132" s="89" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="C132" s="6">
-        <v>43550</v>
-      </c>
-      <c r="D132" s="32" t="s">
-        <v>484</v>
+        <v>43552</v>
+      </c>
+      <c r="D132" s="91" t="s">
+        <v>503</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="F132" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="I132" s="32" t="s">
-        <v>428</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="H132" s="94"/>
+      <c r="I132" s="32"/>
       <c r="J132" s="32"/>
       <c r="K132" s="32"/>
       <c r="L132" s="32">
@@ -15314,42 +15309,40 @@
       <c r="M132" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N132" s="32" t="s">
-        <v>20</v>
+      <c r="N132" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="O132" s="21">
-        <v>43550</v>
-      </c>
-      <c r="P132" s="96"/>
-      <c r="Q132" s="5"/>
-      <c r="R132" s="33"/>
+        <v>43552</v>
+      </c>
+      <c r="P132" s="97"/>
+      <c r="Q132" s="14"/>
+      <c r="R132" s="32"/>
       <c r="S132" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T132" s="32"/>
-      <c r="U132" s="32"/>
-    </row>
-    <row r="133" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="U132" s="33"/>
+    </row>
+    <row r="133" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A133" s="92">
-        <v>135</v>
-      </c>
-      <c r="B133" s="89" t="s">
-        <v>503</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B133" s="31"/>
       <c r="C133" s="6">
         <v>43552</v>
       </c>
-      <c r="D133" s="91" t="s">
-        <v>505</v>
+      <c r="D133" s="32" t="s">
+        <v>504</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F133" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H133" s="94"/>
       <c r="I133" s="32"/>
@@ -15361,31 +15354,31 @@
       <c r="M133" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N133" s="21" t="s">
+      <c r="N133" s="32" t="s">
         <v>153</v>
       </c>
       <c r="O133" s="21">
         <v>43552</v>
       </c>
-      <c r="P133" s="97"/>
-      <c r="Q133" s="14"/>
-      <c r="R133" s="32"/>
-      <c r="S133" s="14" t="s">
-        <v>498</v>
-      </c>
-      <c r="T133" s="32"/>
+      <c r="P133" s="96"/>
+      <c r="Q133" s="33"/>
+      <c r="R133" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="S133" s="32"/>
+      <c r="T133" s="33"/>
       <c r="U133" s="33"/>
     </row>
-    <row r="134" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:21" ht="266" x14ac:dyDescent="0.35">
       <c r="A134" s="92">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B134" s="31"/>
       <c r="C134" s="6">
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15394,7 +15387,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H134" s="94"/>
       <c r="I134" s="32"/>
@@ -15413,24 +15406,24 @@
         <v>43552</v>
       </c>
       <c r="P134" s="96"/>
-      <c r="Q134" s="33"/>
+      <c r="Q134" s="32"/>
       <c r="R134" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="S134" s="32"/>
+        <v>513</v>
+      </c>
+      <c r="S134" s="33"/>
       <c r="T134" s="33"/>
       <c r="U134" s="33"/>
     </row>
-    <row r="135" spans="1:21" ht="266" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A135" s="92">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B135" s="31"/>
       <c r="C135" s="6">
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15439,7 +15432,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H135" s="94"/>
       <c r="I135" s="32"/>
@@ -15457,25 +15450,25 @@
       <c r="O135" s="21">
         <v>43552</v>
       </c>
-      <c r="P135" s="96"/>
-      <c r="Q135" s="32"/>
-      <c r="R135" s="5" t="s">
-        <v>515</v>
+      <c r="P135" s="10"/>
+      <c r="Q135" s="33"/>
+      <c r="R135" s="33" t="s">
+        <v>513</v>
       </c>
       <c r="S135" s="33"/>
       <c r="T135" s="33"/>
       <c r="U135" s="33"/>
     </row>
-    <row r="136" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A136" s="92">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B136" s="31"/>
       <c r="C136" s="6">
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -15484,13 +15477,13 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H136" s="94"/>
       <c r="I136" s="32"/>
       <c r="J136" s="32"/>
-      <c r="K136" s="32"/>
-      <c r="L136" s="32">
+      <c r="K136" s="21"/>
+      <c r="L136" s="14">
         <v>1</v>
       </c>
       <c r="M136" s="32" t="s">
@@ -15505,22 +15498,22 @@
       <c r="P136" s="10"/>
       <c r="Q136" s="33"/>
       <c r="R136" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S136" s="33"/>
       <c r="T136" s="33"/>
       <c r="U136" s="33"/>
     </row>
-    <row r="137" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:21" ht="98" x14ac:dyDescent="0.35">
       <c r="A137" s="92">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B137" s="31"/>
       <c r="C137" s="6">
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -15529,12 +15522,12 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H137" s="94"/>
       <c r="I137" s="32"/>
-      <c r="J137" s="32"/>
-      <c r="K137" s="21"/>
+      <c r="J137" s="21"/>
+      <c r="K137" s="5"/>
       <c r="L137" s="14">
         <v>1</v>
       </c>
@@ -15550,22 +15543,22 @@
       <c r="P137" s="10"/>
       <c r="Q137" s="33"/>
       <c r="R137" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S137" s="33"/>
       <c r="T137" s="33"/>
       <c r="U137" s="33"/>
     </row>
-    <row r="138" spans="1:21" ht="98" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A138" s="92">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B138" s="31"/>
       <c r="C138" s="6">
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -15574,14 +15567,14 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H138" s="94"/>
-      <c r="I138" s="32"/>
-      <c r="J138" s="21"/>
-      <c r="K138" s="5"/>
-      <c r="L138" s="14">
-        <v>1</v>
+      <c r="I138" s="21"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="33"/>
+      <c r="L138" s="32">
+        <v>2</v>
       </c>
       <c r="M138" s="32" t="s">
         <v>74</v>
@@ -15595,22 +15588,22 @@
       <c r="P138" s="10"/>
       <c r="Q138" s="33"/>
       <c r="R138" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
       <c r="U138" s="33"/>
     </row>
-    <row r="139" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A139" s="92">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B139" s="31"/>
       <c r="C139" s="6">
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -15619,13 +15612,13 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>512</v>
-      </c>
-      <c r="H139" s="94"/>
-      <c r="I139" s="21"/>
-      <c r="J139" s="5"/>
-      <c r="K139" s="33"/>
-      <c r="L139" s="32">
+        <v>511</v>
+      </c>
+      <c r="H139" s="95"/>
+      <c r="I139" s="5"/>
+      <c r="J139" s="33"/>
+      <c r="K139" s="32"/>
+      <c r="L139" s="14">
         <v>2</v>
       </c>
       <c r="M139" s="32" t="s">
@@ -15640,7 +15633,7 @@
       <c r="P139" s="10"/>
       <c r="Q139" s="33"/>
       <c r="R139" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S139" s="33"/>
       <c r="T139" s="33"/>
@@ -15648,14 +15641,14 @@
     </row>
     <row r="140" spans="1:21" ht="196" x14ac:dyDescent="0.35">
       <c r="A140" s="92">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B140" s="31"/>
       <c r="C140" s="6">
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -15664,14 +15657,14 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>513</v>
-      </c>
-      <c r="H140" s="95"/>
-      <c r="I140" s="5"/>
-      <c r="J140" s="33"/>
-      <c r="K140" s="32"/>
+        <v>512</v>
+      </c>
+      <c r="H140" s="96"/>
+      <c r="I140" s="33"/>
+      <c r="J140" s="32"/>
+      <c r="K140" s="33"/>
       <c r="L140" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M140" s="32" t="s">
         <v>74</v>
@@ -15685,22 +15678,22 @@
       <c r="P140" s="10"/>
       <c r="Q140" s="33"/>
       <c r="R140" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S140" s="33"/>
       <c r="T140" s="33"/>
       <c r="U140" s="33"/>
     </row>
-    <row r="141" spans="1:21" ht="196" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A141" s="92">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B141" s="31"/>
       <c r="C141" s="6">
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -15711,10 +15704,10 @@
       <c r="G141" s="32" t="s">
         <v>514</v>
       </c>
-      <c r="H141" s="96"/>
-      <c r="I141" s="33"/>
-      <c r="J141" s="32"/>
-      <c r="K141" s="33"/>
+      <c r="H141" s="33"/>
+      <c r="I141" s="32"/>
+      <c r="J141" s="33"/>
+      <c r="K141" s="14"/>
       <c r="L141" s="14">
         <v>1</v>
       </c>
@@ -15727,25 +15720,25 @@
       <c r="O141" s="21">
         <v>43552</v>
       </c>
-      <c r="P141" s="10"/>
+      <c r="P141" s="93"/>
       <c r="Q141" s="33"/>
       <c r="R141" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S141" s="33"/>
       <c r="T141" s="33"/>
       <c r="U141" s="33"/>
     </row>
-    <row r="142" spans="1:21" ht="70" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A142" s="92">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B142" s="31"/>
       <c r="C142" s="6">
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -15754,19 +15747,19 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>516</v>
-      </c>
-      <c r="H142" s="33"/>
-      <c r="I142" s="32"/>
-      <c r="J142" s="33"/>
+        <v>515</v>
+      </c>
+      <c r="H142" s="32"/>
+      <c r="I142" s="33"/>
+      <c r="J142" s="14"/>
       <c r="K142" s="14"/>
-      <c r="L142" s="14">
+      <c r="L142" s="32">
         <v>1</v>
       </c>
       <c r="M142" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N142" s="32" t="s">
+      <c r="N142" s="21" t="s">
         <v>153</v>
       </c>
       <c r="O142" s="21">
@@ -15775,22 +15768,22 @@
       <c r="P142" s="93"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S142" s="33"/>
       <c r="T142" s="33"/>
       <c r="U142" s="33"/>
     </row>
-    <row r="143" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:21" ht="112" x14ac:dyDescent="0.35">
       <c r="A143" s="92">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B143" s="31"/>
       <c r="C143" s="6">
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -15799,16 +15792,16 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>517</v>
-      </c>
-      <c r="H143" s="32"/>
-      <c r="I143" s="33"/>
+        <v>516</v>
+      </c>
+      <c r="H143" s="33"/>
+      <c r="I143" s="14"/>
       <c r="J143" s="14"/>
-      <c r="K143" s="14"/>
+      <c r="K143" s="32"/>
       <c r="L143" s="32">
         <v>1</v>
       </c>
-      <c r="M143" s="32" t="s">
+      <c r="M143" s="21" t="s">
         <v>74</v>
       </c>
       <c r="N143" s="21" t="s">
@@ -15817,28 +15810,28 @@
       <c r="O143" s="21">
         <v>43552</v>
       </c>
-      <c r="P143" s="93"/>
+      <c r="P143" s="10"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S143" s="33"/>
       <c r="T143" s="33"/>
       <c r="U143" s="33"/>
     </row>
-    <row r="144" spans="1:21" ht="112" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:21" ht="84" x14ac:dyDescent="0.35">
       <c r="A144" s="92">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B144" s="31"/>
       <c r="C144" s="6">
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E144" s="32" t="s">
-        <v>39</v>
+        <v>212</v>
       </c>
       <c r="F144" s="32" t="s">
         <v>26</v>
@@ -15846,9 +15839,9 @@
       <c r="G144" s="32" t="s">
         <v>518</v>
       </c>
-      <c r="H144" s="33"/>
+      <c r="H144" s="14"/>
       <c r="I144" s="14"/>
-      <c r="J144" s="14"/>
+      <c r="J144" s="32"/>
       <c r="K144" s="32"/>
       <c r="L144" s="32">
         <v>1</v>
@@ -15865,22 +15858,22 @@
       <c r="P144" s="10"/>
       <c r="Q144" s="33"/>
       <c r="R144" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S144" s="33"/>
       <c r="T144" s="33"/>
       <c r="U144" s="33"/>
     </row>
-    <row r="145" spans="1:21" ht="84" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A145" s="92">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B145" s="31"/>
       <c r="C145" s="6">
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>212</v>
@@ -15889,19 +15882,19 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="H145" s="14"/>
-      <c r="I145" s="14"/>
+      <c r="I145" s="32"/>
       <c r="J145" s="32"/>
-      <c r="K145" s="32"/>
+      <c r="K145" s="21"/>
       <c r="L145" s="32">
         <v>1</v>
       </c>
       <c r="M145" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N145" s="21" t="s">
+      <c r="N145" s="10" t="s">
         <v>153</v>
       </c>
       <c r="O145" s="21">
@@ -15910,7 +15903,7 @@
       <c r="P145" s="10"/>
       <c r="Q145" s="33"/>
       <c r="R145" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S145" s="33"/>
       <c r="T145" s="33"/>
@@ -15918,17 +15911,17 @@
     </row>
     <row r="146" spans="1:21" ht="70" x14ac:dyDescent="0.35">
       <c r="A146" s="92">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B146" s="31"/>
       <c r="C146" s="6">
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E146" s="32" t="s">
-        <v>212</v>
+        <v>39</v>
       </c>
       <c r="F146" s="32" t="s">
         <v>26</v>
@@ -15936,9 +15929,9 @@
       <c r="G146" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="H146" s="14"/>
+      <c r="H146" s="32"/>
       <c r="I146" s="32"/>
-      <c r="J146" s="32"/>
+      <c r="J146" s="21"/>
       <c r="K146" s="21"/>
       <c r="L146" s="32">
         <v>1</v>
@@ -15955,115 +15948,120 @@
       <c r="P146" s="10"/>
       <c r="Q146" s="33"/>
       <c r="R146" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S146" s="33"/>
       <c r="T146" s="33"/>
       <c r="U146" s="33"/>
     </row>
-    <row r="147" spans="1:21" ht="70" x14ac:dyDescent="0.35">
-      <c r="A147" s="92">
-        <v>149</v>
-      </c>
-      <c r="B147" s="31"/>
-      <c r="C147" s="6">
+    <row r="147" spans="1:21" ht="140" x14ac:dyDescent="0.35">
+      <c r="A147" s="100">
+        <v>150</v>
+      </c>
+      <c r="B147" s="90"/>
+      <c r="C147" s="37">
         <v>43552</v>
       </c>
-      <c r="D147" s="32" t="s">
-        <v>506</v>
-      </c>
-      <c r="E147" s="32" t="s">
+      <c r="D147" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="E147" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="F147" s="32" t="s">
+      <c r="F147" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G147" s="32" t="s">
-        <v>521</v>
+      <c r="G147" s="28" t="s">
+        <v>520</v>
       </c>
       <c r="H147" s="32"/>
-      <c r="I147" s="32"/>
-      <c r="J147" s="21"/>
-      <c r="K147" s="21"/>
-      <c r="L147" s="32">
+      <c r="I147" s="38"/>
+      <c r="J147" s="38"/>
+      <c r="K147" s="38"/>
+      <c r="L147" s="28">
         <v>1</v>
       </c>
-      <c r="M147" s="21" t="s">
+      <c r="M147" s="38" t="s">
         <v>74</v>
       </c>
       <c r="N147" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="O147" s="21">
+      <c r="O147" s="38">
         <v>43552</v>
       </c>
       <c r="P147" s="10"/>
-      <c r="Q147" s="33"/>
-      <c r="R147" s="33" t="s">
-        <v>515</v>
-      </c>
-      <c r="S147" s="33"/>
-      <c r="T147" s="33"/>
-      <c r="U147" s="33"/>
-    </row>
-    <row r="148" spans="1:21" ht="140" x14ac:dyDescent="0.35">
-      <c r="A148" s="100">
-        <v>150</v>
-      </c>
-      <c r="B148" s="90"/>
-      <c r="C148" s="37">
-        <v>43552</v>
-      </c>
-      <c r="D148" s="28" t="s">
-        <v>506</v>
-      </c>
-      <c r="E148" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F148" s="28" t="s">
+      <c r="Q147" s="88"/>
+      <c r="R147" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="S147" s="88"/>
+      <c r="T147" s="88"/>
+      <c r="U147" s="88"/>
+    </row>
+    <row r="148" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A148" s="5">
+        <f>1+A125</f>
+        <v>129</v>
+      </c>
+      <c r="B148" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="C148" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D148" s="32" t="s">
+        <v>526</v>
+      </c>
+      <c r="E148" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F148" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G148" s="28" t="s">
-        <v>522</v>
-      </c>
-      <c r="H148" s="32"/>
-      <c r="I148" s="38"/>
-      <c r="J148" s="38"/>
-      <c r="K148" s="38"/>
-      <c r="L148" s="28">
+      <c r="G148" s="32" t="s">
+        <v>527</v>
+      </c>
+      <c r="I148" s="32"/>
+      <c r="J148" s="32"/>
+      <c r="K148" s="32"/>
+      <c r="L148" s="32">
         <v>1</v>
       </c>
-      <c r="M148" s="38" t="s">
+      <c r="M148" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N148" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="O148" s="38">
-        <v>43552</v>
-      </c>
-      <c r="P148" s="10"/>
-      <c r="Q148" s="88"/>
-      <c r="R148" s="88" t="s">
-        <v>515</v>
-      </c>
-      <c r="S148" s="88"/>
-      <c r="T148" s="88"/>
-      <c r="U148" s="88"/>
+      <c r="N148" s="32" t="s">
+        <v>577</v>
+      </c>
+      <c r="O148" s="6">
+        <v>43553</v>
+      </c>
+      <c r="Q148" s="5">
+        <v>15</v>
+      </c>
+      <c r="R148" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="S148" s="33"/>
+      <c r="T148" s="5">
+        <v>11</v>
+      </c>
+      <c r="U148" s="32"/>
     </row>
     <row r="149" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
-        <f>1+A126</f>
-        <v>129</v>
+        <f t="shared" ref="A149:A152" si="8">1+A126</f>
+        <v>130</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C149" s="6">
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -16072,7 +16070,7 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I149" s="32"/>
       <c r="J149" s="32"/>
@@ -16084,13 +16082,13 @@
         <v>74</v>
       </c>
       <c r="N149" s="32" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="O149" s="6">
         <v>43553</v>
       </c>
       <c r="Q149" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R149" s="5" t="s">
         <v>269</v>
@@ -16103,17 +16101,17 @@
     </row>
     <row r="150" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
-        <f t="shared" ref="A150:A153" si="8">1+A127</f>
-        <v>130</v>
+        <f t="shared" si="8"/>
+        <v>131</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C150" s="6">
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -16122,19 +16120,19 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I150" s="32"/>
       <c r="J150" s="32"/>
       <c r="K150" s="32"/>
-      <c r="L150" s="32">
-        <v>1</v>
+      <c r="L150" s="32" t="s">
+        <v>140</v>
       </c>
       <c r="M150" s="28" t="s">
         <v>74</v>
       </c>
       <c r="N150" s="32" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="O150" s="6">
         <v>43553</v>
@@ -16145,25 +16143,22 @@
       <c r="R150" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="S150" s="33"/>
-      <c r="T150" s="5">
-        <v>11</v>
-      </c>
+      <c r="S150" s="10"/>
       <c r="U150" s="32"/>
     </row>
-    <row r="151" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <f t="shared" si="8"/>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C151" s="6">
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16172,45 +16167,42 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I151" s="32"/>
       <c r="J151" s="32"/>
       <c r="K151" s="32"/>
-      <c r="L151" s="32" t="s">
-        <v>140</v>
+      <c r="L151" s="32">
+        <v>2</v>
       </c>
       <c r="M151" s="28" t="s">
         <v>74</v>
       </c>
       <c r="N151" s="32" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="O151" s="6">
         <v>43553</v>
       </c>
-      <c r="Q151" s="5">
-        <v>12</v>
-      </c>
-      <c r="R151" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="S151" s="10"/>
+      <c r="Q151" s="5"/>
+      <c r="R151" s="5"/>
+      <c r="S151" s="33"/>
+      <c r="T151" s="5"/>
       <c r="U151" s="32"/>
     </row>
-    <row r="152" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <f t="shared" si="8"/>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C152" s="6">
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16219,91 +16211,92 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I152" s="32"/>
       <c r="J152" s="32"/>
       <c r="K152" s="32"/>
       <c r="L152" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M152" s="28" t="s">
         <v>74</v>
       </c>
       <c r="N152" s="32" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="O152" s="6">
         <v>43553</v>
       </c>
-      <c r="Q152" s="5"/>
-      <c r="R152" s="5"/>
+      <c r="Q152" s="5">
+        <v>15</v>
+      </c>
+      <c r="R152" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="S152" s="33"/>
-      <c r="T152" s="5"/>
+      <c r="T152" s="5">
+        <v>11</v>
+      </c>
       <c r="U152" s="32"/>
     </row>
-    <row r="153" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A153" s="5">
-        <f t="shared" si="8"/>
-        <v>133</v>
+    <row r="153" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+      <c r="A153" s="92">
+        <v>151</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="C153" s="6">
-        <v>43553</v>
+        <v>43550</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="E153" s="32" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F153" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="I153" s="32"/>
+        <v>534</v>
+      </c>
+      <c r="H153" s="21"/>
+      <c r="I153" s="21"/>
       <c r="J153" s="32"/>
       <c r="K153" s="32"/>
       <c r="L153" s="32">
         <v>1</v>
       </c>
-      <c r="M153" s="28" t="s">
+      <c r="M153" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="N153" s="32" t="s">
-        <v>579</v>
-      </c>
-      <c r="O153" s="6">
-        <v>43553</v>
-      </c>
-      <c r="Q153" s="5">
-        <v>15</v>
-      </c>
-      <c r="R153" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="S153" s="33"/>
-      <c r="T153" s="5">
-        <v>11</v>
-      </c>
+      <c r="N153" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O153" s="21">
+        <v>43550</v>
+      </c>
+      <c r="P153" s="33"/>
+      <c r="Q153" s="14"/>
+      <c r="R153" s="14"/>
+      <c r="S153" s="14"/>
+      <c r="T153" s="5"/>
       <c r="U153" s="32"/>
     </row>
-    <row r="154" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="92">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C154" s="6">
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E154" s="32" t="s">
         <v>32</v>
@@ -16315,19 +16308,19 @@
         <v>536</v>
       </c>
       <c r="H154" s="21"/>
-      <c r="I154" s="21"/>
+      <c r="I154" s="32"/>
       <c r="J154" s="32"/>
       <c r="K154" s="32"/>
       <c r="L154" s="32">
         <v>1</v>
       </c>
-      <c r="M154" s="33" t="s">
+      <c r="M154" s="21" t="s">
         <v>74</v>
       </c>
       <c r="N154" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="O154" s="21">
+      <c r="O154" s="105">
         <v>43550</v>
       </c>
       <c r="P154" s="33"/>
@@ -16339,7 +16332,7 @@
     </row>
     <row r="155" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A155" s="92">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B155" s="31" t="s">
         <v>537</v>
@@ -16359,7 +16352,7 @@
       <c r="G155" s="32" t="s">
         <v>538</v>
       </c>
-      <c r="H155" s="21"/>
+      <c r="H155" s="32"/>
       <c r="I155" s="32"/>
       <c r="J155" s="32"/>
       <c r="K155" s="32"/>
@@ -16382,15 +16375,15 @@
       <c r="T155" s="5"/>
       <c r="U155" s="32"/>
     </row>
-    <row r="156" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="92">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B156" s="31" t="s">
         <v>539</v>
       </c>
       <c r="C156" s="6">
-        <v>43550</v>
+        <v>43556</v>
       </c>
       <c r="D156" s="32" t="s">
         <v>540</v>
@@ -16415,10 +16408,10 @@
         <v>74</v>
       </c>
       <c r="N156" s="21" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="O156" s="105">
-        <v>43550</v>
+        <v>43556</v>
       </c>
       <c r="P156" s="33"/>
       <c r="Q156" s="14"/>
@@ -16427,15 +16420,15 @@
       <c r="T156" s="5"/>
       <c r="U156" s="32"/>
     </row>
-    <row r="157" spans="1:21" ht="42" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="92">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B157" s="31" t="s">
         <v>541</v>
       </c>
       <c r="C157" s="6">
-        <v>43556</v>
+        <v>43552</v>
       </c>
       <c r="D157" s="32" t="s">
         <v>542</v>
@@ -16447,7 +16440,7 @@
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H157" s="32"/>
       <c r="I157" s="32"/>
@@ -16460,10 +16453,10 @@
         <v>74</v>
       </c>
       <c r="N157" s="21" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="O157" s="105">
-        <v>43556</v>
+        <v>43552</v>
       </c>
       <c r="P157" s="33"/>
       <c r="Q157" s="14"/>
@@ -16473,62 +16466,67 @@
       <c r="U157" s="32"/>
     </row>
     <row r="158" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A158" s="92">
-        <v>155</v>
+      <c r="A158" s="5">
+        <v>134</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="C158" s="6">
-        <v>43552</v>
+        <v>43546</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F158" s="32" t="s">
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="H158" s="32"/>
       <c r="I158" s="32"/>
       <c r="J158" s="32"/>
-      <c r="K158" s="32"/>
       <c r="L158" s="32">
         <v>1</v>
       </c>
       <c r="M158" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N158" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="O158" s="105">
-        <v>43552</v>
-      </c>
-      <c r="P158" s="33"/>
-      <c r="Q158" s="14"/>
-      <c r="R158" s="14"/>
-      <c r="S158" s="14"/>
+      <c r="N158" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="O158" s="6">
+        <v>43546</v>
+      </c>
+      <c r="P158" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q158" s="5">
+        <v>10</v>
+      </c>
+      <c r="R158" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="S158" s="32"/>
       <c r="T158" s="5"/>
       <c r="U158" s="32"/>
     </row>
-    <row r="159" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:21" ht="210" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="C159" s="6">
-        <v>43546</v>
+        <v>43528</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>550</v>
+        <v>482</v>
       </c>
       <c r="E159" s="32" t="s">
         <v>15</v>
@@ -16537,7 +16535,7 @@
         <v>26</v>
       </c>
       <c r="G159" s="32" t="s">
-        <v>551</v>
+        <v>579</v>
       </c>
       <c r="H159" s="32"/>
       <c r="I159" s="32"/>
@@ -16545,20 +16543,20 @@
       <c r="L159" s="32">
         <v>1</v>
       </c>
-      <c r="M159" s="21" t="s">
+      <c r="M159" s="28" t="s">
         <v>74</v>
       </c>
       <c r="N159" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="O159" s="6">
-        <v>43546</v>
+      <c r="O159" s="101">
+        <v>43528</v>
       </c>
       <c r="P159" s="5">
         <v>4</v>
       </c>
       <c r="Q159" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R159" s="5" t="s">
         <v>269</v>
@@ -16567,115 +16565,116 @@
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:21" ht="210" x14ac:dyDescent="0.35">
-      <c r="A160" s="5">
-        <v>135</v>
-      </c>
-      <c r="B160" s="31" t="s">
+    <row r="160" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+      <c r="A160" s="39">
+        <v>136</v>
+      </c>
+      <c r="B160" s="90" t="s">
         <v>554</v>
       </c>
-      <c r="C160" s="6">
-        <v>43528</v>
-      </c>
-      <c r="D160" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="E160" s="32" t="s">
+      <c r="C160" s="37">
+        <v>43481</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="E160" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F160" s="32" t="s">
+      <c r="F160" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G160" s="32" t="s">
-        <v>581</v>
-      </c>
-      <c r="H160" s="32"/>
-      <c r="I160" s="32"/>
-      <c r="J160" s="32"/>
-      <c r="L160" s="32">
+      <c r="G160" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="I160" s="28"/>
+      <c r="J160" s="28"/>
+      <c r="K160" s="28"/>
+      <c r="L160" s="28">
         <v>1</v>
       </c>
       <c r="M160" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="N160" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="O160" s="101">
-        <v>43528</v>
-      </c>
-      <c r="P160" s="5">
-        <v>4</v>
-      </c>
-      <c r="Q160" s="5">
-        <v>9</v>
-      </c>
-      <c r="R160" s="5" t="s">
+      <c r="N160" s="28"/>
+      <c r="O160" s="37">
+        <v>43481</v>
+      </c>
+      <c r="Q160" s="39">
+        <v>12</v>
+      </c>
+      <c r="R160" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="S160" s="32"/>
-      <c r="T160" s="5"/>
-      <c r="U160" s="32"/>
+      <c r="S160" s="88"/>
+      <c r="T160" s="39">
+        <v>8</v>
+      </c>
+      <c r="U160" s="28"/>
     </row>
     <row r="161" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A161" s="39">
-        <v>136</v>
-      </c>
-      <c r="B161" s="90" t="s">
-        <v>556</v>
-      </c>
-      <c r="C161" s="37">
-        <v>43481</v>
-      </c>
-      <c r="D161" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="E161" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F161" s="28" t="s">
+      <c r="A161" s="5">
+        <v>138</v>
+      </c>
+      <c r="B161" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C161" s="6">
+        <v>43542</v>
+      </c>
+      <c r="D161" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="E161" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F161" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="G161" s="28" t="s">
-        <v>557</v>
-      </c>
-      <c r="I161" s="28"/>
-      <c r="J161" s="28"/>
-      <c r="K161" s="28"/>
-      <c r="L161" s="28">
+      <c r="G161" s="32" t="s">
+        <v>567</v>
+      </c>
+      <c r="H161" s="14"/>
+      <c r="I161" s="32"/>
+      <c r="J161" s="32"/>
+      <c r="K161" s="32"/>
+      <c r="L161" s="32">
         <v>1</v>
       </c>
-      <c r="M161" s="28" t="s">
+      <c r="M161" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N161" s="28"/>
-      <c r="O161" s="37">
-        <v>43481</v>
-      </c>
-      <c r="Q161" s="39">
-        <v>12</v>
-      </c>
-      <c r="R161" s="39" t="s">
-        <v>269</v>
-      </c>
-      <c r="S161" s="88"/>
-      <c r="T161" s="39">
-        <v>8</v>
-      </c>
-      <c r="U161" s="28"/>
+      <c r="N161" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="O161" s="6">
+        <v>43542</v>
+      </c>
+      <c r="P161" s="31"/>
+      <c r="Q161" s="5">
+        <v>11</v>
+      </c>
+      <c r="R161" s="5"/>
+      <c r="S161" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="T161" s="5">
+        <v>10</v>
+      </c>
+      <c r="U161" s="32"/>
     </row>
     <row r="162" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B162" s="31" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C162" s="6">
         <v>43542</v>
       </c>
       <c r="D162" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E162" s="32" t="s">
         <v>80</v>
@@ -16684,13 +16683,13 @@
         <v>26</v>
       </c>
       <c r="G162" s="32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H162" s="14"/>
       <c r="I162" s="32"/>
       <c r="J162" s="32"/>
       <c r="K162" s="32"/>
-      <c r="L162" s="32">
+      <c r="L162" s="28">
         <v>1</v>
       </c>
       <c r="M162" s="32" t="s">
@@ -16708,7 +16707,7 @@
       </c>
       <c r="R162" s="5"/>
       <c r="S162" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T162" s="5">
         <v>10</v>
@@ -16717,16 +16716,16 @@
     </row>
     <row r="163" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C163" s="6">
         <v>43542</v>
       </c>
       <c r="D163" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E163" s="32" t="s">
         <v>80</v>
@@ -16735,13 +16734,13 @@
         <v>26</v>
       </c>
       <c r="G163" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H163" s="14"/>
       <c r="I163" s="32"/>
       <c r="J163" s="32"/>
       <c r="K163" s="32"/>
-      <c r="L163" s="28">
+      <c r="L163" s="32">
         <v>1</v>
       </c>
       <c r="M163" s="32" t="s">
@@ -16755,11 +16754,11 @@
       </c>
       <c r="P163" s="31"/>
       <c r="Q163" s="5">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="R163" s="5"/>
       <c r="S163" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T163" s="5">
         <v>10</v>
@@ -16768,16 +16767,16 @@
     </row>
     <row r="164" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C164" s="6">
         <v>43542</v>
       </c>
       <c r="D164" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E164" s="32" t="s">
         <v>80</v>
@@ -16786,13 +16785,13 @@
         <v>26</v>
       </c>
       <c r="G164" s="32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H164" s="14"/>
       <c r="I164" s="32"/>
       <c r="J164" s="32"/>
       <c r="K164" s="32"/>
-      <c r="L164" s="32">
+      <c r="L164" s="28">
         <v>1</v>
       </c>
       <c r="M164" s="32" t="s">
@@ -16806,11 +16805,11 @@
       </c>
       <c r="P164" s="31"/>
       <c r="Q164" s="5">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="R164" s="5"/>
       <c r="S164" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T164" s="5">
         <v>10</v>
@@ -16819,16 +16818,16 @@
     </row>
     <row r="165" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C165" s="6">
         <v>43542</v>
       </c>
       <c r="D165" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E165" s="32" t="s">
         <v>80</v>
@@ -16837,13 +16836,13 @@
         <v>26</v>
       </c>
       <c r="G165" s="32" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H165" s="14"/>
       <c r="I165" s="32"/>
       <c r="J165" s="32"/>
       <c r="K165" s="32"/>
-      <c r="L165" s="28">
+      <c r="L165" s="32">
         <v>1</v>
       </c>
       <c r="M165" s="32" t="s">
@@ -16857,11 +16856,11 @@
       </c>
       <c r="P165" s="31"/>
       <c r="Q165" s="5">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="R165" s="5"/>
       <c r="S165" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T165" s="5">
         <v>10</v>
@@ -16870,16 +16869,16 @@
     </row>
     <row r="166" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C166" s="6">
         <v>43542</v>
       </c>
       <c r="D166" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E166" s="32" t="s">
         <v>80</v>
@@ -16888,13 +16887,13 @@
         <v>26</v>
       </c>
       <c r="G166" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H166" s="14"/>
       <c r="I166" s="32"/>
       <c r="J166" s="32"/>
       <c r="K166" s="32"/>
-      <c r="L166" s="32">
+      <c r="L166" s="28">
         <v>1</v>
       </c>
       <c r="M166" s="32" t="s">
@@ -16908,11 +16907,11 @@
       </c>
       <c r="P166" s="31"/>
       <c r="Q166" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R166" s="5"/>
       <c r="S166" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T166" s="5">
         <v>10</v>
@@ -16921,16 +16920,16 @@
     </row>
     <row r="167" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C167" s="6">
         <v>43542</v>
       </c>
       <c r="D167" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E167" s="32" t="s">
         <v>80</v>
@@ -16939,13 +16938,13 @@
         <v>26</v>
       </c>
       <c r="G167" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H167" s="14"/>
       <c r="I167" s="32"/>
       <c r="J167" s="32"/>
       <c r="K167" s="32"/>
-      <c r="L167" s="28">
+      <c r="L167" s="32">
         <v>1</v>
       </c>
       <c r="M167" s="32" t="s">
@@ -16959,11 +16958,11 @@
       </c>
       <c r="P167" s="31"/>
       <c r="Q167" s="5">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="R167" s="5"/>
       <c r="S167" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T167" s="5">
         <v>10</v>
@@ -16972,16 +16971,16 @@
     </row>
     <row r="168" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C168" s="6">
         <v>43542</v>
       </c>
       <c r="D168" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E168" s="32" t="s">
         <v>80</v>
@@ -16990,13 +16989,13 @@
         <v>26</v>
       </c>
       <c r="G168" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H168" s="14"/>
       <c r="I168" s="32"/>
       <c r="J168" s="32"/>
       <c r="K168" s="32"/>
-      <c r="L168" s="32">
+      <c r="L168" s="28">
         <v>1</v>
       </c>
       <c r="M168" s="32" t="s">
@@ -17010,11 +17009,11 @@
       </c>
       <c r="P168" s="31"/>
       <c r="Q168" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="R168" s="5"/>
       <c r="S168" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T168" s="5">
         <v>10</v>
@@ -17023,16 +17022,16 @@
     </row>
     <row r="169" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C169" s="6">
         <v>43542</v>
       </c>
       <c r="D169" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E169" s="32" t="s">
         <v>80</v>
@@ -17041,13 +17040,13 @@
         <v>26</v>
       </c>
       <c r="G169" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H169" s="14"/>
       <c r="I169" s="32"/>
       <c r="J169" s="32"/>
       <c r="K169" s="32"/>
-      <c r="L169" s="28">
+      <c r="L169" s="32">
         <v>1</v>
       </c>
       <c r="M169" s="32" t="s">
@@ -17061,11 +17060,11 @@
       </c>
       <c r="P169" s="31"/>
       <c r="Q169" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R169" s="5"/>
       <c r="S169" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T169" s="5">
         <v>10</v>
@@ -17074,16 +17073,16 @@
     </row>
     <row r="170" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C170" s="6">
         <v>43542</v>
       </c>
       <c r="D170" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E170" s="32" t="s">
         <v>80</v>
@@ -17092,7 +17091,7 @@
         <v>26</v>
       </c>
       <c r="G170" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H170" s="14"/>
       <c r="I170" s="32"/>
@@ -17116,74 +17115,68 @@
       </c>
       <c r="R170" s="5"/>
       <c r="S170" s="33" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T170" s="5">
         <v>10</v>
       </c>
       <c r="U170" s="32"/>
     </row>
-    <row r="171" spans="1:21" ht="28" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:21" s="106" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
-        <v>149</v>
-      </c>
-      <c r="B171" s="31" t="s">
-        <v>568</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B171" s="5"/>
       <c r="C171" s="6">
-        <v>43542</v>
-      </c>
-      <c r="D171" s="32" t="s">
-        <v>580</v>
-      </c>
-      <c r="E171" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F171" s="32" t="s">
+        <v>43552</v>
+      </c>
+      <c r="D171" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="E171" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F171" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G171" s="32" t="s">
-        <v>578</v>
-      </c>
-      <c r="H171" s="14"/>
-      <c r="I171" s="32"/>
-      <c r="J171" s="32"/>
-      <c r="K171" s="32"/>
-      <c r="L171" s="32">
+        <v>583</v>
+      </c>
+      <c r="H171" s="16"/>
+      <c r="I171" s="14"/>
+      <c r="J171" s="14"/>
+      <c r="K171" s="14"/>
+      <c r="L171" s="14">
         <v>1</v>
       </c>
       <c r="M171" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="N171" s="32" t="s">
-        <v>153</v>
+      <c r="N171" s="14" t="s">
+        <v>586</v>
       </c>
       <c r="O171" s="6">
-        <v>43542</v>
-      </c>
-      <c r="P171" s="31"/>
-      <c r="Q171" s="5">
-        <v>5</v>
-      </c>
+        <v>43552</v>
+      </c>
+      <c r="P171" s="2"/>
+      <c r="Q171" s="5"/>
       <c r="R171" s="5"/>
-      <c r="S171" s="33" t="s">
-        <v>500</v>
-      </c>
-      <c r="T171" s="5">
-        <v>10</v>
-      </c>
-      <c r="U171" s="32"/>
+      <c r="S171" s="33"/>
+      <c r="T171" s="5"/>
+      <c r="U171" s="14"/>
     </row>
     <row r="172" spans="1:21" s="106" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
-        <v>150</v>
-      </c>
-      <c r="B172" s="5"/>
+        <v>151</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>580</v>
+      </c>
       <c r="C172" s="6">
         <v>43552</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E172" s="14" t="s">
         <v>125</v>
@@ -17192,7 +17185,7 @@
         <v>26</v>
       </c>
       <c r="G172" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H172" s="16"/>
       <c r="I172" s="14"/>
@@ -17205,30 +17198,34 @@
         <v>74</v>
       </c>
       <c r="N172" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="O172" s="6">
         <v>43552</v>
       </c>
       <c r="P172" s="2"/>
-      <c r="Q172" s="5"/>
-      <c r="R172" s="5"/>
+      <c r="Q172" s="5">
+        <v>4</v>
+      </c>
+      <c r="R172" s="5">
+        <v>4</v>
+      </c>
       <c r="S172" s="33"/>
-      <c r="T172" s="5"/>
+      <c r="T172" s="5">
+        <v>10</v>
+      </c>
       <c r="U172" s="14"/>
     </row>
-    <row r="173" spans="1:21" s="106" customFormat="1" ht="70" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:21" s="106" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
-        <v>151</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>582</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B173" s="5"/>
       <c r="C173" s="6">
-        <v>43552</v>
-      </c>
-      <c r="D173" s="28" t="s">
-        <v>506</v>
+        <v>43556</v>
+      </c>
+      <c r="D173" s="32" t="s">
+        <v>581</v>
       </c>
       <c r="E173" s="14" t="s">
         <v>125</v>
@@ -17237,7 +17234,7 @@
         <v>26</v>
       </c>
       <c r="G173" s="32" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="H173" s="16"/>
       <c r="I173" s="14"/>
@@ -17250,34 +17247,28 @@
         <v>74</v>
       </c>
       <c r="N173" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="O173" s="6">
-        <v>43552</v>
+        <v>43556</v>
       </c>
       <c r="P173" s="2"/>
-      <c r="Q173" s="5">
-        <v>4</v>
-      </c>
-      <c r="R173" s="5">
-        <v>4</v>
-      </c>
+      <c r="Q173" s="5"/>
+      <c r="R173" s="5"/>
       <c r="S173" s="33"/>
-      <c r="T173" s="5">
-        <v>10</v>
-      </c>
+      <c r="T173" s="5"/>
       <c r="U173" s="14"/>
     </row>
-    <row r="174" spans="1:21" s="106" customFormat="1" ht="56" x14ac:dyDescent="0.35">
-      <c r="A174" s="5">
-        <v>152</v>
+    <row r="174" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+      <c r="A174" s="2">
+        <v>153</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="6">
         <v>43556</v>
       </c>
       <c r="D174" s="32" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>125</v>
@@ -17286,9 +17277,8 @@
         <v>26</v>
       </c>
       <c r="G174" s="32" t="s">
-        <v>584</v>
-      </c>
-      <c r="H174" s="16"/>
+        <v>585</v>
+      </c>
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
       <c r="K174" s="14"/>
@@ -17299,74 +17289,31 @@
         <v>74</v>
       </c>
       <c r="N174" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="O174" s="6">
         <v>43556</v>
       </c>
-      <c r="P174" s="2"/>
       <c r="Q174" s="5"/>
       <c r="R174" s="5"/>
       <c r="S174" s="33"/>
       <c r="T174" s="5"/>
       <c r="U174" s="14"/>
     </row>
-    <row r="175" spans="1:21" ht="56" x14ac:dyDescent="0.35">
-      <c r="A175" s="2">
-        <v>153</v>
-      </c>
-      <c r="B175" s="5"/>
-      <c r="C175" s="6">
-        <v>43556</v>
-      </c>
-      <c r="D175" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="E175" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F175" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G175" s="32" t="s">
-        <v>587</v>
-      </c>
-      <c r="I175" s="14"/>
-      <c r="J175" s="14"/>
-      <c r="K175" s="14"/>
-      <c r="L175" s="14">
-        <v>1</v>
-      </c>
-      <c r="M175" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="N175" s="14" t="s">
-        <v>588</v>
-      </c>
-      <c r="O175" s="6">
-        <v>43556</v>
-      </c>
-      <c r="Q175" s="5"/>
-      <c r="R175" s="5"/>
-      <c r="S175" s="33"/>
-      <c r="T175" s="5"/>
-      <c r="U175" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:U171"/>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
-    <hyperlink ref="B127" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
-    <hyperlink ref="B128" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
-    <hyperlink ref="B129" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
-    <hyperlink ref="B130" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
-    <hyperlink ref="B131" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
-    <hyperlink ref="B132" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
-    <hyperlink ref="B133" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
-    <hyperlink ref="D133" r:id="rId9"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D132" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -17601,6 +17548,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17772,39 +17751,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17820,28 +17791,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Questions in CR Tracker for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B98624FC-475C-4D72-BAA8-FB9979399A33}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57FB9515-A5D6-4D5F-BDD7-62BBC13279E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="593">
   <si>
     <t>S.No.</t>
   </si>
@@ -4693,11 +4693,6 @@
     <t>Discussion with Sasi - refer email dated 01-Mar-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Auth APIs now will be authenticated by Partners using VID only
-Auth APIs now will be authenticated by Partners using VID only
-</t>
-  </si>
-  <si>
     <t>Discussion with Shrikant, Ramesh and Sasi - 04-Mar-19</t>
   </si>
   <si>
@@ -5568,7 +5563,17 @@
 </t>
   </si>
   <si>
-    <t>Currently we are supporting only exact match. If in V2 phonetics match has to be implemented, we might need to reintroduce 'Matching Strategy' which will confirm the type of match : phonetics or exact match and 'Matching Threshold' indicating the acceptable match range. Please confirm</t>
+    <t>Currently we are supporting only exact match. What is the high-level business logic when phonetics match will be  invoked?. Do we need to define a set of business rules by which phonetics match will be defined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auth APIs now will be authenticated by Partners using VID only
+</t>
+  </si>
+  <si>
+    <t>UIN/VID concept is configurable for a country</t>
+  </si>
+  <si>
+    <t>Based on Sasi's inputs, Biometric matching would be independent of type of Biometric device i.e., mantra/cogent, in this case decoupling based on biometric type is not applicable. We will modify current matcher implementation to match using a generic biometric matcher using Biometric Function API provided by Ramesh</t>
   </si>
 </sst>
 </file>
@@ -7470,7 +7475,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7822,9 +7827,9 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V177" sqref="V177"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7944,7 +7949,7 @@
         <v>13</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="4" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
@@ -8600,7 +8605,7 @@
       <c r="T13" s="30"/>
       <c r="U13" s="21"/>
       <c r="V13" s="21" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
@@ -9141,7 +9146,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C23" s="6">
         <v>43402</v>
@@ -9367,7 +9372,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C27" s="6">
         <v>43402</v>
@@ -9428,7 +9433,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="81" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C28" s="6">
         <v>43418</v>
@@ -9712,11 +9717,11 @@
         <v>269</v>
       </c>
       <c r="S32" s="30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T32" s="30"/>
       <c r="U32" s="32" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="V32" s="21"/>
     </row>
@@ -9847,7 +9852,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="81" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C35" s="6">
         <v>43430</v>
@@ -10029,7 +10034,7 @@
         <v>160</v>
       </c>
       <c r="V37" s="21" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="156.75" x14ac:dyDescent="0.25">
@@ -10222,7 +10227,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C41" s="6">
         <v>43430</v>
@@ -10336,7 +10341,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="85" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C43" s="6">
         <v>43427</v>
@@ -11092,7 +11097,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="81" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C56" s="6">
         <v>43427</v>
@@ -11152,7 +11157,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="81" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C57" s="6">
         <v>43427</v>
@@ -11212,7 +11217,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="82" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C58" s="6">
         <v>43427</v>
@@ -11383,7 +11388,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C61" s="6">
         <v>43432</v>
@@ -11426,7 +11431,7 @@
         <v>4</v>
       </c>
       <c r="Q61" s="79" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="R61" s="30" t="s">
         <v>269</v>
@@ -11720,7 +11725,7 @@
         <v>269</v>
       </c>
       <c r="S66" s="14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="T66" s="5" t="s">
         <v>172</v>
@@ -11845,7 +11850,7 @@
         <v>269</v>
       </c>
       <c r="S68" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T68" s="5"/>
       <c r="U68" s="32" t="s">
@@ -11858,7 +11863,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="81" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C69" s="6">
         <v>43446</v>
@@ -11919,7 +11924,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="81" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C70" s="6">
         <v>43446</v>
@@ -11978,7 +11983,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="81" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C71" s="6">
         <v>43451</v>
@@ -12088,7 +12093,7 @@
         <v>269</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T72" s="5"/>
       <c r="U72" s="32" t="s">
@@ -12341,7 +12346,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="85" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C77" s="6">
         <v>43465</v>
@@ -12464,7 +12469,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="82" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C79" s="6">
         <v>43465</v>
@@ -12586,7 +12591,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C81" s="6">
         <v>43465</v>
@@ -12646,7 +12651,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="82" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C82" s="6">
         <v>43465</v>
@@ -13061,7 +13066,7 @@
         <v>269</v>
       </c>
       <c r="S88" s="14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="T88" s="5" t="s">
         <v>172</v>
@@ -13126,7 +13131,7 @@
         <v>270</v>
       </c>
       <c r="V89" s="21" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="90" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
@@ -13232,7 +13237,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="82" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C92" s="6">
         <v>43486</v>
@@ -13293,7 +13298,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="81" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C93" s="6">
         <v>43489</v>
@@ -13635,7 +13640,7 @@
       <c r="Q98" s="80"/>
       <c r="R98" s="5"/>
       <c r="S98" s="33" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T98" s="5"/>
       <c r="U98" s="32"/>
@@ -13646,7 +13651,7 @@
         <v>96</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C99" s="6">
         <v>43489</v>
@@ -14169,7 +14174,7 @@
       <c r="Q107" s="5"/>
       <c r="R107" s="5"/>
       <c r="S107" s="33" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T107" s="5"/>
       <c r="U107" s="32"/>
@@ -14736,7 +14741,7 @@
         <v>120</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C118" s="6">
         <v>43517</v>
@@ -14775,11 +14780,11 @@
       <c r="Q118" s="5"/>
       <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T118" s="5"/>
       <c r="U118" s="32" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="V118" s="21"/>
     </row>
@@ -14836,7 +14841,7 @@
         <v>123</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C120" s="6">
         <v>43525</v>
@@ -14884,7 +14889,7 @@
         <v>124</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C121" s="6">
         <v>43525</v>
@@ -14899,7 +14904,7 @@
         <v>26</v>
       </c>
       <c r="G121" s="32" t="s">
-        <v>453</v>
+        <v>590</v>
       </c>
       <c r="H121" s="14"/>
       <c r="I121" s="32" t="s">
@@ -14924,7 +14929,9 @@
       <c r="R121" s="14"/>
       <c r="S121" s="14"/>
       <c r="T121" s="5"/>
-      <c r="U121" s="32"/>
+      <c r="U121" s="32" t="s">
+        <v>591</v>
+      </c>
       <c r="V121" s="21"/>
     </row>
     <row r="122" spans="1:22" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
@@ -14932,13 +14939,13 @@
         <v>125</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C122" s="6">
         <v>43528</v>
       </c>
       <c r="D122" s="32" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E122" s="32" t="s">
         <v>15</v>
@@ -14947,7 +14954,7 @@
         <v>26</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H122" s="14"/>
       <c r="I122" s="32" t="s">
@@ -14990,7 +14997,7 @@
         <v>43528</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E123" s="32" t="s">
         <v>39</v>
@@ -14999,7 +15006,7 @@
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="32" t="s">
@@ -15032,13 +15039,13 @@
         <v>127</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C124" s="6">
         <v>43529</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>80</v>
@@ -15047,7 +15054,7 @@
         <v>26</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I124" s="32" t="s">
         <v>427</v>
@@ -15069,7 +15076,7 @@
       <c r="Q124" s="5"/>
       <c r="R124" s="5"/>
       <c r="S124" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T124" s="5"/>
       <c r="U124" s="32"/>
@@ -15080,13 +15087,13 @@
         <v>128</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C125" s="6">
         <v>43531</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E125" s="32" t="s">
         <v>15</v>
@@ -15095,7 +15102,7 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I125" s="32" t="s">
         <v>427</v>
@@ -15125,13 +15132,13 @@
         <v>129</v>
       </c>
       <c r="B126" s="88" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C126" s="6">
         <v>43550</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E126" s="32" t="s">
         <v>80</v>
@@ -15140,7 +15147,7 @@
         <v>26</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I126" s="28" t="s">
         <v>427</v>
@@ -15162,11 +15169,11 @@
       <c r="Q126" s="5"/>
       <c r="R126" s="5"/>
       <c r="S126" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T126" s="5"/>
       <c r="U126" s="32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="V126" s="21"/>
     </row>
@@ -15175,13 +15182,13 @@
         <v>130</v>
       </c>
       <c r="B127" s="97" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C127" s="37">
         <v>43550</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E127" s="28" t="s">
         <v>80</v>
@@ -15190,7 +15197,7 @@
         <v>26</v>
       </c>
       <c r="G127" s="28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I127" s="28" t="s">
         <v>427</v>
@@ -15213,11 +15220,11 @@
       <c r="Q127" s="39"/>
       <c r="R127" s="87"/>
       <c r="S127" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T127" s="28"/>
       <c r="U127" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="V127" s="21"/>
     </row>
@@ -15226,13 +15233,13 @@
         <v>131</v>
       </c>
       <c r="B128" s="88" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C128" s="6">
         <v>43550</v>
       </c>
       <c r="D128" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E128" s="32" t="s">
         <v>80</v>
@@ -15241,7 +15248,7 @@
         <v>26</v>
       </c>
       <c r="G128" s="32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I128" s="32" t="s">
         <v>427</v>
@@ -15264,7 +15271,7 @@
       <c r="Q128" s="5"/>
       <c r="R128" s="33"/>
       <c r="S128" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T128" s="32"/>
       <c r="U128" s="32"/>
@@ -15275,13 +15282,13 @@
         <v>132</v>
       </c>
       <c r="B129" s="88" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C129" s="6">
         <v>43550</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E129" s="32" t="s">
         <v>80</v>
@@ -15290,7 +15297,7 @@
         <v>26</v>
       </c>
       <c r="G129" s="32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I129" s="32" t="s">
         <v>427</v>
@@ -15313,7 +15320,7 @@
       <c r="Q129" s="5"/>
       <c r="R129" s="33"/>
       <c r="S129" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T129" s="32"/>
       <c r="U129" s="32"/>
@@ -15324,13 +15331,13 @@
         <v>133</v>
       </c>
       <c r="B130" s="88" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C130" s="6">
         <v>43550</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E130" s="32" t="s">
         <v>80</v>
@@ -15339,7 +15346,7 @@
         <v>26</v>
       </c>
       <c r="G130" s="32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I130" s="32" t="s">
         <v>427</v>
@@ -15362,7 +15369,7 @@
       <c r="Q130" s="5"/>
       <c r="R130" s="33"/>
       <c r="S130" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T130" s="32"/>
       <c r="U130" s="32"/>
@@ -15373,13 +15380,13 @@
         <v>134</v>
       </c>
       <c r="B131" s="88" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C131" s="6">
         <v>43550</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E131" s="32" t="s">
         <v>80</v>
@@ -15388,7 +15395,7 @@
         <v>26</v>
       </c>
       <c r="G131" s="32" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I131" s="32" t="s">
         <v>427</v>
@@ -15411,24 +15418,24 @@
       <c r="Q131" s="5"/>
       <c r="R131" s="33"/>
       <c r="S131" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T131" s="32"/>
       <c r="U131" s="32"/>
       <c r="V131" s="21"/>
     </row>
-    <row r="132" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A132" s="91">
         <v>135</v>
       </c>
       <c r="B132" s="88" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C132" s="6">
         <v>43552</v>
       </c>
       <c r="D132" s="90" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E132" s="32" t="s">
         <v>32</v>
@@ -15437,7 +15444,7 @@
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H132" s="93"/>
       <c r="I132" s="32"/>
@@ -15459,11 +15466,13 @@
       <c r="Q132" s="14"/>
       <c r="R132" s="32"/>
       <c r="S132" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T132" s="32"/>
       <c r="U132" s="33"/>
-      <c r="V132" s="21"/>
+      <c r="V132" s="21" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="133" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="91">
@@ -15474,7 +15483,7 @@
         <v>43552</v>
       </c>
       <c r="D133" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E133" s="32" t="s">
         <v>39</v>
@@ -15483,7 +15492,7 @@
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H133" s="93"/>
       <c r="I133" s="32"/>
@@ -15504,7 +15513,7 @@
       <c r="P133" s="95"/>
       <c r="Q133" s="33"/>
       <c r="R133" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S133" s="32"/>
       <c r="T133" s="33"/>
@@ -15520,7 +15529,7 @@
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15529,7 +15538,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H134" s="93"/>
       <c r="I134" s="32"/>
@@ -15550,7 +15559,7 @@
       <c r="P134" s="95"/>
       <c r="Q134" s="32"/>
       <c r="R134" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S134" s="33"/>
       <c r="T134" s="33"/>
@@ -15566,7 +15575,7 @@
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15575,7 +15584,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H135" s="93"/>
       <c r="I135" s="32"/>
@@ -15596,7 +15605,7 @@
       <c r="P135" s="10"/>
       <c r="Q135" s="33"/>
       <c r="R135" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S135" s="33"/>
       <c r="T135" s="33"/>
@@ -15612,7 +15621,7 @@
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -15621,7 +15630,7 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H136" s="93"/>
       <c r="I136" s="32"/>
@@ -15642,7 +15651,7 @@
       <c r="P136" s="10"/>
       <c r="Q136" s="33"/>
       <c r="R136" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S136" s="33"/>
       <c r="T136" s="33"/>
@@ -15658,7 +15667,7 @@
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -15667,7 +15676,7 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H137" s="93"/>
       <c r="I137" s="32"/>
@@ -15688,7 +15697,7 @@
       <c r="P137" s="10"/>
       <c r="Q137" s="33"/>
       <c r="R137" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S137" s="33"/>
       <c r="T137" s="33"/>
@@ -15704,7 +15713,7 @@
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -15713,7 +15722,7 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H138" s="93"/>
       <c r="I138" s="21"/>
@@ -15734,7 +15743,7 @@
       <c r="P138" s="10"/>
       <c r="Q138" s="33"/>
       <c r="R138" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S138" s="33"/>
       <c r="T138" s="33"/>
@@ -15750,7 +15759,7 @@
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -15759,7 +15768,7 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H139" s="94"/>
       <c r="I139" s="5"/>
@@ -15780,7 +15789,7 @@
       <c r="P139" s="10"/>
       <c r="Q139" s="33"/>
       <c r="R139" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S139" s="33"/>
       <c r="T139" s="33"/>
@@ -15796,7 +15805,7 @@
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -15805,7 +15814,7 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H140" s="95"/>
       <c r="I140" s="33"/>
@@ -15826,7 +15835,7 @@
       <c r="P140" s="10"/>
       <c r="Q140" s="33"/>
       <c r="R140" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S140" s="33"/>
       <c r="T140" s="33"/>
@@ -15842,7 +15851,7 @@
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -15851,7 +15860,7 @@
         <v>26</v>
       </c>
       <c r="G141" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H141" s="33"/>
       <c r="I141" s="32"/>
@@ -15872,7 +15881,7 @@
       <c r="P141" s="92"/>
       <c r="Q141" s="33"/>
       <c r="R141" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S141" s="33"/>
       <c r="T141" s="33"/>
@@ -15888,7 +15897,7 @@
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -15897,7 +15906,7 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H142" s="32"/>
       <c r="I142" s="33"/>
@@ -15918,7 +15927,7 @@
       <c r="P142" s="92"/>
       <c r="Q142" s="33"/>
       <c r="R142" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S142" s="33"/>
       <c r="T142" s="33"/>
@@ -15934,7 +15943,7 @@
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -15943,7 +15952,7 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H143" s="33"/>
       <c r="I143" s="14"/>
@@ -15964,7 +15973,7 @@
       <c r="P143" s="10"/>
       <c r="Q143" s="33"/>
       <c r="R143" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S143" s="33"/>
       <c r="T143" s="33"/>
@@ -15980,7 +15989,7 @@
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>212</v>
@@ -15989,7 +15998,7 @@
         <v>26</v>
       </c>
       <c r="G144" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
@@ -16010,7 +16019,7 @@
       <c r="P144" s="10"/>
       <c r="Q144" s="33"/>
       <c r="R144" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S144" s="33"/>
       <c r="T144" s="33"/>
@@ -16026,7 +16035,7 @@
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>212</v>
@@ -16035,7 +16044,7 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H145" s="14"/>
       <c r="I145" s="32"/>
@@ -16056,7 +16065,7 @@
       <c r="P145" s="10"/>
       <c r="Q145" s="33"/>
       <c r="R145" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S145" s="33"/>
       <c r="T145" s="33"/>
@@ -16072,7 +16081,7 @@
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>39</v>
@@ -16081,7 +16090,7 @@
         <v>26</v>
       </c>
       <c r="G146" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H146" s="32"/>
       <c r="I146" s="32"/>
@@ -16102,7 +16111,7 @@
       <c r="P146" s="10"/>
       <c r="Q146" s="33"/>
       <c r="R146" s="33" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S146" s="33"/>
       <c r="T146" s="33"/>
@@ -16118,7 +16127,7 @@
         <v>43552</v>
       </c>
       <c r="D147" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E147" s="28" t="s">
         <v>39</v>
@@ -16127,7 +16136,7 @@
         <v>26</v>
       </c>
       <c r="G147" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H147" s="32"/>
       <c r="I147" s="38"/>
@@ -16148,7 +16157,7 @@
       <c r="P147" s="10"/>
       <c r="Q147" s="87"/>
       <c r="R147" s="87" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S147" s="87"/>
       <c r="T147" s="87"/>
@@ -16161,13 +16170,13 @@
         <v>129</v>
       </c>
       <c r="B148" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C148" s="6">
         <v>43553</v>
       </c>
       <c r="D148" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E148" s="32" t="s">
         <v>15</v>
@@ -16176,7 +16185,7 @@
         <v>26</v>
       </c>
       <c r="G148" s="32" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I148" s="32"/>
       <c r="J148" s="32"/>
@@ -16188,7 +16197,7 @@
         <v>74</v>
       </c>
       <c r="N148" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O148" s="6">
         <v>43553</v>
@@ -16212,13 +16221,13 @@
         <v>130</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C149" s="6">
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -16227,7 +16236,7 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I149" s="32"/>
       <c r="J149" s="32"/>
@@ -16239,7 +16248,7 @@
         <v>74</v>
       </c>
       <c r="N149" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O149" s="6">
         <v>43553</v>
@@ -16263,13 +16272,13 @@
         <v>131</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C150" s="6">
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -16278,7 +16287,7 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I150" s="32"/>
       <c r="J150" s="32"/>
@@ -16290,7 +16299,7 @@
         <v>74</v>
       </c>
       <c r="N150" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O150" s="6">
         <v>43553</v>
@@ -16311,13 +16320,13 @@
         <v>132</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C151" s="6">
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16326,7 +16335,7 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I151" s="32"/>
       <c r="J151" s="32"/>
@@ -16338,7 +16347,7 @@
         <v>74</v>
       </c>
       <c r="N151" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O151" s="6">
         <v>43553</v>
@@ -16356,13 +16365,13 @@
         <v>133</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C152" s="6">
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16371,7 +16380,7 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I152" s="32"/>
       <c r="J152" s="32"/>
@@ -16383,7 +16392,7 @@
         <v>74</v>
       </c>
       <c r="N152" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O152" s="6">
         <v>43553</v>
@@ -16406,13 +16415,13 @@
         <v>151</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C153" s="6">
         <v>43550</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E153" s="32" t="s">
         <v>32</v>
@@ -16421,7 +16430,7 @@
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H153" s="21"/>
       <c r="I153" s="21"/>
@@ -16452,13 +16461,13 @@
         <v>152</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C154" s="6">
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E154" s="32" t="s">
         <v>32</v>
@@ -16467,7 +16476,7 @@
         <v>26</v>
       </c>
       <c r="G154" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H154" s="21"/>
       <c r="I154" s="32"/>
@@ -16498,13 +16507,13 @@
         <v>153</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C155" s="6">
         <v>43550</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E155" s="32" t="s">
         <v>32</v>
@@ -16513,7 +16522,7 @@
         <v>26</v>
       </c>
       <c r="G155" s="32" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H155" s="32"/>
       <c r="I155" s="32"/>
@@ -16544,13 +16553,13 @@
         <v>154</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C156" s="6">
         <v>43556</v>
       </c>
       <c r="D156" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E156" s="32" t="s">
         <v>32</v>
@@ -16559,7 +16568,7 @@
         <v>26</v>
       </c>
       <c r="G156" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H156" s="32"/>
       <c r="I156" s="32"/>
@@ -16590,13 +16599,13 @@
         <v>155</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C157" s="6">
         <v>43552</v>
       </c>
       <c r="D157" s="32" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E157" s="32" t="s">
         <v>32</v>
@@ -16605,7 +16614,7 @@
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H157" s="32"/>
       <c r="I157" s="32"/>
@@ -16636,13 +16645,13 @@
         <v>134</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C158" s="6">
         <v>43546</v>
       </c>
       <c r="D158" s="32" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E158" s="32" t="s">
         <v>15</v>
@@ -16651,7 +16660,7 @@
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H158" s="32"/>
       <c r="I158" s="32"/>
@@ -16686,13 +16695,13 @@
         <v>135</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C159" s="6">
         <v>43528</v>
       </c>
       <c r="D159" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E159" s="32" t="s">
         <v>15</v>
@@ -16701,7 +16710,7 @@
         <v>26</v>
       </c>
       <c r="G159" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H159" s="32"/>
       <c r="I159" s="32"/>
@@ -16736,13 +16745,13 @@
         <v>136</v>
       </c>
       <c r="B160" s="89" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C160" s="37">
         <v>43481</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E160" s="28" t="s">
         <v>15</v>
@@ -16751,7 +16760,7 @@
         <v>26</v>
       </c>
       <c r="G160" s="28" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I160" s="28"/>
       <c r="J160" s="28"/>
@@ -16783,13 +16792,13 @@
         <v>138</v>
       </c>
       <c r="B161" s="31" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C161" s="6">
         <v>43542</v>
       </c>
       <c r="D161" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E161" s="32" t="s">
         <v>80</v>
@@ -16798,7 +16807,7 @@
         <v>26</v>
       </c>
       <c r="G161" s="32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H161" s="14"/>
       <c r="I161" s="32"/>
@@ -16822,7 +16831,7 @@
       </c>
       <c r="R161" s="5"/>
       <c r="S161" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T161" s="5">
         <v>10</v>
@@ -16834,13 +16843,13 @@
         <v>140</v>
       </c>
       <c r="B162" s="31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C162" s="6">
         <v>43542</v>
       </c>
       <c r="D162" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E162" s="32" t="s">
         <v>80</v>
@@ -16849,7 +16858,7 @@
         <v>26</v>
       </c>
       <c r="G162" s="32" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H162" s="14"/>
       <c r="I162" s="32"/>
@@ -16873,7 +16882,7 @@
       </c>
       <c r="R162" s="5"/>
       <c r="S162" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T162" s="5">
         <v>10</v>
@@ -16885,13 +16894,13 @@
         <v>141</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C163" s="6">
         <v>43542</v>
       </c>
       <c r="D163" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E163" s="32" t="s">
         <v>80</v>
@@ -16900,7 +16909,7 @@
         <v>26</v>
       </c>
       <c r="G163" s="32" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H163" s="14"/>
       <c r="I163" s="32"/>
@@ -16924,7 +16933,7 @@
       </c>
       <c r="R163" s="5"/>
       <c r="S163" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T163" s="5">
         <v>10</v>
@@ -16936,13 +16945,13 @@
         <v>142</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C164" s="6">
         <v>43542</v>
       </c>
       <c r="D164" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E164" s="32" t="s">
         <v>80</v>
@@ -16951,7 +16960,7 @@
         <v>26</v>
       </c>
       <c r="G164" s="32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H164" s="14"/>
       <c r="I164" s="32"/>
@@ -16975,7 +16984,7 @@
       </c>
       <c r="R164" s="5"/>
       <c r="S164" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T164" s="5">
         <v>10</v>
@@ -16987,13 +16996,13 @@
         <v>143</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C165" s="6">
         <v>43542</v>
       </c>
       <c r="D165" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E165" s="32" t="s">
         <v>80</v>
@@ -17002,7 +17011,7 @@
         <v>26</v>
       </c>
       <c r="G165" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H165" s="14"/>
       <c r="I165" s="32"/>
@@ -17026,7 +17035,7 @@
       </c>
       <c r="R165" s="5"/>
       <c r="S165" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T165" s="5">
         <v>10</v>
@@ -17038,13 +17047,13 @@
         <v>144</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C166" s="6">
         <v>43542</v>
       </c>
       <c r="D166" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E166" s="32" t="s">
         <v>80</v>
@@ -17053,7 +17062,7 @@
         <v>26</v>
       </c>
       <c r="G166" s="32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H166" s="14"/>
       <c r="I166" s="32"/>
@@ -17077,7 +17086,7 @@
       </c>
       <c r="R166" s="5"/>
       <c r="S166" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T166" s="5">
         <v>10</v>
@@ -17089,13 +17098,13 @@
         <v>145</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C167" s="6">
         <v>43542</v>
       </c>
       <c r="D167" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E167" s="32" t="s">
         <v>80</v>
@@ -17104,7 +17113,7 @@
         <v>26</v>
       </c>
       <c r="G167" s="32" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H167" s="14"/>
       <c r="I167" s="32"/>
@@ -17128,7 +17137,7 @@
       </c>
       <c r="R167" s="5"/>
       <c r="S167" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T167" s="5">
         <v>10</v>
@@ -17140,13 +17149,13 @@
         <v>146</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C168" s="6">
         <v>43542</v>
       </c>
       <c r="D168" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E168" s="32" t="s">
         <v>80</v>
@@ -17155,7 +17164,7 @@
         <v>26</v>
       </c>
       <c r="G168" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H168" s="14"/>
       <c r="I168" s="32"/>
@@ -17179,7 +17188,7 @@
       </c>
       <c r="R168" s="5"/>
       <c r="S168" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T168" s="5">
         <v>10</v>
@@ -17191,13 +17200,13 @@
         <v>148</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C169" s="6">
         <v>43542</v>
       </c>
       <c r="D169" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E169" s="32" t="s">
         <v>80</v>
@@ -17206,7 +17215,7 @@
         <v>26</v>
       </c>
       <c r="G169" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H169" s="14"/>
       <c r="I169" s="32"/>
@@ -17230,7 +17239,7 @@
       </c>
       <c r="R169" s="5"/>
       <c r="S169" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T169" s="5">
         <v>10</v>
@@ -17242,13 +17251,13 @@
         <v>149</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C170" s="6">
         <v>43542</v>
       </c>
       <c r="D170" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E170" s="32" t="s">
         <v>80</v>
@@ -17257,7 +17266,7 @@
         <v>26</v>
       </c>
       <c r="G170" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H170" s="14"/>
       <c r="I170" s="32"/>
@@ -17281,7 +17290,7 @@
       </c>
       <c r="R170" s="5"/>
       <c r="S170" s="33" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T170" s="5">
         <v>10</v>
@@ -17297,7 +17306,7 @@
         <v>43552</v>
       </c>
       <c r="D171" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E171" s="14" t="s">
         <v>125</v>
@@ -17306,7 +17315,7 @@
         <v>26</v>
       </c>
       <c r="G171" s="32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H171" s="16"/>
       <c r="I171" s="14"/>
@@ -17319,7 +17328,7 @@
         <v>74</v>
       </c>
       <c r="N171" s="14" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O171" s="6">
         <v>43552</v>
@@ -17336,13 +17345,13 @@
         <v>151</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C172" s="6">
         <v>43552</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E172" s="14" t="s">
         <v>125</v>
@@ -17351,7 +17360,7 @@
         <v>26</v>
       </c>
       <c r="G172" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H172" s="16"/>
       <c r="I172" s="14"/>
@@ -17364,7 +17373,7 @@
         <v>74</v>
       </c>
       <c r="N172" s="14" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O172" s="6">
         <v>43552</v>
@@ -17391,7 +17400,7 @@
         <v>43556</v>
       </c>
       <c r="D173" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E173" s="14" t="s">
         <v>125</v>
@@ -17400,7 +17409,7 @@
         <v>26</v>
       </c>
       <c r="G173" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H173" s="16"/>
       <c r="I173" s="14"/>
@@ -17413,7 +17422,7 @@
         <v>74</v>
       </c>
       <c r="N173" s="14" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O173" s="6">
         <v>43556</v>
@@ -17434,7 +17443,7 @@
         <v>43556</v>
       </c>
       <c r="D174" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E174" s="14" t="s">
         <v>125</v>
@@ -17443,7 +17452,7 @@
         <v>26</v>
       </c>
       <c r="G174" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
@@ -17455,7 +17464,7 @@
         <v>74</v>
       </c>
       <c r="N174" s="14" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="O174" s="6">
         <v>43556</v>
@@ -17467,7 +17476,7 @@
       <c r="U174" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W174" xr:uid="{3F80A47E-B4AE-4DD6-9886-9680B25FF410}">
+  <autoFilter ref="A2:W174" xr:uid="{83982D90-49D8-4EAF-B5B9-C80E0BC56E60}">
     <filterColumn colId="4">
       <filters>
         <filter val="ID Authentication"/>
@@ -17721,6 +17730,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17892,39 +17933,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17940,28 +17973,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added estimates for Reg client for Location hierarchy
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57FB9515-A5D6-4D5F-BDD7-62BBC13279E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,9 +20,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$W$174</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -5579,7 +5578,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -6297,7 +6296,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6314,7 +6313,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:U70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7475,7 +7474,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7823,43 +7822,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R118" sqref="R118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="60" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="11.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="22.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="51.5703125" style="10" customWidth="1"/>
-    <col min="23" max="16384" width="20.42578125" style="10"/>
+    <col min="16" max="16" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="51.54296875" style="10" customWidth="1"/>
+    <col min="23" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="106" t="s">
         <v>209</v>
       </c>
@@ -7884,7 +7883,7 @@
       <c r="T1" s="108"/>
       <c r="U1" s="110"/>
     </row>
-    <row r="2" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7952,7 +7951,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8014,7 +8013,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -8075,7 +8074,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8137,7 +8136,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -8199,7 +8198,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="4" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8261,7 +8260,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8323,7 +8322,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8383,7 +8382,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -8443,7 +8442,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8497,7 +8496,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="21"/>
     </row>
-    <row r="12" spans="1:22" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8554,7 +8553,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8608,7 +8607,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8669,7 +8668,7 @@
       </c>
       <c r="V14" s="21"/>
     </row>
-    <row r="15" spans="1:22" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -8732,7 +8731,7 @@
       </c>
       <c r="V15" s="21"/>
     </row>
-    <row r="16" spans="1:22" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -8795,7 +8794,7 @@
       </c>
       <c r="V16" s="21"/>
     </row>
-    <row r="17" spans="1:22" s="4" customFormat="1" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -8858,7 +8857,7 @@
       </c>
       <c r="V17" s="21"/>
     </row>
-    <row r="18" spans="1:22" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -8919,7 +8918,7 @@
       </c>
       <c r="V18" s="21"/>
     </row>
-    <row r="19" spans="1:22" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -8982,7 +8981,7 @@
       </c>
       <c r="V19" s="21"/>
     </row>
-    <row r="20" spans="1:22" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9031,7 +9030,7 @@
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
     </row>
-    <row r="21" spans="1:22" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9080,7 +9079,7 @@
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
     </row>
-    <row r="22" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9141,7 +9140,7 @@
       </c>
       <c r="V22" s="21"/>
     </row>
-    <row r="23" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -9202,7 +9201,7 @@
       </c>
       <c r="V23" s="21"/>
     </row>
-    <row r="24" spans="1:22" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9265,7 +9264,7 @@
       </c>
       <c r="V24" s="21"/>
     </row>
-    <row r="25" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9316,7 +9315,7 @@
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
     </row>
-    <row r="26" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9367,7 +9366,7 @@
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
     </row>
-    <row r="27" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -9428,7 +9427,7 @@
       </c>
       <c r="V27" s="21"/>
     </row>
-    <row r="28" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9491,7 +9490,7 @@
       </c>
       <c r="V28" s="21"/>
     </row>
-    <row r="29" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9542,7 +9541,7 @@
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
     </row>
-    <row r="30" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9599,7 +9598,7 @@
       <c r="U30" s="14"/>
       <c r="V30" s="21"/>
     </row>
-    <row r="31" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9662,7 +9661,7 @@
       </c>
       <c r="V31" s="21"/>
     </row>
-    <row r="32" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9725,7 +9724,7 @@
       </c>
       <c r="V32" s="21"/>
     </row>
-    <row r="33" spans="1:22" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9784,7 +9783,7 @@
       </c>
       <c r="V33" s="21"/>
     </row>
-    <row r="34" spans="1:22" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9847,7 +9846,7 @@
       </c>
       <c r="V34" s="21"/>
     </row>
-    <row r="35" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -9905,7 +9904,7 @@
       <c r="U35" s="14"/>
       <c r="V35" s="21"/>
     </row>
-    <row r="36" spans="1:22" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -9970,7 +9969,7 @@
       </c>
       <c r="V36" s="21"/>
     </row>
-    <row r="37" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -10037,7 +10036,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10102,7 +10101,7 @@
       </c>
       <c r="V38" s="21"/>
     </row>
-    <row r="39" spans="1:22" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10167,7 +10166,7 @@
       </c>
       <c r="V39" s="21"/>
     </row>
-    <row r="40" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -10222,7 +10221,7 @@
       <c r="U40" s="32"/>
       <c r="V40" s="21"/>
     </row>
-    <row r="41" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -10281,7 +10280,7 @@
       <c r="U41" s="32"/>
       <c r="V41" s="21"/>
     </row>
-    <row r="42" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10336,7 +10335,7 @@
       <c r="U42" s="32"/>
       <c r="V42" s="21"/>
     </row>
-    <row r="43" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10395,7 +10394,7 @@
       <c r="U43" s="32"/>
       <c r="V43" s="21"/>
     </row>
-    <row r="44" spans="1:22" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10456,7 +10455,7 @@
       </c>
       <c r="V44" s="21"/>
     </row>
-    <row r="45" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10515,7 +10514,7 @@
       </c>
       <c r="V45" s="21"/>
     </row>
-    <row r="46" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10578,7 +10577,7 @@
       </c>
       <c r="V46" s="21"/>
     </row>
-    <row r="47" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10641,7 +10640,7 @@
       </c>
       <c r="V47" s="21"/>
     </row>
-    <row r="48" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10692,7 +10691,7 @@
       <c r="U48" s="32"/>
       <c r="V48" s="21"/>
     </row>
-    <row r="49" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10755,7 +10754,7 @@
       </c>
       <c r="V49" s="21"/>
     </row>
-    <row r="50" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10819,7 +10818,7 @@
       </c>
       <c r="V50" s="21"/>
     </row>
-    <row r="51" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10874,7 +10873,7 @@
       <c r="U51" s="32"/>
       <c r="V51" s="21"/>
     </row>
-    <row r="52" spans="1:22" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10925,7 +10924,7 @@
       <c r="U52" s="32"/>
       <c r="V52" s="21"/>
     </row>
-    <row r="53" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10986,7 +10985,7 @@
       </c>
       <c r="V53" s="21"/>
     </row>
-    <row r="54" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -11037,7 +11036,7 @@
       <c r="U54" s="32"/>
       <c r="V54" s="21"/>
     </row>
-    <row r="55" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -11092,7 +11091,7 @@
       <c r="U55" s="32"/>
       <c r="V55" s="21"/>
     </row>
-    <row r="56" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -11152,7 +11151,7 @@
       </c>
       <c r="V56" s="21"/>
     </row>
-    <row r="57" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -11212,7 +11211,7 @@
       </c>
       <c r="V57" s="21"/>
     </row>
-    <row r="58" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11273,7 +11272,7 @@
       </c>
       <c r="V58" s="21"/>
     </row>
-    <row r="59" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11328,7 +11327,7 @@
       <c r="U59" s="32"/>
       <c r="V59" s="21"/>
     </row>
-    <row r="60" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11383,7 +11382,7 @@
       <c r="U60" s="32"/>
       <c r="V60" s="21"/>
     </row>
-    <row r="61" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -11441,7 +11440,7 @@
       <c r="U61" s="32"/>
       <c r="V61" s="21"/>
     </row>
-    <row r="62" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -11505,7 +11504,7 @@
       </c>
       <c r="V62" s="21"/>
     </row>
-    <row r="63" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -11567,7 +11566,7 @@
       </c>
       <c r="V63" s="21"/>
     </row>
-    <row r="64" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11619,7 +11618,7 @@
       <c r="U64" s="32"/>
       <c r="V64" s="21"/>
     </row>
-    <row r="65" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11671,7 +11670,7 @@
       <c r="U65" s="32"/>
       <c r="V65" s="21"/>
     </row>
-    <row r="66" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -11735,7 +11734,7 @@
       </c>
       <c r="V66" s="21"/>
     </row>
-    <row r="67" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11796,7 +11795,7 @@
       </c>
       <c r="V67" s="21"/>
     </row>
-    <row r="68" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -11858,7 +11857,7 @@
       </c>
       <c r="V68" s="21"/>
     </row>
-    <row r="69" spans="1:23" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -11919,7 +11918,7 @@
       </c>
       <c r="V69" s="21"/>
     </row>
-    <row r="70" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -11978,7 +11977,7 @@
       <c r="U70" s="32"/>
       <c r="V70" s="21"/>
     </row>
-    <row r="71" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -12039,7 +12038,7 @@
       </c>
       <c r="V71" s="21"/>
     </row>
-    <row r="72" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -12102,7 +12101,7 @@
       <c r="V72" s="21"/>
       <c r="W72" s="32"/>
     </row>
-    <row r="73" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -12162,7 +12161,7 @@
       <c r="V73" s="21"/>
       <c r="W73" s="28"/>
     </row>
-    <row r="74" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12217,7 +12216,7 @@
       <c r="V74" s="21"/>
       <c r="W74" s="32"/>
     </row>
-    <row r="75" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -12279,7 +12278,7 @@
       </c>
       <c r="V75" s="21"/>
     </row>
-    <row r="76" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -12341,7 +12340,7 @@
       </c>
       <c r="V76" s="21"/>
     </row>
-    <row r="77" spans="1:23" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -12402,7 +12401,7 @@
       </c>
       <c r="V77" s="21"/>
     </row>
-    <row r="78" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -12464,7 +12463,7 @@
       <c r="V78" s="21"/>
       <c r="W78" s="32"/>
     </row>
-    <row r="79" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>76</v>
       </c>
@@ -12524,7 +12523,7 @@
       <c r="V79" s="21"/>
       <c r="W79" s="32"/>
     </row>
-    <row r="80" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -12586,7 +12585,7 @@
       <c r="V80" s="21"/>
       <c r="W80" s="32"/>
     </row>
-    <row r="81" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>78</v>
       </c>
@@ -12646,7 +12645,7 @@
       <c r="V81" s="21"/>
       <c r="W81" s="32"/>
     </row>
-    <row r="82" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -12708,7 +12707,7 @@
       <c r="V82" s="21"/>
       <c r="W82" s="32"/>
     </row>
-    <row r="83" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>80</v>
       </c>
@@ -12768,7 +12767,7 @@
       </c>
       <c r="V83" s="21"/>
     </row>
-    <row r="84" spans="1:23" ht="228" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -12830,7 +12829,7 @@
       <c r="V84" s="21"/>
       <c r="W84" s="32"/>
     </row>
-    <row r="85" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>82</v>
       </c>
@@ -12893,7 +12892,7 @@
       </c>
       <c r="V85" s="21"/>
     </row>
-    <row r="86" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -12954,7 +12953,7 @@
       <c r="U86" s="32"/>
       <c r="V86" s="21"/>
     </row>
-    <row r="87" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>84</v>
       </c>
@@ -13014,7 +13013,7 @@
       </c>
       <c r="V87" s="21"/>
     </row>
-    <row r="88" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -13076,7 +13075,7 @@
       </c>
       <c r="V88" s="21"/>
     </row>
-    <row r="89" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>86</v>
       </c>
@@ -13134,7 +13133,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -13184,7 +13183,7 @@
       <c r="U90" s="32"/>
       <c r="V90" s="21"/>
     </row>
-    <row r="91" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>88</v>
       </c>
@@ -13232,7 +13231,7 @@
       <c r="U91" s="32"/>
       <c r="V91" s="21"/>
     </row>
-    <row r="92" spans="1:23" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -13293,7 +13292,7 @@
       </c>
       <c r="V92" s="21"/>
     </row>
-    <row r="93" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>90</v>
       </c>
@@ -13352,7 +13351,7 @@
       <c r="U93" s="32"/>
       <c r="V93" s="21"/>
     </row>
-    <row r="94" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -13413,7 +13412,7 @@
       </c>
       <c r="V94" s="21"/>
     </row>
-    <row r="95" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>92</v>
       </c>
@@ -13474,7 +13473,7 @@
       </c>
       <c r="V95" s="21"/>
     </row>
-    <row r="96" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -13535,7 +13534,7 @@
       </c>
       <c r="V96" s="21"/>
     </row>
-    <row r="97" spans="1:22" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>94</v>
       </c>
@@ -13594,7 +13593,7 @@
       <c r="U97" s="32"/>
       <c r="V97" s="21"/>
     </row>
-    <row r="98" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -13646,7 +13645,7 @@
       <c r="U98" s="32"/>
       <c r="V98" s="21"/>
     </row>
-    <row r="99" spans="1:22" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>96</v>
       </c>
@@ -13705,7 +13704,7 @@
       <c r="U99" s="32"/>
       <c r="V99" s="21"/>
     </row>
-    <row r="100" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -13766,7 +13765,7 @@
       </c>
       <c r="V100" s="21"/>
     </row>
-    <row r="101" spans="1:22" ht="299.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>98</v>
       </c>
@@ -13827,7 +13826,7 @@
       </c>
       <c r="V101" s="21"/>
     </row>
-    <row r="102" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -13886,7 +13885,7 @@
       <c r="U102" s="32"/>
       <c r="V102" s="21"/>
     </row>
-    <row r="103" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>100</v>
       </c>
@@ -13947,7 +13946,7 @@
       </c>
       <c r="V103" s="21"/>
     </row>
-    <row r="104" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -14008,7 +14007,7 @@
       </c>
       <c r="V104" s="21"/>
     </row>
-    <row r="105" spans="1:22" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>102</v>
       </c>
@@ -14068,7 +14067,7 @@
       <c r="U105" s="33"/>
       <c r="V105" s="21"/>
     </row>
-    <row r="106" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -14128,7 +14127,7 @@
       </c>
       <c r="V106" s="21"/>
     </row>
-    <row r="107" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>104</v>
       </c>
@@ -14180,7 +14179,7 @@
       <c r="U107" s="32"/>
       <c r="V107" s="21"/>
     </row>
-    <row r="108" spans="1:22" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -14240,7 +14239,7 @@
       </c>
       <c r="V108" s="21"/>
     </row>
-    <row r="109" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>111</v>
       </c>
@@ -14296,7 +14295,7 @@
       <c r="U109" s="32"/>
       <c r="V109" s="21"/>
     </row>
-    <row r="110" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>112</v>
       </c>
@@ -14352,7 +14351,7 @@
       <c r="U110" s="32"/>
       <c r="V110" s="21"/>
     </row>
-    <row r="111" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>113</v>
       </c>
@@ -14410,7 +14409,7 @@
       <c r="U111" s="32"/>
       <c r="V111" s="21"/>
     </row>
-    <row r="112" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>114</v>
       </c>
@@ -14468,7 +14467,7 @@
       <c r="U112" s="32"/>
       <c r="V112" s="21"/>
     </row>
-    <row r="113" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>115</v>
       </c>
@@ -14526,7 +14525,7 @@
       <c r="U113" s="32"/>
       <c r="V113" s="21"/>
     </row>
-    <row r="114" spans="1:22" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>116</v>
       </c>
@@ -14584,7 +14583,7 @@
       <c r="U114" s="32"/>
       <c r="V114" s="21"/>
     </row>
-    <row r="115" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>117</v>
       </c>
@@ -14640,7 +14639,7 @@
       <c r="U115" s="32"/>
       <c r="V115" s="21"/>
     </row>
-    <row r="116" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>118</v>
       </c>
@@ -14687,7 +14686,7 @@
       <c r="U116" s="32"/>
       <c r="V116" s="21"/>
     </row>
-    <row r="117" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="39">
         <v>119</v>
       </c>
@@ -14736,7 +14735,7 @@
       <c r="U117" s="28"/>
       <c r="V117" s="21"/>
     </row>
-    <row r="118" spans="1:22" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>120</v>
       </c>
@@ -14777,8 +14776,12 @@
         <v>43517</v>
       </c>
       <c r="P118" s="31"/>
-      <c r="Q118" s="5"/>
-      <c r="R118" s="5"/>
+      <c r="Q118" s="5">
+        <v>30</v>
+      </c>
+      <c r="R118" s="5">
+        <v>20</v>
+      </c>
       <c r="S118" s="33" t="s">
         <v>494</v>
       </c>
@@ -14788,7 +14791,7 @@
       </c>
       <c r="V118" s="21"/>
     </row>
-    <row r="119" spans="1:22" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>121</v>
       </c>
@@ -14836,7 +14839,7 @@
       <c r="U119" s="32"/>
       <c r="V119" s="21"/>
     </row>
-    <row r="120" spans="1:22" ht="57" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>123</v>
       </c>
@@ -14884,7 +14887,7 @@
       <c r="U120" s="32"/>
       <c r="V120" s="21"/>
     </row>
-    <row r="121" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>124</v>
       </c>
@@ -14934,7 +14937,7 @@
       </c>
       <c r="V121" s="21"/>
     </row>
-    <row r="122" spans="1:22" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" ht="112" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>125</v>
       </c>
@@ -14988,7 +14991,7 @@
       <c r="U122" s="32"/>
       <c r="V122" s="21"/>
     </row>
-    <row r="123" spans="1:22" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>126</v>
       </c>
@@ -15034,7 +15037,7 @@
       <c r="U123" s="32"/>
       <c r="V123" s="21"/>
     </row>
-    <row r="124" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>127</v>
       </c>
@@ -15082,7 +15085,7 @@
       <c r="U124" s="32"/>
       <c r="V124" s="21"/>
     </row>
-    <row r="125" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>128</v>
       </c>
@@ -15127,7 +15130,7 @@
       <c r="U125" s="32"/>
       <c r="V125" s="21"/>
     </row>
-    <row r="126" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>129</v>
       </c>
@@ -15177,7 +15180,7 @@
       </c>
       <c r="V126" s="21"/>
     </row>
-    <row r="127" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>130</v>
       </c>
@@ -15228,7 +15231,7 @@
       </c>
       <c r="V127" s="21"/>
     </row>
-    <row r="128" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A128" s="91">
         <v>131</v>
       </c>
@@ -15277,7 +15280,7 @@
       <c r="U128" s="32"/>
       <c r="V128" s="21"/>
     </row>
-    <row r="129" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="91">
         <v>132</v>
       </c>
@@ -15326,7 +15329,7 @@
       <c r="U129" s="32"/>
       <c r="V129" s="21"/>
     </row>
-    <row r="130" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="91">
         <v>133</v>
       </c>
@@ -15375,7 +15378,7 @@
       <c r="U130" s="32"/>
       <c r="V130" s="21"/>
     </row>
-    <row r="131" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="91">
         <v>134</v>
       </c>
@@ -15424,7 +15427,7 @@
       <c r="U131" s="32"/>
       <c r="V131" s="21"/>
     </row>
-    <row r="132" spans="1:22" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A132" s="91">
         <v>135</v>
       </c>
@@ -15474,7 +15477,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A133" s="91">
         <v>136</v>
       </c>
@@ -15520,7 +15523,7 @@
       <c r="U133" s="33"/>
       <c r="V133" s="21"/>
     </row>
-    <row r="134" spans="1:22" ht="270.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" ht="266" x14ac:dyDescent="0.35">
       <c r="A134" s="91">
         <v>137</v>
       </c>
@@ -15566,7 +15569,7 @@
       <c r="U134" s="33"/>
       <c r="V134" s="21"/>
     </row>
-    <row r="135" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A135" s="91">
         <v>138</v>
       </c>
@@ -15612,7 +15615,7 @@
       <c r="U135" s="33"/>
       <c r="V135" s="21"/>
     </row>
-    <row r="136" spans="1:22" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" ht="196" x14ac:dyDescent="0.35">
       <c r="A136" s="91">
         <v>139</v>
       </c>
@@ -15658,7 +15661,7 @@
       <c r="U136" s="33"/>
       <c r="V136" s="21"/>
     </row>
-    <row r="137" spans="1:22" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" ht="98" x14ac:dyDescent="0.35">
       <c r="A137" s="91">
         <v>140</v>
       </c>
@@ -15704,7 +15707,7 @@
       <c r="U137" s="33"/>
       <c r="V137" s="21"/>
     </row>
-    <row r="138" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A138" s="91">
         <v>141</v>
       </c>
@@ -15750,7 +15753,7 @@
       <c r="U138" s="33"/>
       <c r="V138" s="21"/>
     </row>
-    <row r="139" spans="1:22" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" ht="196" x14ac:dyDescent="0.35">
       <c r="A139" s="91">
         <v>142</v>
       </c>
@@ -15796,7 +15799,7 @@
       <c r="U139" s="33"/>
       <c r="V139" s="21"/>
     </row>
-    <row r="140" spans="1:22" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" ht="196" x14ac:dyDescent="0.35">
       <c r="A140" s="91">
         <v>143</v>
       </c>
@@ -15842,7 +15845,7 @@
       <c r="U140" s="33"/>
       <c r="V140" s="21"/>
     </row>
-    <row r="141" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A141" s="91">
         <v>144</v>
       </c>
@@ -15888,7 +15891,7 @@
       <c r="U141" s="33"/>
       <c r="V141" s="21"/>
     </row>
-    <row r="142" spans="1:22" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A142" s="91">
         <v>145</v>
       </c>
@@ -15934,7 +15937,7 @@
       <c r="U142" s="33"/>
       <c r="V142" s="21"/>
     </row>
-    <row r="143" spans="1:22" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" ht="112" x14ac:dyDescent="0.35">
       <c r="A143" s="91">
         <v>146</v>
       </c>
@@ -15980,7 +15983,7 @@
       <c r="U143" s="33"/>
       <c r="V143" s="21"/>
     </row>
-    <row r="144" spans="1:22" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" ht="84" x14ac:dyDescent="0.35">
       <c r="A144" s="91">
         <v>147</v>
       </c>
@@ -16026,7 +16029,7 @@
       <c r="U144" s="33"/>
       <c r="V144" s="21"/>
     </row>
-    <row r="145" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A145" s="91">
         <v>148</v>
       </c>
@@ -16072,7 +16075,7 @@
       <c r="U145" s="33"/>
       <c r="V145" s="21"/>
     </row>
-    <row r="146" spans="1:22" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" ht="70" x14ac:dyDescent="0.35">
       <c r="A146" s="91">
         <v>149</v>
       </c>
@@ -16118,7 +16121,7 @@
       <c r="U146" s="33"/>
       <c r="V146" s="21"/>
     </row>
-    <row r="147" spans="1:22" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" ht="140" x14ac:dyDescent="0.35">
       <c r="A147" s="99">
         <v>150</v>
       </c>
@@ -16164,7 +16167,7 @@
       <c r="U147" s="87"/>
       <c r="V147" s="21"/>
     </row>
-    <row r="148" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <f>1+A125</f>
         <v>129</v>
@@ -16215,7 +16218,7 @@
       <c r="U148" s="32"/>
       <c r="V148" s="21"/>
     </row>
-    <row r="149" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <f t="shared" ref="A149:A152" si="8">1+A126</f>
         <v>130</v>
@@ -16266,7 +16269,7 @@
       <c r="U149" s="32"/>
       <c r="V149" s="21"/>
     </row>
-    <row r="150" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <f t="shared" si="8"/>
         <v>131</v>
@@ -16314,7 +16317,7 @@
       <c r="U150" s="32"/>
       <c r="V150" s="21"/>
     </row>
-    <row r="151" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <f t="shared" si="8"/>
         <v>132</v>
@@ -16359,7 +16362,7 @@
       <c r="U151" s="32"/>
       <c r="V151" s="21"/>
     </row>
-    <row r="152" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <f t="shared" si="8"/>
         <v>133</v>
@@ -16410,7 +16413,7 @@
       <c r="U152" s="32"/>
       <c r="V152" s="21"/>
     </row>
-    <row r="153" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A153" s="91">
         <v>151</v>
       </c>
@@ -16456,7 +16459,7 @@
       <c r="U153" s="32"/>
       <c r="V153" s="21"/>
     </row>
-    <row r="154" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="91">
         <v>152</v>
       </c>
@@ -16502,7 +16505,7 @@
       <c r="U154" s="32"/>
       <c r="V154" s="21"/>
     </row>
-    <row r="155" spans="1:22" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A155" s="91">
         <v>153</v>
       </c>
@@ -16548,7 +16551,7 @@
       <c r="U155" s="32"/>
       <c r="V155" s="21"/>
     </row>
-    <row r="156" spans="1:22" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:22" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="91">
         <v>154</v>
       </c>
@@ -16594,7 +16597,7 @@
       <c r="U156" s="32"/>
       <c r="V156" s="21"/>
     </row>
-    <row r="157" spans="1:22" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="91">
         <v>155</v>
       </c>
@@ -16640,7 +16643,7 @@
       <c r="U157" s="32"/>
       <c r="V157" s="21"/>
     </row>
-    <row r="158" spans="1:22" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>134</v>
       </c>
@@ -16690,7 +16693,7 @@
       <c r="T158" s="5"/>
       <c r="U158" s="32"/>
     </row>
-    <row r="159" spans="1:22" ht="228" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" ht="210" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>135</v>
       </c>
@@ -16740,7 +16743,7 @@
       <c r="T159" s="5"/>
       <c r="U159" s="32"/>
     </row>
-    <row r="160" spans="1:22" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:22" ht="28" x14ac:dyDescent="0.35">
       <c r="A160" s="39">
         <v>136</v>
       </c>
@@ -16787,7 +16790,7 @@
       </c>
       <c r="U160" s="28"/>
     </row>
-    <row r="161" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>138</v>
       </c>
@@ -16838,7 +16841,7 @@
       </c>
       <c r="U161" s="32"/>
     </row>
-    <row r="162" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>140</v>
       </c>
@@ -16889,7 +16892,7 @@
       </c>
       <c r="U162" s="32"/>
     </row>
-    <row r="163" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>141</v>
       </c>
@@ -16940,7 +16943,7 @@
       </c>
       <c r="U163" s="32"/>
     </row>
-    <row r="164" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>142</v>
       </c>
@@ -16991,7 +16994,7 @@
       </c>
       <c r="U164" s="32"/>
     </row>
-    <row r="165" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>143</v>
       </c>
@@ -17042,7 +17045,7 @@
       </c>
       <c r="U165" s="32"/>
     </row>
-    <row r="166" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>144</v>
       </c>
@@ -17093,7 +17096,7 @@
       </c>
       <c r="U166" s="32"/>
     </row>
-    <row r="167" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>145</v>
       </c>
@@ -17144,7 +17147,7 @@
       </c>
       <c r="U167" s="32"/>
     </row>
-    <row r="168" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>146</v>
       </c>
@@ -17195,7 +17198,7 @@
       </c>
       <c r="U168" s="32"/>
     </row>
-    <row r="169" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>148</v>
       </c>
@@ -17246,7 +17249,7 @@
       </c>
       <c r="U169" s="32"/>
     </row>
-    <row r="170" spans="1:21" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>149</v>
       </c>
@@ -17297,7 +17300,7 @@
       </c>
       <c r="U170" s="32"/>
     </row>
-    <row r="171" spans="1:21" s="105" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" s="105" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>150</v>
       </c>
@@ -17340,7 +17343,7 @@
       <c r="T171" s="5"/>
       <c r="U171" s="14"/>
     </row>
-    <row r="172" spans="1:21" s="105" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" s="105" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>151</v>
       </c>
@@ -17391,7 +17394,7 @@
       </c>
       <c r="U172" s="14"/>
     </row>
-    <row r="173" spans="1:21" s="105" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" s="105" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>152</v>
       </c>
@@ -17434,7 +17437,7 @@
       <c r="T173" s="5"/>
       <c r="U173" s="14"/>
     </row>
-    <row r="174" spans="1:21" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="56" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>153</v>
       </c>
@@ -17476,26 +17479,19 @@
       <c r="U174" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W174" xr:uid="{83982D90-49D8-4EAF-B5B9-C80E0BC56E60}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="ID Authentication"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D132" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D132" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
@@ -17503,57 +17499,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9"/>
     </row>
   </sheetData>
@@ -17563,19 +17559,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>145</v>
       </c>
@@ -17586,7 +17582,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -17597,7 +17593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -17608,7 +17604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -17619,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -17630,7 +17626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -17641,7 +17637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -17652,7 +17648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -17663,7 +17659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>146</v>
       </c>
@@ -17681,17 +17677,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="65" t="s">
         <v>207</v>
       </c>
@@ -17699,25 +17695,25 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69"/>
       <c r="C3" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="70"/>
       <c r="C4" s="68" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71"/>
       <c r="C5" s="72" t="s">
         <v>206</v>
@@ -17753,15 +17749,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17933,6 +17920,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
@@ -17950,14 +17946,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17973,4 +17961,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added estimates for Location hierarchy
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -7826,9 +7826,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R118" sqref="R118"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R119" sqref="R119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -14776,12 +14776,8 @@
         <v>43517</v>
       </c>
       <c r="P118" s="31"/>
-      <c r="Q118" s="5">
-        <v>30</v>
-      </c>
-      <c r="R118" s="5">
-        <v>20</v>
-      </c>
+      <c r="Q118" s="5"/>
+      <c r="R118" s="5"/>
       <c r="S118" s="33" t="s">
         <v>494</v>
       </c>
@@ -14832,8 +14828,12 @@
         <v>43517</v>
       </c>
       <c r="P119" s="31"/>
-      <c r="Q119" s="5"/>
-      <c r="R119" s="5"/>
+      <c r="Q119" s="5">
+        <v>30</v>
+      </c>
+      <c r="R119" s="5">
+        <v>20</v>
+      </c>
       <c r="S119" s="33"/>
       <c r="T119" s="5"/>
       <c r="U119" s="32"/>
@@ -17726,26 +17726,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17921,26 +17907,32 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17964,9 +17956,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the Features Roadmap for IDA
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8233CA09-B05C-4431-9ED0-FEB4D4DE9EB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6EFB36EC-3A66-49D2-8F07-C706B7A6E519}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -5513,6 +5513,64 @@
     <t>Mocked Implementation Completed</t>
   </si>
   <si>
+    <t xml:space="preserve">Auth APIs now will be authenticated by Partners using VID only
+</t>
+  </si>
+  <si>
+    <t>UIN/VID concept is configurable for a country</t>
+  </si>
+  <si>
+    <t>Based on Sasi's inputs, Biometric matching would be independent of type of Biometric device i.e., mantra/cogent, in this case decoupling based on biometric type is not applicable. We will modify current matcher implementation to match using a generic biometric matcher using Biometric Function API provided by Ramesh</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Design/Technical</t>
+  </si>
+  <si>
+    <t>Partner Management Portal</t>
+  </si>
+  <si>
+    <t>Resident Services</t>
+  </si>
+  <si>
+    <t>Admin/Reports</t>
+  </si>
+  <si>
+    <t>For UIN Update of Child, capture the UIN, Name and one biometric of the Parent/Guardian</t>
+  </si>
+  <si>
+    <t>For new registration of child capture any one biometric of the Parent/Guardian</t>
+  </si>
+  <si>
+    <t>Registration Client should send a token to Registration processor, when Officer or Supervisor authenticate themselves during Packet Creation</t>
+  </si>
+  <si>
+    <t>Generate packet using centre id and unique machine id</t>
+  </si>
+  <si>
+    <t>Enable registration only when packets pending EoD approval are within configured limits</t>
+  </si>
+  <si>
+    <t>Review with Sasi/Ramesh</t>
+  </si>
+  <si>
+    <t>Review with Sasi/Ramesh
+Email 
+Dated: 28th Mar 2019
+Subject: Detailed out the Suggestions that were Provided by Sasi for Registration Processor</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">&lt;Quote from Mail Dated April 1st &gt;
 “New Approach - MOSIP can collect consent at time of registration to transfer their ID information details to the Social Registry
@@ -5527,74 +5585,40 @@
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
-      <t>If the parent provides the UIN of the child, and the consent for data transfer is provided by child during Registration, then the OTP/Biometrics of the parent has to be authenticated before transferring the data.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Should all the biometric devices  send an NFIQ score or any other quality standards should be adhered to and send in the authentication request?
+      <t>If the parent provides the UIN of the child, and the consent for data transfer is provided by child during Registration, then the OTP/Biometrics of the parent has to be authenticated before transferring the data.
+The question is in reference to the requirement which will be finalised after discussion with Morroco</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Should all the biometric devices  send an NFIQ score or any other quality standards should be adhered to and send in the authentication request?
 2. The intimation is to be triggered for the scenario below: configured number of authentication failure cases consequtively for a UIN and for a configure high NFIQ score. Please confirm
 </t>
-  </si>
-  <si>
-    <t>Currently we are supporting only exact match. What is the high-level business logic when phonetics match will be  invoked?. Do we need to define a set of business rules by which phonetics match will be defined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auth APIs now will be authenticated by Partners using VID only
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>The Question is in reference to version 2 Implementation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Currently we are supporting only exact match. What is the high-level business logic when phonetics match will be  invoked?. Do we need to define a set of business rules by which phonetics match will be defined
 </t>
-  </si>
-  <si>
-    <t>UIN/VID concept is configurable for a country</t>
-  </si>
-  <si>
-    <t>Based on Sasi's inputs, Biometric matching would be independent of type of Biometric device i.e., mantra/cogent, in this case decoupling based on biometric type is not applicable. We will modify current matcher implementation to match using a generic biometric matcher using Biometric Function API provided by Ramesh</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Design/Technical</t>
-  </si>
-  <si>
-    <t>Partner Management Portal</t>
-  </si>
-  <si>
-    <t>Resident Services</t>
-  </si>
-  <si>
-    <t>Admin/Reports</t>
-  </si>
-  <si>
-    <t>For UIN Update of Child, capture the UIN, Name and one biometric of the Parent/Guardian</t>
-  </si>
-  <si>
-    <t>For new registration of child capture any one biometric of the Parent/Guardian</t>
-  </si>
-  <si>
-    <t>Registration Client should send a token to Registration processor, when Officer or Supervisor authenticate themselves during Packet Creation</t>
-  </si>
-  <si>
-    <t>Generate packet using centre id and unique machine id</t>
-  </si>
-  <si>
-    <t>Enable registration only when packets pending EoD approval are within configured limits</t>
-  </si>
-  <si>
-    <t>Review with Sasi/Ramesh</t>
-  </si>
-  <si>
-    <t>Review with Sasi/Ramesh
-Email 
-Dated: 28th Mar 2019
-Subject: Detailed out the Suggestions that were Provided by Sasi for Registration Processor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>The Question is in reference to version 2 Implementation</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6256,6 +6280,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6271,7 +6296,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7480,7 +7504,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7829,12 +7853,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:X174"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A174" sqref="A174"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W177" sqref="W177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7865,30 +7889,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="108"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="109"/>
     </row>
     <row r="2" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -7910,7 +7934,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="H2" s="17" t="s">
         <v>5</v>
@@ -7961,7 +7985,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7981,7 +8005,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>356</v>
@@ -8026,7 +8050,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -8046,7 +8070,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H4" s="32" t="s">
         <v>436</v>
@@ -8090,7 +8114,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8110,7 +8134,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>21</v>
@@ -8155,7 +8179,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -8175,7 +8199,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H6" s="32" t="s">
         <v>441</v>
@@ -8220,7 +8244,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8240,7 +8264,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>23</v>
@@ -8285,7 +8309,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8305,7 +8329,7 @@
         <v>16</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>442</v>
@@ -8350,7 +8374,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8370,7 +8394,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>24</v>
@@ -8413,7 +8437,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -8433,7 +8457,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>444</v>
@@ -8476,7 +8500,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8494,7 +8518,7 @@
         <v>33</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>27</v>
@@ -8533,7 +8557,7 @@
       <c r="U11" s="30"/>
       <c r="V11" s="21"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8591,7 +8615,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8611,7 +8635,7 @@
         <v>33</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H13" s="43" t="s">
         <v>34</v>
@@ -8645,10 +8669,10 @@
       <c r="U13" s="30"/>
       <c r="V13" s="21"/>
       <c r="W13" s="21" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8668,7 +8692,7 @@
         <v>26</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>331</v>
@@ -8712,7 +8736,7 @@
       </c>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -8732,7 +8756,7 @@
         <v>26</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H15" s="51" t="s">
         <v>178</v>
@@ -8778,7 +8802,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -8798,7 +8822,7 @@
         <v>26</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H16" s="51" t="s">
         <v>177</v>
@@ -8844,7 +8868,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -8864,7 +8888,7 @@
         <v>26</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>43</v>
@@ -8910,7 +8934,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -8928,7 +8952,7 @@
         <v>26</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H18" s="42" t="s">
         <v>46</v>
@@ -8974,7 +8998,7 @@
       </c>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -8994,7 +9018,7 @@
         <v>26</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>49</v>
@@ -9040,7 +9064,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -9056,7 +9080,7 @@
         <v>26</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H20" s="45" t="s">
         <v>53</v>
@@ -9092,7 +9116,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -9108,7 +9132,7 @@
         <v>26</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H21" s="42" t="s">
         <v>55</v>
@@ -9144,7 +9168,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -9164,7 +9188,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>58</v>
@@ -9208,7 +9232,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -9228,7 +9252,7 @@
         <v>26</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>348</v>
@@ -9272,7 +9296,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -9292,7 +9316,7 @@
         <v>26</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>59</v>
@@ -9338,7 +9362,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -9356,7 +9380,7 @@
         <v>26</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>64</v>
@@ -9392,7 +9416,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -9410,7 +9434,7 @@
         <v>26</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H26" s="46" t="s">
         <v>65</v>
@@ -9446,7 +9470,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -9466,7 +9490,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H27" s="46" t="s">
         <v>67</v>
@@ -9510,7 +9534,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -9530,7 +9554,7 @@
         <v>26</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H28" s="46" t="s">
         <v>69</v>
@@ -9576,7 +9600,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -9594,7 +9618,7 @@
         <v>26</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H29" s="42" t="s">
         <v>70</v>
@@ -9630,7 +9654,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -9648,7 +9672,7 @@
         <v>26</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="H30" s="47" t="s">
         <v>73</v>
@@ -9690,7 +9714,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -9710,7 +9734,7 @@
         <v>26</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H31" s="46" t="s">
         <v>77</v>
@@ -9756,7 +9780,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -9776,7 +9800,7 @@
         <v>26</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>149</v>
@@ -9822,7 +9846,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -9840,7 +9864,7 @@
         <v>33</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H33" s="46" t="s">
         <v>332</v>
@@ -9884,7 +9908,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -9904,7 +9928,7 @@
         <v>26</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H34" s="46" t="s">
         <v>84</v>
@@ -9950,7 +9974,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -9970,7 +9994,7 @@
         <v>26</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H35" s="48" t="s">
         <v>333</v>
@@ -10031,7 +10055,7 @@
         <v>26</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H36" s="49" t="s">
         <v>89</v>
@@ -10079,7 +10103,7 @@
       </c>
       <c r="W36" s="21"/>
     </row>
-    <row r="37" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="114" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -10099,7 +10123,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H37" s="46" t="s">
         <v>92</v>
@@ -10146,7 +10170,7 @@
         <v>159</v>
       </c>
       <c r="W37" s="21" t="s">
-        <v>580</v>
+        <v>598</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
@@ -10169,7 +10193,7 @@
         <v>26</v>
       </c>
       <c r="G38" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H38" s="46" t="s">
         <v>94</v>
@@ -10237,7 +10261,7 @@
         <v>26</v>
       </c>
       <c r="G39" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H39" s="46" t="s">
         <v>96</v>
@@ -10285,7 +10309,7 @@
       </c>
       <c r="W39" s="21"/>
     </row>
-    <row r="40" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -10305,7 +10329,7 @@
         <v>33</v>
       </c>
       <c r="G40" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H40" s="19" t="s">
         <v>98</v>
@@ -10343,7 +10367,7 @@
       <c r="V40" s="32"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -10363,7 +10387,7 @@
         <v>26</v>
       </c>
       <c r="G41" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H41" s="19" t="s">
         <v>334</v>
@@ -10405,7 +10429,7 @@
       <c r="V41" s="32"/>
       <c r="W41" s="21"/>
     </row>
-    <row r="42" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -10423,7 +10447,7 @@
         <v>33</v>
       </c>
       <c r="G42" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H42" s="19" t="s">
         <v>101</v>
@@ -10463,7 +10487,7 @@
       <c r="V42" s="32"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -10483,7 +10507,7 @@
         <v>26</v>
       </c>
       <c r="G43" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>335</v>
@@ -10525,7 +10549,7 @@
       <c r="V43" s="32"/>
       <c r="W43" s="21"/>
     </row>
-    <row r="44" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -10545,7 +10569,7 @@
         <v>26</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H44" s="19" t="s">
         <v>103</v>
@@ -10589,7 +10613,7 @@
       </c>
       <c r="W44" s="21"/>
     </row>
-    <row r="45" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -10609,7 +10633,7 @@
         <v>33</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H45" s="19" t="s">
         <v>105</v>
@@ -10651,7 +10675,7 @@
       </c>
       <c r="W45" s="21"/>
     </row>
-    <row r="46" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -10671,7 +10695,7 @@
         <v>26</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H46" s="19" t="s">
         <v>106</v>
@@ -10717,7 +10741,7 @@
       </c>
       <c r="W46" s="21"/>
     </row>
-    <row r="47" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -10737,7 +10761,7 @@
         <v>26</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H47" s="19" t="s">
         <v>187</v>
@@ -10783,7 +10807,7 @@
       </c>
       <c r="W47" s="21"/>
     </row>
-    <row r="48" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -10801,7 +10825,7 @@
         <v>26</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H48" s="19" t="s">
         <v>151</v>
@@ -10837,7 +10861,7 @@
       <c r="V48" s="32"/>
       <c r="W48" s="21"/>
     </row>
-    <row r="49" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -10857,7 +10881,7 @@
         <v>26</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H49" s="19" t="s">
         <v>108</v>
@@ -10923,7 +10947,7 @@
         <v>26</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H50" s="19" t="s">
         <v>109</v>
@@ -10970,7 +10994,7 @@
       </c>
       <c r="W50" s="21"/>
     </row>
-    <row r="51" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -10988,7 +11012,7 @@
         <v>33</v>
       </c>
       <c r="G51" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H51" s="19" t="s">
         <v>111</v>
@@ -11028,7 +11052,7 @@
       <c r="V51" s="32"/>
       <c r="W51" s="21"/>
     </row>
-    <row r="52" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -11046,7 +11070,7 @@
         <v>26</v>
       </c>
       <c r="G52" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H52" s="19" t="s">
         <v>112</v>
@@ -11082,7 +11106,7 @@
       <c r="V52" s="32"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -11102,7 +11126,7 @@
         <v>26</v>
       </c>
       <c r="G53" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H53" s="19" t="s">
         <v>114</v>
@@ -11146,7 +11170,7 @@
       </c>
       <c r="W53" s="21"/>
     </row>
-    <row r="54" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -11164,7 +11188,7 @@
         <v>26</v>
       </c>
       <c r="G54" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H54" s="19" t="s">
         <v>116</v>
@@ -11200,7 +11224,7 @@
       <c r="V54" s="32"/>
       <c r="W54" s="21"/>
     </row>
-    <row r="55" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -11218,7 +11242,7 @@
         <v>33</v>
       </c>
       <c r="G55" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H55" s="19" t="s">
         <v>117</v>
@@ -11258,7 +11282,7 @@
       <c r="V55" s="32"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -11278,7 +11302,7 @@
         <v>26</v>
       </c>
       <c r="G56" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H56" s="19" t="s">
         <v>336</v>
@@ -11321,7 +11345,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -11341,7 +11365,7 @@
         <v>26</v>
       </c>
       <c r="G57" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H57" s="19" t="s">
         <v>350</v>
@@ -11384,7 +11408,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11404,7 +11428,7 @@
         <v>26</v>
       </c>
       <c r="G58" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H58" s="19" t="s">
         <v>119</v>
@@ -11448,7 +11472,7 @@
       </c>
       <c r="W58" s="21"/>
     </row>
-    <row r="59" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11466,7 +11490,7 @@
         <v>33</v>
       </c>
       <c r="G59" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H59" s="19" t="s">
         <v>121</v>
@@ -11506,7 +11530,7 @@
       <c r="V59" s="32"/>
       <c r="W59" s="21"/>
     </row>
-    <row r="60" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11524,7 +11548,7 @@
         <v>33</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H60" s="19" t="s">
         <v>122</v>
@@ -11564,7 +11588,7 @@
       <c r="V60" s="32"/>
       <c r="W60" s="21"/>
     </row>
-    <row r="61" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -11584,7 +11608,7 @@
         <v>26</v>
       </c>
       <c r="G61" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H61" s="19" t="s">
         <v>126</v>
@@ -11645,7 +11669,7 @@
         <v>26</v>
       </c>
       <c r="G62" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>127</v>
@@ -11692,7 +11716,7 @@
       </c>
       <c r="W62" s="21"/>
     </row>
-    <row r="63" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -11712,7 +11736,7 @@
         <v>26</v>
       </c>
       <c r="G63" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>129</v>
@@ -11757,7 +11781,7 @@
       </c>
       <c r="W63" s="21"/>
     </row>
-    <row r="64" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11777,7 +11801,7 @@
         <v>33</v>
       </c>
       <c r="G64" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>131</v>
@@ -11812,7 +11836,7 @@
       <c r="V64" s="32"/>
       <c r="W64" s="21"/>
     </row>
-    <row r="65" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11832,7 +11856,7 @@
         <v>33</v>
       </c>
       <c r="G65" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>154</v>
@@ -11887,7 +11911,7 @@
         <v>26</v>
       </c>
       <c r="G66" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>156</v>
@@ -11934,7 +11958,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -11954,7 +11978,7 @@
         <v>26</v>
       </c>
       <c r="G67" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>137</v>
@@ -11998,7 +12022,7 @@
       </c>
       <c r="W67" s="21"/>
     </row>
-    <row r="68" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -12018,7 +12042,7 @@
         <v>26</v>
       </c>
       <c r="G68" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H68" s="19" t="s">
         <v>137</v>
@@ -12063,7 +12087,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -12083,7 +12107,7 @@
         <v>26</v>
       </c>
       <c r="G69" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H69" s="19" t="s">
         <v>142</v>
@@ -12127,7 +12151,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -12147,7 +12171,7 @@
         <v>26</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H70" s="19" t="s">
         <v>337</v>
@@ -12189,7 +12213,7 @@
       <c r="V70" s="32"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -12209,7 +12233,7 @@
         <v>26</v>
       </c>
       <c r="G71" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H71" s="19" t="s">
         <v>338</v>
@@ -12253,7 +12277,7 @@
       </c>
       <c r="W71" s="21"/>
     </row>
-    <row r="72" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -12273,7 +12297,7 @@
         <v>26</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H72" s="19" t="s">
         <v>161</v>
@@ -12319,7 +12343,7 @@
       <c r="W72" s="21"/>
       <c r="X72" s="32"/>
     </row>
-    <row r="73" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -12339,7 +12363,7 @@
         <v>26</v>
       </c>
       <c r="G73" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H73" s="19" t="s">
         <v>162</v>
@@ -12382,7 +12406,7 @@
       <c r="W73" s="21"/>
       <c r="X73" s="28"/>
     </row>
-    <row r="74" spans="1:24" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12400,7 +12424,7 @@
         <v>33</v>
       </c>
       <c r="G74" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H74" s="32" t="s">
         <v>167</v>
@@ -12440,7 +12464,7 @@
       <c r="W74" s="21"/>
       <c r="X74" s="32"/>
     </row>
-    <row r="75" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -12460,7 +12484,7 @@
         <v>26</v>
       </c>
       <c r="G75" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>169</v>
@@ -12505,7 +12529,7 @@
       </c>
       <c r="W75" s="21"/>
     </row>
-    <row r="76" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -12525,7 +12549,7 @@
         <v>26</v>
       </c>
       <c r="G76" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H76" s="32" t="s">
         <v>172</v>
@@ -12570,7 +12594,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -12590,7 +12614,7 @@
         <v>26</v>
       </c>
       <c r="G77" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H77" s="32" t="s">
         <v>355</v>
@@ -12634,7 +12658,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -12654,7 +12678,7 @@
         <v>26</v>
       </c>
       <c r="G78" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H78" s="32" t="s">
         <v>440</v>
@@ -12699,7 +12723,7 @@
       <c r="W78" s="21"/>
       <c r="X78" s="32"/>
     </row>
-    <row r="79" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -12719,7 +12743,7 @@
         <v>26</v>
       </c>
       <c r="G79" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H79" s="32" t="s">
         <v>339</v>
@@ -12762,7 +12786,7 @@
       <c r="W79" s="21"/>
       <c r="X79" s="32"/>
     </row>
-    <row r="80" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -12782,7 +12806,7 @@
         <v>26</v>
       </c>
       <c r="G80" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H80" s="32" t="s">
         <v>189</v>
@@ -12827,7 +12851,7 @@
       <c r="W80" s="21"/>
       <c r="X80" s="32"/>
     </row>
-    <row r="81" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -12847,7 +12871,7 @@
         <v>26</v>
       </c>
       <c r="G81" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H81" s="32" t="s">
         <v>342</v>
@@ -12890,7 +12914,7 @@
       <c r="W81" s="21"/>
       <c r="X81" s="32"/>
     </row>
-    <row r="82" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -12910,7 +12934,7 @@
         <v>26</v>
       </c>
       <c r="G82" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H82" s="32" t="s">
         <v>379</v>
@@ -12955,7 +12979,7 @@
       <c r="W82" s="21"/>
       <c r="X82" s="32"/>
     </row>
-    <row r="83" spans="1:24" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -12973,7 +12997,7 @@
         <v>33</v>
       </c>
       <c r="G83" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H83" s="19" t="s">
         <v>213</v>
@@ -13018,7 +13042,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="228" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="228" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -13038,7 +13062,7 @@
         <v>26</v>
       </c>
       <c r="G84" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H84" s="32" t="s">
         <v>449</v>
@@ -13083,7 +13107,7 @@
       <c r="W84" s="21"/>
       <c r="X84" s="32"/>
     </row>
-    <row r="85" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -13103,7 +13127,7 @@
         <v>26</v>
       </c>
       <c r="G85" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H85" s="19" t="s">
         <v>214</v>
@@ -13149,7 +13173,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -13169,7 +13193,7 @@
         <v>26</v>
       </c>
       <c r="G86" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H86" s="32" t="s">
         <v>215</v>
@@ -13213,7 +13237,7 @@
       <c r="V86" s="32"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -13233,7 +13257,7 @@
         <v>26</v>
       </c>
       <c r="G87" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H87" s="32" t="s">
         <v>216</v>
@@ -13296,7 +13320,7 @@
         <v>26</v>
       </c>
       <c r="G88" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H88" s="32" t="s">
         <v>217</v>
@@ -13341,7 +13365,7 @@
       </c>
       <c r="W88" s="21"/>
     </row>
-    <row r="89" spans="1:24" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -13361,7 +13385,7 @@
         <v>26</v>
       </c>
       <c r="G89" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H89" s="32" t="s">
         <v>224</v>
@@ -13399,10 +13423,10 @@
         <v>269</v>
       </c>
       <c r="W89" s="21" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -13420,7 +13444,7 @@
         <v>26</v>
       </c>
       <c r="G90" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H90" s="32" t="s">
         <v>218</v>
@@ -13455,7 +13479,7 @@
       <c r="V90" s="32"/>
       <c r="W90" s="21"/>
     </row>
-    <row r="91" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -13473,7 +13497,7 @@
         <v>26</v>
       </c>
       <c r="G91" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H91" s="32" t="s">
         <v>219</v>
@@ -13506,7 +13530,7 @@
       <c r="V91" s="32"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="171" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="171" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -13526,7 +13550,7 @@
         <v>26</v>
       </c>
       <c r="G92" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H92" s="32" t="s">
         <v>226</v>
@@ -13570,7 +13594,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -13590,7 +13614,7 @@
         <v>26</v>
       </c>
       <c r="G93" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H93" s="32" t="s">
         <v>320</v>
@@ -13632,7 +13656,7 @@
       <c r="V93" s="32"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -13652,7 +13676,7 @@
         <v>26</v>
       </c>
       <c r="G94" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H94" s="32" t="s">
         <v>319</v>
@@ -13696,7 +13720,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -13716,7 +13740,7 @@
         <v>26</v>
       </c>
       <c r="G95" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H95" s="32" t="s">
         <v>351</v>
@@ -13760,7 +13784,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -13780,7 +13804,7 @@
         <v>26</v>
       </c>
       <c r="G96" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H96" s="32" t="s">
         <v>352</v>
@@ -13824,7 +13848,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -13844,7 +13868,7 @@
         <v>26</v>
       </c>
       <c r="G97" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H97" s="32" t="s">
         <v>353</v>
@@ -13886,7 +13910,7 @@
       <c r="V97" s="32"/>
       <c r="W97" s="21"/>
     </row>
-    <row r="98" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -13906,7 +13930,7 @@
         <v>26</v>
       </c>
       <c r="G98" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H98" s="32" t="s">
         <v>318</v>
@@ -13941,7 +13965,7 @@
       <c r="V98" s="32"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -13961,7 +13985,7 @@
         <v>26</v>
       </c>
       <c r="G99" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H99" s="32" t="s">
         <v>340</v>
@@ -14003,7 +14027,7 @@
       <c r="V99" s="32"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -14023,7 +14047,7 @@
         <v>26</v>
       </c>
       <c r="G100" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H100" s="32" t="s">
         <v>343</v>
@@ -14067,7 +14091,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" ht="299.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -14087,7 +14111,7 @@
         <v>26</v>
       </c>
       <c r="G101" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H101" s="32" t="s">
         <v>316</v>
@@ -14131,7 +14155,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -14151,7 +14175,7 @@
         <v>26</v>
       </c>
       <c r="G102" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H102" s="32" t="s">
         <v>317</v>
@@ -14193,7 +14217,7 @@
       <c r="V102" s="32"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -14213,7 +14237,7 @@
         <v>26</v>
       </c>
       <c r="G103" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H103" s="32" t="s">
         <v>315</v>
@@ -14257,7 +14281,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -14277,7 +14301,7 @@
         <v>26</v>
       </c>
       <c r="G104" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H104" s="32" t="s">
         <v>447</v>
@@ -14341,7 +14365,7 @@
         <v>26</v>
       </c>
       <c r="G105" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H105" s="74" t="s">
         <v>246</v>
@@ -14404,7 +14428,7 @@
         <v>26</v>
       </c>
       <c r="G106" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H106" s="32" t="s">
         <v>266</v>
@@ -14447,7 +14471,7 @@
       </c>
       <c r="W106" s="21"/>
     </row>
-    <row r="107" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -14467,7 +14491,7 @@
         <v>26</v>
       </c>
       <c r="G107" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H107" s="32" t="s">
         <v>272</v>
@@ -14502,7 +14526,7 @@
       <c r="V107" s="32"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -14522,7 +14546,7 @@
         <v>26</v>
       </c>
       <c r="G108" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H108" s="32" t="s">
         <v>273</v>
@@ -14565,7 +14589,7 @@
       </c>
       <c r="W108" s="21"/>
     </row>
-    <row r="109" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -14585,7 +14609,7 @@
         <v>26</v>
       </c>
       <c r="G109" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H109" s="32" t="s">
         <v>321</v>
@@ -14624,7 +14648,7 @@
       <c r="V109" s="32"/>
       <c r="W109" s="21"/>
     </row>
-    <row r="110" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>108</v>
       </c>
@@ -14644,7 +14668,7 @@
         <v>26</v>
       </c>
       <c r="G110" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H110" s="32" t="s">
         <v>322</v>
@@ -14683,7 +14707,7 @@
       <c r="V110" s="32"/>
       <c r="W110" s="21"/>
     </row>
-    <row r="111" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -14703,7 +14727,7 @@
         <v>26</v>
       </c>
       <c r="G111" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H111" s="32" t="s">
         <v>323</v>
@@ -14744,7 +14768,7 @@
       <c r="V111" s="32"/>
       <c r="W111" s="21"/>
     </row>
-    <row r="112" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -14764,7 +14788,7 @@
         <v>26</v>
       </c>
       <c r="G112" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H112" s="32" t="s">
         <v>324</v>
@@ -14805,7 +14829,7 @@
       <c r="V112" s="32"/>
       <c r="W112" s="21"/>
     </row>
-    <row r="113" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -14825,7 +14849,7 @@
         <v>26</v>
       </c>
       <c r="G113" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H113" s="32" t="s">
         <v>325</v>
@@ -14866,7 +14890,7 @@
       <c r="V113" s="32"/>
       <c r="W113" s="21"/>
     </row>
-    <row r="114" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -14886,7 +14910,7 @@
         <v>26</v>
       </c>
       <c r="G114" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H114" s="32" t="s">
         <v>326</v>
@@ -14927,7 +14951,7 @@
       <c r="V114" s="32"/>
       <c r="W114" s="21"/>
     </row>
-    <row r="115" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -14947,7 +14971,7 @@
         <v>26</v>
       </c>
       <c r="G115" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H115" s="32" t="s">
         <v>327</v>
@@ -14986,7 +15010,7 @@
       <c r="V115" s="32"/>
       <c r="W115" s="21"/>
     </row>
-    <row r="116" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -15006,7 +15030,7 @@
         <v>26</v>
       </c>
       <c r="G116" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H116" s="32" t="s">
         <v>416</v>
@@ -15036,7 +15060,7 @@
       <c r="V116" s="32"/>
       <c r="W116" s="21"/>
     </row>
-    <row r="117" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -15056,7 +15080,7 @@
         <v>26</v>
       </c>
       <c r="G117" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H117" s="28" t="s">
         <v>419</v>
@@ -15088,7 +15112,7 @@
       <c r="V117" s="28"/>
       <c r="W117" s="21"/>
     </row>
-    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -15108,7 +15132,7 @@
         <v>26</v>
       </c>
       <c r="G118" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H118" s="32" t="s">
         <v>427</v>
@@ -15143,7 +15167,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -15163,7 +15187,7 @@
         <v>26</v>
       </c>
       <c r="G119" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H119" s="32" t="s">
         <v>427</v>
@@ -15218,7 +15242,7 @@
         <v>26</v>
       </c>
       <c r="G120" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H120" s="32" t="s">
         <v>450</v>
@@ -15269,10 +15293,10 @@
         <v>26</v>
       </c>
       <c r="G121" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H121" s="32" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I121" s="14"/>
       <c r="J121" s="32" t="s">
@@ -15298,11 +15322,11 @@
       <c r="T121" s="14"/>
       <c r="U121" s="5"/>
       <c r="V121" s="32" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -15322,7 +15346,7 @@
         <v>26</v>
       </c>
       <c r="G122" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H122" s="32" t="s">
         <v>454</v>
@@ -15359,7 +15383,7 @@
       <c r="V122" s="32"/>
       <c r="W122" s="21"/>
     </row>
-    <row r="123" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>121</v>
       </c>
@@ -15377,7 +15401,7 @@
         <v>26</v>
       </c>
       <c r="G123" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H123" s="32" t="s">
         <v>454</v>
@@ -15408,7 +15432,7 @@
       <c r="V123" s="32"/>
       <c r="W123" s="21"/>
     </row>
-    <row r="124" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -15428,7 +15452,7 @@
         <v>26</v>
       </c>
       <c r="G124" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H124" s="32" t="s">
         <v>456</v>
@@ -15459,7 +15483,7 @@
       <c r="V124" s="32"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -15479,7 +15503,7 @@
         <v>26</v>
       </c>
       <c r="G125" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H125" s="32" t="s">
         <v>458</v>
@@ -15507,7 +15531,7 @@
       <c r="V125" s="32"/>
       <c r="W125" s="21"/>
     </row>
-    <row r="126" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -15527,7 +15551,7 @@
         <v>26</v>
       </c>
       <c r="G126" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>478</v>
@@ -15560,7 +15584,7 @@
       </c>
       <c r="W126" s="21"/>
     </row>
-    <row r="127" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -15580,7 +15604,7 @@
         <v>26</v>
       </c>
       <c r="G127" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H127" s="28" t="s">
         <v>482</v>
@@ -15614,7 +15638,7 @@
       </c>
       <c r="W127" s="21"/>
     </row>
-    <row r="128" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -15634,7 +15658,7 @@
         <v>26</v>
       </c>
       <c r="G128" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H128" s="32" t="s">
         <v>484</v>
@@ -15666,7 +15690,7 @@
       <c r="V128" s="32"/>
       <c r="W128" s="21"/>
     </row>
-    <row r="129" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -15686,7 +15710,7 @@
         <v>26</v>
       </c>
       <c r="G129" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H129" s="32" t="s">
         <v>486</v>
@@ -15718,7 +15742,7 @@
       <c r="V129" s="32"/>
       <c r="W129" s="21"/>
     </row>
-    <row r="130" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -15738,7 +15762,7 @@
         <v>26</v>
       </c>
       <c r="G130" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H130" s="32" t="s">
         <v>488</v>
@@ -15770,7 +15794,7 @@
       <c r="V130" s="32"/>
       <c r="W130" s="21"/>
     </row>
-    <row r="131" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -15790,7 +15814,7 @@
         <v>26</v>
       </c>
       <c r="G131" s="28" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H131" s="32" t="s">
         <v>489</v>
@@ -15842,7 +15866,7 @@
         <v>26</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H132" s="32" t="s">
         <v>499</v>
@@ -15872,10 +15896,10 @@
       <c r="U132" s="32"/>
       <c r="V132" s="33"/>
       <c r="W132" s="21" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="133" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>131</v>
       </c>
@@ -15884,7 +15908,7 @@
         <v>43552</v>
       </c>
       <c r="D133" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E133" s="32" t="s">
         <v>39</v>
@@ -15893,7 +15917,7 @@
         <v>26</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H133" s="32" t="s">
         <v>502</v>
@@ -15924,7 +15948,7 @@
       <c r="V133" s="33"/>
       <c r="W133" s="21"/>
     </row>
-    <row r="134" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="270.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>132</v>
       </c>
@@ -15933,7 +15957,7 @@
         <v>43552</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E134" s="32" t="s">
         <v>39</v>
@@ -15942,7 +15966,7 @@
         <v>26</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H134" s="32" t="s">
         <v>503</v>
@@ -15973,7 +15997,7 @@
       <c r="V134" s="33"/>
       <c r="W134" s="21"/>
     </row>
-    <row r="135" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>133</v>
       </c>
@@ -15982,7 +16006,7 @@
         <v>43552</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E135" s="32" t="s">
         <v>39</v>
@@ -15991,7 +16015,7 @@
         <v>26</v>
       </c>
       <c r="G135" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H135" s="32" t="s">
         <v>504</v>
@@ -16022,7 +16046,7 @@
       <c r="V135" s="33"/>
       <c r="W135" s="21"/>
     </row>
-    <row r="136" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>134</v>
       </c>
@@ -16031,7 +16055,7 @@
         <v>43552</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E136" s="32" t="s">
         <v>39</v>
@@ -16040,7 +16064,7 @@
         <v>26</v>
       </c>
       <c r="G136" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H136" s="32" t="s">
         <v>505</v>
@@ -16071,7 +16095,7 @@
       <c r="V136" s="33"/>
       <c r="W136" s="21"/>
     </row>
-    <row r="137" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>135</v>
       </c>
@@ -16080,7 +16104,7 @@
         <v>43552</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E137" s="32" t="s">
         <v>39</v>
@@ -16089,7 +16113,7 @@
         <v>26</v>
       </c>
       <c r="G137" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H137" s="32" t="s">
         <v>506</v>
@@ -16120,7 +16144,7 @@
       <c r="V137" s="33"/>
       <c r="W137" s="21"/>
     </row>
-    <row r="138" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>136</v>
       </c>
@@ -16129,7 +16153,7 @@
         <v>43552</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E138" s="32" t="s">
         <v>39</v>
@@ -16138,7 +16162,7 @@
         <v>26</v>
       </c>
       <c r="G138" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H138" s="32" t="s">
         <v>507</v>
@@ -16169,7 +16193,7 @@
       <c r="V138" s="33"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>137</v>
       </c>
@@ -16178,7 +16202,7 @@
         <v>43552</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E139" s="32" t="s">
         <v>39</v>
@@ -16187,7 +16211,7 @@
         <v>26</v>
       </c>
       <c r="G139" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H139" s="32" t="s">
         <v>508</v>
@@ -16218,7 +16242,7 @@
       <c r="V139" s="33"/>
       <c r="W139" s="21"/>
     </row>
-    <row r="140" spans="1:23" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>138</v>
       </c>
@@ -16227,7 +16251,7 @@
         <v>43552</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E140" s="32" t="s">
         <v>39</v>
@@ -16236,7 +16260,7 @@
         <v>26</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H140" s="32" t="s">
         <v>509</v>
@@ -16267,7 +16291,7 @@
       <c r="V140" s="33"/>
       <c r="W140" s="21"/>
     </row>
-    <row r="141" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -16276,7 +16300,7 @@
         <v>43552</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E141" s="32" t="s">
         <v>39</v>
@@ -16285,7 +16309,7 @@
         <v>26</v>
       </c>
       <c r="G141" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H141" s="32" t="s">
         <v>511</v>
@@ -16316,7 +16340,7 @@
       <c r="V141" s="33"/>
       <c r="W141" s="21"/>
     </row>
-    <row r="142" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>140</v>
       </c>
@@ -16325,7 +16349,7 @@
         <v>43552</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E142" s="32" t="s">
         <v>39</v>
@@ -16334,7 +16358,7 @@
         <v>26</v>
       </c>
       <c r="G142" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H142" s="32" t="s">
         <v>512</v>
@@ -16365,7 +16389,7 @@
       <c r="V142" s="33"/>
       <c r="W142" s="21"/>
     </row>
-    <row r="143" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>141</v>
       </c>
@@ -16374,7 +16398,7 @@
         <v>43552</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E143" s="32" t="s">
         <v>39</v>
@@ -16383,7 +16407,7 @@
         <v>26</v>
       </c>
       <c r="G143" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H143" s="32" t="s">
         <v>513</v>
@@ -16414,7 +16438,7 @@
       <c r="V143" s="33"/>
       <c r="W143" s="21"/>
     </row>
-    <row r="144" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>142</v>
       </c>
@@ -16423,7 +16447,7 @@
         <v>43552</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E144" s="32" t="s">
         <v>211</v>
@@ -16432,7 +16456,7 @@
         <v>26</v>
       </c>
       <c r="G144" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H144" s="32" t="s">
         <v>515</v>
@@ -16463,7 +16487,7 @@
       <c r="V144" s="33"/>
       <c r="W144" s="21"/>
     </row>
-    <row r="145" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>143</v>
       </c>
@@ -16472,7 +16496,7 @@
         <v>43552</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E145" s="32" t="s">
         <v>211</v>
@@ -16481,7 +16505,7 @@
         <v>26</v>
       </c>
       <c r="G145" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H145" s="32" t="s">
         <v>514</v>
@@ -16512,7 +16536,7 @@
       <c r="V145" s="33"/>
       <c r="W145" s="21"/>
     </row>
-    <row r="146" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>144</v>
       </c>
@@ -16521,7 +16545,7 @@
         <v>43552</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E146" s="32" t="s">
         <v>39</v>
@@ -16530,7 +16554,7 @@
         <v>26</v>
       </c>
       <c r="G146" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H146" s="32" t="s">
         <v>516</v>
@@ -16561,7 +16585,7 @@
       <c r="V146" s="33"/>
       <c r="W146" s="21"/>
     </row>
-    <row r="147" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>145</v>
       </c>
@@ -16570,7 +16594,7 @@
         <v>43552</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E147" s="28" t="s">
         <v>39</v>
@@ -16579,7 +16603,7 @@
         <v>26</v>
       </c>
       <c r="G147" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H147" s="28" t="s">
         <v>517</v>
@@ -16610,7 +16634,7 @@
       <c r="V147" s="87"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -16621,7 +16645,7 @@
         <v>43553</v>
       </c>
       <c r="D148" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E148" s="32" t="s">
         <v>15</v>
@@ -16630,7 +16654,7 @@
         <v>26</v>
       </c>
       <c r="G148" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H148" s="32" t="s">
         <v>523</v>
@@ -16663,7 +16687,7 @@
       <c r="V148" s="32"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -16674,7 +16698,7 @@
         <v>43553</v>
       </c>
       <c r="D149" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E149" s="32" t="s">
         <v>15</v>
@@ -16683,10 +16707,10 @@
         <v>26</v>
       </c>
       <c r="G149" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H149" s="32" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="J149" s="32"/>
       <c r="K149" s="32"/>
@@ -16716,7 +16740,7 @@
       <c r="V149" s="32"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -16727,7 +16751,7 @@
         <v>43553</v>
       </c>
       <c r="D150" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E150" s="32" t="s">
         <v>15</v>
@@ -16736,10 +16760,10 @@
         <v>26</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H150" s="32" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="J150" s="32"/>
       <c r="K150" s="32"/>
@@ -16766,7 +16790,7 @@
       <c r="V150" s="32"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -16777,7 +16801,7 @@
         <v>43553</v>
       </c>
       <c r="D151" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E151" s="32" t="s">
         <v>15</v>
@@ -16786,10 +16810,10 @@
         <v>26</v>
       </c>
       <c r="G151" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H151" s="32" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J151" s="32"/>
       <c r="K151" s="32"/>
@@ -16813,7 +16837,7 @@
       <c r="V151" s="32"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -16824,7 +16848,7 @@
         <v>43553</v>
       </c>
       <c r="D152" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E152" s="32" t="s">
         <v>15</v>
@@ -16833,10 +16857,10 @@
         <v>26</v>
       </c>
       <c r="G152" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H152" s="32" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="J152" s="32"/>
       <c r="K152" s="32"/>
@@ -16877,7 +16901,7 @@
         <v>43550</v>
       </c>
       <c r="D153" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E153" s="32" t="s">
         <v>32</v>
@@ -16886,7 +16910,7 @@
         <v>26</v>
       </c>
       <c r="G153" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H153" s="32" t="s">
         <v>525</v>
@@ -16926,7 +16950,7 @@
         <v>43550</v>
       </c>
       <c r="D154" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E154" s="32" t="s">
         <v>32</v>
@@ -16935,7 +16959,7 @@
         <v>26</v>
       </c>
       <c r="G154" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H154" s="32" t="s">
         <v>527</v>
@@ -16975,7 +16999,7 @@
         <v>43550</v>
       </c>
       <c r="D155" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E155" s="32" t="s">
         <v>32</v>
@@ -16984,7 +17008,7 @@
         <v>26</v>
       </c>
       <c r="G155" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H155" s="32" t="s">
         <v>529</v>
@@ -17033,7 +17057,7 @@
         <v>26</v>
       </c>
       <c r="G156" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H156" s="32" t="s">
         <v>531</v>
@@ -17082,7 +17106,7 @@
         <v>26</v>
       </c>
       <c r="G157" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H157" s="32" t="s">
         <v>534</v>
@@ -17111,7 +17135,7 @@
       <c r="V157" s="32"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -17131,7 +17155,7 @@
         <v>26</v>
       </c>
       <c r="G158" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H158" s="32" t="s">
         <v>540</v>
@@ -17165,7 +17189,7 @@
       <c r="V158" s="32"/>
       <c r="W158" s="33"/>
     </row>
-    <row r="159" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" ht="228" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -17185,7 +17209,7 @@
         <v>26</v>
       </c>
       <c r="G159" s="32" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H159" s="32" t="s">
         <v>568</v>
@@ -17219,7 +17243,7 @@
       <c r="V159" s="32"/>
       <c r="W159" s="33"/>
     </row>
-    <row r="160" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -17239,10 +17263,10 @@
         <v>26</v>
       </c>
       <c r="G160" s="28" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H160" s="28" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="J160" s="28"/>
       <c r="K160" s="28"/>
@@ -17270,7 +17294,7 @@
       <c r="V160" s="28"/>
       <c r="W160" s="33"/>
     </row>
-    <row r="161" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>159</v>
       </c>
@@ -17281,7 +17305,7 @@
         <v>43542</v>
       </c>
       <c r="D161" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E161" s="32" t="s">
         <v>80</v>
@@ -17290,7 +17314,7 @@
         <v>26</v>
       </c>
       <c r="G161" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H161" s="32" t="s">
         <v>557</v>
@@ -17325,7 +17349,7 @@
       <c r="V161" s="32"/>
       <c r="W161" s="33"/>
     </row>
-    <row r="162" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>160</v>
       </c>
@@ -17336,7 +17360,7 @@
         <v>43542</v>
       </c>
       <c r="D162" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E162" s="32" t="s">
         <v>80</v>
@@ -17345,7 +17369,7 @@
         <v>26</v>
       </c>
       <c r="G162" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H162" s="32" t="s">
         <v>558</v>
@@ -17380,7 +17404,7 @@
       <c r="V162" s="32"/>
       <c r="W162" s="33"/>
     </row>
-    <row r="163" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
         <v>161</v>
       </c>
@@ -17391,7 +17415,7 @@
         <v>43542</v>
       </c>
       <c r="D163" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E163" s="32" t="s">
         <v>80</v>
@@ -17400,7 +17424,7 @@
         <v>26</v>
       </c>
       <c r="G163" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H163" s="32" t="s">
         <v>559</v>
@@ -17435,7 +17459,7 @@
       <c r="V163" s="32"/>
       <c r="W163" s="33"/>
     </row>
-    <row r="164" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>162</v>
       </c>
@@ -17446,7 +17470,7 @@
         <v>43542</v>
       </c>
       <c r="D164" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E164" s="32" t="s">
         <v>80</v>
@@ -17455,7 +17479,7 @@
         <v>26</v>
       </c>
       <c r="G164" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H164" s="32" t="s">
         <v>560</v>
@@ -17490,7 +17514,7 @@
       <c r="V164" s="32"/>
       <c r="W164" s="33"/>
     </row>
-    <row r="165" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>163</v>
       </c>
@@ -17501,7 +17525,7 @@
         <v>43542</v>
       </c>
       <c r="D165" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E165" s="32" t="s">
         <v>80</v>
@@ -17510,7 +17534,7 @@
         <v>26</v>
       </c>
       <c r="G165" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H165" s="32" t="s">
         <v>561</v>
@@ -17545,7 +17569,7 @@
       <c r="V165" s="32"/>
       <c r="W165" s="33"/>
     </row>
-    <row r="166" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>164</v>
       </c>
@@ -17556,7 +17580,7 @@
         <v>43542</v>
       </c>
       <c r="D166" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E166" s="32" t="s">
         <v>80</v>
@@ -17565,7 +17589,7 @@
         <v>26</v>
       </c>
       <c r="G166" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H166" s="32" t="s">
         <v>562</v>
@@ -17600,7 +17624,7 @@
       <c r="V166" s="32"/>
       <c r="W166" s="33"/>
     </row>
-    <row r="167" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>165</v>
       </c>
@@ -17611,7 +17635,7 @@
         <v>43542</v>
       </c>
       <c r="D167" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E167" s="32" t="s">
         <v>80</v>
@@ -17620,7 +17644,7 @@
         <v>26</v>
       </c>
       <c r="G167" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H167" s="32" t="s">
         <v>563</v>
@@ -17655,7 +17679,7 @@
       <c r="V167" s="32"/>
       <c r="W167" s="33"/>
     </row>
-    <row r="168" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>166</v>
       </c>
@@ -17666,7 +17690,7 @@
         <v>43542</v>
       </c>
       <c r="D168" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E168" s="32" t="s">
         <v>80</v>
@@ -17675,7 +17699,7 @@
         <v>26</v>
       </c>
       <c r="G168" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H168" s="32" t="s">
         <v>564</v>
@@ -17710,7 +17734,7 @@
       <c r="V168" s="32"/>
       <c r="W168" s="33"/>
     </row>
-    <row r="169" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>167</v>
       </c>
@@ -17721,7 +17745,7 @@
         <v>43542</v>
       </c>
       <c r="D169" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E169" s="32" t="s">
         <v>80</v>
@@ -17730,7 +17754,7 @@
         <v>26</v>
       </c>
       <c r="G169" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H169" s="32" t="s">
         <v>565</v>
@@ -17765,7 +17789,7 @@
       <c r="V169" s="32"/>
       <c r="W169" s="33"/>
     </row>
-    <row r="170" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>168</v>
       </c>
@@ -17776,7 +17800,7 @@
         <v>43542</v>
       </c>
       <c r="D170" s="32" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E170" s="32" t="s">
         <v>80</v>
@@ -17785,7 +17809,7 @@
         <v>26</v>
       </c>
       <c r="G170" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H170" s="32" t="s">
         <v>566</v>
@@ -17820,7 +17844,7 @@
       <c r="V170" s="32"/>
       <c r="W170" s="33"/>
     </row>
-    <row r="171" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" s="103" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>169</v>
       </c>
@@ -17838,7 +17862,7 @@
         <v>26</v>
       </c>
       <c r="G171" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H171" s="32" t="s">
         <v>572</v>
@@ -17865,9 +17889,9 @@
       <c r="T171" s="33"/>
       <c r="U171" s="5"/>
       <c r="V171" s="14"/>
-      <c r="W171" s="109"/>
-    </row>
-    <row r="172" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="W171" s="104"/>
+    </row>
+    <row r="172" spans="1:23" s="103" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>170</v>
       </c>
@@ -17887,7 +17911,7 @@
         <v>26</v>
       </c>
       <c r="G172" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H172" s="32" t="s">
         <v>573</v>
@@ -17920,9 +17944,9 @@
         <v>10</v>
       </c>
       <c r="V172" s="14"/>
-      <c r="W172" s="109"/>
-    </row>
-    <row r="173" spans="1:23" s="103" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+      <c r="W172" s="104"/>
+    </row>
+    <row r="173" spans="1:23" s="103" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>171</v>
       </c>
@@ -17940,7 +17964,7 @@
         <v>26</v>
       </c>
       <c r="G173" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H173" s="32" t="s">
         <v>571</v>
@@ -17967,9 +17991,9 @@
       <c r="T173" s="33"/>
       <c r="U173" s="5"/>
       <c r="V173" s="14"/>
-      <c r="W173" s="109"/>
-    </row>
-    <row r="174" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+      <c r="W173" s="104"/>
+    </row>
+    <row r="174" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>172</v>
       </c>
@@ -17987,7 +18011,7 @@
         <v>26</v>
       </c>
       <c r="G174" s="14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H174" s="32" t="s">
         <v>574</v>
@@ -18015,6 +18039,13 @@
       <c r="W174" s="33"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:X174" xr:uid="{6C8A7F8F-6E5A-48C3-B40D-B34E2585C37A}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="ID Authentication"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
@@ -18065,7 +18096,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -18073,7 +18104,7 @@
         <v>80</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -18081,7 +18112,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -18089,7 +18120,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -18106,19 +18137,19 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -18295,6 +18326,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18466,15 +18506,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -18499,6 +18530,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18512,14 +18551,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added new UI feedback changes
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6EFB36EC-3A66-49D2-8F07-C706B7A6E519}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,9 +20,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$X$174</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="634">
   <si>
     <t>S.No.</t>
   </si>
@@ -5620,15 +5619,477 @@
       <t>The Question is in reference to version 2 Implementation</t>
     </r>
   </si>
+  <si>
+    <t>Sprint 9 demo on 2/4/2019</t>
+  </si>
+  <si>
+    <t>MOS 21860</t>
+  </si>
+  <si>
+    <t>MOS 21861</t>
+  </si>
+  <si>
+    <t>MOS 21863</t>
+  </si>
+  <si>
+    <t>MOS 21870</t>
+  </si>
+  <si>
+    <t>MOS 21873</t>
+  </si>
+  <si>
+    <t>MOS 21887</t>
+  </si>
+  <si>
+    <t>MOS-21888</t>
+  </si>
+  <si>
+    <t>MOS-21897</t>
+  </si>
+  <si>
+    <t>MOS-21920</t>
+  </si>
+  <si>
+    <t>MOS-21921</t>
+  </si>
+  <si>
+    <t>MOS-21922</t>
+  </si>
+  <si>
+    <t>MOS-21923</t>
+  </si>
+  <si>
+    <t>MOS-21924</t>
+  </si>
+  <si>
+    <t>MOS-21926</t>
+  </si>
+  <si>
+    <t>MOS-21927</t>
+  </si>
+  <si>
+    <t>MOS-21928</t>
+  </si>
+  <si>
+    <t>MOS-21929</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Transliteration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+The virtual keyboard icon is repeated three times. Can we make it appear in just one place? </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+The address is too spaced out. Utilize the space better. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Demographic fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Should age, date of birth, phone number and email be displayed twice, considering RHS is not editable?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Optimize the vertical scroll bar—keep it as minimum as possible.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Explore the option of having the exception marking on the same screen as the document upload. Utilize the space on the right.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Fingerprint exception marking to be more intuitive. Do not colour the entire finger. The exception fingers should to be crossed out.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Morocco screens will have iris exception only. Create a new screen with iris exceptions aligned better.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+RO should be able to go back and forth between demographic, document and biometric screens. Retain the captured data in each screen. For biometrics - retain data whenever possible i.e. for those biometrics not marked as exceptions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Biometric screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+a. 'Start Over/Reset' buttons: what happens on click? Revisit the flow.
+b. 'Scan' button - instead of having the button at the bottom, provide a scan icon on the slap image itself for each biometric.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+a. RHS progress bar - can we make them links? Implement if feasible. User should be able to jump to any page using RHS and top navigation links.
+b. Validations - all validations should happen on the preview page when user tries to submit. Display a consolidated error message highlighting which pages have errors. User should be able to jump to the page having errors, make the changes and jump back to preview</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - consent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+The consent feature is under discussion. It could result in additional attributes for seeking consent.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Acknowledgement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+The acknowledgement printout should fit on half an A4 page. Hence on click of print, mirror it and print two copies on a single A4 sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New Registration - Acknowledgement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+The QR code should have only the RID. Remove the other details such as demographics and photo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Re-register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Rename 'Re-register' to 'Notification for Re-registration'. This should be done on the home page and the Re-register page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Upload packet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+Provide a search feature for the lsit of packets on the upload page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+There are navigation links at the top of the new reg. screen. Can we make them clickable? User should be able to navigate to the screens in any order.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Age/Date of Birth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+If we enter age, the DoB should display 01/Jan/xxxx. 
+If we enter DoB, the age should be auto calculated and displayed. 
+Both fields should remain editable.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5739,6 +6200,14 @@
       <color rgb="FF0070C0"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -5985,7 +6454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6296,6 +6765,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6326,7 +6798,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6343,7 +6815,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:V70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -7504,7 +7976,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -7852,43 +8324,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:X174"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:X192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W177" sqref="W177"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="3" customWidth="1"/>
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" style="3" customWidth="1"/>
     <col min="12" max="12" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="22.81640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="51.5703125" style="10" customWidth="1"/>
-    <col min="24" max="16384" width="20.42578125" style="10"/>
+    <col min="17" max="17" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="51.54296875" style="10" customWidth="1"/>
+    <col min="24" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="105" t="s">
         <v>208</v>
       </c>
@@ -7914,7 +8386,7 @@
       <c r="U1" s="107"/>
       <c r="V1" s="109"/>
     </row>
-    <row r="2" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7985,7 +8457,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8050,7 +8522,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -8114,7 +8586,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8179,7 +8651,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -8244,7 +8716,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8309,7 +8781,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8374,7 +8846,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8437,7 +8909,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -8500,7 +8972,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -8557,7 +9029,7 @@
       <c r="U11" s="30"/>
       <c r="V11" s="21"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -8615,7 +9087,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -8672,7 +9144,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -8736,7 +9208,7 @@
       </c>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -8802,7 +9274,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -8868,7 +9340,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -8934,7 +9406,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -8998,7 +9470,7 @@
       </c>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -9064,7 +9536,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -9116,7 +9588,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -9168,7 +9640,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -9232,7 +9704,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -9296,7 +9768,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -9362,7 +9834,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -9416,7 +9888,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -9470,7 +9942,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -9534,7 +10006,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -9600,7 +10072,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -9654,7 +10126,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -9714,7 +10186,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -9780,7 +10252,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -9846,7 +10318,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -9908,7 +10380,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -9974,7 +10446,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -10035,7 +10507,7 @@
       <c r="V35" s="14"/>
       <c r="W35" s="21"/>
     </row>
-    <row r="36" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -10103,7 +10575,7 @@
       </c>
       <c r="W36" s="21"/>
     </row>
-    <row r="37" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -10173,7 +10645,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -10241,7 +10713,7 @@
       </c>
       <c r="W38" s="21"/>
     </row>
-    <row r="39" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -10309,7 +10781,7 @@
       </c>
       <c r="W39" s="21"/>
     </row>
-    <row r="40" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -10367,7 +10839,7 @@
       <c r="V40" s="32"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -10429,7 +10901,7 @@
       <c r="V41" s="32"/>
       <c r="W41" s="21"/>
     </row>
-    <row r="42" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -10487,7 +10959,7 @@
       <c r="V42" s="32"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -10549,7 +11021,7 @@
       <c r="V43" s="32"/>
       <c r="W43" s="21"/>
     </row>
-    <row r="44" spans="1:23" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -10613,7 +11085,7 @@
       </c>
       <c r="W44" s="21"/>
     </row>
-    <row r="45" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -10675,7 +11147,7 @@
       </c>
       <c r="W45" s="21"/>
     </row>
-    <row r="46" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -10741,7 +11213,7 @@
       </c>
       <c r="W46" s="21"/>
     </row>
-    <row r="47" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -10807,7 +11279,7 @@
       </c>
       <c r="W47" s="21"/>
     </row>
-    <row r="48" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -10861,7 +11333,7 @@
       <c r="V48" s="32"/>
       <c r="W48" s="21"/>
     </row>
-    <row r="49" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -10927,7 +11399,7 @@
       </c>
       <c r="W49" s="21"/>
     </row>
-    <row r="50" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -10994,7 +11466,7 @@
       </c>
       <c r="W50" s="21"/>
     </row>
-    <row r="51" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -11052,7 +11524,7 @@
       <c r="V51" s="32"/>
       <c r="W51" s="21"/>
     </row>
-    <row r="52" spans="1:23" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -11106,7 +11578,7 @@
       <c r="V52" s="32"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -11170,7 +11642,7 @@
       </c>
       <c r="W53" s="21"/>
     </row>
-    <row r="54" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -11224,7 +11696,7 @@
       <c r="V54" s="32"/>
       <c r="W54" s="21"/>
     </row>
-    <row r="55" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -11282,7 +11754,7 @@
       <c r="V55" s="32"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -11345,7 +11817,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -11408,7 +11880,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11472,7 +11944,7 @@
       </c>
       <c r="W58" s="21"/>
     </row>
-    <row r="59" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -11530,7 +12002,7 @@
       <c r="V59" s="32"/>
       <c r="W59" s="21"/>
     </row>
-    <row r="60" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -11588,7 +12060,7 @@
       <c r="V60" s="32"/>
       <c r="W60" s="21"/>
     </row>
-    <row r="61" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -11649,7 +12121,7 @@
       <c r="V61" s="32"/>
       <c r="W61" s="21"/>
     </row>
-    <row r="62" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -11716,7 +12188,7 @@
       </c>
       <c r="W62" s="21"/>
     </row>
-    <row r="63" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -11781,7 +12253,7 @@
       </c>
       <c r="W63" s="21"/>
     </row>
-    <row r="64" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -11836,7 +12308,7 @@
       <c r="V64" s="32"/>
       <c r="W64" s="21"/>
     </row>
-    <row r="65" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -11891,7 +12363,7 @@
       <c r="V65" s="32"/>
       <c r="W65" s="21"/>
     </row>
-    <row r="66" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -11958,7 +12430,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -12022,7 +12494,7 @@
       </c>
       <c r="W67" s="21"/>
     </row>
-    <row r="68" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -12087,7 +12559,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="256.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -12151,7 +12623,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -12213,7 +12685,7 @@
       <c r="V70" s="32"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -12277,7 +12749,7 @@
       </c>
       <c r="W71" s="21"/>
     </row>
-    <row r="72" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -12343,7 +12815,7 @@
       <c r="W72" s="21"/>
       <c r="X72" s="32"/>
     </row>
-    <row r="73" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -12406,7 +12878,7 @@
       <c r="W73" s="21"/>
       <c r="X73" s="28"/>
     </row>
-    <row r="74" spans="1:24" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12464,7 +12936,7 @@
       <c r="W74" s="21"/>
       <c r="X74" s="32"/>
     </row>
-    <row r="75" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -12529,7 +13001,7 @@
       </c>
       <c r="W75" s="21"/>
     </row>
-    <row r="76" spans="1:24" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -12594,7 +13066,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -12658,7 +13130,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -12723,7 +13195,7 @@
       <c r="W78" s="21"/>
       <c r="X78" s="32"/>
     </row>
-    <row r="79" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -12786,7 +13258,7 @@
       <c r="W79" s="21"/>
       <c r="X79" s="32"/>
     </row>
-    <row r="80" spans="1:24" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -12851,7 +13323,7 @@
       <c r="W80" s="21"/>
       <c r="X80" s="32"/>
     </row>
-    <row r="81" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -12914,7 +13386,7 @@
       <c r="W81" s="21"/>
       <c r="X81" s="32"/>
     </row>
-    <row r="82" spans="1:24" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -12979,7 +13451,7 @@
       <c r="W82" s="21"/>
       <c r="X82" s="32"/>
     </row>
-    <row r="83" spans="1:24" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -13042,7 +13514,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="228" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -13107,7 +13579,7 @@
       <c r="W84" s="21"/>
       <c r="X84" s="32"/>
     </row>
-    <row r="85" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -13173,7 +13645,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -13237,7 +13709,7 @@
       <c r="V86" s="32"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:24" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -13300,7 +13772,7 @@
       </c>
       <c r="W87" s="21"/>
     </row>
-    <row r="88" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -13365,7 +13837,7 @@
       </c>
       <c r="W88" s="21"/>
     </row>
-    <row r="89" spans="1:24" ht="313.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="294" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -13426,7 +13898,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -13479,7 +13951,7 @@
       <c r="V90" s="32"/>
       <c r="W90" s="21"/>
     </row>
-    <row r="91" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -13530,7 +14002,7 @@
       <c r="V91" s="32"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -13594,7 +14066,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -13656,7 +14128,7 @@
       <c r="V93" s="32"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -13720,7 +14192,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -13784,7 +14256,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -13848,7 +14320,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -13910,7 +14382,7 @@
       <c r="V97" s="32"/>
       <c r="W97" s="21"/>
     </row>
-    <row r="98" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -13965,7 +14437,7 @@
       <c r="V98" s="32"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -14027,7 +14499,7 @@
       <c r="V99" s="32"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -14091,7 +14563,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="299.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -14155,7 +14627,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -14217,7 +14689,7 @@
       <c r="V102" s="32"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -14281,7 +14753,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -14345,7 +14817,7 @@
       </c>
       <c r="W104" s="21"/>
     </row>
-    <row r="105" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -14408,7 +14880,7 @@
       <c r="V105" s="33"/>
       <c r="W105" s="21"/>
     </row>
-    <row r="106" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -14471,7 +14943,7 @@
       </c>
       <c r="W106" s="21"/>
     </row>
-    <row r="107" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -14526,7 +14998,7 @@
       <c r="V107" s="32"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -14589,7 +15061,7 @@
       </c>
       <c r="W108" s="21"/>
     </row>
-    <row r="109" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -14648,7 +15120,7 @@
       <c r="V109" s="32"/>
       <c r="W109" s="21"/>
     </row>
-    <row r="110" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>108</v>
       </c>
@@ -14707,7 +15179,7 @@
       <c r="V110" s="32"/>
       <c r="W110" s="21"/>
     </row>
-    <row r="111" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -14768,7 +15240,7 @@
       <c r="V111" s="32"/>
       <c r="W111" s="21"/>
     </row>
-    <row r="112" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -14829,7 +15301,7 @@
       <c r="V112" s="32"/>
       <c r="W112" s="21"/>
     </row>
-    <row r="113" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -14890,7 +15362,7 @@
       <c r="V113" s="32"/>
       <c r="W113" s="21"/>
     </row>
-    <row r="114" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -14951,7 +15423,7 @@
       <c r="V114" s="32"/>
       <c r="W114" s="21"/>
     </row>
-    <row r="115" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -15010,7 +15482,7 @@
       <c r="V115" s="32"/>
       <c r="W115" s="21"/>
     </row>
-    <row r="116" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -15060,7 +15532,7 @@
       <c r="V116" s="32"/>
       <c r="W116" s="21"/>
     </row>
-    <row r="117" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -15112,7 +15584,7 @@
       <c r="V117" s="28"/>
       <c r="W117" s="21"/>
     </row>
-    <row r="118" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -15167,7 +15639,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -15222,7 +15694,7 @@
       <c r="V119" s="32"/>
       <c r="W119" s="21"/>
     </row>
-    <row r="120" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>118</v>
       </c>
@@ -15273,7 +15745,7 @@
       <c r="V120" s="32"/>
       <c r="W120" s="21"/>
     </row>
-    <row r="121" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>119</v>
       </c>
@@ -15326,7 +15798,7 @@
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -15383,7 +15855,7 @@
       <c r="V122" s="32"/>
       <c r="W122" s="21"/>
     </row>
-    <row r="123" spans="1:23" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>121</v>
       </c>
@@ -15432,7 +15904,7 @@
       <c r="V123" s="32"/>
       <c r="W123" s="21"/>
     </row>
-    <row r="124" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -15483,7 +15955,7 @@
       <c r="V124" s="32"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -15531,7 +16003,7 @@
       <c r="V125" s="32"/>
       <c r="W125" s="21"/>
     </row>
-    <row r="126" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -15584,7 +16056,7 @@
       </c>
       <c r="W126" s="21"/>
     </row>
-    <row r="127" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -15638,7 +16110,7 @@
       </c>
       <c r="W127" s="21"/>
     </row>
-    <row r="128" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -15690,7 +16162,7 @@
       <c r="V128" s="32"/>
       <c r="W128" s="21"/>
     </row>
-    <row r="129" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -15742,7 +16214,7 @@
       <c r="V129" s="32"/>
       <c r="W129" s="21"/>
     </row>
-    <row r="130" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -15794,7 +16266,7 @@
       <c r="V130" s="32"/>
       <c r="W130" s="21"/>
     </row>
-    <row r="131" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -15846,7 +16318,7 @@
       <c r="V131" s="32"/>
       <c r="W131" s="21"/>
     </row>
-    <row r="132" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>130</v>
       </c>
@@ -15899,7 +16371,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>131</v>
       </c>
@@ -15948,7 +16420,7 @@
       <c r="V133" s="33"/>
       <c r="W133" s="21"/>
     </row>
-    <row r="134" spans="1:23" ht="270.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="266" x14ac:dyDescent="0.35">
       <c r="A134" s="5">
         <v>132</v>
       </c>
@@ -15997,7 +16469,7 @@
       <c r="V134" s="33"/>
       <c r="W134" s="21"/>
     </row>
-    <row r="135" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>133</v>
       </c>
@@ -16046,7 +16518,7 @@
       <c r="V135" s="33"/>
       <c r="W135" s="21"/>
     </row>
-    <row r="136" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
         <v>134</v>
       </c>
@@ -16095,7 +16567,7 @@
       <c r="V136" s="33"/>
       <c r="W136" s="21"/>
     </row>
-    <row r="137" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A137" s="5">
         <v>135</v>
       </c>
@@ -16144,7 +16616,7 @@
       <c r="V137" s="33"/>
       <c r="W137" s="21"/>
     </row>
-    <row r="138" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A138" s="5">
         <v>136</v>
       </c>
@@ -16193,7 +16665,7 @@
       <c r="V138" s="33"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A139" s="5">
         <v>137</v>
       </c>
@@ -16242,7 +16714,7 @@
       <c r="V139" s="33"/>
       <c r="W139" s="21"/>
     </row>
-    <row r="140" spans="1:23" ht="213.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A140" s="5">
         <v>138</v>
       </c>
@@ -16291,7 +16763,7 @@
       <c r="V140" s="33"/>
       <c r="W140" s="21"/>
     </row>
-    <row r="141" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -16340,7 +16812,7 @@
       <c r="V141" s="33"/>
       <c r="W141" s="21"/>
     </row>
-    <row r="142" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>140</v>
       </c>
@@ -16389,7 +16861,7 @@
       <c r="V142" s="33"/>
       <c r="W142" s="21"/>
     </row>
-    <row r="143" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A143" s="5">
         <v>141</v>
       </c>
@@ -16438,7 +16910,7 @@
       <c r="V143" s="33"/>
       <c r="W143" s="21"/>
     </row>
-    <row r="144" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>142</v>
       </c>
@@ -16487,7 +16959,7 @@
       <c r="V144" s="33"/>
       <c r="W144" s="21"/>
     </row>
-    <row r="145" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>143</v>
       </c>
@@ -16536,7 +17008,7 @@
       <c r="V145" s="33"/>
       <c r="W145" s="21"/>
     </row>
-    <row r="146" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A146" s="5">
         <v>144</v>
       </c>
@@ -16585,7 +17057,7 @@
       <c r="V146" s="33"/>
       <c r="W146" s="21"/>
     </row>
-    <row r="147" spans="1:23" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A147" s="5">
         <v>145</v>
       </c>
@@ -16634,7 +17106,7 @@
       <c r="V147" s="87"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -16687,7 +17159,7 @@
       <c r="V148" s="32"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -16740,7 +17212,7 @@
       <c r="V149" s="32"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -16790,7 +17262,7 @@
       <c r="V150" s="32"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -16837,7 +17309,7 @@
       <c r="V151" s="32"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -16890,7 +17362,7 @@
       <c r="V152" s="32"/>
       <c r="W152" s="21"/>
     </row>
-    <row r="153" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>151</v>
       </c>
@@ -16939,7 +17411,7 @@
       <c r="V153" s="32"/>
       <c r="W153" s="21"/>
     </row>
-    <row r="154" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>152</v>
       </c>
@@ -16988,7 +17460,7 @@
       <c r="V154" s="32"/>
       <c r="W154" s="21"/>
     </row>
-    <row r="155" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>153</v>
       </c>
@@ -17037,7 +17509,7 @@
       <c r="V155" s="32"/>
       <c r="W155" s="21"/>
     </row>
-    <row r="156" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>154</v>
       </c>
@@ -17086,7 +17558,7 @@
       <c r="V156" s="32"/>
       <c r="W156" s="21"/>
     </row>
-    <row r="157" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>155</v>
       </c>
@@ -17135,7 +17607,7 @@
       <c r="V157" s="32"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -17189,7 +17661,7 @@
       <c r="V158" s="32"/>
       <c r="W158" s="33"/>
     </row>
-    <row r="159" spans="1:23" ht="228" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -17243,7 +17715,7 @@
       <c r="V159" s="32"/>
       <c r="W159" s="33"/>
     </row>
-    <row r="160" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -17294,7 +17766,7 @@
       <c r="V160" s="28"/>
       <c r="W160" s="33"/>
     </row>
-    <row r="161" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>159</v>
       </c>
@@ -17349,7 +17821,7 @@
       <c r="V161" s="32"/>
       <c r="W161" s="33"/>
     </row>
-    <row r="162" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>160</v>
       </c>
@@ -17404,7 +17876,7 @@
       <c r="V162" s="32"/>
       <c r="W162" s="33"/>
     </row>
-    <row r="163" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>161</v>
       </c>
@@ -17459,7 +17931,7 @@
       <c r="V163" s="32"/>
       <c r="W163" s="33"/>
     </row>
-    <row r="164" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>162</v>
       </c>
@@ -17514,7 +17986,7 @@
       <c r="V164" s="32"/>
       <c r="W164" s="33"/>
     </row>
-    <row r="165" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>163</v>
       </c>
@@ -17569,7 +18041,7 @@
       <c r="V165" s="32"/>
       <c r="W165" s="33"/>
     </row>
-    <row r="166" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>164</v>
       </c>
@@ -17624,7 +18096,7 @@
       <c r="V166" s="32"/>
       <c r="W166" s="33"/>
     </row>
-    <row r="167" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>165</v>
       </c>
@@ -17679,7 +18151,7 @@
       <c r="V167" s="32"/>
       <c r="W167" s="33"/>
     </row>
-    <row r="168" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>166</v>
       </c>
@@ -17734,7 +18206,7 @@
       <c r="V168" s="32"/>
       <c r="W168" s="33"/>
     </row>
-    <row r="169" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>167</v>
       </c>
@@ -17789,7 +18261,7 @@
       <c r="V169" s="32"/>
       <c r="W169" s="33"/>
     </row>
-    <row r="170" spans="1:23" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>168</v>
       </c>
@@ -17844,7 +18316,7 @@
       <c r="V170" s="32"/>
       <c r="W170" s="33"/>
     </row>
-    <row r="171" spans="1:23" s="103" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>169</v>
       </c>
@@ -17891,7 +18363,7 @@
       <c r="V171" s="14"/>
       <c r="W171" s="104"/>
     </row>
-    <row r="172" spans="1:23" s="103" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>170</v>
       </c>
@@ -17946,11 +18418,13 @@
       <c r="V172" s="14"/>
       <c r="W172" s="104"/>
     </row>
-    <row r="173" spans="1:23" s="103" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" s="103" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>171</v>
       </c>
-      <c r="B173" s="5"/>
+      <c r="B173" s="6" t="s">
+        <v>604</v>
+      </c>
       <c r="C173" s="6">
         <v>43556</v>
       </c>
@@ -17993,11 +18467,13 @@
       <c r="V173" s="14"/>
       <c r="W173" s="104"/>
     </row>
-    <row r="174" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>172</v>
       </c>
-      <c r="B174" s="5"/>
+      <c r="B174" s="6" t="s">
+        <v>605</v>
+      </c>
       <c r="C174" s="6">
         <v>43556</v>
       </c>
@@ -18038,38 +18514,556 @@
       <c r="V174" s="14"/>
       <c r="W174" s="33"/>
     </row>
+    <row r="175" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+      <c r="A175" s="5">
+        <f>1+A174</f>
+        <v>173</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="C175" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D175" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E175" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F175" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G175" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H175" s="32" t="s">
+        <v>632</v>
+      </c>
+      <c r="J175" s="32"/>
+      <c r="K175" s="32"/>
+      <c r="L175" s="32"/>
+      <c r="M175" s="32">
+        <v>1</v>
+      </c>
+      <c r="N175" s="28"/>
+      <c r="O175" s="32"/>
+      <c r="P175" s="6"/>
+      <c r="R175" s="5"/>
+      <c r="S175" s="5"/>
+      <c r="T175" s="33"/>
+      <c r="U175" s="5"/>
+      <c r="V175" s="32"/>
+      <c r="W175" s="21"/>
+    </row>
+    <row r="176" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+      <c r="A176" s="5">
+        <f t="shared" ref="A176:A185" si="8">1+A175</f>
+        <v>174</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="C176" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D176" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E176" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F176" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G176" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H176" s="32" t="s">
+        <v>633</v>
+      </c>
+      <c r="M176" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A177" s="5">
+        <f t="shared" si="8"/>
+        <v>175</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="C177" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D177" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E177" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F177" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G177" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H177" s="32" t="s">
+        <v>617</v>
+      </c>
+      <c r="M177" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A178" s="5">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="C178" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D178" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E178" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F178" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G178" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H178" s="32" t="s">
+        <v>618</v>
+      </c>
+      <c r="M178" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A179" s="5">
+        <f t="shared" si="8"/>
+        <v>177</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="C179" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D179" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E179" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F179" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G179" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H179" s="32" t="s">
+        <v>619</v>
+      </c>
+      <c r="M179" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A180" s="5">
+        <f t="shared" si="8"/>
+        <v>178</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C180" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D180" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E180" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G180" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H180" s="32" t="s">
+        <v>620</v>
+      </c>
+      <c r="M180" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A181" s="5">
+        <f t="shared" si="8"/>
+        <v>179</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="C181" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D181" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E181" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G181" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H181" s="32" t="s">
+        <v>621</v>
+      </c>
+      <c r="M181" s="32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A182" s="5">
+        <f>1+A181</f>
+        <v>180</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C182" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D182" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E182" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F182" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G182" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H182" s="32" t="s">
+        <v>622</v>
+      </c>
+      <c r="M182" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A183" s="5">
+        <f t="shared" si="8"/>
+        <v>181</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="C183" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D183" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E183" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G183" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H183" s="32" t="s">
+        <v>623</v>
+      </c>
+      <c r="M183" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A184" s="5">
+        <f t="shared" si="8"/>
+        <v>182</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C184" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D184" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E184" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F184" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G184" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H184" s="32" t="s">
+        <v>624</v>
+      </c>
+      <c r="M184" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A185" s="5">
+        <f t="shared" si="8"/>
+        <v>183</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="C185" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D185" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E185" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F185" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G185" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H185" s="32" t="s">
+        <v>625</v>
+      </c>
+      <c r="M185" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A186" s="2">
+        <f>1+A185</f>
+        <v>184</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="C186" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D186" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E186" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G186" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H186" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="M186" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A187" s="2">
+        <f>1+A186</f>
+        <v>185</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="C187" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D187" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E187" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F187" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G187" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H187" s="32" t="s">
+        <v>627</v>
+      </c>
+      <c r="M187" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A188" s="2">
+        <f t="shared" ref="A188:A191" si="9">1+A187</f>
+        <v>186</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C188" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D188" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E188" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F188" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G188" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H188" s="32" t="s">
+        <v>628</v>
+      </c>
+      <c r="M188" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A189" s="2">
+        <f t="shared" si="9"/>
+        <v>187</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="C189" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D189" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E189" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F189" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G189" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H189" s="32" t="s">
+        <v>629</v>
+      </c>
+      <c r="M189" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A190" s="2">
+        <f t="shared" si="9"/>
+        <v>188</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="C190" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D190" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E190" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G190" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H190" s="32" t="s">
+        <v>630</v>
+      </c>
+      <c r="M190" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A191" s="2">
+        <f t="shared" si="9"/>
+        <v>189</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="C191" s="6">
+        <v>43553</v>
+      </c>
+      <c r="D191" s="32" t="s">
+        <v>599</v>
+      </c>
+      <c r="E191" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F191" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G191" s="32" t="s">
+        <v>582</v>
+      </c>
+      <c r="H191" s="32" t="s">
+        <v>631</v>
+      </c>
+      <c r="M191" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B192" s="110"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:X174" xr:uid="{6C8A7F8F-6E5A-48C3-B40D-B34E2585C37A}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="ID Authentication"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D132" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D132" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9EA61013-F3C9-4524-80A2-4A4BA088EF9E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Values!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G174</xm:sqref>
+          <xm:sqref>G3:G191</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18078,20 +19072,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -18099,7 +19093,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
@@ -18107,7 +19101,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
@@ -18115,7 +19109,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
@@ -18123,31 +19117,31 @@
         <v>585</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>588</v>
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>587</v>
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>586</v>
       </c>
@@ -18159,19 +19153,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>144</v>
       </c>
@@ -18182,7 +19176,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -18193,7 +19187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -18204,7 +19198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -18215,7 +19209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -18226,7 +19220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -18237,7 +19231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -18248,7 +19242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -18259,7 +19253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>145</v>
       </c>
@@ -18277,17 +19271,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="65" t="s">
         <v>206</v>
       </c>
@@ -18295,25 +19289,25 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69"/>
       <c r="C3" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="70"/>
       <c r="C4" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71"/>
       <c r="C5" s="72" t="s">
         <v>205</v>
@@ -18326,12 +19320,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18507,32 +19515,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18556,17 +19558,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited font for few CR's
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\PROJECTS\MOSIP\Bootcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D49E6084-F384-4976-BD20-ECAC08DA4E54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2655" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$X$191</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -5670,344 +5669,6 @@
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Transliteration</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-The virtual keyboard icon is repeated three times. Can we make it appear in just one place? </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Address</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-The address is too spaced out. Utilize the space better. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Demographic fields</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Should age, date of birth, phone number and email be displayed twice, considering RHS is not editable?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - all screens</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Optimize the vertical scroll bar—keep it as minimum as possible.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Biometric exceptions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Explore the option of having the exception marking on the same screen as the document upload. Utilize the space on the right.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Biometric exceptions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Fingerprint exception marking to be more intuitive. Do not colour the entire finger. The exception fingers should to be crossed out.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Biometric exceptions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Morocco screens will have iris exception only. Create a new screen with iris exceptions aligned better.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - all screens</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-RO should be able to go back and forth between demographic, document and biometric screens. Retain the captured data in each screen. For biometrics - retain data whenever possible i.e. for those biometrics not marked as exceptions.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Biometric screens</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-a. 'Start Over/Reset' buttons: what happens on click? Revisit the flow.
-b. 'Scan' button - instead of having the button at the bottom, provide a scan icon on the slap image itself for each biometric.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - all screens</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-a. RHS progress bar - can we make them links? Implement if feasible. User should be able to jump to any page using RHS and top navigation links.
-b. Validations - all validations should happen on the preview page when user tries to submit. Display a consolidated error message highlighting which pages have errors. User should be able to jump to the page having errors, make the changes and jump back to preview</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - consent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-The consent feature is under discussion. It could result in additional attributes for seeking consent.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Acknowledgement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-The acknowledgement printout should fit on half an A4 page. Hence on click of print, mirror it and print two copies on a single A4 sheet.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New Registration - Acknowledgement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-The QR code should have only the RID. Remove the other details such as demographics and photo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Re-register</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-Rename 'Re-register' to 'Notification for Re-registration'. This should be done on the home page and the Re-register page.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
@@ -6055,14 +5716,335 @@
     <t>UX analysis in progress</t>
   </si>
   <si>
+    <t>Consent wrt HoH requirement under discussion with GoM - Pending with GoM/CPU team for requirement finalization</t>
+  </si>
+  <si>
+    <t>Functional Change: Allow partial search in center selection page</t>
+  </si>
+  <si>
+    <t>VD needs to changed/ any other intuitive way should be decided - UX analysis in progress</t>
+  </si>
+  <si>
+    <t>Sprint 9 - UI Demo Feedback from Shrikant on 02Apr19</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Transliteration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+The virtual keyboard icon is repeated three times. Can we make it appear in just one place? </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+The address is too spaced out. Utilize the space better. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Demographic fields</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Should age, date of birth, phone number and email be displayed twice, considering RHS is not editable?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Optimize the vertical scroll bar—keep it as minimum as possible.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Explore the option of having the exception marking on the same screen as the document upload. Utilize the space on the right.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Fingerprint exception marking to be more intuitive. Do not colour the entire finger. The exception fingers should to be crossed out.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Biometric exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Morocco screens will have iris exception only. Create a new screen with iris exceptions aligned better.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+RO should be able to go back and forth between demographic, document and biometric screens. Retain the captured data in each screen. For biometrics - retain data whenever possible i.e. for those biometrics not marked as exceptions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Biometric screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+a. 'Start Over/Reset' buttons: what happens on click? Revisit the flow.
+b. 'Scan' button - instead of having the button at the bottom, provide a scan icon on the slap image itself for each biometric.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - all screens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+a. RHS progress bar - can we make them links? Implement if feasible. User should be able to jump to any page using RHS and top navigation links.
+b. Validations - all validations should happen on the preview page when user tries to submit. Display a consolidated error message highlighting which pages have errors. User should be able to jump to the page having errors, make the changes and jump back to preview</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - consent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The consent feature is under discussion. It could result in additional attributes for seeking consent.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Acknowledgement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The acknowledgement printout should fit on half an A4 page. Hence on click of print, mirror it and print two copies on a single A4 sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>New Registration - Acknowledgement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The QR code should have only the RID. Remove the other details such as demographics and photo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Re-register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Rename 'Re-register' to 'Notification for Re-registration'. This should be done on the home page and the Re-register page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>Upload packet</t>
     </r>
@@ -6070,35 +6052,22 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t>:
 Provide a search feature for the list of packets on the upload page - Partial Search mechanism</t>
     </r>
-  </si>
-  <si>
-    <t>Consent wrt HoH requirement under discussion with GoM - Pending with GoM/CPU team for requirement finalization</t>
-  </si>
-  <si>
-    <t>Functional Change: Allow partial search in center selection page</t>
-  </si>
-  <si>
-    <t>VD needs to changed/ any other intuitive way should be decided - UX analysis in progress</t>
-  </si>
-  <si>
-    <t>Sprint 9 - UI Demo Feedback from Shrikant on 02Apr19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6209,14 +6178,6 @@
       <color rgb="FF0070C0"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -6476,7 +6437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6772,6 +6733,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6787,19 +6758,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6830,7 +6788,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -6847,7 +6805,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:V70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -8008,7 +7966,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -8356,70 +8314,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A192" sqref="A192"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G190" sqref="G190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="27" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="32" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="3" customWidth="1"/>
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" style="3" customWidth="1"/>
     <col min="12" max="12" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="22.81640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="27" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="51.5703125" style="10" customWidth="1"/>
-    <col min="24" max="16384" width="20.42578125" style="10"/>
+    <col min="17" max="17" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="51.54296875" style="10" customWidth="1"/>
+    <col min="24" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="109" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="109"/>
-    </row>
-    <row r="2" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+      <c r="B1" s="110"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="113"/>
+    </row>
+    <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -8490,7 +8448,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -8554,9 +8512,9 @@
       <c r="V3" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="W3" s="113"/>
-    </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="W3" s="107"/>
+    </row>
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -8619,9 +8577,9 @@
       <c r="V4" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="W4" s="113"/>
-    </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="W4" s="107"/>
+    </row>
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -8685,9 +8643,9 @@
       <c r="V5" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="W5" s="113"/>
-    </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="W5" s="107"/>
+    </row>
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -8751,9 +8709,9 @@
       <c r="V6" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="W6" s="113"/>
-    </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="W6" s="107"/>
+    </row>
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -8817,9 +8775,9 @@
       <c r="V7" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="W7" s="113"/>
-    </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+      <c r="W7" s="107"/>
+    </row>
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -8883,9 +8841,9 @@
       <c r="V8" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="W8" s="113"/>
-    </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="W8" s="107"/>
+    </row>
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -8947,9 +8905,9 @@
       <c r="V9" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="W9" s="113"/>
-    </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+      <c r="W9" s="107"/>
+    </row>
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -9011,9 +8969,9 @@
       <c r="V10" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="W10" s="113"/>
-    </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="W10" s="107"/>
+    </row>
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -9069,9 +9027,9 @@
       <c r="T11" s="30"/>
       <c r="U11" s="30"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="114"/>
-    </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="W11" s="108"/>
+    </row>
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -9128,9 +9086,9 @@
       <c r="V12" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="W12" s="114"/>
-    </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="W12" s="108"/>
+    </row>
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -9187,7 +9145,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -9251,7 +9209,7 @@
       </c>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -9317,7 +9275,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -9383,7 +9341,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="4" customFormat="1" ht="182" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -9449,7 +9407,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -9513,7 +9471,7 @@
       </c>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -9579,7 +9537,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -9631,7 +9589,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -9683,7 +9641,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -9747,7 +9705,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -9811,7 +9769,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -9877,7 +9835,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -9931,7 +9889,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -9985,7 +9943,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -10049,7 +10007,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -10115,7 +10073,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -10169,7 +10127,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -10229,7 +10187,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -10295,7 +10253,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -10361,7 +10319,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -10423,7 +10381,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -10489,7 +10447,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -10550,7 +10508,7 @@
       <c r="V35" s="14"/>
       <c r="W35" s="21"/>
     </row>
-    <row r="36" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -10618,7 +10576,7 @@
       </c>
       <c r="W36" s="21"/>
     </row>
-    <row r="37" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -10688,7 +10646,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -10756,7 +10714,7 @@
       </c>
       <c r="W38" s="21"/>
     </row>
-    <row r="39" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -10824,7 +10782,7 @@
       </c>
       <c r="W39" s="21"/>
     </row>
-    <row r="40" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -10882,7 +10840,7 @@
       <c r="V40" s="32"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -10944,7 +10902,7 @@
       <c r="V41" s="32"/>
       <c r="W41" s="21"/>
     </row>
-    <row r="42" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -11002,7 +10960,7 @@
       <c r="V42" s="32"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -11064,7 +11022,7 @@
       <c r="V43" s="32"/>
       <c r="W43" s="21"/>
     </row>
-    <row r="44" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="252" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -11128,7 +11086,7 @@
       </c>
       <c r="W44" s="21"/>
     </row>
-    <row r="45" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -11190,7 +11148,7 @@
       </c>
       <c r="W45" s="21"/>
     </row>
-    <row r="46" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -11256,7 +11214,7 @@
       </c>
       <c r="W46" s="21"/>
     </row>
-    <row r="47" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -11322,7 +11280,7 @@
       </c>
       <c r="W47" s="21"/>
     </row>
-    <row r="48" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -11376,7 +11334,7 @@
       <c r="V48" s="32"/>
       <c r="W48" s="21"/>
     </row>
-    <row r="49" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -11442,7 +11400,7 @@
       </c>
       <c r="W49" s="21"/>
     </row>
-    <row r="50" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -11509,7 +11467,7 @@
       </c>
       <c r="W50" s="21"/>
     </row>
-    <row r="51" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -11567,7 +11525,7 @@
       <c r="V51" s="32"/>
       <c r="W51" s="21"/>
     </row>
-    <row r="52" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -11621,7 +11579,7 @@
       <c r="V52" s="32"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -11685,7 +11643,7 @@
       </c>
       <c r="W53" s="21"/>
     </row>
-    <row r="54" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -11739,7 +11697,7 @@
       <c r="V54" s="32"/>
       <c r="W54" s="21"/>
     </row>
-    <row r="55" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -11797,7 +11755,7 @@
       <c r="V55" s="32"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -11860,7 +11818,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -11923,7 +11881,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -11987,7 +11945,7 @@
       </c>
       <c r="W58" s="21"/>
     </row>
-    <row r="59" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -12045,7 +12003,7 @@
       <c r="V59" s="32"/>
       <c r="W59" s="21"/>
     </row>
-    <row r="60" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -12103,7 +12061,7 @@
       <c r="V60" s="32"/>
       <c r="W60" s="21"/>
     </row>
-    <row r="61" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -12164,7 +12122,7 @@
       <c r="V61" s="32"/>
       <c r="W61" s="21"/>
     </row>
-    <row r="62" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -12231,7 +12189,7 @@
       </c>
       <c r="W62" s="21"/>
     </row>
-    <row r="63" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -12296,7 +12254,7 @@
       </c>
       <c r="W63" s="21"/>
     </row>
-    <row r="64" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -12351,7 +12309,7 @@
       <c r="V64" s="32"/>
       <c r="W64" s="21"/>
     </row>
-    <row r="65" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -12406,7 +12364,7 @@
       <c r="V65" s="32"/>
       <c r="W65" s="21"/>
     </row>
-    <row r="66" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -12473,7 +12431,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -12537,7 +12495,7 @@
       </c>
       <c r="W67" s="21"/>
     </row>
-    <row r="68" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -12602,7 +12560,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -12666,7 +12624,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -12728,7 +12686,7 @@
       <c r="V70" s="32"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -12792,7 +12750,7 @@
       </c>
       <c r="W71" s="21"/>
     </row>
-    <row r="72" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -12856,9 +12814,9 @@
         <v>165</v>
       </c>
       <c r="W72" s="21"/>
-      <c r="X72" s="112"/>
-    </row>
-    <row r="73" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="X72" s="106"/>
+    </row>
+    <row r="73" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -12921,7 +12879,7 @@
       <c r="W73" s="21"/>
       <c r="X73" s="97"/>
     </row>
-    <row r="74" spans="1:24" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -12977,9 +12935,9 @@
       <c r="U74" s="5"/>
       <c r="V74" s="5"/>
       <c r="W74" s="21"/>
-      <c r="X74" s="112"/>
-    </row>
-    <row r="75" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+      <c r="X74" s="106"/>
+    </row>
+    <row r="75" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -13044,7 +13002,7 @@
       </c>
       <c r="W75" s="21"/>
     </row>
-    <row r="76" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -13109,7 +13067,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -13173,7 +13131,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -13236,9 +13194,9 @@
         <v>253</v>
       </c>
       <c r="W78" s="21"/>
-      <c r="X78" s="112"/>
-    </row>
-    <row r="79" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+      <c r="X78" s="106"/>
+    </row>
+    <row r="79" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -13299,9 +13257,9 @@
       <c r="U79" s="5"/>
       <c r="V79" s="5"/>
       <c r="W79" s="21"/>
-      <c r="X79" s="112"/>
-    </row>
-    <row r="80" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="X79" s="106"/>
+    </row>
+    <row r="80" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -13364,9 +13322,9 @@
         <v>258</v>
       </c>
       <c r="W80" s="21"/>
-      <c r="X80" s="112"/>
-    </row>
-    <row r="81" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="X80" s="106"/>
+    </row>
+    <row r="81" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -13427,9 +13385,9 @@
       <c r="U81" s="5"/>
       <c r="V81" s="5"/>
       <c r="W81" s="21"/>
-      <c r="X81" s="112"/>
-    </row>
-    <row r="82" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="X81" s="106"/>
+    </row>
+    <row r="82" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -13492,9 +13450,9 @@
         <v>259</v>
       </c>
       <c r="W82" s="21"/>
-      <c r="X82" s="112"/>
-    </row>
-    <row r="83" spans="1:24" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="X82" s="106"/>
+    </row>
+    <row r="83" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -13557,7 +13515,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="228" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -13620,9 +13578,9 @@
         <v>446</v>
       </c>
       <c r="W84" s="21"/>
-      <c r="X84" s="112"/>
-    </row>
-    <row r="85" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="X84" s="106"/>
+    </row>
+    <row r="85" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -13688,7 +13646,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -13752,7 +13710,7 @@
       <c r="V86" s="32"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -13815,7 +13773,7 @@
       </c>
       <c r="W87" s="21"/>
     </row>
-    <row r="88" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -13880,7 +13838,7 @@
       </c>
       <c r="W88" s="21"/>
     </row>
-    <row r="89" spans="1:24" ht="313.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="294" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -13941,7 +13899,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -13994,7 +13952,7 @@
       <c r="V90" s="32"/>
       <c r="W90" s="21"/>
     </row>
-    <row r="91" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -14045,7 +14003,7 @@
       <c r="V91" s="32"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="171" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -14109,7 +14067,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -14171,7 +14129,7 @@
       <c r="V93" s="32"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -14235,7 +14193,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -14299,7 +14257,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -14363,7 +14321,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -14425,7 +14383,7 @@
       <c r="V97" s="32"/>
       <c r="W97" s="21"/>
     </row>
-    <row r="98" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -14480,7 +14438,7 @@
       <c r="V98" s="32"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -14542,7 +14500,7 @@
       <c r="V99" s="32"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -14606,7 +14564,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -14670,7 +14628,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -14732,7 +14690,7 @@
       <c r="V102" s="32"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -14796,7 +14754,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -14860,7 +14818,7 @@
       </c>
       <c r="W104" s="21"/>
     </row>
-    <row r="105" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -14923,7 +14881,7 @@
       <c r="V105" s="33"/>
       <c r="W105" s="21"/>
     </row>
-    <row r="106" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -14986,7 +14944,7 @@
       </c>
       <c r="W106" s="21"/>
     </row>
-    <row r="107" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -15041,7 +14999,7 @@
       <c r="V107" s="32"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -15104,7 +15062,7 @@
       </c>
       <c r="W108" s="21"/>
     </row>
-    <row r="109" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -15163,7 +15121,7 @@
       <c r="V109" s="32"/>
       <c r="W109" s="21"/>
     </row>
-    <row r="110" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>108</v>
       </c>
@@ -15222,7 +15180,7 @@
       <c r="V110" s="32"/>
       <c r="W110" s="21"/>
     </row>
-    <row r="111" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -15283,7 +15241,7 @@
       <c r="V111" s="32"/>
       <c r="W111" s="21"/>
     </row>
-    <row r="112" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -15344,7 +15302,7 @@
       <c r="V112" s="32"/>
       <c r="W112" s="21"/>
     </row>
-    <row r="113" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -15405,7 +15363,7 @@
       <c r="V113" s="32"/>
       <c r="W113" s="21"/>
     </row>
-    <row r="114" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -15466,7 +15424,7 @@
       <c r="V114" s="32"/>
       <c r="W114" s="21"/>
     </row>
-    <row r="115" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -15525,7 +15483,7 @@
       <c r="V115" s="32"/>
       <c r="W115" s="21"/>
     </row>
-    <row r="116" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -15575,7 +15533,7 @@
       <c r="V116" s="32"/>
       <c r="W116" s="21"/>
     </row>
-    <row r="117" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -15627,7 +15585,7 @@
       <c r="V117" s="28"/>
       <c r="W117" s="21"/>
     </row>
-    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -15682,7 +15640,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -15737,7 +15695,7 @@
       <c r="V119" s="32"/>
       <c r="W119" s="21"/>
     </row>
-    <row r="120" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>118</v>
       </c>
@@ -15788,7 +15746,7 @@
       <c r="V120" s="32"/>
       <c r="W120" s="21"/>
     </row>
-    <row r="121" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>119</v>
       </c>
@@ -15841,7 +15799,7 @@
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -15898,7 +15856,7 @@
       <c r="V122" s="32"/>
       <c r="W122" s="21"/>
     </row>
-    <row r="123" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>121</v>
       </c>
@@ -15947,7 +15905,7 @@
       <c r="V123" s="32"/>
       <c r="W123" s="21"/>
     </row>
-    <row r="124" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -15998,7 +15956,7 @@
       <c r="V124" s="32"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -16046,7 +16004,7 @@
       <c r="V125" s="32"/>
       <c r="W125" s="21"/>
     </row>
-    <row r="126" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -16099,7 +16057,7 @@
       </c>
       <c r="W126" s="21"/>
     </row>
-    <row r="127" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -16149,11 +16107,11 @@
       </c>
       <c r="U127" s="28"/>
       <c r="V127" s="3" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="W127" s="21"/>
     </row>
-    <row r="128" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -16203,11 +16161,11 @@
       </c>
       <c r="U128" s="32"/>
       <c r="V128" s="32" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="W128" s="21"/>
     </row>
-    <row r="129" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -16257,11 +16215,11 @@
       </c>
       <c r="U129" s="32"/>
       <c r="V129" s="32" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="W129" s="21"/>
     </row>
-    <row r="130" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -16284,7 +16242,7 @@
         <v>580</v>
       </c>
       <c r="H130" s="32" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="J130" s="32" t="s">
         <v>426</v>
@@ -16311,11 +16269,11 @@
       </c>
       <c r="U130" s="32"/>
       <c r="V130" s="32" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="W130" s="21"/>
     </row>
-    <row r="131" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -16365,11 +16323,11 @@
       </c>
       <c r="U131" s="32"/>
       <c r="V131" s="32" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="W131" s="21"/>
     </row>
-    <row r="132" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>130</v>
       </c>
@@ -16422,7 +16380,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>131</v>
       </c>
@@ -16471,7 +16429,7 @@
       <c r="V133" s="33"/>
       <c r="W133" s="21"/>
     </row>
-    <row r="134" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="266" x14ac:dyDescent="0.35">
       <c r="A134" s="5">
         <v>132</v>
       </c>
@@ -16520,7 +16478,7 @@
       <c r="V134" s="33"/>
       <c r="W134" s="21"/>
     </row>
-    <row r="135" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>133</v>
       </c>
@@ -16569,7 +16527,7 @@
       <c r="V135" s="33"/>
       <c r="W135" s="21"/>
     </row>
-    <row r="136" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
         <v>134</v>
       </c>
@@ -16618,7 +16576,7 @@
       <c r="V136" s="33"/>
       <c r="W136" s="21"/>
     </row>
-    <row r="137" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A137" s="5">
         <v>135</v>
       </c>
@@ -16667,7 +16625,7 @@
       <c r="V137" s="33"/>
       <c r="W137" s="21"/>
     </row>
-    <row r="138" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A138" s="5">
         <v>136</v>
       </c>
@@ -16716,7 +16674,7 @@
       <c r="V138" s="33"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A139" s="5">
         <v>137</v>
       </c>
@@ -16765,7 +16723,7 @@
       <c r="V139" s="33"/>
       <c r="W139" s="21"/>
     </row>
-    <row r="140" spans="1:23" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A140" s="5">
         <v>138</v>
       </c>
@@ -16814,7 +16772,7 @@
       <c r="V140" s="33"/>
       <c r="W140" s="21"/>
     </row>
-    <row r="141" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -16863,7 +16821,7 @@
       <c r="V141" s="33"/>
       <c r="W141" s="21"/>
     </row>
-    <row r="142" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>140</v>
       </c>
@@ -16912,7 +16870,7 @@
       <c r="V142" s="33"/>
       <c r="W142" s="21"/>
     </row>
-    <row r="143" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A143" s="5">
         <v>141</v>
       </c>
@@ -16961,7 +16919,7 @@
       <c r="V143" s="33"/>
       <c r="W143" s="21"/>
     </row>
-    <row r="144" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>142</v>
       </c>
@@ -17010,7 +16968,7 @@
       <c r="V144" s="33"/>
       <c r="W144" s="21"/>
     </row>
-    <row r="145" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>143</v>
       </c>
@@ -17059,7 +17017,7 @@
       <c r="V145" s="33"/>
       <c r="W145" s="21"/>
     </row>
-    <row r="146" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A146" s="5">
         <v>144</v>
       </c>
@@ -17108,7 +17066,7 @@
       <c r="V146" s="33"/>
       <c r="W146" s="21"/>
     </row>
-    <row r="147" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" ht="140" x14ac:dyDescent="0.35">
       <c r="A147" s="5">
         <v>145</v>
       </c>
@@ -17157,7 +17115,7 @@
       <c r="V147" s="87"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -17210,7 +17168,7 @@
       <c r="V148" s="32"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -17263,7 +17221,7 @@
       <c r="V149" s="32"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -17313,7 +17271,7 @@
       <c r="V150" s="32"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -17360,7 +17318,7 @@
       <c r="V151" s="32"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -17413,7 +17371,7 @@
       <c r="V152" s="32"/>
       <c r="W152" s="21"/>
     </row>
-    <row r="153" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>151</v>
       </c>
@@ -17462,7 +17420,7 @@
       <c r="V153" s="32"/>
       <c r="W153" s="21"/>
     </row>
-    <row r="154" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>152</v>
       </c>
@@ -17511,7 +17469,7 @@
       <c r="V154" s="32"/>
       <c r="W154" s="21"/>
     </row>
-    <row r="155" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>153</v>
       </c>
@@ -17560,7 +17518,7 @@
       <c r="V155" s="32"/>
       <c r="W155" s="21"/>
     </row>
-    <row r="156" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>154</v>
       </c>
@@ -17609,7 +17567,7 @@
       <c r="V156" s="32"/>
       <c r="W156" s="21"/>
     </row>
-    <row r="157" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>155</v>
       </c>
@@ -17658,7 +17616,7 @@
       <c r="V157" s="32"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -17712,7 +17670,7 @@
       <c r="V158" s="32"/>
       <c r="W158" s="33"/>
     </row>
-    <row r="159" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -17766,7 +17724,7 @@
       <c r="V159" s="32"/>
       <c r="W159" s="33"/>
     </row>
-    <row r="160" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -17817,7 +17775,7 @@
       <c r="V160" s="28"/>
       <c r="W160" s="33"/>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>159</v>
       </c>
@@ -17872,7 +17830,7 @@
       <c r="V161" s="32"/>
       <c r="W161" s="33"/>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>160</v>
       </c>
@@ -17927,7 +17885,7 @@
       <c r="V162" s="32"/>
       <c r="W162" s="33"/>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>161</v>
       </c>
@@ -17982,7 +17940,7 @@
       <c r="V163" s="32"/>
       <c r="W163" s="33"/>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>162</v>
       </c>
@@ -18037,7 +17995,7 @@
       <c r="V164" s="32"/>
       <c r="W164" s="33"/>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>163</v>
       </c>
@@ -18092,7 +18050,7 @@
       <c r="V165" s="32"/>
       <c r="W165" s="33"/>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>164</v>
       </c>
@@ -18147,7 +18105,7 @@
       <c r="V166" s="32"/>
       <c r="W166" s="33"/>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>165</v>
       </c>
@@ -18202,7 +18160,7 @@
       <c r="V167" s="32"/>
       <c r="W167" s="33"/>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>166</v>
       </c>
@@ -18257,7 +18215,7 @@
       <c r="V168" s="32"/>
       <c r="W168" s="33"/>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>167</v>
       </c>
@@ -18312,7 +18270,7 @@
       <c r="V169" s="32"/>
       <c r="W169" s="33"/>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>168</v>
       </c>
@@ -18367,7 +18325,7 @@
       <c r="V170" s="32"/>
       <c r="W170" s="33"/>
     </row>
-    <row r="171" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>169</v>
       </c>
@@ -18414,7 +18372,7 @@
       <c r="V171" s="14"/>
       <c r="W171" s="104"/>
     </row>
-    <row r="172" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>170</v>
       </c>
@@ -18469,7 +18427,7 @@
       <c r="V172" s="14"/>
       <c r="W172" s="104"/>
     </row>
-    <row r="173" spans="1:23" s="103" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" s="103" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>171</v>
       </c>
@@ -18518,7 +18476,7 @@
       <c r="V173" s="14"/>
       <c r="W173" s="104"/>
     </row>
-    <row r="174" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>172</v>
       </c>
@@ -18565,7 +18523,7 @@
       <c r="V174" s="14"/>
       <c r="W174" s="33"/>
     </row>
-    <row r="175" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A175" s="39">
         <f>1+A174</f>
         <v>173</v>
@@ -18577,7 +18535,7 @@
         <v>43557</v>
       </c>
       <c r="D175" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E175" s="28" t="s">
         <v>15</v>
@@ -18589,7 +18547,7 @@
         <v>581</v>
       </c>
       <c r="H175" s="28" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="J175" s="28"/>
       <c r="K175" s="28"/>
@@ -18607,7 +18565,7 @@
       <c r="V175" s="28"/>
       <c r="W175" s="38"/>
     </row>
-    <row r="176" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <f t="shared" ref="A176:A185" si="8">1+A175</f>
         <v>174</v>
@@ -18619,7 +18577,7 @@
         <v>43557</v>
       </c>
       <c r="D176" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E176" s="32" t="s">
         <v>15</v>
@@ -18631,7 +18589,7 @@
         <v>580</v>
       </c>
       <c r="H176" s="32" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="I176" s="14"/>
       <c r="J176" s="32"/>
@@ -18644,7 +18602,7 @@
         <v>74</v>
       </c>
       <c r="O176" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P176" s="21">
         <v>43557</v>
@@ -18653,13 +18611,13 @@
       <c r="R176" s="14"/>
       <c r="S176" s="14"/>
       <c r="T176" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U176" s="5"/>
       <c r="V176" s="32"/>
       <c r="W176" s="33"/>
     </row>
-    <row r="177" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
         <f t="shared" si="8"/>
         <v>175</v>
@@ -18671,7 +18629,7 @@
         <v>43557</v>
       </c>
       <c r="D177" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E177" s="32" t="s">
         <v>15</v>
@@ -18683,7 +18641,7 @@
         <v>581</v>
       </c>
       <c r="H177" s="32" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="I177" s="14"/>
       <c r="J177" s="32"/>
@@ -18696,7 +18654,7 @@
         <v>74</v>
       </c>
       <c r="O177" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P177" s="21">
         <v>43557</v>
@@ -18705,13 +18663,13 @@
       <c r="R177" s="14"/>
       <c r="S177" s="14"/>
       <c r="T177" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U177" s="5"/>
       <c r="V177" s="32"/>
       <c r="W177" s="33"/>
     </row>
-    <row r="178" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <f t="shared" si="8"/>
         <v>176</v>
@@ -18723,7 +18681,7 @@
         <v>43557</v>
       </c>
       <c r="D178" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E178" s="32" t="s">
         <v>15</v>
@@ -18735,7 +18693,7 @@
         <v>581</v>
       </c>
       <c r="H178" s="32" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="I178" s="14"/>
       <c r="J178" s="32"/>
@@ -18748,7 +18706,7 @@
         <v>74</v>
       </c>
       <c r="O178" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P178" s="21">
         <v>43557</v>
@@ -18757,13 +18715,13 @@
       <c r="R178" s="14"/>
       <c r="S178" s="14"/>
       <c r="T178" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U178" s="5"/>
       <c r="V178" s="32"/>
       <c r="W178" s="33"/>
     </row>
-    <row r="179" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <f t="shared" si="8"/>
         <v>177</v>
@@ -18775,7 +18733,7 @@
         <v>43557</v>
       </c>
       <c r="D179" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E179" s="32" t="s">
         <v>15</v>
@@ -18787,7 +18745,7 @@
         <v>581</v>
       </c>
       <c r="H179" s="32" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="I179" s="14"/>
       <c r="J179" s="32"/>
@@ -18800,7 +18758,7 @@
         <v>74</v>
       </c>
       <c r="O179" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P179" s="21">
         <v>43557</v>
@@ -18809,13 +18767,13 @@
       <c r="R179" s="14"/>
       <c r="S179" s="14"/>
       <c r="T179" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U179" s="5"/>
       <c r="V179" s="32"/>
       <c r="W179" s="33"/>
     </row>
-    <row r="180" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <f t="shared" si="8"/>
         <v>178</v>
@@ -18827,7 +18785,7 @@
         <v>43557</v>
       </c>
       <c r="D180" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E180" s="32" t="s">
         <v>15</v>
@@ -18839,7 +18797,7 @@
         <v>581</v>
       </c>
       <c r="H180" s="32" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="I180" s="14"/>
       <c r="J180" s="32"/>
@@ -18852,7 +18810,7 @@
         <v>74</v>
       </c>
       <c r="O180" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P180" s="21">
         <v>43557</v>
@@ -18861,13 +18819,13 @@
       <c r="R180" s="14"/>
       <c r="S180" s="14"/>
       <c r="T180" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U180" s="5"/>
       <c r="V180" s="32"/>
       <c r="W180" s="33"/>
     </row>
-    <row r="181" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <f t="shared" si="8"/>
         <v>179</v>
@@ -18879,7 +18837,7 @@
         <v>43557</v>
       </c>
       <c r="D181" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E181" s="32" t="s">
         <v>15</v>
@@ -18891,7 +18849,7 @@
         <v>581</v>
       </c>
       <c r="H181" s="32" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="I181" s="14"/>
       <c r="J181" s="32"/>
@@ -18904,7 +18862,7 @@
         <v>74</v>
       </c>
       <c r="O181" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P181" s="21">
         <v>43557</v>
@@ -18913,13 +18871,13 @@
       <c r="R181" s="14"/>
       <c r="S181" s="14"/>
       <c r="T181" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U181" s="5"/>
       <c r="V181" s="32"/>
       <c r="W181" s="33"/>
     </row>
-    <row r="182" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <f>1+A181</f>
         <v>180</v>
@@ -18931,7 +18889,7 @@
         <v>43557</v>
       </c>
       <c r="D182" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E182" s="32" t="s">
         <v>15</v>
@@ -18943,7 +18901,7 @@
         <v>581</v>
       </c>
       <c r="H182" s="32" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="I182" s="14"/>
       <c r="J182" s="32"/>
@@ -18956,7 +18914,7 @@
         <v>74</v>
       </c>
       <c r="O182" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P182" s="21">
         <v>43557</v>
@@ -18965,13 +18923,13 @@
       <c r="R182" s="14"/>
       <c r="S182" s="14"/>
       <c r="T182" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U182" s="5"/>
       <c r="V182" s="32"/>
       <c r="W182" s="33"/>
     </row>
-    <row r="183" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <f t="shared" si="8"/>
         <v>181</v>
@@ -18983,7 +18941,7 @@
         <v>43557</v>
       </c>
       <c r="D183" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E183" s="32" t="s">
         <v>15</v>
@@ -18995,7 +18953,7 @@
         <v>581</v>
       </c>
       <c r="H183" s="32" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="I183" s="14"/>
       <c r="J183" s="32"/>
@@ -19008,7 +18966,7 @@
         <v>74</v>
       </c>
       <c r="O183" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P183" s="21">
         <v>43557</v>
@@ -19017,13 +18975,13 @@
       <c r="R183" s="14"/>
       <c r="S183" s="14"/>
       <c r="T183" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U183" s="5"/>
       <c r="V183" s="32"/>
       <c r="W183" s="33"/>
     </row>
-    <row r="184" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <f t="shared" si="8"/>
         <v>182</v>
@@ -19035,7 +18993,7 @@
         <v>43557</v>
       </c>
       <c r="D184" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E184" s="32" t="s">
         <v>15</v>
@@ -19047,7 +19005,7 @@
         <v>581</v>
       </c>
       <c r="H184" s="32" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="I184" s="14"/>
       <c r="J184" s="32"/>
@@ -19060,7 +19018,7 @@
         <v>74</v>
       </c>
       <c r="O184" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P184" s="21">
         <v>43557</v>
@@ -19069,13 +19027,13 @@
       <c r="R184" s="14"/>
       <c r="S184" s="14"/>
       <c r="T184" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U184" s="5"/>
       <c r="V184" s="32"/>
       <c r="W184" s="33"/>
     </row>
-    <row r="185" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A185" s="5">
         <f t="shared" si="8"/>
         <v>183</v>
@@ -19087,7 +19045,7 @@
         <v>43557</v>
       </c>
       <c r="D185" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E185" s="32" t="s">
         <v>15</v>
@@ -19099,7 +19057,7 @@
         <v>581</v>
       </c>
       <c r="H185" s="32" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="I185" s="14"/>
       <c r="J185" s="32"/>
@@ -19112,7 +19070,7 @@
         <v>74</v>
       </c>
       <c r="O185" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P185" s="21">
         <v>43557</v>
@@ -19121,13 +19079,13 @@
       <c r="R185" s="14"/>
       <c r="S185" s="14"/>
       <c r="T185" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U185" s="5"/>
       <c r="V185" s="32"/>
       <c r="W185" s="33"/>
     </row>
-    <row r="186" spans="1:23" ht="135" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <f>1+A185</f>
         <v>184</v>
@@ -19139,7 +19097,7 @@
         <v>43557</v>
       </c>
       <c r="D186" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E186" s="32" t="s">
         <v>15</v>
@@ -19151,7 +19109,7 @@
         <v>581</v>
       </c>
       <c r="H186" s="32" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="I186" s="14"/>
       <c r="J186" s="32"/>
@@ -19164,7 +19122,7 @@
         <v>74</v>
       </c>
       <c r="O186" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P186" s="21">
         <v>43557</v>
@@ -19173,13 +19131,13 @@
       <c r="R186" s="14"/>
       <c r="S186" s="14"/>
       <c r="T186" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U186" s="5"/>
       <c r="V186" s="32"/>
       <c r="W186" s="33"/>
     </row>
-    <row r="187" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <f>1+A186</f>
         <v>185</v>
@@ -19191,7 +19149,7 @@
         <v>43557</v>
       </c>
       <c r="D187" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E187" s="32" t="s">
         <v>15</v>
@@ -19203,7 +19161,7 @@
         <v>580</v>
       </c>
       <c r="H187" s="32" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="I187" s="14"/>
       <c r="J187" s="32"/>
@@ -19216,7 +19174,7 @@
         <v>74</v>
       </c>
       <c r="O187" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P187" s="21">
         <v>43557</v>
@@ -19225,15 +19183,15 @@
       <c r="R187" s="14"/>
       <c r="S187" s="14"/>
       <c r="T187" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U187" s="5"/>
       <c r="V187" s="32" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="W187" s="33"/>
     </row>
-    <row r="188" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <f t="shared" ref="A188:A191" si="9">1+A187</f>
         <v>186</v>
@@ -19245,7 +19203,7 @@
         <v>43557</v>
       </c>
       <c r="D188" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E188" s="32" t="s">
         <v>15</v>
@@ -19257,7 +19215,7 @@
         <v>581</v>
       </c>
       <c r="H188" s="32" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="I188" s="14"/>
       <c r="J188" s="32"/>
@@ -19270,7 +19228,7 @@
         <v>74</v>
       </c>
       <c r="O188" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P188" s="21">
         <v>43557</v>
@@ -19279,13 +19237,13 @@
       <c r="R188" s="14"/>
       <c r="S188" s="14"/>
       <c r="T188" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U188" s="5"/>
       <c r="V188" s="32"/>
       <c r="W188" s="33"/>
     </row>
-    <row r="189" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
         <f t="shared" si="9"/>
         <v>187</v>
@@ -19297,7 +19255,7 @@
         <v>43557</v>
       </c>
       <c r="D189" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E189" s="32" t="s">
         <v>15</v>
@@ -19309,7 +19267,7 @@
         <v>580</v>
       </c>
       <c r="H189" s="32" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="I189" s="14"/>
       <c r="J189" s="32"/>
@@ -19322,7 +19280,7 @@
         <v>74</v>
       </c>
       <c r="O189" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P189" s="21">
         <v>43557</v>
@@ -19331,13 +19289,13 @@
       <c r="R189" s="14"/>
       <c r="S189" s="14"/>
       <c r="T189" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U189" s="5"/>
       <c r="V189" s="32"/>
       <c r="W189" s="33"/>
     </row>
-    <row r="190" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A190" s="5">
         <f t="shared" si="9"/>
         <v>188</v>
@@ -19349,7 +19307,7 @@
         <v>43557</v>
       </c>
       <c r="D190" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E190" s="32" t="s">
         <v>15</v>
@@ -19361,7 +19319,7 @@
         <v>580</v>
       </c>
       <c r="H190" s="32" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="I190" s="14"/>
       <c r="J190" s="32"/>
@@ -19374,7 +19332,7 @@
         <v>74</v>
       </c>
       <c r="O190" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P190" s="21">
         <v>43557</v>
@@ -19383,13 +19341,13 @@
       <c r="R190" s="14"/>
       <c r="S190" s="14"/>
       <c r="T190" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U190" s="5"/>
       <c r="V190" s="32"/>
       <c r="W190" s="33"/>
     </row>
-    <row r="191" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <f t="shared" si="9"/>
         <v>189</v>
@@ -19401,7 +19359,7 @@
         <v>43557</v>
       </c>
       <c r="D191" s="28" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E191" s="32" t="s">
         <v>15</v>
@@ -19412,8 +19370,8 @@
       <c r="G191" s="32" t="s">
         <v>580</v>
       </c>
-      <c r="H191" s="111" t="s">
-        <v>632</v>
+      <c r="H191" s="32" t="s">
+        <v>636</v>
       </c>
       <c r="I191" s="14"/>
       <c r="J191" s="32"/>
@@ -19426,7 +19384,7 @@
         <v>74</v>
       </c>
       <c r="O191" s="32" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="P191" s="21">
         <v>43557</v>
@@ -19435,37 +19393,37 @@
       <c r="R191" s="14"/>
       <c r="S191" s="14"/>
       <c r="T191" s="14" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="U191" s="5"/>
       <c r="V191" s="32"/>
       <c r="W191" s="33"/>
     </row>
-    <row r="192" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="B192" s="110"/>
+    <row r="192" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B192" s="105"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:X191" xr:uid="{11EADDAE-1EA5-4909-A1FD-209D3B9E7E7D}"/>
+  <autoFilter ref="A2:X191"/>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D132" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D132" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Values!$D$4:$D$6</xm:f>
           </x14:formula1>
@@ -19478,20 +19436,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -19499,7 +19457,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
@@ -19507,7 +19465,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
@@ -19515,7 +19473,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
@@ -19523,31 +19481,31 @@
         <v>583</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>586</v>
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>585</v>
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>584</v>
       </c>
@@ -19559,19 +19517,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>144</v>
       </c>
@@ -19582,7 +19540,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -19593,7 +19551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -19604,7 +19562,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -19615,7 +19573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -19626,7 +19584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -19637,7 +19595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -19648,7 +19606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -19659,7 +19617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>145</v>
       </c>
@@ -19677,17 +19635,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="65" t="s">
         <v>206</v>
       </c>
@@ -19695,25 +19653,25 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69"/>
       <c r="C3" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="70"/>
       <c r="C4" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71"/>
       <c r="C5" s="72" t="s">
         <v>205</v>
@@ -19735,6 +19693,29 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19906,29 +19887,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
@@ -19938,6 +19896,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19953,20 +19927,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added CR's for feedback from client on 4th April
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="668">
   <si>
     <t>S.No.</t>
   </si>
@@ -6058,6 +6058,376 @@
       <t>:
 Provide a search feature for the list of packets on the upload page - Partial Search mechanism</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+If the RO forgets user name - provide a link to the Admin portal so that the user can retrieve the username. Dependency on the Admin portal to define the flow.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+'Forgot password' should be a link instead of a button.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator On-boarding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The landing page should have a placeholder for training content. UX team to come up with the design.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator On-boarding - Exceptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+Morocco screens will capture only irises and not fingerprints. Create a new screen showing iris exceptions aligned at the centre. Similarly if a country captures fingerprints only, the fingerprint exception images should be centre aligned.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator On-boarding - Biometrics capture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:
+When a biometric is captured, validate that its quality meets the threshold before sending to server for authentication. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator On-boarding - Biometrics capture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The exceptions marked in the previous screen need not be displayed as text notes in the subsequent fingerprint and iris capture pages. Remove the exceptions displayed on these pages.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Operator On-boarding - Photo capture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The exception photo should not be captured. Remove this.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>EoD Process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+On load of the EoD page, the first packet should be selected by default.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>EoD Process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The acknowledgement slip should be smaller - no scrolling should be required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>EoD Process</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The 'Approve' and 'Reject' actions should be placed closer to the list. Suggestion - provide 'tick' and 'cross' buttons on each row in the list. Buttons will be greyed out by default and become active when the row is selected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Home page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The content in the 'news and updates' section should be configurable. The Admin should be able to add text content through the Admin portal, such as news, announcements, links and training material, and sync to display on the reg. client.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Upload packet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The list of registrations should include:
+a. A new column for registration date
+b. Sorting of list by ascending and descending order on clicking the headers
+c. Excel icon to export the data in csv format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Upload packet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+The width of the table should be reduced and not run across the entire page.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprint 9 - UI Demo Feedback from Shrikant on 04Apr19</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EoD Process:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>The list of registrations should include:
+a. A Search field to perform partial search on the RID
+b. Sorting of list by ascending and descending order on clicking the headers
+c. Excel icon to export the data in csv format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EoD Process:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Add the registration date as a new column.</t>
+    </r>
+  </si>
+  <si>
+    <t>MOS-21996</t>
+  </si>
+  <si>
+    <t>MOS-21997</t>
+  </si>
+  <si>
+    <t>MOS-21998</t>
+  </si>
+  <si>
+    <t>MOS-21999</t>
+  </si>
+  <si>
+    <t>MOS-22000</t>
+  </si>
+  <si>
+    <t>MOS-22001</t>
+  </si>
+  <si>
+    <t>MOS-22005</t>
+  </si>
+  <si>
+    <t>MOS-22006</t>
+  </si>
+  <si>
+    <t>MOS-22007</t>
+  </si>
+  <si>
+    <t>MOS-22008</t>
+  </si>
+  <si>
+    <t>MOS-22009</t>
+  </si>
+  <si>
+    <t>MOS-22010</t>
+  </si>
+  <si>
+    <t>MOS-22011</t>
+  </si>
+  <si>
+    <t>MOS-22012</t>
+  </si>
+  <si>
+    <t>MOS-22013</t>
   </si>
 </sst>
 </file>
@@ -6437,7 +6807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6733,9 +7103,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6757,6 +7124,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8316,11 +8698,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X192"/>
+  <dimension ref="A1:X237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G190" sqref="G190"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -8352,30 +8734,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="108" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="112"/>
-      <c r="T1" s="112"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="113"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="110"/>
+      <c r="V1" s="112"/>
     </row>
     <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -8512,7 +8894,7 @@
       <c r="V3" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="W3" s="107"/>
+      <c r="W3" s="106"/>
     </row>
     <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
@@ -8577,7 +8959,7 @@
       <c r="V4" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="W4" s="107"/>
+      <c r="W4" s="106"/>
     </row>
     <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
@@ -8643,7 +9025,7 @@
       <c r="V5" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="W5" s="107"/>
+      <c r="W5" s="106"/>
     </row>
     <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
@@ -8709,7 +9091,7 @@
       <c r="V6" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="W6" s="107"/>
+      <c r="W6" s="106"/>
     </row>
     <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
@@ -8775,7 +9157,7 @@
       <c r="V7" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="W7" s="107"/>
+      <c r="W7" s="106"/>
     </row>
     <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
@@ -8841,7 +9223,7 @@
       <c r="V8" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="W8" s="107"/>
+      <c r="W8" s="106"/>
     </row>
     <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
@@ -8905,7 +9287,7 @@
       <c r="V9" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="W9" s="107"/>
+      <c r="W9" s="106"/>
     </row>
     <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
@@ -8969,7 +9351,7 @@
       <c r="V10" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="W10" s="107"/>
+      <c r="W10" s="106"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
@@ -9027,7 +9409,7 @@
       <c r="T11" s="30"/>
       <c r="U11" s="30"/>
       <c r="V11" s="21"/>
-      <c r="W11" s="108"/>
+      <c r="W11" s="107"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
@@ -9086,7 +9468,7 @@
       <c r="V12" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="W12" s="108"/>
+      <c r="W12" s="107"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
@@ -12814,7 +13196,7 @@
         <v>165</v>
       </c>
       <c r="W72" s="21"/>
-      <c r="X72" s="106"/>
+      <c r="X72" s="105"/>
     </row>
     <row r="73" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
@@ -12935,7 +13317,7 @@
       <c r="U74" s="5"/>
       <c r="V74" s="5"/>
       <c r="W74" s="21"/>
-      <c r="X74" s="106"/>
+      <c r="X74" s="105"/>
     </row>
     <row r="75" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
@@ -13194,7 +13576,7 @@
         <v>253</v>
       </c>
       <c r="W78" s="21"/>
-      <c r="X78" s="106"/>
+      <c r="X78" s="105"/>
     </row>
     <row r="79" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
@@ -13257,7 +13639,7 @@
       <c r="U79" s="5"/>
       <c r="V79" s="5"/>
       <c r="W79" s="21"/>
-      <c r="X79" s="106"/>
+      <c r="X79" s="105"/>
     </row>
     <row r="80" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
@@ -13322,7 +13704,7 @@
         <v>258</v>
       </c>
       <c r="W80" s="21"/>
-      <c r="X80" s="106"/>
+      <c r="X80" s="105"/>
     </row>
     <row r="81" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
@@ -13385,7 +13767,7 @@
       <c r="U81" s="5"/>
       <c r="V81" s="5"/>
       <c r="W81" s="21"/>
-      <c r="X81" s="106"/>
+      <c r="X81" s="105"/>
     </row>
     <row r="82" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
@@ -13450,7 +13832,7 @@
         <v>259</v>
       </c>
       <c r="W82" s="21"/>
-      <c r="X82" s="106"/>
+      <c r="X82" s="105"/>
     </row>
     <row r="83" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
@@ -13578,7 +13960,7 @@
         <v>446</v>
       </c>
       <c r="W84" s="21"/>
-      <c r="X84" s="106"/>
+      <c r="X84" s="105"/>
     </row>
     <row r="85" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
@@ -19399,8 +19781,968 @@
       <c r="V191" s="32"/>
       <c r="W191" s="33"/>
     </row>
-    <row r="192" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B192" s="105"/>
+    <row r="192" spans="1:23" ht="56" x14ac:dyDescent="0.3">
+      <c r="A192" s="5">
+        <f>1+A191</f>
+        <v>190</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C192" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D192" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E192" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F192" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G192" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H192" s="116" t="s">
+        <v>637</v>
+      </c>
+      <c r="I192" s="14"/>
+      <c r="J192" s="32"/>
+      <c r="K192" s="32"/>
+      <c r="L192" s="32"/>
+      <c r="M192" s="32">
+        <v>1</v>
+      </c>
+      <c r="N192" s="32"/>
+      <c r="O192" s="32"/>
+      <c r="P192" s="32"/>
+      <c r="Q192" s="31"/>
+      <c r="R192" s="14"/>
+      <c r="S192" s="14"/>
+      <c r="T192" s="14"/>
+      <c r="U192" s="5"/>
+    </row>
+    <row r="193" spans="1:21" ht="28" x14ac:dyDescent="0.3">
+      <c r="A193" s="5">
+        <f t="shared" ref="A193:A206" si="10">1+A192</f>
+        <v>191</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="C193" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D193" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E193" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F193" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G193" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H193" s="116" t="s">
+        <v>638</v>
+      </c>
+      <c r="I193" s="14"/>
+      <c r="J193" s="32"/>
+      <c r="K193" s="32"/>
+      <c r="L193" s="32"/>
+      <c r="M193" s="32">
+        <v>1</v>
+      </c>
+      <c r="N193" s="32"/>
+      <c r="O193" s="32"/>
+      <c r="P193" s="32"/>
+      <c r="Q193" s="31"/>
+      <c r="R193" s="14"/>
+      <c r="S193" s="14"/>
+      <c r="T193" s="14"/>
+      <c r="U193" s="5"/>
+    </row>
+    <row r="194" spans="1:21" ht="42" x14ac:dyDescent="0.3">
+      <c r="A194" s="5">
+        <f t="shared" si="10"/>
+        <v>192</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="C194" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D194" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E194" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F194" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G194" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H194" s="116" t="s">
+        <v>639</v>
+      </c>
+      <c r="I194" s="14"/>
+      <c r="J194" s="32"/>
+      <c r="K194" s="32"/>
+      <c r="L194" s="32"/>
+      <c r="M194" s="32">
+        <v>1</v>
+      </c>
+      <c r="N194" s="32"/>
+      <c r="O194" s="32"/>
+      <c r="P194" s="32"/>
+      <c r="Q194" s="31"/>
+      <c r="R194" s="14"/>
+      <c r="S194" s="14"/>
+      <c r="T194" s="14"/>
+      <c r="U194" s="5"/>
+    </row>
+    <row r="195" spans="1:21" ht="70" x14ac:dyDescent="0.3">
+      <c r="A195" s="5">
+        <f t="shared" si="10"/>
+        <v>193</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="C195" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D195" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E195" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F195" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G195" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H195" s="116" t="s">
+        <v>640</v>
+      </c>
+      <c r="I195" s="14"/>
+      <c r="J195" s="32"/>
+      <c r="K195" s="32"/>
+      <c r="L195" s="32"/>
+      <c r="M195" s="32">
+        <v>1</v>
+      </c>
+      <c r="N195" s="32"/>
+      <c r="O195" s="32"/>
+      <c r="P195" s="32"/>
+      <c r="Q195" s="31"/>
+      <c r="R195" s="14"/>
+      <c r="S195" s="14"/>
+      <c r="T195" s="14"/>
+      <c r="U195" s="5"/>
+    </row>
+    <row r="196" spans="1:21" ht="42" x14ac:dyDescent="0.3">
+      <c r="A196" s="5">
+        <f>1+A195</f>
+        <v>194</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="C196" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D196" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E196" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F196" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G196" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H196" s="116" t="s">
+        <v>641</v>
+      </c>
+      <c r="I196" s="14"/>
+      <c r="J196" s="32"/>
+      <c r="K196" s="32"/>
+      <c r="L196" s="32"/>
+      <c r="M196" s="32">
+        <v>1</v>
+      </c>
+      <c r="N196" s="32"/>
+      <c r="O196" s="32"/>
+      <c r="P196" s="32"/>
+      <c r="Q196" s="31"/>
+      <c r="R196" s="14"/>
+      <c r="S196" s="14"/>
+      <c r="T196" s="14"/>
+      <c r="U196" s="5"/>
+    </row>
+    <row r="197" spans="1:21" ht="56" x14ac:dyDescent="0.3">
+      <c r="A197" s="5">
+        <f t="shared" si="10"/>
+        <v>195</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="C197" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D197" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E197" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F197" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G197" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H197" s="116" t="s">
+        <v>642</v>
+      </c>
+      <c r="I197" s="14"/>
+      <c r="J197" s="32"/>
+      <c r="K197" s="32"/>
+      <c r="L197" s="32"/>
+      <c r="M197" s="32">
+        <v>1</v>
+      </c>
+      <c r="N197" s="32"/>
+      <c r="O197" s="32"/>
+      <c r="P197" s="32"/>
+      <c r="Q197" s="31"/>
+      <c r="R197" s="14"/>
+      <c r="S197" s="14"/>
+      <c r="T197" s="14"/>
+      <c r="U197" s="5"/>
+    </row>
+    <row r="198" spans="1:21" ht="28" x14ac:dyDescent="0.3">
+      <c r="A198" s="5">
+        <f>1+A197</f>
+        <v>196</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="C198" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D198" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E198" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F198" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G198" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H198" s="116" t="s">
+        <v>643</v>
+      </c>
+      <c r="I198" s="14"/>
+      <c r="J198" s="32"/>
+      <c r="K198" s="32"/>
+      <c r="L198" s="32"/>
+      <c r="M198" s="32">
+        <v>1</v>
+      </c>
+      <c r="N198" s="32"/>
+      <c r="O198" s="32"/>
+      <c r="P198" s="32"/>
+      <c r="Q198" s="31"/>
+      <c r="R198" s="14"/>
+      <c r="S198" s="14"/>
+      <c r="T198" s="14"/>
+      <c r="U198" s="5"/>
+    </row>
+    <row r="199" spans="1:21" ht="42" x14ac:dyDescent="0.3">
+      <c r="A199" s="5">
+        <f>1+A198</f>
+        <v>197</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="C199" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D199" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E199" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F199" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G199" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H199" s="116" t="s">
+        <v>644</v>
+      </c>
+      <c r="I199" s="14"/>
+      <c r="J199" s="32"/>
+      <c r="K199" s="32"/>
+      <c r="L199" s="32"/>
+      <c r="M199" s="32">
+        <v>1</v>
+      </c>
+      <c r="N199" s="32"/>
+      <c r="O199" s="32"/>
+      <c r="P199" s="32"/>
+      <c r="Q199" s="31"/>
+      <c r="R199" s="14"/>
+      <c r="S199" s="14"/>
+      <c r="T199" s="14"/>
+      <c r="U199" s="5"/>
+    </row>
+    <row r="200" spans="1:21" ht="42" x14ac:dyDescent="0.3">
+      <c r="A200" s="5">
+        <f>1+A199</f>
+        <v>198</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="C200" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D200" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E200" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F200" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G200" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H200" s="116" t="s">
+        <v>645</v>
+      </c>
+      <c r="I200" s="14"/>
+      <c r="J200" s="32"/>
+      <c r="K200" s="32"/>
+      <c r="L200" s="32"/>
+      <c r="M200" s="32">
+        <v>1</v>
+      </c>
+      <c r="N200" s="32"/>
+      <c r="O200" s="32"/>
+      <c r="P200" s="32"/>
+      <c r="Q200" s="31"/>
+      <c r="R200" s="14"/>
+      <c r="S200" s="14"/>
+      <c r="T200" s="14"/>
+      <c r="U200" s="5"/>
+    </row>
+    <row r="201" spans="1:21" ht="70" x14ac:dyDescent="0.3">
+      <c r="A201" s="5">
+        <f t="shared" si="10"/>
+        <v>199</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="C201" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D201" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E201" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F201" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G201" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H201" s="116" t="s">
+        <v>646</v>
+      </c>
+      <c r="I201" s="14"/>
+      <c r="J201" s="32"/>
+      <c r="K201" s="32"/>
+      <c r="L201" s="32"/>
+      <c r="M201" s="32">
+        <v>1</v>
+      </c>
+      <c r="N201" s="32"/>
+      <c r="O201" s="32"/>
+      <c r="P201" s="32"/>
+      <c r="Q201" s="31"/>
+      <c r="R201" s="14"/>
+      <c r="S201" s="14"/>
+      <c r="T201" s="14"/>
+      <c r="U201" s="5"/>
+    </row>
+    <row r="202" spans="1:21" ht="84" x14ac:dyDescent="0.3">
+      <c r="A202" s="5">
+        <f>1+A201</f>
+        <v>200</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="C202" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D202" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E202" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G202" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H202" s="117" t="s">
+        <v>651</v>
+      </c>
+      <c r="I202" s="14"/>
+      <c r="J202" s="32"/>
+      <c r="K202" s="32"/>
+      <c r="L202" s="32"/>
+      <c r="M202" s="32">
+        <v>1</v>
+      </c>
+      <c r="N202" s="32"/>
+      <c r="O202" s="32"/>
+      <c r="P202" s="32"/>
+      <c r="Q202" s="31"/>
+      <c r="R202" s="14"/>
+      <c r="S202" s="14"/>
+      <c r="T202" s="14"/>
+      <c r="U202" s="5"/>
+    </row>
+    <row r="203" spans="1:21" ht="28" x14ac:dyDescent="0.3">
+      <c r="A203" s="5">
+        <f t="shared" si="10"/>
+        <v>201</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="C203" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D203" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E203" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F203" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G203" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H203" s="117" t="s">
+        <v>652</v>
+      </c>
+      <c r="I203" s="14"/>
+      <c r="J203" s="32"/>
+      <c r="K203" s="32"/>
+      <c r="L203" s="32"/>
+      <c r="M203" s="32">
+        <v>1</v>
+      </c>
+      <c r="N203" s="32"/>
+      <c r="O203" s="32"/>
+      <c r="P203" s="32"/>
+      <c r="Q203" s="31"/>
+      <c r="R203" s="14"/>
+      <c r="S203" s="14"/>
+      <c r="T203" s="14"/>
+      <c r="U203" s="5"/>
+    </row>
+    <row r="204" spans="1:21" ht="70" x14ac:dyDescent="0.3">
+      <c r="A204" s="5">
+        <f t="shared" si="10"/>
+        <v>202</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C204" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D204" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E204" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F204" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G204" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H204" s="116" t="s">
+        <v>647</v>
+      </c>
+      <c r="I204" s="14"/>
+      <c r="J204" s="32"/>
+      <c r="K204" s="32"/>
+      <c r="L204" s="32"/>
+      <c r="M204" s="32">
+        <v>1</v>
+      </c>
+      <c r="N204" s="32"/>
+      <c r="O204" s="32"/>
+      <c r="P204" s="32"/>
+      <c r="Q204" s="31"/>
+      <c r="R204" s="14"/>
+      <c r="S204" s="14"/>
+      <c r="T204" s="14"/>
+      <c r="U204" s="5"/>
+    </row>
+    <row r="205" spans="1:21" ht="84" x14ac:dyDescent="0.3">
+      <c r="A205" s="5">
+        <f t="shared" si="10"/>
+        <v>203</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="C205" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D205" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E205" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F205" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G205" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="H205" s="116" t="s">
+        <v>648</v>
+      </c>
+      <c r="I205" s="14"/>
+      <c r="J205" s="32"/>
+      <c r="K205" s="32"/>
+      <c r="L205" s="32"/>
+      <c r="M205" s="32">
+        <v>1</v>
+      </c>
+      <c r="N205" s="32"/>
+      <c r="O205" s="32"/>
+      <c r="P205" s="32"/>
+      <c r="Q205" s="31"/>
+      <c r="R205" s="14"/>
+      <c r="S205" s="14"/>
+      <c r="T205" s="14"/>
+      <c r="U205" s="5"/>
+    </row>
+    <row r="206" spans="1:21" ht="42" x14ac:dyDescent="0.3">
+      <c r="A206" s="5">
+        <f t="shared" si="10"/>
+        <v>204</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="C206" s="6">
+        <v>43559</v>
+      </c>
+      <c r="D206" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="E206" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F206" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G206" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="H206" s="116" t="s">
+        <v>649</v>
+      </c>
+      <c r="I206" s="14"/>
+      <c r="J206" s="32"/>
+      <c r="K206" s="32"/>
+      <c r="L206" s="32"/>
+      <c r="M206" s="32">
+        <v>1</v>
+      </c>
+      <c r="N206" s="32"/>
+      <c r="O206" s="32"/>
+      <c r="P206" s="32"/>
+      <c r="Q206" s="31"/>
+      <c r="R206" s="14"/>
+      <c r="S206" s="14"/>
+      <c r="T206" s="14"/>
+      <c r="U206" s="5"/>
+    </row>
+    <row r="207" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A207" s="5"/>
+      <c r="B207" s="31"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="32"/>
+      <c r="E207" s="32"/>
+      <c r="F207" s="32"/>
+      <c r="G207" s="113"/>
+      <c r="H207" s="113"/>
+      <c r="I207" s="14"/>
+      <c r="J207" s="32"/>
+      <c r="K207" s="32"/>
+      <c r="L207" s="32"/>
+      <c r="M207" s="32"/>
+      <c r="N207" s="32"/>
+      <c r="O207" s="32"/>
+      <c r="P207" s="32"/>
+      <c r="Q207" s="31"/>
+      <c r="R207" s="14"/>
+      <c r="S207" s="14"/>
+      <c r="T207" s="14"/>
+      <c r="U207" s="5"/>
+    </row>
+    <row r="208" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A208" s="5"/>
+      <c r="B208" s="31"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="32"/>
+      <c r="E208" s="32"/>
+      <c r="F208" s="32"/>
+      <c r="G208" s="113"/>
+      <c r="H208" s="113"/>
+      <c r="I208" s="14"/>
+      <c r="J208" s="32"/>
+      <c r="K208" s="32"/>
+      <c r="L208" s="32"/>
+      <c r="M208" s="32"/>
+      <c r="N208" s="32"/>
+      <c r="O208" s="32"/>
+      <c r="P208" s="32"/>
+      <c r="Q208" s="31"/>
+      <c r="R208" s="14"/>
+      <c r="S208" s="14"/>
+      <c r="T208" s="14"/>
+      <c r="U208" s="5"/>
+    </row>
+    <row r="209" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A209" s="5"/>
+      <c r="B209" s="31"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="32"/>
+      <c r="E209" s="32"/>
+      <c r="F209" s="32"/>
+      <c r="G209" s="113"/>
+      <c r="H209" s="113"/>
+      <c r="I209" s="14"/>
+      <c r="J209" s="32"/>
+      <c r="K209" s="32"/>
+      <c r="L209" s="32"/>
+      <c r="M209" s="32"/>
+      <c r="N209" s="32"/>
+      <c r="O209" s="32"/>
+      <c r="P209" s="32"/>
+      <c r="Q209" s="31"/>
+      <c r="R209" s="14"/>
+      <c r="S209" s="14"/>
+      <c r="T209" s="14"/>
+      <c r="U209" s="5"/>
+    </row>
+    <row r="210" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A210" s="5"/>
+      <c r="B210" s="31"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="32"/>
+      <c r="E210" s="32"/>
+      <c r="F210" s="32"/>
+      <c r="G210" s="113"/>
+      <c r="H210" s="113"/>
+      <c r="I210" s="14"/>
+      <c r="J210" s="32"/>
+      <c r="K210" s="32"/>
+      <c r="L210" s="32"/>
+      <c r="M210" s="32"/>
+      <c r="N210" s="32"/>
+      <c r="O210" s="32"/>
+      <c r="P210" s="32"/>
+      <c r="Q210" s="31"/>
+      <c r="R210" s="14"/>
+      <c r="S210" s="14"/>
+      <c r="T210" s="14"/>
+      <c r="U210" s="5"/>
+    </row>
+    <row r="211" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A211" s="5"/>
+      <c r="B211" s="31"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="32"/>
+      <c r="E211" s="32"/>
+      <c r="F211" s="32"/>
+      <c r="G211" s="113"/>
+      <c r="H211" s="113"/>
+      <c r="I211" s="14"/>
+      <c r="J211" s="32"/>
+      <c r="K211" s="32"/>
+      <c r="L211" s="32"/>
+      <c r="M211" s="32"/>
+      <c r="N211" s="32"/>
+      <c r="O211" s="32"/>
+      <c r="P211" s="32"/>
+      <c r="Q211" s="31"/>
+      <c r="R211" s="14"/>
+      <c r="S211" s="14"/>
+      <c r="T211" s="14"/>
+      <c r="U211" s="5"/>
+    </row>
+    <row r="212" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A212" s="5"/>
+      <c r="B212" s="31"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="32"/>
+      <c r="E212" s="32"/>
+      <c r="F212" s="32"/>
+      <c r="G212" s="113"/>
+      <c r="H212" s="113"/>
+      <c r="I212" s="14"/>
+      <c r="J212" s="32"/>
+      <c r="K212" s="32"/>
+      <c r="L212" s="32"/>
+      <c r="M212" s="32"/>
+      <c r="N212" s="32"/>
+      <c r="O212" s="32"/>
+      <c r="P212" s="32"/>
+      <c r="Q212" s="31"/>
+      <c r="R212" s="14"/>
+      <c r="S212" s="14"/>
+      <c r="T212" s="14"/>
+      <c r="U212" s="5"/>
+    </row>
+    <row r="213" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A213" s="5"/>
+      <c r="B213" s="31"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="32"/>
+      <c r="E213" s="32"/>
+      <c r="F213" s="32"/>
+      <c r="G213" s="113"/>
+      <c r="H213" s="113"/>
+      <c r="I213" s="14"/>
+      <c r="J213" s="32"/>
+      <c r="K213" s="32"/>
+      <c r="L213" s="32"/>
+      <c r="M213" s="32"/>
+      <c r="N213" s="32"/>
+      <c r="O213" s="32"/>
+      <c r="P213" s="32"/>
+      <c r="Q213" s="31"/>
+      <c r="R213" s="14"/>
+      <c r="S213" s="14"/>
+      <c r="T213" s="14"/>
+      <c r="U213" s="5"/>
+    </row>
+    <row r="214" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A214" s="5"/>
+      <c r="B214" s="31"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="32"/>
+      <c r="E214" s="32"/>
+      <c r="F214" s="32"/>
+      <c r="G214" s="113"/>
+      <c r="H214" s="113"/>
+      <c r="I214" s="14"/>
+      <c r="J214" s="32"/>
+      <c r="K214" s="32"/>
+      <c r="L214" s="32"/>
+      <c r="M214" s="32"/>
+      <c r="N214" s="32"/>
+      <c r="O214" s="32"/>
+      <c r="P214" s="32"/>
+      <c r="Q214" s="31"/>
+      <c r="R214" s="14"/>
+      <c r="S214" s="14"/>
+      <c r="T214" s="14"/>
+      <c r="U214" s="5"/>
+    </row>
+    <row r="215" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A215" s="5"/>
+      <c r="B215" s="31"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="32"/>
+      <c r="E215" s="32"/>
+      <c r="F215" s="32"/>
+      <c r="G215" s="113"/>
+      <c r="H215" s="113"/>
+      <c r="I215" s="14"/>
+      <c r="J215" s="32"/>
+      <c r="K215" s="32"/>
+      <c r="L215" s="32"/>
+      <c r="M215" s="32"/>
+      <c r="N215" s="32"/>
+      <c r="O215" s="32"/>
+      <c r="P215" s="32"/>
+      <c r="Q215" s="31"/>
+      <c r="R215" s="14"/>
+      <c r="S215" s="14"/>
+      <c r="T215" s="14"/>
+      <c r="U215" s="5"/>
+    </row>
+    <row r="216" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A216" s="5"/>
+      <c r="B216" s="31"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="32"/>
+      <c r="E216" s="32"/>
+      <c r="F216" s="32"/>
+      <c r="G216" s="113"/>
+      <c r="H216" s="113"/>
+      <c r="I216" s="14"/>
+      <c r="J216" s="32"/>
+      <c r="K216" s="32"/>
+      <c r="L216" s="32"/>
+      <c r="M216" s="32"/>
+      <c r="N216" s="32"/>
+      <c r="O216" s="32"/>
+      <c r="P216" s="32"/>
+      <c r="Q216" s="31"/>
+      <c r="R216" s="14"/>
+      <c r="S216" s="14"/>
+      <c r="T216" s="14"/>
+      <c r="U216" s="5"/>
+    </row>
+    <row r="217" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="5"/>
+      <c r="B217" s="31"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="32"/>
+      <c r="E217" s="32"/>
+      <c r="F217" s="32"/>
+      <c r="G217" s="113"/>
+      <c r="H217" s="113"/>
+      <c r="I217" s="14"/>
+      <c r="J217" s="32"/>
+      <c r="K217" s="32"/>
+      <c r="L217" s="32"/>
+      <c r="M217" s="32"/>
+      <c r="N217" s="32"/>
+      <c r="O217" s="32"/>
+      <c r="P217" s="32"/>
+      <c r="Q217" s="31"/>
+      <c r="R217" s="14"/>
+      <c r="S217" s="14"/>
+      <c r="T217" s="14"/>
+      <c r="U217" s="5"/>
+    </row>
+    <row r="218" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A218" s="5"/>
+      <c r="B218" s="31"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="32"/>
+      <c r="E218" s="32"/>
+      <c r="F218" s="32"/>
+      <c r="G218" s="113"/>
+      <c r="H218" s="113"/>
+      <c r="I218" s="14"/>
+      <c r="J218" s="32"/>
+      <c r="K218" s="32"/>
+      <c r="L218" s="32"/>
+      <c r="M218" s="32"/>
+      <c r="N218" s="32"/>
+      <c r="O218" s="32"/>
+      <c r="P218" s="32"/>
+      <c r="Q218" s="31"/>
+      <c r="R218" s="14"/>
+      <c r="S218" s="14"/>
+      <c r="T218" s="14"/>
+      <c r="U218" s="5"/>
+    </row>
+    <row r="219" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G219" s="115"/>
+      <c r="H219" s="114"/>
+    </row>
+    <row r="220" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G220" s="113"/>
+      <c r="H220" s="114"/>
+    </row>
+    <row r="221" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G221" s="113"/>
+      <c r="H221" s="114"/>
+    </row>
+    <row r="222" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G222" s="113"/>
+    </row>
+    <row r="223" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G223" s="113"/>
+    </row>
+    <row r="224" spans="1:21" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G224" s="113"/>
+    </row>
+    <row r="225" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G225" s="113"/>
+    </row>
+    <row r="226" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G226" s="113"/>
+    </row>
+    <row r="227" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G227" s="113"/>
+    </row>
+    <row r="228" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G228" s="113"/>
+    </row>
+    <row r="229" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G229" s="113"/>
+    </row>
+    <row r="230" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G230" s="113"/>
+    </row>
+    <row r="231" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G231" s="113"/>
+    </row>
+    <row r="232" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G232" s="113"/>
+    </row>
+    <row r="233" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G233" s="113"/>
+    </row>
+    <row r="234" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G234" s="113"/>
+    </row>
+    <row r="235" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G235" s="113"/>
+    </row>
+    <row r="237" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G237" s="113"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:X191"/>
@@ -19427,7 +20769,7 @@
           <x14:formula1>
             <xm:f>Values!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G191</xm:sqref>
+          <xm:sqref>G3:G201</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19684,15 +21026,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -19713,6 +21046,15 @@
     </RatedBy>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19888,14 +21230,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19907,6 +21241,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated Feature Road Map For Karthik
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1047454\git\mosip_master\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA84CC3-B874-4170-80D2-0D7ABDA2E3D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -21,9 +20,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$X$213</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -6662,7 +6661,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -7351,6 +7350,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7365,15 +7373,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7405,7 +7404,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -7422,7 +7421,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:V70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -8583,7 +8582,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -8931,13 +8930,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A147" sqref="A147"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -8950,15 +8949,15 @@
     <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" style="3" customWidth="1"/>
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="16" customWidth="1"/>
     <col min="10" max="10" width="28.453125" style="3" customWidth="1"/>
     <col min="11" max="11" width="38.453125" style="3" customWidth="1"/>
     <col min="12" max="12" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11.1796875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" style="3" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="22.81640625" style="3" customWidth="1"/>
     <col min="15" max="15" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.1796875" style="27" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" style="27" customWidth="1"/>
     <col min="18" max="18" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.81640625" style="16" customWidth="1"/>
     <col min="20" max="20" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
@@ -8969,30 +8968,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="116"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="119"/>
     </row>
     <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
@@ -9065,7 +9064,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -9131,7 +9130,7 @@
       </c>
       <c r="W3" s="106"/>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -9196,7 +9195,7 @@
       </c>
       <c r="W4" s="106"/>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -9262,7 +9261,7 @@
       </c>
       <c r="W5" s="106"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -9328,7 +9327,7 @@
       </c>
       <c r="W6" s="106"/>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -9394,7 +9393,7 @@
       </c>
       <c r="W7" s="106"/>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -9460,7 +9459,7 @@
       </c>
       <c r="W8" s="106"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -9524,7 +9523,7 @@
       </c>
       <c r="W9" s="106"/>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -9588,7 +9587,7 @@
       </c>
       <c r="W10" s="106"/>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -9646,7 +9645,7 @@
       <c r="V11" s="21"/>
       <c r="W11" s="107"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -9705,7 +9704,7 @@
       </c>
       <c r="W12" s="107"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -9762,7 +9761,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -10154,7 +10153,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -10206,7 +10205,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -10258,7 +10257,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -10322,7 +10321,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -10452,7 +10451,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -10506,7 +10505,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -10560,7 +10559,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -10624,7 +10623,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -10690,7 +10689,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -10744,7 +10743,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -10870,7 +10869,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -10936,7 +10935,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" s="8" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -10998,7 +10997,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -11064,7 +11063,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -11125,7 +11124,7 @@
       <c r="V35" s="14"/>
       <c r="W35" s="21"/>
     </row>
-    <row r="36" spans="1:23" ht="182" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -11193,7 +11192,7 @@
       </c>
       <c r="W36" s="21"/>
     </row>
-    <row r="37" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -11263,7 +11262,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -11331,7 +11330,7 @@
       </c>
       <c r="W38" s="21"/>
     </row>
-    <row r="39" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -11399,7 +11398,7 @@
       </c>
       <c r="W39" s="21"/>
     </row>
-    <row r="40" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -11457,7 +11456,7 @@
       <c r="V40" s="32"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -11519,7 +11518,7 @@
       <c r="V41" s="32"/>
       <c r="W41" s="21"/>
     </row>
-    <row r="42" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -11577,7 +11576,7 @@
       <c r="V42" s="32"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -12017,7 +12016,7 @@
       </c>
       <c r="W49" s="21"/>
     </row>
-    <row r="50" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -12084,7 +12083,7 @@
       </c>
       <c r="W50" s="21"/>
     </row>
-    <row r="51" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -12142,7 +12141,7 @@
       <c r="V51" s="32"/>
       <c r="W51" s="21"/>
     </row>
-    <row r="52" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -12196,7 +12195,7 @@
       <c r="V52" s="32"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -12260,7 +12259,7 @@
       </c>
       <c r="W53" s="21"/>
     </row>
-    <row r="54" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -12314,7 +12313,7 @@
       <c r="V54" s="32"/>
       <c r="W54" s="21"/>
     </row>
-    <row r="55" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -12372,7 +12371,7 @@
       <c r="V55" s="32"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -12435,7 +12434,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -12498,7 +12497,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -12562,7 +12561,7 @@
       </c>
       <c r="W58" s="21"/>
     </row>
-    <row r="59" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -12620,7 +12619,7 @@
       <c r="V59" s="32"/>
       <c r="W59" s="21"/>
     </row>
-    <row r="60" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -12678,7 +12677,7 @@
       <c r="V60" s="32"/>
       <c r="W60" s="21"/>
     </row>
-    <row r="61" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -12739,7 +12738,7 @@
       <c r="V61" s="32"/>
       <c r="W61" s="21"/>
     </row>
-    <row r="62" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -12871,7 +12870,7 @@
       </c>
       <c r="W63" s="21"/>
     </row>
-    <row r="64" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -12926,7 +12925,7 @@
       <c r="V64" s="32"/>
       <c r="W64" s="21"/>
     </row>
-    <row r="65" spans="1:24" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -12981,7 +12980,7 @@
       <c r="V65" s="32"/>
       <c r="W65" s="21"/>
     </row>
-    <row r="66" spans="1:24" ht="182" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -13048,7 +13047,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -13112,7 +13111,7 @@
       </c>
       <c r="W67" s="21"/>
     </row>
-    <row r="68" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -13177,7 +13176,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="252" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="252" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -13241,7 +13240,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -13303,7 +13302,7 @@
       <c r="V70" s="32"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -13367,7 +13366,7 @@
       </c>
       <c r="W71" s="21"/>
     </row>
-    <row r="72" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -13433,7 +13432,7 @@
       <c r="W72" s="21"/>
       <c r="X72" s="105"/>
     </row>
-    <row r="73" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -13496,7 +13495,7 @@
       <c r="W73" s="21"/>
       <c r="X73" s="97"/>
     </row>
-    <row r="74" spans="1:24" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:24" ht="84" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -13684,7 +13683,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="196" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" ht="196" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -13748,7 +13747,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" ht="154" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -13813,7 +13812,7 @@
       <c r="W78" s="21"/>
       <c r="X78" s="105"/>
     </row>
-    <row r="79" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -13876,7 +13875,7 @@
       <c r="W79" s="21"/>
       <c r="X79" s="105"/>
     </row>
-    <row r="80" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" ht="126" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -13941,7 +13940,7 @@
       <c r="W80" s="21"/>
       <c r="X80" s="105"/>
     </row>
-    <row r="81" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -14004,7 +14003,7 @@
       <c r="W81" s="21"/>
       <c r="X81" s="105"/>
     </row>
-    <row r="82" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:24" ht="140" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -14132,7 +14131,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="210" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:24" ht="210" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -14197,7 +14196,7 @@
       <c r="W84" s="21"/>
       <c r="X84" s="105"/>
     </row>
-    <row r="85" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -14263,7 +14262,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -14327,7 +14326,7 @@
       <c r="V86" s="32"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:24" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:24" ht="98" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -14390,7 +14389,7 @@
       </c>
       <c r="W87" s="21"/>
     </row>
-    <row r="88" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -14455,7 +14454,7 @@
       </c>
       <c r="W88" s="21"/>
     </row>
-    <row r="89" spans="1:24" ht="294" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:24" ht="294" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -14516,7 +14515,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:24" ht="70" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -14569,7 +14568,7 @@
       <c r="V90" s="32"/>
       <c r="W90" s="21"/>
     </row>
-    <row r="91" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -14620,7 +14619,7 @@
       <c r="V91" s="32"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="168" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:24" ht="168" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -14684,7 +14683,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:24" ht="42" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -14746,7 +14745,7 @@
       <c r="V93" s="32"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -14810,7 +14809,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -14874,7 +14873,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:24" ht="56" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -14938,7 +14937,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -15000,7 +14999,7 @@
       <c r="V97" s="32"/>
       <c r="W97" s="21"/>
     </row>
-    <row r="98" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -15055,7 +15054,7 @@
       <c r="V98" s="32"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -15117,7 +15116,7 @@
       <c r="V99" s="32"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -15181,7 +15180,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="280" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" ht="280" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -15245,7 +15244,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -15307,7 +15306,7 @@
       <c r="V102" s="32"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -15371,7 +15370,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -15435,7 +15434,7 @@
       </c>
       <c r="W104" s="21"/>
     </row>
-    <row r="105" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -15498,7 +15497,7 @@
       <c r="V105" s="33"/>
       <c r="W105" s="21"/>
     </row>
-    <row r="106" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -15561,7 +15560,7 @@
       </c>
       <c r="W106" s="21"/>
     </row>
-    <row r="107" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -15616,7 +15615,7 @@
       <c r="V107" s="32"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -15679,7 +15678,7 @@
       </c>
       <c r="W108" s="21"/>
     </row>
-    <row r="109" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -15797,7 +15796,7 @@
       <c r="V110" s="32"/>
       <c r="W110" s="21"/>
     </row>
-    <row r="111" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -15858,7 +15857,7 @@
       <c r="V111" s="32"/>
       <c r="W111" s="21"/>
     </row>
-    <row r="112" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -15919,7 +15918,7 @@
       <c r="V112" s="32"/>
       <c r="W112" s="21"/>
     </row>
-    <row r="113" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -15980,7 +15979,7 @@
       <c r="V113" s="32"/>
       <c r="W113" s="21"/>
     </row>
-    <row r="114" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -16041,7 +16040,7 @@
       <c r="V114" s="32"/>
       <c r="W114" s="21"/>
     </row>
-    <row r="115" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -16100,7 +16099,7 @@
       <c r="V115" s="32"/>
       <c r="W115" s="21"/>
     </row>
-    <row r="116" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -16150,7 +16149,7 @@
       <c r="V116" s="32"/>
       <c r="W116" s="21"/>
     </row>
-    <row r="117" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -16202,7 +16201,7 @@
       <c r="V117" s="28"/>
       <c r="W117" s="21"/>
     </row>
-    <row r="118" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -16257,7 +16256,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -16312,7 +16311,7 @@
       <c r="V119" s="32"/>
       <c r="W119" s="21"/>
     </row>
-    <row r="120" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>118</v>
       </c>
@@ -16363,7 +16362,7 @@
       <c r="V120" s="32"/>
       <c r="W120" s="21"/>
     </row>
-    <row r="121" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>119</v>
       </c>
@@ -16416,7 +16415,7 @@
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="112" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -16530,7 +16529,7 @@
       <c r="V123" s="32"/>
       <c r="W123" s="21"/>
     </row>
-    <row r="124" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -16581,7 +16580,7 @@
       <c r="V124" s="32"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -16622,6 +16621,9 @@
       </c>
       <c r="P125" s="21">
         <v>43531</v>
+      </c>
+      <c r="Q125" s="27">
+        <v>3</v>
       </c>
       <c r="R125" s="2"/>
       <c r="S125" s="2"/>
@@ -16629,7 +16631,7 @@
       <c r="V125" s="32"/>
       <c r="W125" s="21"/>
     </row>
-    <row r="126" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -16682,7 +16684,7 @@
       </c>
       <c r="W126" s="21"/>
     </row>
-    <row r="127" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -16736,7 +16738,7 @@
       </c>
       <c r="W127" s="21"/>
     </row>
-    <row r="128" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -16790,7 +16792,7 @@
       </c>
       <c r="W128" s="21"/>
     </row>
-    <row r="129" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -16844,7 +16846,7 @@
       </c>
       <c r="W129" s="21"/>
     </row>
-    <row r="130" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -16898,7 +16900,7 @@
       </c>
       <c r="W130" s="21"/>
     </row>
-    <row r="131" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -16952,7 +16954,7 @@
       </c>
       <c r="W131" s="21"/>
     </row>
-    <row r="132" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>130</v>
       </c>
@@ -17594,7 +17596,7 @@
       <c r="V143" s="33"/>
       <c r="W143" s="21"/>
     </row>
-    <row r="144" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>142</v>
       </c>
@@ -17643,7 +17645,7 @@
       <c r="V144" s="33"/>
       <c r="W144" s="21"/>
     </row>
-    <row r="145" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>143</v>
       </c>
@@ -17798,7 +17800,7 @@
       <c r="V147" s="33"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -17851,7 +17853,7 @@
       <c r="V148" s="32"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -17904,7 +17906,7 @@
       <c r="V149" s="32"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -17954,7 +17956,7 @@
       <c r="V150" s="32"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -17993,6 +17995,9 @@
       </c>
       <c r="P151" s="6">
         <v>43553</v>
+      </c>
+      <c r="Q151" s="27">
+        <v>20</v>
       </c>
       <c r="R151" s="5"/>
       <c r="S151" s="5"/>
@@ -18001,7 +18006,7 @@
       <c r="V151" s="32"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -18054,7 +18059,7 @@
       <c r="V152" s="32"/>
       <c r="W152" s="21"/>
     </row>
-    <row r="153" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>151</v>
       </c>
@@ -18103,7 +18108,7 @@
       <c r="V153" s="32"/>
       <c r="W153" s="21"/>
     </row>
-    <row r="154" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>152</v>
       </c>
@@ -18152,7 +18157,7 @@
       <c r="V154" s="32"/>
       <c r="W154" s="21"/>
     </row>
-    <row r="155" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>153</v>
       </c>
@@ -18201,7 +18206,7 @@
       <c r="V155" s="32"/>
       <c r="W155" s="21"/>
     </row>
-    <row r="156" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>154</v>
       </c>
@@ -18250,7 +18255,7 @@
       <c r="V156" s="32"/>
       <c r="W156" s="21"/>
     </row>
-    <row r="157" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>155</v>
       </c>
@@ -18299,7 +18304,7 @@
       <c r="V157" s="32"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -18353,7 +18358,7 @@
       <c r="V158" s="32"/>
       <c r="W158" s="33"/>
     </row>
-    <row r="159" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" ht="210" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -18407,7 +18412,7 @@
       <c r="V159" s="32"/>
       <c r="W159" s="33"/>
     </row>
-    <row r="160" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -18458,7 +18463,7 @@
       <c r="V160" s="28"/>
       <c r="W160" s="33"/>
     </row>
-    <row r="161" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>159</v>
       </c>
@@ -18513,7 +18518,7 @@
       <c r="V161" s="32"/>
       <c r="W161" s="33"/>
     </row>
-    <row r="162" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>160</v>
       </c>
@@ -18568,7 +18573,7 @@
       <c r="V162" s="32"/>
       <c r="W162" s="33"/>
     </row>
-    <row r="163" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>161</v>
       </c>
@@ -18623,7 +18628,7 @@
       <c r="V163" s="32"/>
       <c r="W163" s="33"/>
     </row>
-    <row r="164" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>162</v>
       </c>
@@ -18678,7 +18683,7 @@
       <c r="V164" s="32"/>
       <c r="W164" s="33"/>
     </row>
-    <row r="165" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>163</v>
       </c>
@@ -18733,7 +18738,7 @@
       <c r="V165" s="32"/>
       <c r="W165" s="33"/>
     </row>
-    <row r="166" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>164</v>
       </c>
@@ -18788,7 +18793,7 @@
       <c r="V166" s="32"/>
       <c r="W166" s="33"/>
     </row>
-    <row r="167" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>165</v>
       </c>
@@ -18843,7 +18848,7 @@
       <c r="V167" s="32"/>
       <c r="W167" s="33"/>
     </row>
-    <row r="168" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>166</v>
       </c>
@@ -18898,7 +18903,7 @@
       <c r="V168" s="32"/>
       <c r="W168" s="33"/>
     </row>
-    <row r="169" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>167</v>
       </c>
@@ -18953,7 +18958,7 @@
       <c r="V169" s="32"/>
       <c r="W169" s="33"/>
     </row>
-    <row r="170" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>168</v>
       </c>
@@ -19008,7 +19013,7 @@
       <c r="V170" s="32"/>
       <c r="W170" s="33"/>
     </row>
-    <row r="171" spans="1:23" s="103" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>169</v>
       </c>
@@ -19055,7 +19060,7 @@
       <c r="V171" s="14"/>
       <c r="W171" s="104"/>
     </row>
-    <row r="172" spans="1:23" s="103" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:23" s="103" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>170</v>
       </c>
@@ -19110,7 +19115,7 @@
       <c r="V172" s="14"/>
       <c r="W172" s="104"/>
     </row>
-    <row r="173" spans="1:23" s="103" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" s="103" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>171</v>
       </c>
@@ -19159,7 +19164,7 @@
       <c r="V173" s="14"/>
       <c r="W173" s="104"/>
     </row>
-    <row r="174" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>172</v>
       </c>
@@ -19206,7 +19211,7 @@
       <c r="V174" s="14"/>
       <c r="W174" s="33"/>
     </row>
-    <row r="175" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A175" s="39">
         <f>1+A174</f>
         <v>173</v>
@@ -19241,6 +19246,9 @@
       <c r="N175" s="28"/>
       <c r="O175" s="28"/>
       <c r="P175" s="37"/>
+      <c r="Q175" s="27">
+        <v>10</v>
+      </c>
       <c r="R175" s="39"/>
       <c r="S175" s="39"/>
       <c r="T175" s="87"/>
@@ -19248,7 +19256,7 @@
       <c r="V175" s="28"/>
       <c r="W175" s="38"/>
     </row>
-    <row r="176" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <f t="shared" ref="A176:A185" si="8">1+A175</f>
         <v>174</v>
@@ -19290,7 +19298,9 @@
       <c r="P176" s="21">
         <v>43557</v>
       </c>
-      <c r="Q176" s="31"/>
+      <c r="Q176" s="31">
+        <v>3</v>
+      </c>
       <c r="R176" s="14"/>
       <c r="S176" s="14"/>
       <c r="T176" s="14" t="s">
@@ -19300,7 +19310,7 @@
       <c r="V176" s="32"/>
       <c r="W176" s="33"/>
     </row>
-    <row r="177" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
         <f t="shared" si="8"/>
         <v>175</v>
@@ -19342,7 +19352,9 @@
       <c r="P177" s="21">
         <v>43557</v>
       </c>
-      <c r="Q177" s="31"/>
+      <c r="Q177" s="31">
+        <v>10</v>
+      </c>
       <c r="R177" s="14"/>
       <c r="S177" s="14"/>
       <c r="T177" s="14" t="s">
@@ -19352,7 +19364,7 @@
       <c r="V177" s="32"/>
       <c r="W177" s="33"/>
     </row>
-    <row r="178" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <f t="shared" si="8"/>
         <v>176</v>
@@ -19394,7 +19406,9 @@
       <c r="P178" s="21">
         <v>43557</v>
       </c>
-      <c r="Q178" s="31"/>
+      <c r="Q178" s="31">
+        <v>3</v>
+      </c>
       <c r="R178" s="14"/>
       <c r="S178" s="14"/>
       <c r="T178" s="14" t="s">
@@ -19404,7 +19418,7 @@
       <c r="V178" s="32"/>
       <c r="W178" s="33"/>
     </row>
-    <row r="179" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <f t="shared" si="8"/>
         <v>177</v>
@@ -19446,7 +19460,9 @@
       <c r="P179" s="21">
         <v>43557</v>
       </c>
-      <c r="Q179" s="31"/>
+      <c r="Q179" s="31">
+        <v>3</v>
+      </c>
       <c r="R179" s="14"/>
       <c r="S179" s="14"/>
       <c r="T179" s="14" t="s">
@@ -19456,7 +19472,7 @@
       <c r="V179" s="32"/>
       <c r="W179" s="33"/>
     </row>
-    <row r="180" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <f t="shared" si="8"/>
         <v>178</v>
@@ -19498,7 +19514,9 @@
       <c r="P180" s="21">
         <v>43557</v>
       </c>
-      <c r="Q180" s="31"/>
+      <c r="Q180" s="31">
+        <v>8</v>
+      </c>
       <c r="R180" s="14"/>
       <c r="S180" s="14"/>
       <c r="T180" s="14" t="s">
@@ -19508,7 +19526,7 @@
       <c r="V180" s="32"/>
       <c r="W180" s="33"/>
     </row>
-    <row r="181" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <f t="shared" si="8"/>
         <v>179</v>
@@ -19550,7 +19568,9 @@
       <c r="P181" s="21">
         <v>43557</v>
       </c>
-      <c r="Q181" s="31"/>
+      <c r="Q181" s="31">
+        <v>15</v>
+      </c>
       <c r="R181" s="14"/>
       <c r="S181" s="14"/>
       <c r="T181" s="14" t="s">
@@ -19560,7 +19580,7 @@
       <c r="V181" s="32"/>
       <c r="W181" s="33"/>
     </row>
-    <row r="182" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <f>1+A181</f>
         <v>180</v>
@@ -19602,7 +19622,9 @@
       <c r="P182" s="21">
         <v>43557</v>
       </c>
-      <c r="Q182" s="31"/>
+      <c r="Q182" s="31">
+        <v>3</v>
+      </c>
       <c r="R182" s="14"/>
       <c r="S182" s="14"/>
       <c r="T182" s="14" t="s">
@@ -19612,7 +19634,7 @@
       <c r="V182" s="32"/>
       <c r="W182" s="33"/>
     </row>
-    <row r="183" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <f t="shared" si="8"/>
         <v>181</v>
@@ -19654,7 +19676,9 @@
       <c r="P183" s="21">
         <v>43557</v>
       </c>
-      <c r="Q183" s="31"/>
+      <c r="Q183" s="31">
+        <v>4</v>
+      </c>
       <c r="R183" s="14"/>
       <c r="S183" s="14"/>
       <c r="T183" s="14" t="s">
@@ -19664,7 +19688,7 @@
       <c r="V183" s="32"/>
       <c r="W183" s="33"/>
     </row>
-    <row r="184" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <f t="shared" si="8"/>
         <v>182</v>
@@ -19706,7 +19730,9 @@
       <c r="P184" s="21">
         <v>43557</v>
       </c>
-      <c r="Q184" s="31"/>
+      <c r="Q184" s="31">
+        <v>15</v>
+      </c>
       <c r="R184" s="14"/>
       <c r="S184" s="14"/>
       <c r="T184" s="14" t="s">
@@ -19716,7 +19742,7 @@
       <c r="V184" s="32"/>
       <c r="W184" s="33"/>
     </row>
-    <row r="185" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A185" s="5">
         <f t="shared" si="8"/>
         <v>183</v>
@@ -19758,7 +19784,9 @@
       <c r="P185" s="21">
         <v>43557</v>
       </c>
-      <c r="Q185" s="31"/>
+      <c r="Q185" s="31">
+        <v>5</v>
+      </c>
       <c r="R185" s="14"/>
       <c r="S185" s="14"/>
       <c r="T185" s="14" t="s">
@@ -19768,7 +19796,7 @@
       <c r="V185" s="32"/>
       <c r="W185" s="33"/>
     </row>
-    <row r="186" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <f>1+A185</f>
         <v>184</v>
@@ -19810,7 +19838,9 @@
       <c r="P186" s="21">
         <v>43557</v>
       </c>
-      <c r="Q186" s="31"/>
+      <c r="Q186" s="31">
+        <v>20</v>
+      </c>
       <c r="R186" s="14"/>
       <c r="S186" s="14"/>
       <c r="T186" s="14" t="s">
@@ -19820,7 +19850,7 @@
       <c r="V186" s="32"/>
       <c r="W186" s="33"/>
     </row>
-    <row r="187" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <f>1+A186</f>
         <v>185</v>
@@ -19862,7 +19892,9 @@
       <c r="P187" s="21">
         <v>43557</v>
       </c>
-      <c r="Q187" s="31"/>
+      <c r="Q187" s="31">
+        <v>10</v>
+      </c>
       <c r="R187" s="14"/>
       <c r="S187" s="14"/>
       <c r="T187" s="14" t="s">
@@ -19874,7 +19906,7 @@
       </c>
       <c r="W187" s="33"/>
     </row>
-    <row r="188" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <f t="shared" ref="A188:A191" si="9">1+A187</f>
         <v>186</v>
@@ -19916,7 +19948,9 @@
       <c r="P188" s="21">
         <v>43557</v>
       </c>
-      <c r="Q188" s="31"/>
+      <c r="Q188" s="31">
+        <v>10</v>
+      </c>
       <c r="R188" s="14"/>
       <c r="S188" s="14"/>
       <c r="T188" s="14" t="s">
@@ -19926,7 +19960,7 @@
       <c r="V188" s="32"/>
       <c r="W188" s="33"/>
     </row>
-    <row r="189" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
         <f t="shared" si="9"/>
         <v>187</v>
@@ -19968,7 +20002,9 @@
       <c r="P189" s="21">
         <v>43557</v>
       </c>
-      <c r="Q189" s="31"/>
+      <c r="Q189" s="31">
+        <v>2</v>
+      </c>
       <c r="R189" s="14"/>
       <c r="S189" s="14"/>
       <c r="T189" s="14" t="s">
@@ -19978,7 +20014,7 @@
       <c r="V189" s="32"/>
       <c r="W189" s="33"/>
     </row>
-    <row r="190" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A190" s="5">
         <f t="shared" si="9"/>
         <v>188</v>
@@ -20020,7 +20056,9 @@
       <c r="P190" s="21">
         <v>43557</v>
       </c>
-      <c r="Q190" s="31"/>
+      <c r="Q190" s="31">
+        <v>1</v>
+      </c>
       <c r="R190" s="14"/>
       <c r="S190" s="14"/>
       <c r="T190" s="14" t="s">
@@ -20030,7 +20068,7 @@
       <c r="V190" s="32"/>
       <c r="W190" s="33"/>
     </row>
-    <row r="191" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <f t="shared" si="9"/>
         <v>189</v>
@@ -20072,7 +20110,9 @@
       <c r="P191" s="21">
         <v>43557</v>
       </c>
-      <c r="Q191" s="31"/>
+      <c r="Q191" s="31">
+        <v>10</v>
+      </c>
       <c r="R191" s="14"/>
       <c r="S191" s="14"/>
       <c r="T191" s="14" t="s">
@@ -20082,7 +20122,7 @@
       <c r="V191" s="32"/>
       <c r="W191" s="33"/>
     </row>
-    <row r="192" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="56" x14ac:dyDescent="0.3">
       <c r="A192" s="5">
         <f>1+A191</f>
         <v>190</v>
@@ -20118,7 +20158,9 @@
       <c r="N192" s="32"/>
       <c r="O192" s="32"/>
       <c r="P192" s="32"/>
-      <c r="Q192" s="31"/>
+      <c r="Q192" s="31">
+        <v>1</v>
+      </c>
       <c r="R192" s="14"/>
       <c r="S192" s="14"/>
       <c r="T192" s="14"/>
@@ -20126,7 +20168,7 @@
       <c r="V192" s="32"/>
       <c r="W192" s="33"/>
     </row>
-    <row r="193" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="28" x14ac:dyDescent="0.3">
       <c r="A193" s="5">
         <f t="shared" ref="A193:A206" si="10">1+A192</f>
         <v>191</v>
@@ -20162,7 +20204,9 @@
       <c r="N193" s="32"/>
       <c r="O193" s="32"/>
       <c r="P193" s="32"/>
-      <c r="Q193" s="31"/>
+      <c r="Q193" s="31">
+        <v>1</v>
+      </c>
       <c r="R193" s="14"/>
       <c r="S193" s="14"/>
       <c r="T193" s="14"/>
@@ -20170,7 +20214,7 @@
       <c r="V193" s="32"/>
       <c r="W193" s="33"/>
     </row>
-    <row r="194" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A194" s="5">
         <f t="shared" si="10"/>
         <v>192</v>
@@ -20206,7 +20250,9 @@
       <c r="N194" s="32"/>
       <c r="O194" s="32"/>
       <c r="P194" s="32"/>
-      <c r="Q194" s="31"/>
+      <c r="Q194" s="31">
+        <v>10</v>
+      </c>
       <c r="R194" s="14"/>
       <c r="S194" s="14"/>
       <c r="T194" s="14"/>
@@ -20214,7 +20260,7 @@
       <c r="V194" s="32"/>
       <c r="W194" s="33"/>
     </row>
-    <row r="195" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" ht="70" x14ac:dyDescent="0.3">
       <c r="A195" s="5">
         <f t="shared" si="10"/>
         <v>193</v>
@@ -20250,7 +20296,9 @@
       <c r="N195" s="32"/>
       <c r="O195" s="32"/>
       <c r="P195" s="32"/>
-      <c r="Q195" s="31"/>
+      <c r="Q195" s="31">
+        <v>10</v>
+      </c>
       <c r="R195" s="14"/>
       <c r="S195" s="14"/>
       <c r="T195" s="14"/>
@@ -20258,7 +20306,7 @@
       <c r="V195" s="32"/>
       <c r="W195" s="33"/>
     </row>
-    <row r="196" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A196" s="5">
         <f>1+A195</f>
         <v>194</v>
@@ -20294,7 +20342,9 @@
       <c r="N196" s="32"/>
       <c r="O196" s="32"/>
       <c r="P196" s="32"/>
-      <c r="Q196" s="31"/>
+      <c r="Q196" s="31">
+        <v>5</v>
+      </c>
       <c r="R196" s="14"/>
       <c r="S196" s="14"/>
       <c r="T196" s="14"/>
@@ -20302,7 +20352,7 @@
       <c r="V196" s="32"/>
       <c r="W196" s="33"/>
     </row>
-    <row r="197" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" ht="56" x14ac:dyDescent="0.3">
       <c r="A197" s="5">
         <f t="shared" si="10"/>
         <v>195</v>
@@ -20338,7 +20388,9 @@
       <c r="N197" s="32"/>
       <c r="O197" s="32"/>
       <c r="P197" s="32"/>
-      <c r="Q197" s="31"/>
+      <c r="Q197" s="31">
+        <v>5</v>
+      </c>
       <c r="R197" s="14"/>
       <c r="S197" s="14"/>
       <c r="T197" s="14"/>
@@ -20346,7 +20398,7 @@
       <c r="V197" s="32"/>
       <c r="W197" s="33"/>
     </row>
-    <row r="198" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="28" x14ac:dyDescent="0.3">
       <c r="A198" s="5">
         <f>1+A197</f>
         <v>196</v>
@@ -20382,7 +20434,9 @@
       <c r="N198" s="32"/>
       <c r="O198" s="32"/>
       <c r="P198" s="32"/>
-      <c r="Q198" s="31"/>
+      <c r="Q198" s="31">
+        <v>0</v>
+      </c>
       <c r="R198" s="14"/>
       <c r="S198" s="14"/>
       <c r="T198" s="14"/>
@@ -20390,7 +20444,7 @@
       <c r="V198" s="32"/>
       <c r="W198" s="33"/>
     </row>
-    <row r="199" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A199" s="5">
         <f>1+A198</f>
         <v>197</v>
@@ -20426,7 +20480,9 @@
       <c r="N199" s="32"/>
       <c r="O199" s="32"/>
       <c r="P199" s="32"/>
-      <c r="Q199" s="31"/>
+      <c r="Q199" s="31">
+        <v>3</v>
+      </c>
       <c r="R199" s="14"/>
       <c r="S199" s="14"/>
       <c r="T199" s="14"/>
@@ -20434,7 +20490,7 @@
       <c r="V199" s="32"/>
       <c r="W199" s="33"/>
     </row>
-    <row r="200" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A200" s="5">
         <f>1+A199</f>
         <v>198</v>
@@ -20470,7 +20526,9 @@
       <c r="N200" s="32"/>
       <c r="O200" s="32"/>
       <c r="P200" s="32"/>
-      <c r="Q200" s="31"/>
+      <c r="Q200" s="31">
+        <v>5</v>
+      </c>
       <c r="R200" s="14"/>
       <c r="S200" s="14"/>
       <c r="T200" s="14"/>
@@ -20478,7 +20536,7 @@
       <c r="V200" s="32"/>
       <c r="W200" s="33"/>
     </row>
-    <row r="201" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23" ht="70" x14ac:dyDescent="0.3">
       <c r="A201" s="5">
         <f t="shared" si="10"/>
         <v>199</v>
@@ -20514,7 +20572,9 @@
       <c r="N201" s="32"/>
       <c r="O201" s="32"/>
       <c r="P201" s="32"/>
-      <c r="Q201" s="31"/>
+      <c r="Q201" s="31">
+        <v>3</v>
+      </c>
       <c r="R201" s="14"/>
       <c r="S201" s="14"/>
       <c r="T201" s="14"/>
@@ -20522,7 +20582,7 @@
       <c r="V201" s="32"/>
       <c r="W201" s="33"/>
     </row>
-    <row r="202" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23" ht="84" x14ac:dyDescent="0.3">
       <c r="A202" s="5">
         <f>1+A201</f>
         <v>200</v>
@@ -20558,7 +20618,9 @@
       <c r="N202" s="32"/>
       <c r="O202" s="32"/>
       <c r="P202" s="32"/>
-      <c r="Q202" s="31"/>
+      <c r="Q202" s="31">
+        <v>10</v>
+      </c>
       <c r="R202" s="14"/>
       <c r="S202" s="14"/>
       <c r="T202" s="14"/>
@@ -20566,7 +20628,7 @@
       <c r="V202" s="32"/>
       <c r="W202" s="33"/>
     </row>
-    <row r="203" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23" ht="28" x14ac:dyDescent="0.3">
       <c r="A203" s="5">
         <f t="shared" si="10"/>
         <v>201</v>
@@ -20602,7 +20664,9 @@
       <c r="N203" s="32"/>
       <c r="O203" s="32"/>
       <c r="P203" s="32"/>
-      <c r="Q203" s="31"/>
+      <c r="Q203" s="31">
+        <v>3</v>
+      </c>
       <c r="R203" s="14"/>
       <c r="S203" s="14"/>
       <c r="T203" s="14"/>
@@ -20610,7 +20674,7 @@
       <c r="V203" s="32"/>
       <c r="W203" s="33"/>
     </row>
-    <row r="204" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23" ht="70" x14ac:dyDescent="0.3">
       <c r="A204" s="5">
         <f t="shared" si="10"/>
         <v>202</v>
@@ -20646,7 +20710,9 @@
       <c r="N204" s="32"/>
       <c r="O204" s="32"/>
       <c r="P204" s="32"/>
-      <c r="Q204" s="31"/>
+      <c r="Q204" s="31">
+        <v>5</v>
+      </c>
       <c r="R204" s="14"/>
       <c r="S204" s="14"/>
       <c r="T204" s="14"/>
@@ -20654,7 +20720,7 @@
       <c r="V204" s="32"/>
       <c r="W204" s="33"/>
     </row>
-    <row r="205" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" ht="84" x14ac:dyDescent="0.3">
       <c r="A205" s="5">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -20690,7 +20756,9 @@
       <c r="N205" s="32"/>
       <c r="O205" s="32"/>
       <c r="P205" s="32"/>
-      <c r="Q205" s="31"/>
+      <c r="Q205" s="31">
+        <v>5</v>
+      </c>
       <c r="R205" s="14"/>
       <c r="S205" s="14"/>
       <c r="T205" s="14"/>
@@ -20698,7 +20766,7 @@
       <c r="V205" s="32"/>
       <c r="W205" s="33"/>
     </row>
-    <row r="206" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A206" s="5">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -20734,7 +20802,9 @@
       <c r="N206" s="32"/>
       <c r="O206" s="32"/>
       <c r="P206" s="32"/>
-      <c r="Q206" s="31"/>
+      <c r="Q206" s="31">
+        <v>5</v>
+      </c>
       <c r="R206" s="14"/>
       <c r="S206" s="14"/>
       <c r="T206" s="14"/>
@@ -20742,7 +20812,7 @@
       <c r="V206" s="32"/>
       <c r="W206" s="33"/>
     </row>
-    <row r="207" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:23" ht="42" x14ac:dyDescent="0.3">
       <c r="A207" s="5">
         <v>205</v>
       </c>
@@ -20791,7 +20861,7 @@
       <c r="V207" s="32"/>
       <c r="W207" s="33"/>
     </row>
-    <row r="208" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:23" ht="70" x14ac:dyDescent="0.3">
       <c r="A208" s="5">
         <v>206</v>
       </c>
@@ -20840,7 +20910,7 @@
       <c r="V208" s="32"/>
       <c r="W208" s="33"/>
     </row>
-    <row r="209" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:23" ht="112" x14ac:dyDescent="0.3">
       <c r="A209" s="5">
         <v>207</v>
       </c>
@@ -20927,7 +20997,7 @@
       <c r="O210" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="P210" s="117">
+      <c r="P210" s="112">
         <v>43552</v>
       </c>
       <c r="Q210" s="31"/>
@@ -21037,7 +21107,7 @@
       <c r="O212" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="P212" s="117">
+      <c r="P212" s="112">
         <v>43559</v>
       </c>
       <c r="Q212" s="31"/>
@@ -21092,7 +21162,7 @@
       <c r="O213" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="P213" s="117">
+      <c r="P213" s="112">
         <v>43559</v>
       </c>
       <c r="Q213" s="31"/>
@@ -21231,141 +21301,135 @@
       <c r="W218" s="33"/>
     </row>
     <row r="219" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G219" s="118"/>
+      <c r="G219" s="113"/>
       <c r="H219" s="109"/>
     </row>
     <row r="220" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G220" s="118"/>
+      <c r="G220" s="113"/>
       <c r="H220" s="109"/>
     </row>
     <row r="221" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G221" s="118"/>
+      <c r="G221" s="113"/>
       <c r="H221" s="109"/>
     </row>
     <row r="222" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G222" s="118"/>
+      <c r="G222" s="113"/>
     </row>
     <row r="223" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G223" s="118"/>
+      <c r="G223" s="113"/>
     </row>
     <row r="224" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G224" s="118"/>
+      <c r="G224" s="113"/>
     </row>
     <row r="225" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G225" s="118"/>
+      <c r="G225" s="113"/>
     </row>
     <row r="226" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G226" s="118"/>
+      <c r="G226" s="113"/>
     </row>
     <row r="227" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G227" s="118"/>
+      <c r="G227" s="113"/>
     </row>
     <row r="228" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G228" s="118"/>
+      <c r="G228" s="113"/>
     </row>
     <row r="229" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G229" s="118"/>
+      <c r="G229" s="113"/>
     </row>
     <row r="230" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G230" s="118"/>
+      <c r="G230" s="113"/>
     </row>
     <row r="231" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G231" s="118"/>
+      <c r="G231" s="113"/>
     </row>
     <row r="232" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G232" s="118"/>
+      <c r="G232" s="113"/>
     </row>
     <row r="233" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G233" s="118"/>
+      <c r="G233" s="113"/>
     </row>
     <row r="234" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G234" s="118"/>
+      <c r="G234" s="113"/>
     </row>
     <row r="235" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G235" s="118"/>
+      <c r="G235" s="113"/>
     </row>
     <row r="236" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G236" s="119"/>
+      <c r="G236" s="114"/>
     </row>
     <row r="237" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="G237" s="118"/>
+      <c r="G237" s="113"/>
     </row>
     <row r="238" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G238" s="119"/>
+      <c r="G238" s="114"/>
     </row>
     <row r="239" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G239" s="119"/>
+      <c r="G239" s="114"/>
     </row>
     <row r="240" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G240" s="119"/>
+      <c r="G240" s="114"/>
     </row>
     <row r="241" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G241" s="119"/>
+      <c r="G241" s="114"/>
     </row>
     <row r="242" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G242" s="119"/>
+      <c r="G242" s="114"/>
     </row>
     <row r="243" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G243" s="119"/>
+      <c r="G243" s="114"/>
     </row>
     <row r="244" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G244" s="119"/>
+      <c r="G244" s="114"/>
     </row>
     <row r="245" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G245" s="119"/>
+      <c r="G245" s="114"/>
     </row>
     <row r="246" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G246" s="119"/>
+      <c r="G246" s="114"/>
     </row>
     <row r="247" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G247" s="119"/>
+      <c r="G247" s="114"/>
     </row>
     <row r="248" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G248" s="119"/>
+      <c r="G248" s="114"/>
     </row>
     <row r="249" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G249" s="119"/>
+      <c r="G249" s="114"/>
     </row>
     <row r="250" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G250" s="119"/>
+      <c r="G250" s="114"/>
     </row>
     <row r="251" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G251" s="119"/>
+      <c r="G251" s="114"/>
     </row>
     <row r="252" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G252" s="119"/>
+      <c r="G252" s="114"/>
     </row>
     <row r="253" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G253" s="119"/>
+      <c r="G253" s="114"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:X213" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Registration Processor"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:X213"/>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D132" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
+    <hyperlink ref="D132" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Values!$D$4:$D$6</xm:f>
           </x14:formula1>
@@ -21378,7 +21442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21459,7 +21523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21577,7 +21641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21626,6 +21690,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21797,39 +21893,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21845,28 +21933,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating Feature RoadMap for Gurpreet
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1035497\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mindtree\Projects\MOSIP\IDA\Management\Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$X$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$W$213</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="698">
   <si>
     <t>S.No.</t>
   </si>
@@ -6665,6 +6665,9 @@
   <si>
     <t>UX analysis in progress
 04/04 - VD change in progress, post approval from customer - estimation would be provided</t>
+  </si>
+  <si>
+    <t>Assuming that we have same number of address line items, we will map new attributes with corresponding address attributes in ID Auth</t>
   </si>
 </sst>
 </file>
@@ -8591,7 +8594,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -8940,43 +8943,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:X253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T207" sqref="T207"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V156" sqref="V156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="27" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="32" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="3" customWidth="1"/>
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="24" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="27" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="51.5703125" style="10" customWidth="1"/>
-    <col min="24" max="16384" width="20.42578125" style="10"/>
+    <col min="9" max="9" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="11.1796875" style="3" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="3" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" style="27" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="51.54296875" style="10" customWidth="1"/>
+    <col min="24" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="115" t="s">
         <v>208</v>
       </c>
@@ -9002,7 +9005,7 @@
       <c r="U1" s="117"/>
       <c r="V1" s="119"/>
     </row>
-    <row r="2" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -9073,7 +9076,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -9139,7 +9142,7 @@
       </c>
       <c r="W3" s="106"/>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -9204,7 +9207,7 @@
       </c>
       <c r="W4" s="106"/>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -9270,7 +9273,7 @@
       </c>
       <c r="W5" s="106"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -9336,7 +9339,7 @@
       </c>
       <c r="W6" s="106"/>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -9402,7 +9405,7 @@
       </c>
       <c r="W7" s="106"/>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -9468,7 +9471,7 @@
       </c>
       <c r="W8" s="106"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -9532,7 +9535,7 @@
       </c>
       <c r="W9" s="106"/>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -9596,7 +9599,7 @@
       </c>
       <c r="W10" s="106"/>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -9654,7 +9657,7 @@
       <c r="V11" s="21"/>
       <c r="W11" s="107"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -9713,7 +9716,7 @@
       </c>
       <c r="W12" s="107"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="242.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -9770,7 +9773,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -9834,7 +9837,7 @@
       </c>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -9900,7 +9903,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -9966,7 +9969,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="4" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -10032,7 +10035,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -10096,7 +10099,7 @@
       </c>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -10162,7 +10165,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -10214,7 +10217,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -10266,7 +10269,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -10330,7 +10333,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -10394,7 +10397,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -10460,7 +10463,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -10514,7 +10517,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -10568,7 +10571,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -10632,7 +10635,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -10698,7 +10701,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -10752,7 +10755,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -10812,7 +10815,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -10878,7 +10881,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -10944,7 +10947,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="8" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -11006,7 +11009,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -11072,7 +11075,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -11133,7 +11136,7 @@
       <c r="V35" s="14"/>
       <c r="W35" s="21"/>
     </row>
-    <row r="36" spans="1:23" ht="185.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="182" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -11201,7 +11204,7 @@
       </c>
       <c r="W36" s="21"/>
     </row>
-    <row r="37" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -11271,7 +11274,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="154" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -11339,7 +11342,7 @@
       </c>
       <c r="W38" s="21"/>
     </row>
-    <row r="39" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -11407,7 +11410,7 @@
       </c>
       <c r="W39" s="21"/>
     </row>
-    <row r="40" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -11465,7 +11468,7 @@
       <c r="V40" s="32"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -11527,7 +11530,7 @@
       <c r="V41" s="32"/>
       <c r="W41" s="21"/>
     </row>
-    <row r="42" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -11585,7 +11588,7 @@
       <c r="V42" s="32"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -11647,7 +11650,7 @@
       <c r="V43" s="32"/>
       <c r="W43" s="21"/>
     </row>
-    <row r="44" spans="1:23" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -11711,7 +11714,7 @@
       </c>
       <c r="W44" s="21"/>
     </row>
-    <row r="45" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -11773,7 +11776,7 @@
       </c>
       <c r="W45" s="21"/>
     </row>
-    <row r="46" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -11839,7 +11842,7 @@
       </c>
       <c r="W46" s="21"/>
     </row>
-    <row r="47" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -11905,7 +11908,7 @@
       </c>
       <c r="W47" s="21"/>
     </row>
-    <row r="48" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -11959,7 +11962,7 @@
       <c r="V48" s="32"/>
       <c r="W48" s="21"/>
     </row>
-    <row r="49" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -12025,7 +12028,7 @@
       </c>
       <c r="W49" s="21"/>
     </row>
-    <row r="50" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -12092,7 +12095,7 @@
       </c>
       <c r="W50" s="21"/>
     </row>
-    <row r="51" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -12150,7 +12153,7 @@
       <c r="V51" s="32"/>
       <c r="W51" s="21"/>
     </row>
-    <row r="52" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -12204,7 +12207,7 @@
       <c r="V52" s="32"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -12268,7 +12271,7 @@
       </c>
       <c r="W53" s="21"/>
     </row>
-    <row r="54" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -12322,7 +12325,7 @@
       <c r="V54" s="32"/>
       <c r="W54" s="21"/>
     </row>
-    <row r="55" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -12380,7 +12383,7 @@
       <c r="V55" s="32"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -12443,7 +12446,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -12506,7 +12509,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -12570,7 +12573,7 @@
       </c>
       <c r="W58" s="21"/>
     </row>
-    <row r="59" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -12628,7 +12631,7 @@
       <c r="V59" s="32"/>
       <c r="W59" s="21"/>
     </row>
-    <row r="60" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -12686,7 +12689,7 @@
       <c r="V60" s="32"/>
       <c r="W60" s="21"/>
     </row>
-    <row r="61" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -12747,7 +12750,7 @@
       <c r="V61" s="32"/>
       <c r="W61" s="21"/>
     </row>
-    <row r="62" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -12814,7 +12817,7 @@
       </c>
       <c r="W62" s="21"/>
     </row>
-    <row r="63" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -12879,7 +12882,7 @@
       </c>
       <c r="W63" s="21"/>
     </row>
-    <row r="64" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -12934,7 +12937,7 @@
       <c r="V64" s="32"/>
       <c r="W64" s="21"/>
     </row>
-    <row r="65" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -12989,7 +12992,7 @@
       <c r="V65" s="32"/>
       <c r="W65" s="21"/>
     </row>
-    <row r="66" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="182" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -13056,7 +13059,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -13120,7 +13123,7 @@
       </c>
       <c r="W67" s="21"/>
     </row>
-    <row r="68" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -13185,7 +13188,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -13249,7 +13252,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -13311,7 +13314,7 @@
       <c r="V70" s="32"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -13375,7 +13378,7 @@
       </c>
       <c r="W71" s="21"/>
     </row>
-    <row r="72" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -13441,7 +13444,7 @@
       <c r="W72" s="21"/>
       <c r="X72" s="105"/>
     </row>
-    <row r="73" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -13504,7 +13507,7 @@
       <c r="W73" s="21"/>
       <c r="X73" s="97"/>
     </row>
-    <row r="74" spans="1:24" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -13562,7 +13565,7 @@
       <c r="W74" s="21"/>
       <c r="X74" s="105"/>
     </row>
-    <row r="75" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -13627,7 +13630,7 @@
       </c>
       <c r="W75" s="21"/>
     </row>
-    <row r="76" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -13692,7 +13695,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -13756,7 +13759,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -13821,7 +13824,7 @@
       <c r="W78" s="21"/>
       <c r="X78" s="105"/>
     </row>
-    <row r="79" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -13884,7 +13887,7 @@
       <c r="W79" s="21"/>
       <c r="X79" s="105"/>
     </row>
-    <row r="80" spans="1:24" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -13949,7 +13952,7 @@
       <c r="W80" s="21"/>
       <c r="X80" s="105"/>
     </row>
-    <row r="81" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -14012,7 +14015,7 @@
       <c r="W81" s="21"/>
       <c r="X81" s="105"/>
     </row>
-    <row r="82" spans="1:24" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -14077,7 +14080,7 @@
       <c r="W82" s="21"/>
       <c r="X82" s="105"/>
     </row>
-    <row r="83" spans="1:24" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -14140,7 +14143,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="228" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -14205,7 +14208,7 @@
       <c r="W84" s="21"/>
       <c r="X84" s="105"/>
     </row>
-    <row r="85" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -14271,7 +14274,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -14335,7 +14338,7 @@
       <c r="V86" s="32"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -14398,7 +14401,7 @@
       </c>
       <c r="W87" s="21"/>
     </row>
-    <row r="88" spans="1:24" ht="114" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="112" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -14463,7 +14466,7 @@
       </c>
       <c r="W88" s="21"/>
     </row>
-    <row r="89" spans="1:24" ht="313.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="294" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -14524,7 +14527,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -14577,7 +14580,7 @@
       <c r="V90" s="32"/>
       <c r="W90" s="21"/>
     </row>
-    <row r="91" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -14628,7 +14631,7 @@
       <c r="V91" s="32"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="171" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="168" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -14692,7 +14695,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -14754,7 +14757,7 @@
       <c r="V93" s="32"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -14818,7 +14821,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -14882,7 +14885,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="57" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -14946,7 +14949,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -15008,7 +15011,7 @@
       <c r="V97" s="32"/>
       <c r="W97" s="21"/>
     </row>
-    <row r="98" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -15063,7 +15066,7 @@
       <c r="V98" s="32"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -15125,7 +15128,7 @@
       <c r="V99" s="32"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -15189,7 +15192,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" ht="280" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -15253,7 +15256,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -15315,7 +15318,7 @@
       <c r="V102" s="32"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -15379,7 +15382,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -15443,7 +15446,7 @@
       </c>
       <c r="W104" s="21"/>
     </row>
-    <row r="105" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -15506,7 +15509,7 @@
       <c r="V105" s="33"/>
       <c r="W105" s="21"/>
     </row>
-    <row r="106" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -15569,7 +15572,7 @@
       </c>
       <c r="W106" s="21"/>
     </row>
-    <row r="107" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -15624,7 +15627,7 @@
       <c r="V107" s="32"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -15687,7 +15690,7 @@
       </c>
       <c r="W108" s="21"/>
     </row>
-    <row r="109" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -15746,7 +15749,7 @@
       <c r="V109" s="32"/>
       <c r="W109" s="21"/>
     </row>
-    <row r="110" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>108</v>
       </c>
@@ -15805,7 +15808,7 @@
       <c r="V110" s="32"/>
       <c r="W110" s="21"/>
     </row>
-    <row r="111" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -15866,7 +15869,7 @@
       <c r="V111" s="32"/>
       <c r="W111" s="21"/>
     </row>
-    <row r="112" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -15927,7 +15930,7 @@
       <c r="V112" s="32"/>
       <c r="W112" s="21"/>
     </row>
-    <row r="113" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -15988,7 +15991,7 @@
       <c r="V113" s="32"/>
       <c r="W113" s="21"/>
     </row>
-    <row r="114" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -16049,7 +16052,7 @@
       <c r="V114" s="32"/>
       <c r="W114" s="21"/>
     </row>
-    <row r="115" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -16108,7 +16111,7 @@
       <c r="V115" s="32"/>
       <c r="W115" s="21"/>
     </row>
-    <row r="116" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -16158,7 +16161,7 @@
       <c r="V116" s="32"/>
       <c r="W116" s="21"/>
     </row>
-    <row r="117" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -16210,7 +16213,7 @@
       <c r="V117" s="28"/>
       <c r="W117" s="21"/>
     </row>
-    <row r="118" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -16265,7 +16268,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -16320,7 +16323,7 @@
       <c r="V119" s="32"/>
       <c r="W119" s="21"/>
     </row>
-    <row r="120" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>118</v>
       </c>
@@ -16364,14 +16367,20 @@
         <v>43525</v>
       </c>
       <c r="Q120" s="31"/>
-      <c r="R120" s="14"/>
-      <c r="S120" s="14"/>
-      <c r="T120" s="14"/>
+      <c r="R120" s="14">
+        <v>40</v>
+      </c>
+      <c r="S120" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T120" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U120" s="5"/>
       <c r="V120" s="32"/>
       <c r="W120" s="21"/>
     </row>
-    <row r="121" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>119</v>
       </c>
@@ -16415,16 +16424,22 @@
         <v>43525</v>
       </c>
       <c r="Q121" s="31"/>
-      <c r="R121" s="14"/>
-      <c r="S121" s="14"/>
-      <c r="T121" s="14"/>
+      <c r="R121" s="14">
+        <v>6</v>
+      </c>
+      <c r="S121" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="T121" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U121" s="5"/>
       <c r="V121" s="32" t="s">
         <v>575</v>
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -16471,17 +16486,19 @@
       <c r="R122" s="5">
         <v>30</v>
       </c>
-      <c r="S122" s="5">
-        <v>20</v>
-      </c>
-      <c r="T122" s="33"/>
+      <c r="S122" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="T122" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U122" s="5">
         <v>10</v>
       </c>
       <c r="V122" s="32"/>
       <c r="W122" s="21"/>
     </row>
-    <row r="123" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="5">
         <v>121</v>
       </c>
@@ -16528,17 +16545,17 @@
       <c r="R123" s="5">
         <v>25</v>
       </c>
-      <c r="S123" s="5" t="s">
+      <c r="S123" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T123" s="61" t="s">
-        <v>170</v>
+      <c r="T123" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U123" s="5"/>
       <c r="V123" s="32"/>
       <c r="W123" s="21"/>
     </row>
-    <row r="124" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -16581,15 +16598,13 @@
         <v>43529</v>
       </c>
       <c r="R124" s="5"/>
-      <c r="S124" s="5"/>
-      <c r="T124" s="33" t="s">
-        <v>494</v>
-      </c>
+      <c r="S124" s="14"/>
+      <c r="T124" s="14"/>
       <c r="U124" s="5"/>
       <c r="V124" s="32"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -16635,12 +16650,16 @@
         <v>3</v>
       </c>
       <c r="R125" s="2"/>
-      <c r="S125" s="2"/>
-      <c r="T125" s="33"/>
+      <c r="S125" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T125" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="V125" s="32"/>
       <c r="W125" s="21"/>
     </row>
-    <row r="126" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -16688,9 +16707,11 @@
       <c r="R126" s="5">
         <v>10</v>
       </c>
-      <c r="S126" s="5"/>
-      <c r="T126" s="33" t="s">
-        <v>492</v>
+      <c r="S126" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T126" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U126" s="5"/>
       <c r="V126" s="32" t="s">
@@ -16698,7 +16719,7 @@
       </c>
       <c r="W126" s="21"/>
     </row>
-    <row r="127" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -16742,9 +16763,11 @@
       </c>
       <c r="Q127" s="5"/>
       <c r="R127" s="39"/>
-      <c r="S127" s="87"/>
-      <c r="T127" s="15" t="s">
-        <v>492</v>
+      <c r="S127" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T127" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U127" s="28"/>
       <c r="V127" s="3" t="s">
@@ -16752,7 +16775,7 @@
       </c>
       <c r="W127" s="21"/>
     </row>
-    <row r="128" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -16806,7 +16829,7 @@
       </c>
       <c r="W128" s="21"/>
     </row>
-    <row r="129" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -16860,7 +16883,7 @@
       </c>
       <c r="W129" s="21"/>
     </row>
-    <row r="130" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -16918,7 +16941,7 @@
       </c>
       <c r="W130" s="21"/>
     </row>
-    <row r="131" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -16972,7 +16995,7 @@
       </c>
       <c r="W131" s="21"/>
     </row>
-    <row r="132" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" ht="98" x14ac:dyDescent="0.35">
       <c r="A132" s="5">
         <v>130</v>
       </c>
@@ -17014,10 +17037,14 @@
         <v>43552</v>
       </c>
       <c r="Q132" s="95"/>
-      <c r="R132" s="14"/>
-      <c r="S132" s="32"/>
+      <c r="R132" s="14">
+        <v>40</v>
+      </c>
+      <c r="S132" s="14" t="s">
+        <v>268</v>
+      </c>
       <c r="T132" s="14" t="s">
-        <v>492</v>
+        <v>400</v>
       </c>
       <c r="U132" s="32"/>
       <c r="V132" s="33"/>
@@ -17025,7 +17052,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="5">
         <v>131</v>
       </c>
@@ -17070,17 +17097,17 @@
       <c r="R133" s="5">
         <v>10</v>
       </c>
-      <c r="S133" s="5" t="s">
+      <c r="S133" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T133" s="61" t="s">
-        <v>170</v>
+      <c r="T133" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U133" s="33"/>
       <c r="V133" s="33"/>
       <c r="W133" s="21"/>
     </row>
-    <row r="134" spans="1:23" ht="270.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="266" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="5">
         <v>132</v>
       </c>
@@ -17125,17 +17152,17 @@
       <c r="R134" s="31">
         <v>11</v>
       </c>
-      <c r="S134" s="5" t="s">
+      <c r="S134" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T134" s="61" t="s">
-        <v>170</v>
+      <c r="T134" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U134" s="33"/>
       <c r="V134" s="33"/>
       <c r="W134" s="21"/>
     </row>
-    <row r="135" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="5">
         <v>133</v>
       </c>
@@ -17180,17 +17207,17 @@
       <c r="R135" s="5">
         <v>10</v>
       </c>
-      <c r="S135" s="5" t="s">
+      <c r="S135" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T135" s="61" t="s">
-        <v>170</v>
+      <c r="T135" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U135" s="33"/>
       <c r="V135" s="33"/>
       <c r="W135" s="21"/>
     </row>
-    <row r="136" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="5">
         <v>134</v>
       </c>
@@ -17235,17 +17262,13 @@
       <c r="R136" s="5">
         <v>22</v>
       </c>
-      <c r="S136" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="T136" s="61" t="s">
-        <v>170</v>
-      </c>
+      <c r="S136" s="14"/>
+      <c r="T136" s="14"/>
       <c r="U136" s="33"/>
       <c r="V136" s="33"/>
       <c r="W136" s="21"/>
     </row>
-    <row r="137" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="5">
         <v>135</v>
       </c>
@@ -17290,17 +17313,17 @@
       <c r="R137" s="5">
         <v>9</v>
       </c>
-      <c r="S137" s="5" t="s">
+      <c r="S137" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="T137" s="61" t="s">
-        <v>170</v>
+      <c r="T137" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U137" s="33"/>
       <c r="V137" s="33"/>
       <c r="W137" s="21"/>
     </row>
-    <row r="138" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="5">
         <v>136</v>
       </c>
@@ -17341,15 +17364,17 @@
       </c>
       <c r="Q138" s="10"/>
       <c r="R138" s="33"/>
-      <c r="S138" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="T138" s="33"/>
+      <c r="S138" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T138" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U138" s="33"/>
       <c r="V138" s="33"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" ht="199.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="5">
         <v>137</v>
       </c>
@@ -17390,15 +17415,17 @@
       </c>
       <c r="Q139" s="10"/>
       <c r="R139" s="33"/>
-      <c r="S139" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="T139" s="33"/>
+      <c r="S139" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T139" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U139" s="33"/>
       <c r="V139" s="33"/>
       <c r="W139" s="21"/>
     </row>
-    <row r="140" spans="1:23" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="5">
         <v>138</v>
       </c>
@@ -17453,7 +17480,7 @@
       <c r="V140" s="33"/>
       <c r="W140" s="21"/>
     </row>
-    <row r="141" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -17508,7 +17535,7 @@
       </c>
       <c r="W141" s="21"/>
     </row>
-    <row r="142" spans="1:23" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>140</v>
       </c>
@@ -17563,7 +17590,7 @@
       <c r="V142" s="33"/>
       <c r="W142" s="21"/>
     </row>
-    <row r="143" spans="1:23" ht="114" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="5">
         <v>141</v>
       </c>
@@ -17614,7 +17641,7 @@
       <c r="V143" s="33"/>
       <c r="W143" s="21"/>
     </row>
-    <row r="144" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="5">
         <v>142</v>
       </c>
@@ -17663,7 +17690,7 @@
       <c r="V144" s="33"/>
       <c r="W144" s="21"/>
     </row>
-    <row r="145" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>143</v>
       </c>
@@ -17712,7 +17739,7 @@
       <c r="V145" s="33"/>
       <c r="W145" s="21"/>
     </row>
-    <row r="146" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="5">
         <v>144</v>
       </c>
@@ -17763,7 +17790,7 @@
       <c r="V146" s="33"/>
       <c r="W146" s="21"/>
     </row>
-    <row r="147" spans="1:23" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="5">
         <v>145</v>
       </c>
@@ -17818,7 +17845,7 @@
       <c r="V147" s="33"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -17871,7 +17898,7 @@
       <c r="V148" s="32"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -17924,7 +17951,7 @@
       <c r="V149" s="32"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -17974,7 +18001,7 @@
       <c r="V150" s="32"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -18024,7 +18051,7 @@
       <c r="V151" s="32"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -18077,7 +18104,7 @@
       <c r="V152" s="32"/>
       <c r="W152" s="21"/>
     </row>
-    <row r="153" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A153" s="5">
         <v>151</v>
       </c>
@@ -18119,14 +18146,20 @@
         <v>43550</v>
       </c>
       <c r="Q153" s="33"/>
-      <c r="R153" s="14"/>
-      <c r="S153" s="14"/>
-      <c r="T153" s="14"/>
+      <c r="R153" s="14">
+        <v>8</v>
+      </c>
+      <c r="S153" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T153" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U153" s="5"/>
       <c r="V153" s="32"/>
       <c r="W153" s="21"/>
     </row>
-    <row r="154" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A154" s="5">
         <v>152</v>
       </c>
@@ -18169,13 +18202,17 @@
       </c>
       <c r="Q154" s="33"/>
       <c r="R154" s="14"/>
-      <c r="S154" s="14"/>
-      <c r="T154" s="14"/>
+      <c r="S154" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="T154" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U154" s="5"/>
       <c r="V154" s="32"/>
       <c r="W154" s="21"/>
     </row>
-    <row r="155" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>153</v>
       </c>
@@ -18217,14 +18254,20 @@
         <v>43550</v>
       </c>
       <c r="Q155" s="33"/>
-      <c r="R155" s="14"/>
-      <c r="S155" s="14"/>
-      <c r="T155" s="14"/>
+      <c r="R155" s="14">
+        <v>42</v>
+      </c>
+      <c r="S155" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="T155" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U155" s="5"/>
       <c r="V155" s="32"/>
       <c r="W155" s="21"/>
     </row>
-    <row r="156" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>154</v>
       </c>
@@ -18266,14 +18309,22 @@
         <v>43556</v>
       </c>
       <c r="Q156" s="33"/>
-      <c r="R156" s="14"/>
-      <c r="S156" s="14"/>
-      <c r="T156" s="14"/>
+      <c r="R156" s="14">
+        <v>6</v>
+      </c>
+      <c r="S156" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="T156" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U156" s="5"/>
-      <c r="V156" s="32"/>
+      <c r="V156" s="32" t="s">
+        <v>697</v>
+      </c>
       <c r="W156" s="21"/>
     </row>
-    <row r="157" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>155</v>
       </c>
@@ -18315,14 +18366,20 @@
         <v>43552</v>
       </c>
       <c r="Q157" s="33"/>
-      <c r="R157" s="14"/>
-      <c r="S157" s="14"/>
-      <c r="T157" s="14"/>
+      <c r="R157" s="14">
+        <v>12</v>
+      </c>
+      <c r="S157" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T157" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U157" s="5"/>
       <c r="V157" s="32"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -18368,15 +18425,17 @@
       <c r="R158" s="5">
         <v>10</v>
       </c>
-      <c r="S158" s="5" t="s">
+      <c r="S158" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T158" s="32"/>
+      <c r="T158" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U158" s="5"/>
       <c r="V158" s="32"/>
       <c r="W158" s="33"/>
     </row>
-    <row r="159" spans="1:23" ht="228" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -18422,15 +18481,17 @@
       <c r="R159" s="5">
         <v>9</v>
       </c>
-      <c r="S159" s="5" t="s">
+      <c r="S159" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T159" s="32"/>
+      <c r="T159" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U159" s="5"/>
       <c r="V159" s="32"/>
       <c r="W159" s="33"/>
     </row>
-    <row r="160" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -18471,17 +18532,19 @@
       <c r="R160" s="39">
         <v>12</v>
       </c>
-      <c r="S160" s="39" t="s">
+      <c r="S160" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="T160" s="87"/>
+      <c r="T160" s="14" t="s">
+        <v>400</v>
+      </c>
       <c r="U160" s="39">
         <v>8</v>
       </c>
       <c r="V160" s="28"/>
       <c r="W160" s="33"/>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="5">
         <v>159</v>
       </c>
@@ -18526,17 +18589,15 @@
       <c r="R161" s="5">
         <v>11</v>
       </c>
-      <c r="S161" s="5"/>
-      <c r="T161" s="33" t="s">
-        <v>494</v>
-      </c>
+      <c r="S161" s="14"/>
+      <c r="T161" s="14"/>
       <c r="U161" s="5">
         <v>10</v>
       </c>
       <c r="V161" s="32"/>
       <c r="W161" s="33"/>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="5">
         <v>160</v>
       </c>
@@ -18581,9 +18642,11 @@
       <c r="R162" s="5">
         <v>11</v>
       </c>
-      <c r="S162" s="5"/>
-      <c r="T162" s="33" t="s">
-        <v>494</v>
+      <c r="S162" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T162" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U162" s="5">
         <v>10</v>
@@ -18591,7 +18654,7 @@
       <c r="V162" s="32"/>
       <c r="W162" s="33"/>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>161</v>
       </c>
@@ -18636,9 +18699,11 @@
       <c r="R163" s="5">
         <v>27</v>
       </c>
-      <c r="S163" s="5"/>
-      <c r="T163" s="33" t="s">
-        <v>494</v>
+      <c r="S163" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T163" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U163" s="5">
         <v>10</v>
@@ -18646,7 +18711,7 @@
       <c r="V163" s="32"/>
       <c r="W163" s="33"/>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>162</v>
       </c>
@@ -18691,9 +18756,11 @@
       <c r="R164" s="5">
         <v>11</v>
       </c>
-      <c r="S164" s="5"/>
-      <c r="T164" s="33" t="s">
-        <v>494</v>
+      <c r="S164" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="T164" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="U164" s="5">
         <v>10</v>
@@ -18701,7 +18768,7 @@
       <c r="V164" s="32"/>
       <c r="W164" s="33"/>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>163</v>
       </c>
@@ -18756,7 +18823,7 @@
       <c r="V165" s="32"/>
       <c r="W165" s="33"/>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>164</v>
       </c>
@@ -18811,7 +18878,7 @@
       <c r="V166" s="32"/>
       <c r="W166" s="33"/>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>165</v>
       </c>
@@ -18866,7 +18933,7 @@
       <c r="V167" s="32"/>
       <c r="W167" s="33"/>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>166</v>
       </c>
@@ -18921,7 +18988,7 @@
       <c r="V168" s="32"/>
       <c r="W168" s="33"/>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>167</v>
       </c>
@@ -18976,7 +19043,7 @@
       <c r="V169" s="32"/>
       <c r="W169" s="33"/>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>168</v>
       </c>
@@ -19031,7 +19098,7 @@
       <c r="V170" s="32"/>
       <c r="W170" s="33"/>
     </row>
-    <row r="171" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" s="103" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>169</v>
       </c>
@@ -19078,7 +19145,7 @@
       <c r="V171" s="14"/>
       <c r="W171" s="104"/>
     </row>
-    <row r="172" spans="1:23" s="103" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" s="103" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>170</v>
       </c>
@@ -19133,7 +19200,7 @@
       <c r="V172" s="14"/>
       <c r="W172" s="104"/>
     </row>
-    <row r="173" spans="1:23" s="103" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" s="103" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>171</v>
       </c>
@@ -19182,7 +19249,7 @@
       <c r="V173" s="14"/>
       <c r="W173" s="104"/>
     </row>
-    <row r="174" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>172</v>
       </c>
@@ -19229,7 +19296,7 @@
       <c r="V174" s="14"/>
       <c r="W174" s="33"/>
     </row>
-    <row r="175" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="39">
         <f>1+A174</f>
         <v>173</v>
@@ -19274,7 +19341,7 @@
       <c r="V175" s="28"/>
       <c r="W175" s="38"/>
     </row>
-    <row r="176" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <f t="shared" ref="A176:A185" si="8">1+A175</f>
         <v>174</v>
@@ -19328,7 +19395,7 @@
       <c r="V176" s="32"/>
       <c r="W176" s="33"/>
     </row>
-    <row r="177" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
         <f t="shared" si="8"/>
         <v>175</v>
@@ -19382,7 +19449,7 @@
       <c r="V177" s="32"/>
       <c r="W177" s="33"/>
     </row>
-    <row r="178" spans="1:23" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <f t="shared" si="8"/>
         <v>176</v>
@@ -19436,7 +19503,7 @@
       <c r="V178" s="32"/>
       <c r="W178" s="33"/>
     </row>
-    <row r="179" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <f t="shared" si="8"/>
         <v>177</v>
@@ -19490,7 +19557,7 @@
       <c r="V179" s="32"/>
       <c r="W179" s="33"/>
     </row>
-    <row r="180" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <f t="shared" si="8"/>
         <v>178</v>
@@ -19544,7 +19611,7 @@
       <c r="V180" s="32"/>
       <c r="W180" s="33"/>
     </row>
-    <row r="181" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <f t="shared" si="8"/>
         <v>179</v>
@@ -19598,7 +19665,7 @@
       <c r="V181" s="32"/>
       <c r="W181" s="33"/>
     </row>
-    <row r="182" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <f>1+A181</f>
         <v>180</v>
@@ -19652,7 +19719,7 @@
       <c r="V182" s="32"/>
       <c r="W182" s="33"/>
     </row>
-    <row r="183" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <f t="shared" si="8"/>
         <v>181</v>
@@ -19706,7 +19773,7 @@
       <c r="V183" s="32"/>
       <c r="W183" s="33"/>
     </row>
-    <row r="184" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <f t="shared" si="8"/>
         <v>182</v>
@@ -19760,7 +19827,7 @@
       <c r="V184" s="32"/>
       <c r="W184" s="33"/>
     </row>
-    <row r="185" spans="1:23" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5">
         <f t="shared" si="8"/>
         <v>183</v>
@@ -19814,7 +19881,7 @@
       <c r="V185" s="32"/>
       <c r="W185" s="33"/>
     </row>
-    <row r="186" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <f>1+A185</f>
         <v>184</v>
@@ -19868,7 +19935,7 @@
       <c r="V186" s="32"/>
       <c r="W186" s="33"/>
     </row>
-    <row r="187" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <f>1+A186</f>
         <v>185</v>
@@ -19924,7 +19991,7 @@
       </c>
       <c r="W187" s="33"/>
     </row>
-    <row r="188" spans="1:23" ht="57" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <f t="shared" ref="A188:A191" si="9">1+A187</f>
         <v>186</v>
@@ -19978,7 +20045,7 @@
       <c r="V188" s="32"/>
       <c r="W188" s="33"/>
     </row>
-    <row r="189" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
         <f t="shared" si="9"/>
         <v>187</v>
@@ -20032,7 +20099,7 @@
       <c r="V189" s="32"/>
       <c r="W189" s="33"/>
     </row>
-    <row r="190" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="5">
         <f t="shared" si="9"/>
         <v>188</v>
@@ -20086,7 +20153,7 @@
       <c r="V190" s="32"/>
       <c r="W190" s="33"/>
     </row>
-    <row r="191" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <f t="shared" si="9"/>
         <v>189</v>
@@ -20140,7 +20207,7 @@
       <c r="V191" s="32"/>
       <c r="W191" s="33"/>
     </row>
-    <row r="192" spans="1:23" ht="57" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="5">
         <f>1+A191</f>
         <v>190</v>
@@ -20186,7 +20253,7 @@
       <c r="V192" s="32"/>
       <c r="W192" s="33"/>
     </row>
-    <row r="193" spans="1:23" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="5">
         <f t="shared" ref="A193:A206" si="10">1+A192</f>
         <v>191</v>
@@ -20232,7 +20299,7 @@
       <c r="V193" s="32"/>
       <c r="W193" s="33"/>
     </row>
-    <row r="194" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="5">
         <f t="shared" si="10"/>
         <v>192</v>
@@ -20278,7 +20345,7 @@
       <c r="V194" s="32"/>
       <c r="W194" s="33"/>
     </row>
-    <row r="195" spans="1:23" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5">
         <f t="shared" si="10"/>
         <v>193</v>
@@ -20324,7 +20391,7 @@
       <c r="V195" s="32"/>
       <c r="W195" s="33"/>
     </row>
-    <row r="196" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="5">
         <f>1+A195</f>
         <v>194</v>
@@ -20370,7 +20437,7 @@
       <c r="V196" s="32"/>
       <c r="W196" s="33"/>
     </row>
-    <row r="197" spans="1:23" ht="57" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="5">
         <f t="shared" si="10"/>
         <v>195</v>
@@ -20416,7 +20483,7 @@
       <c r="V197" s="32"/>
       <c r="W197" s="33"/>
     </row>
-    <row r="198" spans="1:23" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="5">
         <f>1+A197</f>
         <v>196</v>
@@ -20462,7 +20529,7 @@
       <c r="V198" s="32"/>
       <c r="W198" s="33"/>
     </row>
-    <row r="199" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="5">
         <f>1+A198</f>
         <v>197</v>
@@ -20508,7 +20575,7 @@
       <c r="V199" s="32"/>
       <c r="W199" s="33"/>
     </row>
-    <row r="200" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="5">
         <f>1+A199</f>
         <v>198</v>
@@ -20554,7 +20621,7 @@
       <c r="V200" s="32"/>
       <c r="W200" s="33"/>
     </row>
-    <row r="201" spans="1:23" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="5">
         <f t="shared" si="10"/>
         <v>199</v>
@@ -20600,7 +20667,7 @@
       <c r="V201" s="32"/>
       <c r="W201" s="33"/>
     </row>
-    <row r="202" spans="1:23" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="5">
         <f>1+A201</f>
         <v>200</v>
@@ -20646,7 +20713,7 @@
       <c r="V202" s="32"/>
       <c r="W202" s="33"/>
     </row>
-    <row r="203" spans="1:23" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="5">
         <f t="shared" si="10"/>
         <v>201</v>
@@ -20692,7 +20759,7 @@
       <c r="V203" s="32"/>
       <c r="W203" s="33"/>
     </row>
-    <row r="204" spans="1:23" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="5">
         <f t="shared" si="10"/>
         <v>202</v>
@@ -20738,7 +20805,7 @@
       <c r="V204" s="32"/>
       <c r="W204" s="33"/>
     </row>
-    <row r="205" spans="1:23" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="5">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -20784,7 +20851,7 @@
       <c r="V205" s="32"/>
       <c r="W205" s="33"/>
     </row>
-    <row r="206" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="5">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -20830,7 +20897,7 @@
       <c r="V206" s="32"/>
       <c r="W206" s="33"/>
     </row>
-    <row r="207" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="5">
         <v>205</v>
       </c>
@@ -20879,7 +20946,7 @@
       <c r="V207" s="32"/>
       <c r="W207" s="33"/>
     </row>
-    <row r="208" spans="1:23" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="5">
         <v>206</v>
       </c>
@@ -20928,7 +20995,7 @@
       <c r="V208" s="32"/>
       <c r="W208" s="33"/>
     </row>
-    <row r="209" spans="1:23" ht="114" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="5">
         <v>207</v>
       </c>
@@ -20977,7 +21044,7 @@
       <c r="V209" s="32"/>
       <c r="W209" s="33"/>
     </row>
-    <row r="210" spans="1:23" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="5">
         <v>208</v>
       </c>
@@ -21032,7 +21099,7 @@
       <c r="V210" s="32"/>
       <c r="W210" s="33"/>
     </row>
-    <row r="211" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" s="5">
         <v>209</v>
       </c>
@@ -21087,7 +21154,7 @@
       <c r="V211" s="32"/>
       <c r="W211" s="33"/>
     </row>
-    <row r="212" spans="1:23" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" s="5">
         <v>210</v>
       </c>
@@ -21142,7 +21209,7 @@
       <c r="V212" s="32"/>
       <c r="W212" s="33"/>
     </row>
-    <row r="213" spans="1:23" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" s="5">
         <v>211</v>
       </c>
@@ -21193,7 +21260,7 @@
       <c r="V213" s="32"/>
       <c r="W213" s="33"/>
     </row>
-    <row r="214" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A214" s="5"/>
       <c r="B214" s="31"/>
       <c r="C214" s="5"/>
@@ -21218,7 +21285,7 @@
       <c r="V214" s="32"/>
       <c r="W214" s="33"/>
     </row>
-    <row r="215" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A215" s="5"/>
       <c r="B215" s="31"/>
       <c r="C215" s="5"/>
@@ -21243,7 +21310,7 @@
       <c r="V215" s="32"/>
       <c r="W215" s="33"/>
     </row>
-    <row r="216" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A216" s="5"/>
       <c r="B216" s="31"/>
       <c r="C216" s="5"/>
@@ -21268,7 +21335,7 @@
       <c r="V216" s="32"/>
       <c r="W216" s="33"/>
     </row>
-    <row r="217" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A217" s="5"/>
       <c r="B217" s="31"/>
       <c r="C217" s="5"/>
@@ -21293,7 +21360,7 @@
       <c r="V217" s="32"/>
       <c r="W217" s="33"/>
     </row>
-    <row r="218" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A218" s="5"/>
       <c r="B218" s="31"/>
       <c r="C218" s="5"/>
@@ -21318,115 +21385,122 @@
       <c r="V218" s="32"/>
       <c r="W218" s="33"/>
     </row>
-    <row r="219" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G219" s="113"/>
       <c r="H219" s="109"/>
     </row>
-    <row r="220" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G220" s="113"/>
       <c r="H220" s="109"/>
     </row>
-    <row r="221" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G221" s="113"/>
       <c r="H221" s="109"/>
     </row>
-    <row r="222" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G222" s="113"/>
     </row>
-    <row r="223" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G223" s="113"/>
     </row>
-    <row r="224" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G224" s="113"/>
     </row>
-    <row r="225" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="225" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G225" s="113"/>
     </row>
-    <row r="226" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="226" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G226" s="113"/>
     </row>
-    <row r="227" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="227" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G227" s="113"/>
     </row>
-    <row r="228" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="228" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G228" s="113"/>
     </row>
-    <row r="229" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="229" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G229" s="113"/>
     </row>
-    <row r="230" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="230" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G230" s="113"/>
     </row>
-    <row r="231" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="231" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G231" s="113"/>
     </row>
-    <row r="232" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="232" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G232" s="113"/>
     </row>
-    <row r="233" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="233" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G233" s="113"/>
     </row>
-    <row r="234" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="234" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G234" s="113"/>
     </row>
-    <row r="235" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="235" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G235" s="113"/>
     </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G236" s="114"/>
     </row>
-    <row r="237" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="237" spans="7:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="G237" s="113"/>
     </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G238" s="114"/>
     </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G239" s="114"/>
     </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G240" s="114"/>
     </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G241" s="114"/>
     </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G242" s="114"/>
     </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G243" s="114"/>
     </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G244" s="114"/>
     </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G245" s="114"/>
     </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G246" s="114"/>
     </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G247" s="114"/>
     </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G248" s="114"/>
     </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G249" s="114"/>
     </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G250" s="114"/>
     </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G251" s="114"/>
     </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G252" s="114"/>
     </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G253" s="114"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:W213">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="ID Authentication"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>
@@ -21466,13 +21540,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
@@ -21480,7 +21554,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
@@ -21488,7 +21562,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
@@ -21496,7 +21570,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
@@ -21504,31 +21578,31 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>584</v>
       </c>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>583</v>
       </c>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>582</v>
       </c>
@@ -21545,14 +21619,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>144</v>
       </c>
@@ -21563,7 +21637,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -21574,7 +21648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
         <v>32</v>
       </c>
@@ -21585,7 +21659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>125</v>
       </c>
@@ -21596,7 +21670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>80</v>
       </c>
@@ -21607,7 +21681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
@@ -21618,7 +21692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>39</v>
       </c>
@@ -21629,7 +21703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>52</v>
       </c>
@@ -21640,7 +21714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>145</v>
       </c>
@@ -21663,12 +21737,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="65" t="s">
         <v>206</v>
       </c>
@@ -21676,25 +21750,25 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67"/>
       <c r="C2" s="68" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69"/>
       <c r="C3" s="68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="70"/>
       <c r="C4" s="68" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71"/>
       <c r="C5" s="72" t="s">
         <v>205</v>
@@ -21707,6 +21781,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21878,15 +21961,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -21911,6 +21985,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21928,26 +22010,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MOS-21370 Updating Feature Road Map with JIRA IDs
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87DAD15-396A-4557-BD36-DDF8E6F98F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -20,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$W$213</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="710">
   <si>
     <t>S.No.</t>
   </si>
@@ -6699,11 +6700,17 @@
   <si>
     <t>1.5</t>
   </si>
+  <si>
+    <t>MOS-22032</t>
+  </si>
+  <si>
+    <t>MOS-22034</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7387,7 +7394,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -7404,7 +7411,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:V70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -8565,7 +8572,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -8913,13 +8920,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:X253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S214" sqref="S214:S219"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -9047,7 +9054,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -9113,7 +9120,7 @@
       </c>
       <c r="W3" s="91"/>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -9178,7 +9185,7 @@
       </c>
       <c r="W4" s="91"/>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -9244,7 +9251,7 @@
       </c>
       <c r="W5" s="91"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -9310,7 +9317,7 @@
       </c>
       <c r="W6" s="91"/>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -9376,7 +9383,7 @@
       </c>
       <c r="W7" s="91"/>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -9442,7 +9449,7 @@
       </c>
       <c r="W8" s="91"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -9506,7 +9513,7 @@
       </c>
       <c r="W9" s="91"/>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -9628,7 +9635,7 @@
       <c r="V11" s="21"/>
       <c r="W11" s="92"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -9744,7 +9751,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -10006,11 +10013,13 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="C18" s="6">
         <v>43397</v>
       </c>
@@ -10240,7 +10249,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -10304,7 +10313,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -10542,7 +10551,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="84" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -10606,7 +10615,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -10980,7 +10989,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" s="8" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -11046,7 +11055,7 @@
       </c>
       <c r="W34" s="21"/>
     </row>
-    <row r="35" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -11439,7 +11448,7 @@
       <c r="V40" s="30"/>
       <c r="W40" s="21"/>
     </row>
-    <row r="41" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -11559,7 +11568,7 @@
       <c r="V42" s="30"/>
       <c r="W42" s="21"/>
     </row>
-    <row r="43" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -11879,11 +11888,13 @@
       </c>
       <c r="W47" s="21"/>
     </row>
-    <row r="48" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>46</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="C48" s="6">
         <v>43427</v>
       </c>
@@ -12178,7 +12189,7 @@
       <c r="V52" s="30"/>
       <c r="W52" s="21"/>
     </row>
-    <row r="53" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -12354,7 +12365,7 @@
       <c r="V55" s="30"/>
       <c r="W55" s="21"/>
     </row>
-    <row r="56" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -12417,7 +12428,7 @@
       </c>
       <c r="W56" s="21"/>
     </row>
-    <row r="57" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -12480,7 +12491,7 @@
       </c>
       <c r="W57" s="21"/>
     </row>
-    <row r="58" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -13030,7 +13041,7 @@
       </c>
       <c r="W66" s="21"/>
     </row>
-    <row r="67" spans="1:24" ht="112" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -13159,7 +13170,7 @@
       </c>
       <c r="W68" s="21"/>
     </row>
-    <row r="69" spans="1:24" ht="252" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -13223,7 +13234,7 @@
       </c>
       <c r="W69" s="21"/>
     </row>
-    <row r="70" spans="1:24" ht="56" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -13285,7 +13296,7 @@
       <c r="V70" s="30"/>
       <c r="W70" s="21"/>
     </row>
-    <row r="71" spans="1:24" ht="126" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -13415,7 +13426,7 @@
       <c r="W72" s="21"/>
       <c r="X72" s="90"/>
     </row>
-    <row r="73" spans="1:24" ht="140" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -13666,7 +13677,7 @@
       </c>
       <c r="W76" s="21"/>
     </row>
-    <row r="77" spans="1:24" ht="196" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:24" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -13730,7 +13741,7 @@
       </c>
       <c r="W77" s="21"/>
     </row>
-    <row r="78" spans="1:24" ht="154" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -13795,7 +13806,7 @@
       <c r="W78" s="21"/>
       <c r="X78" s="90"/>
     </row>
-    <row r="79" spans="1:24" ht="112" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -13858,7 +13869,7 @@
       <c r="W79" s="21"/>
       <c r="X79" s="90"/>
     </row>
-    <row r="80" spans="1:24" ht="126" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -13923,7 +13934,7 @@
       <c r="W80" s="21"/>
       <c r="X80" s="90"/>
     </row>
-    <row r="81" spans="1:24" ht="70" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -13986,7 +13997,7 @@
       <c r="W81" s="21"/>
       <c r="X81" s="90"/>
     </row>
-    <row r="82" spans="1:24" ht="140" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:24" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -14114,7 +14125,7 @@
       </c>
       <c r="W83" s="21"/>
     </row>
-    <row r="84" spans="1:24" ht="210" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:24" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -14179,7 +14190,7 @@
       <c r="W84" s="21"/>
       <c r="X84" s="90"/>
     </row>
-    <row r="85" spans="1:24" ht="70" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -14245,7 +14256,7 @@
       </c>
       <c r="W85" s="21"/>
     </row>
-    <row r="86" spans="1:24" ht="70" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:24" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -14602,7 +14613,7 @@
       <c r="V91" s="30"/>
       <c r="W91" s="21"/>
     </row>
-    <row r="92" spans="1:24" ht="168" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:24" ht="168" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -14666,7 +14677,7 @@
       </c>
       <c r="W92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="42" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:24" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -14728,7 +14739,7 @@
       <c r="V93" s="30"/>
       <c r="W93" s="21"/>
     </row>
-    <row r="94" spans="1:24" ht="56" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -14792,7 +14803,7 @@
       </c>
       <c r="W94" s="21"/>
     </row>
-    <row r="95" spans="1:24" ht="56" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -14856,7 +14867,7 @@
       </c>
       <c r="W95" s="21"/>
     </row>
-    <row r="96" spans="1:24" ht="56" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:24" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -14920,7 +14931,7 @@
       </c>
       <c r="W96" s="21"/>
     </row>
-    <row r="97" spans="1:23" ht="154" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -15037,7 +15048,7 @@
       <c r="V98" s="30"/>
       <c r="W98" s="21"/>
     </row>
-    <row r="99" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -15099,7 +15110,7 @@
       <c r="V99" s="30"/>
       <c r="W99" s="21"/>
     </row>
-    <row r="100" spans="1:23" ht="98" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -15163,7 +15174,7 @@
       </c>
       <c r="W100" s="21"/>
     </row>
-    <row r="101" spans="1:23" ht="280" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" ht="280" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -15227,7 +15238,7 @@
       </c>
       <c r="W101" s="21"/>
     </row>
-    <row r="102" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -15289,7 +15300,7 @@
       <c r="V102" s="30"/>
       <c r="W102" s="21"/>
     </row>
-    <row r="103" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -15353,7 +15364,7 @@
       </c>
       <c r="W103" s="21"/>
     </row>
-    <row r="104" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -15598,7 +15609,7 @@
       <c r="V107" s="30"/>
       <c r="W107" s="21"/>
     </row>
-    <row r="108" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -16241,7 +16252,7 @@
       </c>
       <c r="W118" s="21"/>
     </row>
-    <row r="119" spans="1:23" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -16414,7 +16425,7 @@
       </c>
       <c r="W121" s="21"/>
     </row>
-    <row r="122" spans="1:23" ht="112" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -16582,7 +16593,7 @@
       <c r="V124" s="30"/>
       <c r="W124" s="21"/>
     </row>
-    <row r="125" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -17303,11 +17314,13 @@
       <c r="V137" s="31"/>
       <c r="W137" s="21"/>
     </row>
-    <row r="138" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A138" s="5">
         <v>136</v>
       </c>
-      <c r="B138" s="29"/>
+      <c r="B138" s="29" t="s">
+        <v>708</v>
+      </c>
       <c r="C138" s="6">
         <v>43552</v>
       </c>
@@ -17354,11 +17367,13 @@
       <c r="V138" s="31"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" ht="196" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" ht="196" x14ac:dyDescent="0.35">
       <c r="A139" s="5">
         <v>137</v>
       </c>
-      <c r="B139" s="29"/>
+      <c r="B139" s="29" t="s">
+        <v>709</v>
+      </c>
       <c r="C139" s="6">
         <v>43552</v>
       </c>
@@ -17460,7 +17475,7 @@
       <c r="V140" s="31"/>
       <c r="W140" s="21"/>
     </row>
-    <row r="141" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -17825,7 +17840,7 @@
       <c r="V147" s="31"/>
       <c r="W147" s="21"/>
     </row>
-    <row r="148" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="5">
         <v>146</v>
       </c>
@@ -17881,7 +17896,7 @@
       <c r="V148" s="30"/>
       <c r="W148" s="21"/>
     </row>
-    <row r="149" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>147</v>
       </c>
@@ -17937,7 +17952,7 @@
       <c r="V149" s="30"/>
       <c r="W149" s="21"/>
     </row>
-    <row r="150" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="5">
         <v>148</v>
       </c>
@@ -17990,7 +18005,7 @@
       <c r="V150" s="30"/>
       <c r="W150" s="21"/>
     </row>
-    <row r="151" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="5">
         <v>149</v>
       </c>
@@ -18044,7 +18059,7 @@
       <c r="V151" s="30"/>
       <c r="W151" s="21"/>
     </row>
-    <row r="152" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>150</v>
       </c>
@@ -18375,7 +18390,7 @@
       <c r="V157" s="30"/>
       <c r="W157" s="21"/>
     </row>
-    <row r="158" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="5">
         <v>156</v>
       </c>
@@ -18431,7 +18446,7 @@
       <c r="V158" s="30"/>
       <c r="W158" s="31"/>
     </row>
-    <row r="159" spans="1:23" ht="210" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>157</v>
       </c>
@@ -18487,7 +18502,7 @@
       <c r="V159" s="30"/>
       <c r="W159" s="31"/>
     </row>
-    <row r="160" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>158</v>
       </c>
@@ -19296,7 +19311,7 @@
       <c r="V174" s="14"/>
       <c r="W174" s="31"/>
     </row>
-    <row r="175" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="37">
         <f>1+A174</f>
         <v>173</v>
@@ -19345,7 +19360,7 @@
       <c r="V175" s="27"/>
       <c r="W175" s="36"/>
     </row>
-    <row r="176" spans="1:23" ht="56" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="5">
         <f t="shared" ref="A176:A185" si="8">1+A175</f>
         <v>174</v>
@@ -19403,7 +19418,7 @@
       <c r="V176" s="30"/>
       <c r="W176" s="31"/>
     </row>
-    <row r="177" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="5">
         <f t="shared" si="8"/>
         <v>175</v>
@@ -19461,7 +19476,7 @@
       <c r="V177" s="30"/>
       <c r="W177" s="31"/>
     </row>
-    <row r="178" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <f t="shared" si="8"/>
         <v>176</v>
@@ -19519,7 +19534,7 @@
       <c r="V178" s="30"/>
       <c r="W178" s="31"/>
     </row>
-    <row r="179" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <f t="shared" si="8"/>
         <v>177</v>
@@ -19577,7 +19592,7 @@
       <c r="V179" s="30"/>
       <c r="W179" s="31"/>
     </row>
-    <row r="180" spans="1:23" ht="28" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <f t="shared" si="8"/>
         <v>178</v>
@@ -19635,7 +19650,7 @@
       <c r="V180" s="30"/>
       <c r="W180" s="31"/>
     </row>
-    <row r="181" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <f t="shared" si="8"/>
         <v>179</v>
@@ -19693,7 +19708,7 @@
       <c r="V181" s="30"/>
       <c r="W181" s="31"/>
     </row>
-    <row r="182" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <f>1+A181</f>
         <v>180</v>
@@ -19751,7 +19766,7 @@
       <c r="V182" s="30"/>
       <c r="W182" s="31"/>
     </row>
-    <row r="183" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="5">
         <f t="shared" si="8"/>
         <v>181</v>
@@ -19809,7 +19824,7 @@
       <c r="V183" s="30"/>
       <c r="W183" s="31"/>
     </row>
-    <row r="184" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="5">
         <f t="shared" si="8"/>
         <v>182</v>
@@ -19867,7 +19882,7 @@
       <c r="V184" s="30"/>
       <c r="W184" s="31"/>
     </row>
-    <row r="185" spans="1:23" ht="70" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5">
         <f t="shared" si="8"/>
         <v>183</v>
@@ -19925,7 +19940,7 @@
       <c r="V185" s="30"/>
       <c r="W185" s="31"/>
     </row>
-    <row r="186" spans="1:23" ht="126" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <f>1+A185</f>
         <v>184</v>
@@ -19983,7 +19998,7 @@
       <c r="V186" s="30"/>
       <c r="W186" s="31"/>
     </row>
-    <row r="187" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <f>1+A186</f>
         <v>185</v>
@@ -20043,7 +20058,7 @@
       </c>
       <c r="W187" s="31"/>
     </row>
-    <row r="188" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <f t="shared" ref="A188:A191" si="9">1+A187</f>
         <v>186</v>
@@ -20101,7 +20116,7 @@
       <c r="V188" s="30"/>
       <c r="W188" s="31"/>
     </row>
-    <row r="189" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
         <f t="shared" si="9"/>
         <v>187</v>
@@ -20159,7 +20174,7 @@
       <c r="V189" s="30"/>
       <c r="W189" s="31"/>
     </row>
-    <row r="190" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="5">
         <f t="shared" si="9"/>
         <v>188</v>
@@ -20217,7 +20232,7 @@
       <c r="V190" s="30"/>
       <c r="W190" s="31"/>
     </row>
-    <row r="191" spans="1:23" ht="42" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="5">
         <f t="shared" si="9"/>
         <v>189</v>
@@ -20275,7 +20290,7 @@
       <c r="V191" s="30"/>
       <c r="W191" s="31"/>
     </row>
-    <row r="192" spans="1:23" ht="56" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="5">
         <f>1+A191</f>
         <v>190</v>
@@ -20325,7 +20340,7 @@
       <c r="V192" s="30"/>
       <c r="W192" s="31"/>
     </row>
-    <row r="193" spans="1:23" ht="28" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="5">
         <f t="shared" ref="A193:A206" si="10">1+A192</f>
         <v>191</v>
@@ -20375,7 +20390,7 @@
       <c r="V193" s="30"/>
       <c r="W193" s="31"/>
     </row>
-    <row r="194" spans="1:23" ht="42" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="5">
         <f t="shared" si="10"/>
         <v>192</v>
@@ -20425,7 +20440,7 @@
       <c r="V194" s="30"/>
       <c r="W194" s="31"/>
     </row>
-    <row r="195" spans="1:23" ht="70" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5">
         <f t="shared" si="10"/>
         <v>193</v>
@@ -20475,7 +20490,7 @@
       <c r="V195" s="30"/>
       <c r="W195" s="31"/>
     </row>
-    <row r="196" spans="1:23" ht="42" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="5">
         <f>1+A195</f>
         <v>194</v>
@@ -20525,7 +20540,7 @@
       <c r="V196" s="30"/>
       <c r="W196" s="31"/>
     </row>
-    <row r="197" spans="1:23" ht="56" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="5">
         <f t="shared" si="10"/>
         <v>195</v>
@@ -20575,7 +20590,7 @@
       <c r="V197" s="30"/>
       <c r="W197" s="31"/>
     </row>
-    <row r="198" spans="1:23" ht="28" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="5">
         <f>1+A197</f>
         <v>196</v>
@@ -20625,7 +20640,7 @@
       <c r="V198" s="30"/>
       <c r="W198" s="31"/>
     </row>
-    <row r="199" spans="1:23" ht="42" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="5">
         <f>1+A198</f>
         <v>197</v>
@@ -20675,7 +20690,7 @@
       <c r="V199" s="30"/>
       <c r="W199" s="31"/>
     </row>
-    <row r="200" spans="1:23" ht="42" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="5">
         <f>1+A199</f>
         <v>198</v>
@@ -20725,7 +20740,7 @@
       <c r="V200" s="30"/>
       <c r="W200" s="31"/>
     </row>
-    <row r="201" spans="1:23" ht="70" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="5">
         <f t="shared" si="10"/>
         <v>199</v>
@@ -20775,7 +20790,7 @@
       <c r="V201" s="30"/>
       <c r="W201" s="31"/>
     </row>
-    <row r="202" spans="1:23" ht="84" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="5">
         <f>1+A201</f>
         <v>200</v>
@@ -20825,7 +20840,7 @@
       <c r="V202" s="30"/>
       <c r="W202" s="31"/>
     </row>
-    <row r="203" spans="1:23" ht="28" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23" ht="28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="5">
         <f t="shared" si="10"/>
         <v>201</v>
@@ -20875,7 +20890,7 @@
       <c r="V203" s="30"/>
       <c r="W203" s="31"/>
     </row>
-    <row r="204" spans="1:23" ht="70" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="5">
         <f t="shared" si="10"/>
         <v>202</v>
@@ -20925,7 +20940,7 @@
       <c r="V204" s="30"/>
       <c r="W204" s="31"/>
     </row>
-    <row r="205" spans="1:23" ht="84" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="5">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -20975,7 +20990,7 @@
       <c r="V205" s="30"/>
       <c r="W205" s="31"/>
     </row>
-    <row r="206" spans="1:23" ht="42" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="5">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -21622,10 +21637,15 @@
       <c r="G253" s="99"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W213">
+  <autoFilter ref="A2:W213" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters blank="1">
+        <filter val="NA"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="Registration Client"/>
+        <filter val="Registration Processor"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
@@ -21638,22 +21658,22 @@
     <mergeCell ref="A1:V1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100"/>
-    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516"/>
-    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302"/>
-    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303"/>
-    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304"/>
-    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306"/>
-    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308"/>
-    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783"/>
-    <hyperlink ref="D132" r:id="rId9"/>
+    <hyperlink ref="B125" r:id="rId1" display="https://mosipid.atlassian.net/browse/MOS-18100" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B126" r:id="rId2" display="https://mosipid.atlassian.net/browse/MOS-20516" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B127" r:id="rId3" display="https://mosipid.atlassian.net/browse/MOS-20302" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B128" r:id="rId4" display="https://mosipid.atlassian.net/browse/MOS-20303" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B129" r:id="rId5" display="https://mosipid.atlassian.net/browse/MOS-20304" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B130" r:id="rId6" display="https://mosipid.atlassian.net/browse/MOS-20306" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B131" r:id="rId7" display="https://mosipid.atlassian.net/browse/MOS-20308" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B132" r:id="rId8" display="https://mosipid.atlassian.net/browse/MOS-20783" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D132" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Values!$D$4:$D$6</xm:f>
           </x14:formula1>
@@ -21666,7 +21686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21747,7 +21767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21865,7 +21885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21914,6 +21934,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22085,39 +22137,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22133,28 +22177,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added 1 new CR
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
+++ b/docs/requirements/MOSIP_FeaturesRoadmap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1037145\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{92DC5969-260F-4CE1-86CE-4452CA520CA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_Feature_Roadmap" sheetId="5" r:id="rId1"/>
@@ -19,9 +18,9 @@
     <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$W$215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_Feature_Roadmap!$A$2:$W$222</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="742">
   <si>
     <t>S.No.</t>
   </si>
@@ -6804,11 +6803,23 @@
   <si>
     <t>Redesign Internal API to accomodate biometric authentication request for a Supervisor/Operator for RegClient/Reg Processor - retrieve UIN for RID</t>
   </si>
+  <si>
+    <t>MOS-22397</t>
+  </si>
+  <si>
+    <t>As the MOSIP Registration Client, I should enforce security-related rules for first time login and sync</t>
+  </si>
+  <si>
+    <t>FIT 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review with Sasi </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7492,7 +7503,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -7509,7 +7520,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:V70" sheet="MOSIP_Feature_Roadmap"/>
   </cacheSource>
@@ -8670,7 +8681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -9018,44 +9029,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:XFD253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D223" sqref="D223"/>
+      <pane ySplit="2" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D224" sqref="D224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="14" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="26" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="32" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="3" customWidth="1"/>
     <col min="8" max="8" width="60" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="16" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="16" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="38.453125" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="24" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="11.140625" style="3" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" style="3" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="26" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="83.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="51.5703125" style="10" customWidth="1"/>
-    <col min="24" max="16384" width="20.42578125" style="10"/>
+    <col min="17" max="17" width="22.1796875" style="26" customWidth="1"/>
+    <col min="18" max="18" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.81640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="22.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="83.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="51.54296875" style="10" customWidth="1"/>
+    <col min="24" max="16384" width="20.453125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="100" t="s">
         <v>208</v>
       </c>
@@ -9081,7 +9092,7 @@
       <c r="U1" s="102"/>
       <c r="V1" s="104"/>
     </row>
-    <row r="2" spans="1:23" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -9152,7 +9163,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -9218,7 +9229,7 @@
       </c>
       <c r="W3" s="91"/>
     </row>
-    <row r="4" spans="1:23" s="4" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -9283,7 +9294,7 @@
       </c>
       <c r="W4" s="91"/>
     </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -9349,7 +9360,7 @@
       </c>
       <c r="W5" s="91"/>
     </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -9415,7 +9426,7 @@
       </c>
       <c r="W6" s="91"/>
     </row>
-    <row r="7" spans="1:23" s="4" customFormat="1" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -9481,7 +9492,7 @@
       </c>
       <c r="W7" s="91"/>
     </row>
-    <row r="8" spans="1:23" s="4" customFormat="1" ht="171" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="140" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -9547,7 +9558,7 @@
       </c>
       <c r="W8" s="91"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -9611,7 +9622,7 @@
       </c>
       <c r="W9" s="91"/>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -9675,7 +9686,7 @@
       </c>
       <c r="W10" s="91"/>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -9733,7 +9744,7 @@
       <c r="V11" s="21"/>
       <c r="W11" s="92"/>
     </row>
-    <row r="12" spans="1:23" s="1" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -9792,7 +9803,7 @@
       </c>
       <c r="W12" s="92"/>
     </row>
-    <row r="13" spans="1:23" s="1" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" s="1" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -9849,7 +9860,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="1" customFormat="1" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -9913,7 +9924,7 @@
       </c>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -9979,7 +9990,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" s="1" customFormat="1" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" s="1" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -10045,7 +10056,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" s="4" customFormat="1" ht="185.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="4" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -10111,7 +10122,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -10177,7 +10188,7 @@
       </c>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="4" customFormat="1" ht="128.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="4" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -10243,7 +10254,7 @@
       </c>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -10295,7 +10306,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="4" customFormat="1" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -10347,7 +10358,7 @@
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -10411,7 +10422,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -10475,7 +10486,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="114" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -10541,7 +10552,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -10595,7 +10606,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -10649,7 +10660,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -10713,7 +10724,7 @@
       </c>
       <c r="W27" s="21"/>
     </row>
-    <row r="28" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="70" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -10779,7 +10790,7 @@
       </c>
       <c r="W28" s="21"/>
     </row>
-    <row r="29" spans="1:23" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -10833,7 +10844,7 @@
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
     </row>
-    <row r="30" spans="1:23" ht="71.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -10893,7 +10904,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -10959,7 +10970,7 @@
       </c>
       <c r="W31" s="21"/>
     </row>
-    <row r="32" spans="1:23" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -11025,7 +11036,7 @@
       </c>
       <c r="W32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1